<commit_message>
[feat][System][Clean Architecture, DDD, Kafka]
</commit_message>
<xml_diff>
--- a/System/Documents.xlsx
+++ b/System/Documents.xlsx
@@ -1,32 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WorkSpace\my-work-space\My-Documents\System\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9967B7F4-2F2B-4D89-A342-07E8B660A6A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" firstSheet="1" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView windowWidth="28695" windowHeight="13530" firstSheet="10" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" state="hidden" r:id="rId1"/>
-    <sheet name="1. DataBase" sheetId="23" r:id="rId2"/>
-    <sheet name="2.Cache" sheetId="11" r:id="rId3"/>
-    <sheet name="3.Architechture" sheetId="22" r:id="rId4"/>
-    <sheet name="4.Microservice" sheetId="3" r:id="rId5"/>
-    <sheet name="Load Balancing" sheetId="24" r:id="rId6"/>
-    <sheet name="API Gateway" sheetId="25" r:id="rId7"/>
+    <sheet name="2.Cache" sheetId="11" r:id="rId2"/>
+    <sheet name="3.Architechture" sheetId="22" r:id="rId3"/>
+    <sheet name="4.Microservice" sheetId="3" r:id="rId4"/>
+    <sheet name="Load Balancing" sheetId="24" r:id="rId5"/>
+    <sheet name="API Gateway" sheetId="25" r:id="rId6"/>
+    <sheet name="Hexagonal Architecture" sheetId="26" r:id="rId7"/>
+    <sheet name="Clean Architecture" sheetId="27" r:id="rId8"/>
+    <sheet name="Onion Architecture" sheetId="28" r:id="rId9"/>
+    <sheet name="Domain Driven Design" sheetId="29" r:id="rId10"/>
+    <sheet name="DesignPattern - SOLID - KISS" sheetId="30" r:id="rId11"/>
+    <sheet name="Event Driven Architecture" sheetId="32" r:id="rId12"/>
+    <sheet name="Saga Pattern" sheetId="33" r:id="rId13"/>
+    <sheet name="Outbox Pattern" sheetId="34" r:id="rId14"/>
+    <sheet name="CQRS" sheetId="35" r:id="rId15"/>
+    <sheet name="KAFKA" sheetId="36" r:id="rId16"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="193" uniqueCount="193">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="211">
   <si>
     <t>Kiến Trúc về Microservice</t>
   </si>
@@ -2482,18 +2485,6 @@
     <t>FallBack Techniques</t>
   </si>
   <si>
-    <t>Service-Level Load balancing</t>
-  </si>
-  <si>
-    <t>Network-Level Load balancing</t>
-  </si>
-  <si>
-    <t>Global Load balancing</t>
-  </si>
-  <si>
-    <t>Cross-Domain Load Balancing</t>
-  </si>
-  <si>
     <t>Load Balancing</t>
   </si>
   <si>
@@ -2511,13 +2502,14 @@
     <t>DNS Load Balacing</t>
   </si>
   <si>
-    <t>Application Level (HTTP/HTTPS)</t>
-  </si>
-  <si>
-    <t>Database Load Balancing</t>
-  </si>
-  <si>
-    <r>
+    <r>
+      <rPr>
+        <sz val="14"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve"> - DNS (Domain Name System) load balancing is a technique used to distribute network and application traffic across many servers or data centers, </t>
     </r>
     <r>
@@ -2526,7 +2518,7 @@
         <sz val="14"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>by leveraging DNS respond mechanism</t>
@@ -2536,7 +2528,7 @@
         <sz val="14"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">.
@@ -2549,7 +2541,7 @@
         <sz val="14"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>DNS server then responds with the IP address of one of the available servers that host the content or application</t>
@@ -2559,7 +2551,7 @@
         <sz val="14"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t xml:space="preserve">.
@@ -2571,7 +2563,7 @@
         <sz val="14"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>DNS Load Balancing is not aware of the server's health or capacity, that's why it is commonly used in combination with other methods at transport or application level to ensure effective load balancing</t>
@@ -2581,18 +2573,21 @@
         <sz val="14"/>
         <color theme="1"/>
         <rFont val="Calibri"/>
-        <family val="2"/>
+        <charset val="134"/>
         <scheme val="minor"/>
       </rPr>
       <t>.</t>
     </r>
+  </si>
+  <si>
+    <t>https://www.nginx.com/resources/glossary/dns-load-balancing/</t>
+  </si>
+  <si>
+    <t>Global Load balancing</t>
   </si>
   <si>
     <t xml:space="preserve"> - Global Server Load Balancing (GSLB) is a method used to distribute traffic across multiple servers or data centers that are geographically dispersed. Unlike traditional load balancing, which distributes traffic among servers within a single data center, GSLB enables traffic distribution among servers in different locations around the world.
 - A GSLB solution uses DNS and ensures that when a user or device makes a request for a service, that request is served by the "best" available site. What constitutes the "best" site can be driven by a range of factors like geographic proximity, the performance of a site, or even the cost of service from a particular data center.</t>
-  </si>
-  <si>
-    <t>https://www.nginx.com/resources/glossary/dns-load-balancing/</t>
   </si>
   <si>
     <t>Transport Level (TCP/UDP) 
@@ -2600,15 +2595,238 @@
 (Layer 4 load balancing)</t>
   </si>
   <si>
+    <t>Application Level (HTTP/HTTPS)</t>
+  </si>
+  <si>
+    <t>Database Load Balancing</t>
+  </si>
+  <si>
+    <t>Service-Level Load balancing</t>
+  </si>
+  <si>
+    <t>Network-Level Load balancing</t>
+  </si>
+  <si>
     <t xml:space="preserve"> - A network load balancer is a load balancer that distributes traffic across multiple local and wide area networks 
 so that large volumes of user requests are handled in a manner that maximizes performance and reliability</t>
+  </si>
+  <si>
+    <t>Cross-Domain Load Balancing</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Separation of concerns by dividing the software into different layers
+ - Use Dependency Inversion (DI) and Polymorphism to create a denependency rule to make the domain layer most independent and stable layer
+ - Source code dependencies can only </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>point inward</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(hướng vào trong), </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>towards</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(hướng tới) to domain layer
+ - Testable domain layer without requiring and external element
+ - Define Entities and Use Cases for domain logic
+ - Same high level principle with hexagonal and onion architectures: Isolate the domain.</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Domain model: Conceptual model of the domain that defines the behaviour and data of system.
+ - The main idea is to sperate the business model from infrastructure.
+ - Domain-Driven Design offers solutions to common problem when building enterprise software.
+ - Both Hexagonal architecture and Domain-Driven design put domain logic in center of the software make it independent out side the world.
+ - Domain Logic: In the center of the software. Independent from other dependencies.
+ - Separating domain logic and infrastructure make the software easier to design, develop, test, build and maintance over time. Help you change the infrastructure components and adapt new technology easily</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">Two side of Domain-Driven Design: 
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Stategic DDD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Introduces boundaries for domain model. Single Bounded context per each domain
+ + What is a Domain? Operational area of your application. eg: Online food ordering.
+ + </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Bounded Context</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Central pattern in DDD. Boundary within a Domain.
+ + 1 Domain can have 1 or more sub domains depends on domain logic.
+ + Ubiquitous Language: Common language used by domain experts and developers. System can be designed, developed, and evolved with well communicated enviroment.
+ </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Tatical DDD</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: Implementation patterns.
+ + Entities: Core Domain object with a unique identity. Embodies set of critical business rules.
+ + Aggregates: Group of Entity objects which always need to be in consistent state.
+ + Aggragates Root (AR): Entry point Entity for an aggragate. All business operations should go through root. An Aggregate should referenced from outside through its root only. AR should have pure, side-effect free functions. So Aggregates owned by Aggregates Root.
+ + Value Objects: Immutable objects without identify. Only value matters. Brings context to value. Brings context, allow business operations inside the object &amp; allow validation in constructor.
+ + Domain Events: Decouple different domains. Describe things that happen and change the state of a domain. Makes the system extendable. Domain event listeners runs in a different transaction than the event publishers In Domain-driven system, domain events  are ab excellent way of achieving eventual consistency. Any system of module that needs to update itself when something happens in another module or system can subscribe to the domain events coming from that system
+ + Eventual(cuối cùng) Consistency: All reads of the system will eventual return the lastest value, provided that no new updates are made.
+ + Domain Services: Business logic that cannot fit in the aggregate. Used when multiple aggregates required in business logic Can interact with other domain services. A domain service coordinates the business logic spans multiple aggreagtes, can put business logic methods into business service if the methods does not fit logically into entities. Domain service can communicate with other domain services if necessary.
+ + Application Services: Allows the isolated domain to communicate with outside. Orchestrate transaction, security, looking up proper aggregates and saving state changes of the domain to the database. Does not contain any business logic. Domain event listeners are special kind of Application services that is triggered by domain events. Each domain event listener can have a sperate doamin service to handle business logic.
+</t>
+    </r>
+  </si>
+  <si>
+    <t>Singleton</t>
+  </si>
+  <si>
+    <t>Hiểu được ý nghĩa, implementation</t>
+  </si>
+  <si>
+    <t>https://java-design-patterns.com/patterns/</t>
+  </si>
+  <si>
+    <t>Builder</t>
+  </si>
+  <si>
+    <t>Factory</t>
+  </si>
+  <si>
+    <t>Adapter</t>
+  </si>
+  <si>
+    <t>CQRS</t>
+  </si>
+  <si>
+    <t>Dependency Injection</t>
+  </si>
+  <si>
+    <t>Nguyên lý SOLID</t>
+  </si>
+  <si>
+    <t>Materialized view pattern</t>
+  </si>
+  <si>
+    <t>Strategy design pattern</t>
+  </si>
+  <si>
+    <t>Creator Design Pattern</t>
+  </si>
+  <si>
+    <t>ObserverPartern</t>
+  </si>
+  <si>
+    <t>Factory Design Pattern</t>
+  </si>
+  <si>
+    <t>Abstract Factory Design Pattern</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="20">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="36">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2617,10 +2835,36 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2661,13 +2905,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -2698,18 +2935,140 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color theme="10"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF000000"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <i/>
@@ -2736,35 +3095,25 @@
       <name val="Calibri"/>
       <charset val="134"/>
     </font>
-    <font>
-      <sz val="18"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="14"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="4">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9EAD3"/>
+        <bgColor rgb="FFD9EAD3"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor rgb="FFFFFFFF"/>
+      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -2778,8 +3127,182 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -2787,146 +3310,468 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF000000"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="32" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="16" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="48" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="3" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="48" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="33" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="23" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="48" applyFont="1"/>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="33" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" quotePrefix="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="3" quotePrefix="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="48" applyFont="1" applyAlignment="1" quotePrefix="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="2" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="4">
-    <cellStyle name="Bad" xfId="1" builtinId="27"/>
-    <cellStyle name="Good" xfId="2" builtinId="26"/>
-    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="60% - Accent6" xfId="1" builtinId="52"/>
+    <cellStyle name="40% - Accent6" xfId="2" builtinId="51"/>
+    <cellStyle name="60% - Accent5" xfId="3" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="4" builtinId="49"/>
+    <cellStyle name="40% - Accent5" xfId="5" builtinId="47"/>
+    <cellStyle name="20% - Accent5" xfId="6" builtinId="46"/>
+    <cellStyle name="60% - Accent4" xfId="7" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="8" builtinId="45"/>
+    <cellStyle name="40% - Accent4" xfId="9" builtinId="43"/>
+    <cellStyle name="Accent4" xfId="10" builtinId="41"/>
+    <cellStyle name="Linked Cell" xfId="11" builtinId="24"/>
+    <cellStyle name="40% - Accent3" xfId="12" builtinId="39"/>
+    <cellStyle name="60% - Accent2" xfId="13" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="14" builtinId="37"/>
+    <cellStyle name="40% - Accent2" xfId="15" builtinId="35"/>
+    <cellStyle name="20% - Accent2" xfId="16" builtinId="34"/>
+    <cellStyle name="Accent2" xfId="17" builtinId="33"/>
+    <cellStyle name="40% - Accent1" xfId="18" builtinId="31"/>
+    <cellStyle name="20% - Accent1" xfId="19" builtinId="30"/>
+    <cellStyle name="Accent1" xfId="20" builtinId="29"/>
+    <cellStyle name="Neutral" xfId="21" builtinId="28"/>
+    <cellStyle name="60% - Accent1" xfId="22" builtinId="32"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="20% - Accent4" xfId="24" builtinId="42"/>
+    <cellStyle name="Total" xfId="25" builtinId="25"/>
+    <cellStyle name="Output" xfId="26" builtinId="21"/>
+    <cellStyle name="Currency" xfId="27" builtinId="4"/>
+    <cellStyle name="20% - Accent3" xfId="28" builtinId="38"/>
+    <cellStyle name="Note" xfId="29" builtinId="10"/>
+    <cellStyle name="Input" xfId="30" builtinId="20"/>
+    <cellStyle name="Heading 4" xfId="31" builtinId="19"/>
+    <cellStyle name="Calculation" xfId="32" builtinId="22"/>
+    <cellStyle name="Good" xfId="33" builtinId="26"/>
+    <cellStyle name="Heading 3" xfId="34" builtinId="18"/>
+    <cellStyle name="CExplanatory Text" xfId="35" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="36" builtinId="16"/>
+    <cellStyle name="Comma [0]" xfId="37" builtinId="6"/>
+    <cellStyle name="20% - Accent6" xfId="38" builtinId="50"/>
+    <cellStyle name="Title" xfId="39" builtinId="15"/>
+    <cellStyle name="Currency [0]" xfId="40" builtinId="7"/>
+    <cellStyle name="Warning Text" xfId="41" builtinId="11"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9"/>
+    <cellStyle name="Heading 2" xfId="43" builtinId="17"/>
+    <cellStyle name="Comma" xfId="44" builtinId="3"/>
+    <cellStyle name="Check Cell" xfId="45" builtinId="23"/>
+    <cellStyle name="60% - Accent3" xfId="46" builtinId="40"/>
+    <cellStyle name="Percent" xfId="47" builtinId="5"/>
+    <cellStyle name="Hyperlink" xfId="48" builtinId="8"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>3</xdr:col>
@@ -2942,19 +3787,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Ảnh 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="3" name="Ảnh 2"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -2986,19 +3825,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="4" name="Ảnh 3">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="4" name="Ảnh 3"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:blip r:embed="rId2"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3030,19 +3863,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="5" name="Ảnh 4">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000005000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="5" name="Ảnh 4"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:blip r:embed="rId3"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3063,7 +3890,7 @@
 </file>
 
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>4</xdr:col>
@@ -3079,19 +3906,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="2" name="Picture 1">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000002000000}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
       </xdr:nvPicPr>
       <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:blip r:embed="rId1"/>
         <a:stretch>
           <a:fillRect/>
         </a:stretch>
@@ -3363,778 +4184,995 @@
     </a:fmtScheme>
   </a:themeElements>
   <a:objectDefaults/>
-  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView topLeftCell="B9" workbookViewId="0">
       <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="12.75" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="9.140625" style="19"/>
-    <col min="2" max="2" width="39.5703125" style="19" customWidth="1"/>
-    <col min="3" max="3" width="95.5703125" style="19" customWidth="1"/>
-    <col min="4" max="4" width="60.7109375" style="19" customWidth="1"/>
-    <col min="5" max="5" width="58.85546875" style="19" customWidth="1"/>
-    <col min="6" max="6" width="50" style="19" customWidth="1"/>
-    <col min="7" max="7" width="49.7109375" style="19" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="19"/>
+    <col min="1" max="1" width="9.14" style="37"/>
+    <col min="2" max="2" width="39.5733333333333" style="37" customWidth="1"/>
+    <col min="3" max="3" width="95.5733333333333" style="37" customWidth="1"/>
+    <col min="4" max="4" width="60.7133333333333" style="37" customWidth="1"/>
+    <col min="5" max="5" width="58.8533333333333" style="37" customWidth="1"/>
+    <col min="6" max="6" width="50" style="37" customWidth="1"/>
+    <col min="7" max="7" width="49.7133333333333" style="37" customWidth="1"/>
+    <col min="8" max="16384" width="9.14" style="37"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="90">
-      <c r="A1" s="19">
+    <row r="1" ht="76.5" spans="1:3">
+      <c r="A1" s="37">
         <v>1</v>
       </c>
-      <c r="B1" s="19" t="s">
+      <c r="B1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="41" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="75">
-      <c r="A2" s="19">
+    <row r="2" ht="63.75" spans="1:3">
+      <c r="A2" s="37">
         <v>2</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="23" t="s">
+      <c r="C2" s="41" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:7" ht="45">
-      <c r="A3" s="19">
+    <row r="3" ht="38.25" spans="1:3">
+      <c r="A3" s="37">
         <v>3</v>
       </c>
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="23" t="s">
+      <c r="C3" s="41" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="45">
-      <c r="A4" s="19">
+    <row r="4" ht="38.25" spans="1:3">
+      <c r="A4" s="37">
         <v>4</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="37" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="42" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:7" ht="240">
-      <c r="A5" s="19">
+    <row r="5" ht="178.5" spans="1:3">
+      <c r="A5" s="37">
         <v>5</v>
       </c>
-      <c r="B5" s="19" t="s">
+      <c r="B5" s="37" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="1" t="s">
+      <c r="C5" s="15" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="6" spans="1:7" ht="30">
-      <c r="A6" s="19">
+    <row r="6" ht="25.5" spans="1:3">
+      <c r="A6" s="37">
         <v>6</v>
       </c>
-      <c r="B6" s="19" t="s">
+      <c r="B6" s="37" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="42" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="300">
-      <c r="A7" s="19">
+    <row r="7" ht="229.5" spans="1:3">
+      <c r="A7" s="37">
         <v>7</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="38" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="245.25" customHeight="1">
-      <c r="A8" s="19">
+    <row r="8" ht="245.25" customHeight="1" spans="1:3">
+      <c r="A8" s="37">
         <v>8</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="37" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="C8" s="38" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:7" ht="223.5" customHeight="1">
-      <c r="A9" s="19">
+    <row r="9" ht="223.5" customHeight="1" spans="1:3">
+      <c r="A9" s="37">
         <v>9</v>
       </c>
-      <c r="B9" s="19" t="s">
+      <c r="B9" s="37" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="23" t="s">
+      <c r="C9" s="41" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="10" spans="1:7" ht="300">
-      <c r="A10" s="19">
+    <row r="10" ht="204" spans="1:4">
+      <c r="A10" s="37">
         <v>10</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="B10" s="37" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="1" t="s">
+      <c r="C10" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="22" t="s">
+      <c r="D10" s="40" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:7" ht="30">
-      <c r="B11" s="19" t="s">
+    <row r="11" ht="25.5" spans="2:3">
+      <c r="B11" s="37" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:7" ht="150">
-      <c r="B12" s="19" t="s">
+    <row r="12" ht="102" spans="2:3">
+      <c r="B12" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="15" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:7" ht="180">
-      <c r="B13" s="19" t="s">
+    <row r="13" ht="140.25" spans="2:3">
+      <c r="B13" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="15" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="14" spans="1:7" ht="288.75" customHeight="1">
-      <c r="B14" s="19" t="s">
+    <row r="14" ht="288.75" customHeight="1" spans="2:7">
+      <c r="B14" s="37" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="1" t="s">
+      <c r="C14" s="15" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="20" t="s">
+      <c r="D14" s="38" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="1" t="s">
+      <c r="E14" s="15" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="F14" s="15" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="1" t="s">
+      <c r="G14" s="15" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="15" spans="1:7" ht="60">
-      <c r="B15" s="19" t="s">
+    <row r="15" ht="38.25" spans="2:3">
+      <c r="B15" s="37" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="C15" s="15" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="1:7" ht="240.75" customHeight="1">
-      <c r="B16" s="19" t="s">
+    <row r="16" ht="240.75" customHeight="1" spans="2:2">
+      <c r="B16" s="37" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="17" spans="2:3" ht="180">
-      <c r="B17" s="19" t="s">
+    <row r="17" ht="153" spans="2:3">
+      <c r="B17" s="37" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="20" t="s">
+      <c r="C17" s="38" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="2:3" ht="180">
-      <c r="B18" s="19" t="s">
+    <row r="18" ht="153" spans="2:3">
+      <c r="B18" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="20" t="s">
+      <c r="C18" s="38" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D10" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
+    <hyperlink ref="D10" r:id="rId2" display="https://topdev.vn/blog/trien-khai-ci-cd-voi-gitlab/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId2"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="D1:D2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="3"/>
+  <cols>
+    <col min="4" max="4" width="151.9" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="89.25" spans="4:4">
+      <c r="D1" s="7" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="2" ht="350" customHeight="1" spans="4:4">
+      <c r="D2" s="8" t="s">
+        <v>195</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:C19"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D46" sqref="D46"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
+  <cols>
+    <col min="1" max="1" width="27.2866666666667" customWidth="1"/>
+    <col min="2" max="2" width="23.4266666666667" customWidth="1"/>
+    <col min="3" max="3" width="45.4266666666667" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2" s="4" t="s">
+        <v>199</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="4"/>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="B3" s="5"/>
+      <c r="C3" s="1"/>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" s="4" t="s">
+        <v>201</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="4"/>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="1"/>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" s="4" t="s">
+        <v>203</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="4"/>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="1"/>
+    </row>
+    <row r="8" customFormat="1"/>
+    <row r="9" customFormat="1"/>
+    <row r="10" customFormat="1"/>
+    <row r="11" customFormat="1"/>
+    <row r="12" customFormat="1" spans="1:2">
+      <c r="A12" t="s">
+        <v>202</v>
+      </c>
+      <c r="B12" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="13" customFormat="1"/>
+    <row r="14" customFormat="1"/>
+    <row r="15" customFormat="1" spans="1:1">
+      <c r="A15" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="16" customFormat="1" spans="1:1">
+      <c r="A16" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="17" customFormat="1" spans="1:1">
+      <c r="A17" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="18" customFormat="1" spans="1:1">
+      <c r="A18" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="19" customFormat="1" spans="1:1">
+      <c r="A19" t="s">
+        <v>210</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:B7"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="C1" r:id="rId1" display="https://java-design-patterns.com/patterns/"/>
+  </hyperlinks>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H29" sqref="H29"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P20" sqref="P20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H28" sqref="H28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:B47"/>
   <sheetViews>
     <sheetView topLeftCell="A40" workbookViewId="0">
       <selection activeCell="B61" sqref="B61"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="38.140625" customWidth="1"/>
-    <col min="2" max="2" width="110.85546875" customWidth="1"/>
+    <col min="1" max="1" width="38.14" customWidth="1"/>
+    <col min="2" max="2" width="110.853333333333" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="105">
-      <c r="A1" s="26" t="s">
+    <row r="1" ht="89.25" spans="1:2">
+      <c r="A1" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="7" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="105">
-      <c r="A2" s="26"/>
-      <c r="B2" s="16" t="s">
+    <row r="2" ht="89.25" spans="1:2">
+      <c r="A2" s="30"/>
+      <c r="B2" s="31" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="135">
-      <c r="A3" s="26"/>
-      <c r="B3" s="15" t="s">
+    <row r="3" ht="102" spans="1:2">
+      <c r="A3" s="30"/>
+      <c r="B3" s="7" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="90">
-      <c r="A4" s="26" t="s">
+    <row r="4" ht="63.75" spans="1:2">
+      <c r="A4" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="15" t="s">
+      <c r="B4" s="7" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="75">
-      <c r="A5" s="26"/>
-      <c r="B5" s="16" t="s">
+    <row r="5" ht="63.75" spans="1:2">
+      <c r="A5" s="30"/>
+      <c r="B5" s="31" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="26"/>
-      <c r="B6" s="16" t="s">
+      <c r="A6" s="30"/>
+      <c r="B6" s="31" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="7" spans="1:2" ht="60">
-      <c r="A7" s="26" t="s">
+    <row r="7" ht="38.25" spans="1:2">
+      <c r="A7" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="16" t="s">
+      <c r="B7" s="31" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="8" spans="1:2" ht="45">
-      <c r="A8" s="26"/>
-      <c r="B8" s="16" t="s">
+    <row r="8" ht="38.25" spans="1:2">
+      <c r="A8" s="30"/>
+      <c r="B8" s="31" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="26"/>
-      <c r="B9" s="16" t="s">
+      <c r="A9" s="30"/>
+      <c r="B9" s="31" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="26"/>
-      <c r="B10" s="16" t="s">
+      <c r="A10" s="30"/>
+      <c r="B10" s="31" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="26"/>
-      <c r="B11" s="16" t="s">
+      <c r="A11" s="30"/>
+      <c r="B11" s="31" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="12" spans="1:2" ht="60">
-      <c r="A12" s="26" t="s">
+    <row r="12" ht="51" spans="1:2">
+      <c r="A12" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="31" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:2" ht="90">
-      <c r="A13" s="26"/>
-      <c r="B13" s="16" t="s">
+    <row r="13" ht="63.75" spans="1:2">
+      <c r="A13" s="30"/>
+      <c r="B13" s="31" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:2" ht="165">
-      <c r="A14" s="26"/>
-      <c r="B14" s="16" t="s">
+    <row r="14" ht="127.5" spans="1:2">
+      <c r="A14" s="30"/>
+      <c r="B14" s="31" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="26"/>
-      <c r="B15" s="16" t="s">
+      <c r="A15" s="30"/>
+      <c r="B15" s="31" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="26"/>
-      <c r="B16" s="16" t="s">
+      <c r="A16" s="30"/>
+      <c r="B16" s="31" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="120">
-      <c r="A17" s="26"/>
-      <c r="B17" s="16" t="s">
+    <row r="17" ht="102" spans="1:2">
+      <c r="A17" s="30"/>
+      <c r="B17" s="31" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="60">
-      <c r="A18" s="26"/>
-      <c r="B18" s="16" t="s">
+    <row r="18" ht="38.25" spans="1:2">
+      <c r="A18" s="30"/>
+      <c r="B18" s="31" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="26"/>
-      <c r="B19" s="16" t="s">
+      <c r="A19" s="30"/>
+      <c r="B19" s="31" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="26"/>
-      <c r="B20" s="17" t="s">
+      <c r="A20" s="30"/>
+      <c r="B20" s="32" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="21" spans="1:2" ht="195">
-      <c r="A21" s="27" t="s">
+    <row r="21" ht="165.75" spans="1:2">
+      <c r="A21" s="33" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="16" t="s">
+      <c r="B21" s="31" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:2" ht="300">
-      <c r="A22" s="27"/>
-      <c r="B22" s="16" t="s">
+    <row r="22" ht="242.25" spans="1:2">
+      <c r="A22" s="33"/>
+      <c r="B22" s="31" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="23" spans="1:2" ht="195">
-      <c r="A23" s="27"/>
-      <c r="B23" s="16" t="s">
+    <row r="23" ht="153" spans="1:2">
+      <c r="A23" s="33"/>
+      <c r="B23" s="31" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="24" spans="1:2" ht="45">
-      <c r="A24" s="27"/>
-      <c r="B24" s="16" t="s">
+    <row r="24" ht="38.25" spans="1:2">
+      <c r="A24" s="33"/>
+      <c r="B24" s="31" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="25" spans="1:2" ht="45">
-      <c r="A25" s="27"/>
-      <c r="B25" s="16" t="s">
+    <row r="25" ht="25.5" spans="1:2">
+      <c r="A25" s="33"/>
+      <c r="B25" s="31" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="26" spans="1:2" ht="75">
-      <c r="A26" s="27"/>
-      <c r="B26" s="16" t="s">
+    <row r="26" ht="51" spans="1:2">
+      <c r="A26" s="33"/>
+      <c r="B26" s="31" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="27"/>
-      <c r="B27" s="16" t="s">
+      <c r="A27" s="33"/>
+      <c r="B27" s="31" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="27"/>
-      <c r="B28" s="17" t="s">
+      <c r="A28" s="33"/>
+      <c r="B28" s="32" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="29" spans="1:2" ht="45">
-      <c r="A29" s="28" t="s">
+    <row r="29" ht="38.25" spans="1:2">
+      <c r="A29" s="34" t="s">
         <v>73</v>
       </c>
-      <c r="B29" s="16" t="s">
+      <c r="B29" s="31" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="26"/>
-      <c r="B30" s="16" t="s">
+      <c r="A30" s="30"/>
+      <c r="B30" s="31" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="26"/>
-      <c r="B31" s="16" t="s">
+      <c r="A31" s="30"/>
+      <c r="B31" s="31" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="26"/>
-      <c r="B32" s="16" t="s">
+      <c r="A32" s="30"/>
+      <c r="B32" s="31" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="26"/>
-      <c r="B33" s="16" t="s">
+      <c r="A33" s="30"/>
+      <c r="B33" s="31" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="75">
-      <c r="A34" s="27" t="s">
+    <row r="34" ht="51" spans="1:2">
+      <c r="A34" s="33" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="35" spans="1:2" ht="60">
-      <c r="A35" s="26"/>
-      <c r="B35" s="15" t="s">
+    <row r="35" ht="38.25" spans="1:2">
+      <c r="A35" s="30"/>
+      <c r="B35" s="7" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="36" spans="1:2" ht="75">
-      <c r="A36" s="26"/>
-      <c r="B36" s="15" t="s">
+    <row r="36" ht="51" spans="1:2">
+      <c r="A36" s="30"/>
+      <c r="B36" s="7" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="1:2" ht="75">
-      <c r="A37" s="26"/>
-      <c r="B37" s="15" t="s">
+    <row r="37" ht="51" spans="1:2">
+      <c r="A37" s="30"/>
+      <c r="B37" s="7" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="38" spans="1:2" ht="45">
-      <c r="A38" s="26" t="s">
+    <row r="38" ht="25.5" spans="1:2">
+      <c r="A38" s="30" t="s">
         <v>84</v>
       </c>
-      <c r="B38" s="15" t="s">
+      <c r="B38" s="7" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="39" spans="1:2" ht="90">
-      <c r="A39" s="26"/>
-      <c r="B39" s="15" t="s">
+    <row r="39" ht="76.5" spans="1:2">
+      <c r="A39" s="30"/>
+      <c r="B39" s="7" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="40" spans="1:2" ht="30">
-      <c r="A40" s="26"/>
-      <c r="B40" s="15" t="s">
+    <row r="40" ht="25.5" spans="1:2">
+      <c r="A40" s="30"/>
+      <c r="B40" s="7" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="41" spans="1:2" ht="30">
-      <c r="A41" s="26"/>
-      <c r="B41" s="15" t="s">
+    <row r="41" ht="25.5" spans="1:2">
+      <c r="A41" s="30"/>
+      <c r="B41" s="7" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="26"/>
-      <c r="B42" s="15" t="s">
+      <c r="A42" s="30"/>
+      <c r="B42" s="7" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="43" spans="1:2" ht="30">
-      <c r="A43" s="26"/>
-      <c r="B43" s="15" t="s">
+    <row r="43" ht="25.5" spans="1:2">
+      <c r="A43" s="30"/>
+      <c r="B43" s="7" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="14"/>
-      <c r="B44" s="15"/>
-    </row>
-    <row r="45" spans="1:2" ht="26.25" customHeight="1">
-      <c r="A45" s="29" t="s">
+      <c r="A44" s="30"/>
+      <c r="B44" s="7"/>
+    </row>
+    <row r="45" ht="26.25" customHeight="1" spans="1:2">
+      <c r="A45" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="B45" s="29"/>
+      <c r="B45" s="35"/>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="29"/>
-      <c r="B46" s="29"/>
-    </row>
-    <row r="47" spans="1:2" ht="60">
-      <c r="A47" s="14" t="s">
+      <c r="A46" s="35"/>
+      <c r="B46" s="35"/>
+    </row>
+    <row r="47" ht="51" spans="1:2">
+      <c r="A47" s="30" t="s">
         <v>92</v>
       </c>
-      <c r="B47" s="18" t="s">
+      <c r="B47" s="36" t="s">
         <v>93</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="9">
-    <mergeCell ref="A29:A33"/>
-    <mergeCell ref="A34:A37"/>
-    <mergeCell ref="A38:A43"/>
-    <mergeCell ref="A45:B46"/>
     <mergeCell ref="A1:A3"/>
     <mergeCell ref="A4:A6"/>
     <mergeCell ref="A7:A11"/>
     <mergeCell ref="A12:A20"/>
     <mergeCell ref="A21:A28"/>
+    <mergeCell ref="A29:A33"/>
+    <mergeCell ref="A34:A37"/>
+    <mergeCell ref="A38:A43"/>
+    <mergeCell ref="A45:B46"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="B47" r:id="rId1" display="https://developer.redis.com/develop/java/redis-and-spring-course/lesson_9_x000a_https://www.bezkoder.com/spring-boot-redis-cache-example/_x000a_https://faun.pub/redis-master-slave-configuration-and-tested-in-spring-boot-3a68e7314b90_x000a_https://www.vinsguru.com/category/redis/" xr:uid="{00000000-0004-0000-0200-000000000000}"/>
+    <hyperlink ref="B47" r:id="rId2" display="https://developer.redis.com/develop/java/redis-and-spring-course/lesson_9&#10;https://www.bezkoder.com/spring-boot-redis-cache-example/&#10;https://faun.pub/redis-master-slave-configuration-and-tested-in-spring-boot-3a68e7314b90&#10;https://www.vinsguru.com/category/redis/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <drawing r:id="rId2"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C40"/>
   <sheetViews>
     <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="B35" sqref="B35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="26.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="55.85546875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="54.140625" style="7" customWidth="1"/>
-    <col min="3" max="3" width="101.7109375" style="8" customWidth="1"/>
+    <col min="1" max="1" width="55.8533333333333" style="22" customWidth="1"/>
+    <col min="2" max="2" width="54.14" style="23" customWidth="1"/>
+    <col min="3" max="3" width="101.713333333333" style="24" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="18.75">
-      <c r="A1" s="30" t="s">
+    <row r="1" ht="12.75" spans="1:1">
+      <c r="A1" s="25" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="15">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31"/>
-      <c r="C2" s="11"/>
-    </row>
-    <row r="3" spans="1:3" ht="15">
-      <c r="A3" s="30"/>
-      <c r="B3" s="31"/>
-    </row>
-    <row r="4" spans="1:3" ht="15">
-      <c r="A4" s="30"/>
-      <c r="B4" s="31"/>
-    </row>
-    <row r="5" spans="1:3" ht="15">
-      <c r="A5" s="30"/>
-      <c r="B5" s="31"/>
-    </row>
-    <row r="6" spans="1:3" ht="15">
-      <c r="A6" s="30"/>
-      <c r="B6" s="31"/>
-    </row>
-    <row r="7" spans="1:3" ht="15">
-      <c r="A7" s="30"/>
-      <c r="B7" s="31"/>
-    </row>
-    <row r="8" spans="1:3" ht="15">
-      <c r="A8" s="30"/>
-      <c r="B8" s="31"/>
-    </row>
-    <row r="9" spans="1:3" ht="15">
-      <c r="A9" s="30"/>
-      <c r="B9" s="31"/>
-    </row>
-    <row r="10" spans="1:3" ht="15">
-      <c r="A10" s="30"/>
-      <c r="B10" s="31"/>
-    </row>
-    <row r="11" spans="1:3" ht="15">
-      <c r="A11" s="30"/>
-      <c r="B11" s="31"/>
-    </row>
-    <row r="12" spans="1:3" ht="15">
-      <c r="A12" s="30"/>
-      <c r="B12" s="31"/>
-    </row>
-    <row r="13" spans="1:3" ht="15">
-      <c r="A13" s="30"/>
-      <c r="B13" s="31"/>
-    </row>
-    <row r="14" spans="1:3" ht="15">
-      <c r="A14" s="30"/>
-      <c r="B14" s="31"/>
-    </row>
-    <row r="15" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A15" s="30"/>
-      <c r="B15" s="31"/>
-    </row>
-    <row r="16" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A16" s="30"/>
-      <c r="B16" s="31"/>
-    </row>
-    <row r="17" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A17" s="30"/>
-      <c r="B17" s="31"/>
-    </row>
-    <row r="18" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A18" s="30"/>
-      <c r="B18" s="31"/>
-    </row>
-    <row r="19" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A19" s="30"/>
-      <c r="B19" s="31"/>
-    </row>
-    <row r="20" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A20" s="30"/>
-      <c r="B20" s="31"/>
-    </row>
-    <row r="21" spans="1:3" ht="18.75" customHeight="1">
-      <c r="A21" s="30"/>
-      <c r="B21" s="31"/>
-    </row>
-    <row r="22" spans="1:3" ht="18.75">
-      <c r="A22" s="30"/>
-      <c r="B22" s="10"/>
-    </row>
-    <row r="23" spans="1:3" ht="18.75">
-      <c r="A23" s="30"/>
-      <c r="B23" s="10"/>
-    </row>
-    <row r="24" spans="1:3" ht="18.75">
-      <c r="A24" s="30"/>
-      <c r="B24" s="12"/>
-    </row>
-    <row r="26" spans="1:3" ht="18.75">
-      <c r="A26" s="30" t="s">
+    <row r="2" ht="12.75" spans="1:3">
+      <c r="A2" s="25"/>
+      <c r="B2" s="26"/>
+      <c r="C2" s="27"/>
+    </row>
+    <row r="3" ht="12.75" spans="1:2">
+      <c r="A3" s="25"/>
+      <c r="B3" s="26"/>
+    </row>
+    <row r="4" ht="12.75" spans="1:2">
+      <c r="A4" s="25"/>
+      <c r="B4" s="26"/>
+    </row>
+    <row r="5" ht="12.75" spans="1:2">
+      <c r="A5" s="25"/>
+      <c r="B5" s="26"/>
+    </row>
+    <row r="6" ht="12.75" spans="1:2">
+      <c r="A6" s="25"/>
+      <c r="B6" s="26"/>
+    </row>
+    <row r="7" ht="12.75" spans="1:2">
+      <c r="A7" s="25"/>
+      <c r="B7" s="26"/>
+    </row>
+    <row r="8" ht="12.75" spans="1:2">
+      <c r="A8" s="25"/>
+      <c r="B8" s="26"/>
+    </row>
+    <row r="9" ht="12.75" spans="1:2">
+      <c r="A9" s="25"/>
+      <c r="B9" s="26"/>
+    </row>
+    <row r="10" ht="12.75" spans="1:2">
+      <c r="A10" s="25"/>
+      <c r="B10" s="26"/>
+    </row>
+    <row r="11" ht="12.75" spans="1:2">
+      <c r="A11" s="25"/>
+      <c r="B11" s="26"/>
+    </row>
+    <row r="12" ht="12.75" spans="1:2">
+      <c r="A12" s="25"/>
+      <c r="B12" s="26"/>
+    </row>
+    <row r="13" ht="12.75" spans="1:2">
+      <c r="A13" s="25"/>
+      <c r="B13" s="26"/>
+    </row>
+    <row r="14" ht="12.75" spans="1:2">
+      <c r="A14" s="25"/>
+      <c r="B14" s="26"/>
+    </row>
+    <row r="15" ht="18.75" customHeight="1" spans="1:2">
+      <c r="A15" s="25"/>
+      <c r="B15" s="26"/>
+    </row>
+    <row r="16" ht="18.75" customHeight="1" spans="1:2">
+      <c r="A16" s="25"/>
+      <c r="B16" s="26"/>
+    </row>
+    <row r="17" ht="18.75" customHeight="1" spans="1:2">
+      <c r="A17" s="25"/>
+      <c r="B17" s="26"/>
+    </row>
+    <row r="18" ht="18.75" customHeight="1" spans="1:2">
+      <c r="A18" s="25"/>
+      <c r="B18" s="26"/>
+    </row>
+    <row r="19" ht="18.75" customHeight="1" spans="1:2">
+      <c r="A19" s="25"/>
+      <c r="B19" s="26"/>
+    </row>
+    <row r="20" ht="18.75" customHeight="1" spans="1:2">
+      <c r="A20" s="25"/>
+      <c r="B20" s="26"/>
+    </row>
+    <row r="21" ht="18.75" customHeight="1" spans="1:2">
+      <c r="A21" s="25"/>
+      <c r="B21" s="26"/>
+    </row>
+    <row r="22" ht="17.25" spans="1:2">
+      <c r="A22" s="25"/>
+      <c r="B22" s="26"/>
+    </row>
+    <row r="23" ht="17.25" spans="1:2">
+      <c r="A23" s="25"/>
+      <c r="B23" s="26"/>
+    </row>
+    <row r="24" ht="17.25" spans="1:2">
+      <c r="A24" s="25"/>
+      <c r="B24" s="28"/>
+    </row>
+    <row r="26" ht="17.25" spans="1:2">
+      <c r="A26" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="B26" s="7" t="s">
+      <c r="B26" s="23" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="18.75">
-      <c r="A27" s="30"/>
-      <c r="B27" s="7" t="s">
+    <row r="27" ht="17.25" spans="1:2">
+      <c r="A27" s="25"/>
+      <c r="B27" s="23" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="28" spans="1:3" ht="18.75">
-      <c r="A28" s="30"/>
-      <c r="B28" s="7" t="s">
+    <row r="28" ht="17.25" spans="1:2">
+      <c r="A28" s="25"/>
+      <c r="B28" s="23" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
-      <c r="A29" s="9"/>
-    </row>
-    <row r="30" spans="1:3" ht="15">
-      <c r="A30" s="30" t="s">
+    <row r="29" spans="1:1">
+      <c r="A29" s="25"/>
+    </row>
+    <row r="30" ht="12.75" spans="1:3">
+      <c r="A30" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="B30" s="32" t="s">
+      <c r="B30" s="23" t="s">
         <v>100</v>
       </c>
-      <c r="C30" s="8" t="s">
+      <c r="C30" s="24" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="31" spans="1:3" ht="15">
-      <c r="A31" s="30"/>
-      <c r="B31" s="32"/>
-      <c r="C31" s="8" t="s">
+    <row r="31" ht="12.75" spans="1:3">
+      <c r="A31" s="25"/>
+      <c r="C31" s="24" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="32" spans="1:3" ht="15">
-      <c r="A32" s="30"/>
-      <c r="B32" s="32"/>
-      <c r="C32" s="8" t="s">
+    <row r="32" ht="12.75" spans="1:3">
+      <c r="A32" s="25"/>
+      <c r="C32" s="24" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="33" spans="1:3" ht="15">
-      <c r="A33" s="30"/>
-      <c r="B33" s="32"/>
-      <c r="C33" s="8" t="s">
+    <row r="33" ht="12.75" spans="1:3">
+      <c r="A33" s="25"/>
+      <c r="C33" s="24" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="35" spans="1:3" ht="165">
-      <c r="A35" s="30" t="s">
+    <row r="35" ht="114.75" spans="1:3">
+      <c r="A35" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="B35" s="7" t="s">
+      <c r="B35" s="23" t="s">
         <v>106</v>
       </c>
-      <c r="C35" s="25" t="s">
+      <c r="C35" s="43" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="36" spans="1:3" ht="105">
-      <c r="A36" s="30"/>
-      <c r="B36" s="7" t="s">
+    <row r="36" ht="89.25" spans="1:3">
+      <c r="A36" s="25"/>
+      <c r="B36" s="23" t="s">
         <v>108</v>
       </c>
-      <c r="C36" s="25" t="s">
+      <c r="C36" s="43" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="37" spans="1:3" ht="105">
-      <c r="A37" s="30"/>
-      <c r="B37" s="7" t="s">
+    <row r="37" ht="76.5" spans="1:3">
+      <c r="A37" s="25"/>
+      <c r="B37" s="23" t="s">
         <v>110</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="29" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="60">
-      <c r="A38" s="30"/>
-      <c r="B38" s="7" t="s">
+    <row r="38" ht="51" spans="1:3">
+      <c r="A38" s="25"/>
+      <c r="B38" s="23" t="s">
         <v>112</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="29" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
-      <c r="A40" s="9" t="s">
+    <row r="40" spans="1:1">
+      <c r="A40" s="25" t="s">
         <v>114</v>
       </c>
     </row>
@@ -4149,305 +5187,307 @@
     <mergeCell ref="B30:B33"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
+  <pageSetup paperSize="1" orientation="portrait"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C64"/>
   <sheetViews>
-    <sheetView topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B64" sqref="B64"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="32" style="1" customWidth="1"/>
-    <col min="2" max="2" width="109" style="1" customWidth="1"/>
+    <col min="1" max="1" width="32" style="15" customWidth="1"/>
+    <col min="2" max="2" width="109" style="15" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="150">
-      <c r="A1" s="2" t="s">
+    <row r="1" ht="127.5" spans="1:3">
+      <c r="A1" s="16" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="42" t="s">
         <v>116</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="17" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="200.25" customHeight="1">
-      <c r="A2" s="1" t="s">
+    <row r="2" ht="200.25" customHeight="1" spans="1:2">
+      <c r="A2" s="15" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="15" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="120">
-      <c r="A3" s="1" t="s">
+    <row r="3" ht="102" spans="1:2">
+      <c r="A3" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="15" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="4" spans="1:3" ht="45">
-      <c r="A4" s="1" t="s">
+    <row r="4" ht="25.5" spans="1:2">
+      <c r="A4" s="15" t="s">
         <v>122</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="42" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30">
-      <c r="A5" s="1" t="s">
+    <row r="5" ht="25.5" spans="1:2">
+      <c r="A5" s="15" t="s">
         <v>124</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="15" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="6" spans="1:3" ht="45">
-      <c r="A6" s="1" t="s">
+    <row r="6" ht="38.25" spans="1:1">
+      <c r="A6" s="15" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="45">
-      <c r="A7" s="1" t="s">
+    <row r="7" ht="38.25" spans="1:2">
+      <c r="A7" s="15" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="15" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="8" spans="1:3" ht="150">
-      <c r="A8" s="1" t="s">
+    <row r="8" ht="114.75" spans="1:2">
+      <c r="A8" s="15" t="s">
         <v>129</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="15" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="12" spans="1:3" ht="60">
-      <c r="A12" s="1" t="s">
+    <row r="12" ht="51" spans="1:2">
+      <c r="A12" s="15" t="s">
         <v>131</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="B12" s="15" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="13" spans="1:3" ht="60">
-      <c r="A13" s="1" t="s">
+    <row r="13" ht="51" spans="1:2">
+      <c r="A13" s="15" t="s">
         <v>133</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="B13" s="15" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="120">
-      <c r="A14" s="1" t="s">
+    <row r="14" ht="89.25" spans="1:2">
+      <c r="A14" s="15" t="s">
         <v>135</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="B14" s="15" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="15" spans="1:3" ht="120">
-      <c r="A15" s="1" t="s">
+    <row r="15" ht="102" spans="1:2">
+      <c r="A15" s="15" t="s">
         <v>137</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="B15" s="15" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
-      <c r="A16" s="1" t="s">
+    <row r="16" spans="1:2">
+      <c r="A16" s="15" t="s">
         <v>139</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="B16" s="15" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="17" spans="1:2" ht="225">
-      <c r="A17" s="1" t="s">
+    <row r="17" ht="178.5" spans="1:2">
+      <c r="A17" s="15" t="s">
         <v>141</v>
       </c>
-      <c r="B17" s="1" t="s">
+      <c r="B17" s="15" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="18" spans="1:2" ht="30">
-      <c r="A18" s="1" t="s">
+    <row r="18" ht="25.5" spans="1:2">
+      <c r="A18" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="B18" s="15" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="19" spans="1:2" ht="345">
-      <c r="A19" s="1" t="s">
+    <row r="19" ht="280.5" spans="1:2">
+      <c r="A19" s="15" t="s">
         <v>145</v>
       </c>
-      <c r="B19" s="1" t="s">
+      <c r="B19" s="15" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="20" spans="1:2">
-      <c r="A20" s="1" t="s">
+    <row r="20" spans="1:1">
+      <c r="A20" s="15" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="22" spans="1:2">
-      <c r="A22" s="1" t="s">
+    <row r="22" spans="1:1">
+      <c r="A22" s="15" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="23" spans="1:2">
-      <c r="B23" s="4"/>
-    </row>
-    <row r="25" spans="1:2">
-      <c r="A25" s="1" t="s">
+    <row r="23" spans="2:2">
+      <c r="B23" s="18"/>
+    </row>
+    <row r="25" spans="1:1">
+      <c r="A25" s="15" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="28" spans="1:2">
-      <c r="A28" s="1" t="s">
+    <row r="28" spans="1:1">
+      <c r="A28" s="15" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="1" t="s">
+      <c r="A31" s="15" t="s">
         <v>151</v>
       </c>
-      <c r="B31" s="1" t="s">
+      <c r="B31" s="15" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="33" spans="1:2" ht="45">
-      <c r="A33" s="1" t="s">
+    <row r="33" ht="38.25" spans="1:2">
+      <c r="A33" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="B33" s="15" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="34" spans="1:2" ht="135">
-      <c r="A34" s="1" t="s">
+    <row r="34" ht="114.75" spans="1:2">
+      <c r="A34" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="B34" s="15" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="36" spans="1:2">
-      <c r="A36" s="1" t="s">
+    <row r="36" spans="1:1">
+      <c r="A36" s="15" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="38" spans="1:2">
-      <c r="A38" s="1" t="s">
+    <row r="38" spans="1:1">
+      <c r="A38" s="15" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="40" spans="1:2">
-      <c r="A40" s="1" t="s">
+    <row r="40" spans="1:1">
+      <c r="A40" s="15" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="42" spans="1:2">
-      <c r="A42" s="1" t="s">
+    <row r="42" spans="1:1">
+      <c r="A42" s="15" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="44" spans="1:2">
-      <c r="A44" s="1" t="s">
+    <row r="44" spans="1:1">
+      <c r="A44" s="15" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="46" spans="1:2">
-      <c r="A46" s="1" t="s">
+    <row r="46" spans="1:1">
+      <c r="A46" s="15" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="48" spans="1:2">
-      <c r="A48" s="1" t="s">
+    <row r="48" spans="1:1">
+      <c r="A48" s="15" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="50" spans="1:2">
-      <c r="A50" s="1" t="s">
+    <row r="50" spans="1:1">
+      <c r="A50" s="15" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="52" spans="1:2">
-      <c r="A52" s="1" t="s">
+    <row r="52" spans="1:1">
+      <c r="A52" s="15" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="33" t="s">
+      <c r="A54" s="19" t="s">
         <v>166</v>
       </c>
-      <c r="B54" s="1" t="s">
+      <c r="B54" s="15" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="33"/>
-      <c r="B55" s="1" t="s">
+      <c r="A55" s="19"/>
+      <c r="B55" s="15" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="33"/>
-      <c r="B56" s="1" t="s">
+      <c r="A56" s="19"/>
+      <c r="B56" s="15" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="58" spans="1:2" ht="30">
-      <c r="A58" s="34" t="s">
+    <row r="58" ht="25.5" spans="1:2">
+      <c r="A58" s="20" t="s">
         <v>170</v>
       </c>
-      <c r="B58" s="1" t="s">
+      <c r="B58" s="15" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="34"/>
-      <c r="B59" s="5" t="s">
+      <c r="A59" s="20"/>
+      <c r="B59" s="21" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="60" spans="1:2">
-      <c r="A60" s="34"/>
-      <c r="B60" s="5" t="s">
+      <c r="A60" s="20"/>
+      <c r="B60" s="21" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="61" spans="1:2">
-      <c r="A61" s="34"/>
-      <c r="B61" s="5" t="s">
+      <c r="A61" s="20"/>
+      <c r="B61" s="21" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="62" spans="1:2">
-      <c r="A62" s="34"/>
-      <c r="B62" s="5" t="s">
+      <c r="A62" s="20"/>
+      <c r="B62" s="21" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="63" spans="1:2">
-      <c r="A63" s="34"/>
-      <c r="B63" s="5" t="s">
+      <c r="A63" s="20"/>
+      <c r="B63" s="21" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="34"/>
-      <c r="B64" s="5" t="s">
+      <c r="A64" s="20"/>
+      <c r="B64" s="21" t="s">
         <v>177</v>
       </c>
     </row>
@@ -4457,95 +5497,96 @@
     <mergeCell ref="A58:A64"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C1" r:id="rId1" xr:uid="{00000000-0004-0000-0400-000000000000}"/>
+    <hyperlink ref="C1" r:id="rId1" display="HƯỚNG DẪN CÁC BƯỚC PHÁT TRIỂN HỆ THỐNG MICROSERVICE VỚI DOCKER | CO-WELL Asia"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B631DE72-CB4E-4B95-ACE9-0C817A0FF87F}">
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="23.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="21.75" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="47" style="39" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="125" style="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60" style="36" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="36"/>
+    <col min="1" max="1" width="47" style="9" customWidth="1"/>
+    <col min="2" max="2" width="125" style="10" customWidth="1"/>
+    <col min="3" max="3" width="60" style="11" customWidth="1"/>
+    <col min="4" max="16384" width="9.14" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="131.25">
-      <c r="A1" s="35" t="s">
+    <row r="1" ht="120.75" spans="1:2">
+      <c r="A1" s="9" t="s">
+        <v>178</v>
+      </c>
+      <c r="B1" s="12" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="2" ht="138" spans="2:2">
+      <c r="B2" s="12" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="3" ht="172.5" spans="1:3">
+      <c r="A3" s="9" t="s">
+        <v>181</v>
+      </c>
+      <c r="B3" s="12" t="s">
         <v>182</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="C3" s="13" t="s">
         <v>183</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="150">
-      <c r="A2" s="35"/>
-      <c r="B2" s="38" t="s">
+    <row r="4" ht="103.5" spans="1:2">
+      <c r="A4" s="9" t="s">
         <v>184</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" ht="225">
-      <c r="A3" s="39" t="s">
+      <c r="B4" s="12" t="s">
         <v>185</v>
       </c>
-      <c r="B3" s="38" t="s">
+    </row>
+    <row r="5" ht="65.25" spans="1:2">
+      <c r="A5" s="14" t="s">
+        <v>186</v>
+      </c>
+      <c r="B5" s="12"/>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="9" t="s">
+        <v>187</v>
+      </c>
+      <c r="B6" s="12"/>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="9" t="s">
         <v>188</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="B7" s="12"/>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="9" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="9" ht="34.5" spans="1:2">
+      <c r="A9" s="9" t="s">
         <v>190</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" ht="150">
-      <c r="A4" s="39" t="s">
-        <v>180</v>
-      </c>
-      <c r="B4" s="38" t="s">
-        <v>189</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="69.75">
-      <c r="A5" s="40" t="s">
+      <c r="B9" s="12" t="s">
         <v>191</v>
       </c>
-      <c r="B5" s="38"/>
-    </row>
-    <row r="6" spans="1:3">
-      <c r="A6" s="39" t="s">
-        <v>186</v>
-      </c>
-      <c r="B6" s="38"/>
-    </row>
-    <row r="7" spans="1:3">
-      <c r="A7" s="39" t="s">
-        <v>187</v>
-      </c>
-      <c r="B7" s="38"/>
-    </row>
-    <row r="8" spans="1:3">
-      <c r="A8" s="39" t="s">
-        <v>178</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="56.25">
-      <c r="A9" s="39" t="s">
-        <v>179</v>
-      </c>
-      <c r="B9" s="38" t="s">
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="9" t="s">
         <v>192</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3">
-      <c r="A10" s="39" t="s">
-        <v>181</v>
       </c>
     </row>
   </sheetData>
@@ -4553,20 +5594,82 @@
     <mergeCell ref="A1:A2"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C3" r:id="rId1" xr:uid="{6915B9AD-3758-445A-B52B-ABA90CDCC71E}"/>
+    <hyperlink ref="C3" r:id="rId1" display="https://www.nginx.com/resources/glossary/dns-load-balancing/"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFBD267F-903D-47F9-8991-FD83D8DCD415}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L31" sqref="L31"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="C1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C25" sqref="C22:C25"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="2"/>
+  <cols>
+    <col min="3" max="3" width="140" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="76.5" spans="3:3">
+      <c r="C1" s="8" t="s">
+        <v>193</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M42" sqref="M42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
[feat][system][DDD, Clean architecture, Saga, Outbox]
</commit_message>
<xml_diff>
--- a/System/Documents.xlsx
+++ b/System/Documents.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13530" firstSheet="10" activeTab="15"/>
+    <workbookView windowWidth="28695" windowHeight="13530" firstSheet="10" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -23,13 +23,14 @@
     <sheet name="Outbox Pattern" sheetId="34" r:id="rId14"/>
     <sheet name="CQRS" sheetId="35" r:id="rId15"/>
     <sheet name="KAFKA" sheetId="36" r:id="rId16"/>
+    <sheet name="Two phases commit" sheetId="37" r:id="rId17"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="212" uniqueCount="211">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="242" uniqueCount="241">
   <si>
     <t>Kiến Trúc về Microservice</t>
   </si>
@@ -2815,21 +2816,705 @@
   <si>
     <t>Abstract Factory Design Pattern</t>
   </si>
+  <si>
+    <t>Introduction</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> - Although microservice architectural style provides numerous benefits, it has several limitations as well. One of the major problems in a microservice architecture is how to handle a "</t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>transaction that spans(trải dài) multiple services</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">".
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Database per Service Pattern</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:
+ - One of the benefits of microservice architecture is that we can choose the technology stack per service.
+ - This model lets the service manage domain data independently on a data store that best suites its data types and schema. Services scale its data stores on demand and insulates it from the failures of other services.
+ - However, at times a </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>transaction can span across multiple services</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, and ensuring data consistency across the service database is a challenge.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Challenges of Distributed Transaction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:
+ - The first challenge is maintaining ACID. In a distributed transaction scenario, as the transaction spans several services, ensuring ACID always remains key.
+ - The second challenge is managing the transaction isolation level. It specifies the amount of data that is visible in a transaction when the other services access the same data simultaneously. In other words, if one object in one of the microservices is persisted in the database while another request reads the data, should the service return the old or new data?
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Saga Pattern</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:
+ - The Saga architecture pattern </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>provides transaction management using a sequence of local transactions</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">.
+ - A local transaction is the unit of work performed by a Saga participant(người tham gia).
+ - Every operation that is part of the Saga can be rolled back by a </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>compensating transaction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. In the Saga pattern, a </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>compensating transaction must be idempotent and retryable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.
+ - the Saga pattern guarantees that either all operations complete successfully or the corresponding compensation transactions are run to undo the work previously completed.
+ - The Saga pattern is a widely used design pattern in microservices architectures to manage distributed transactions in a way that maintains consistency and reliability. 
+ - Unlike traditional distributed transactions, which lock resources across multiple services, the Saga pattern achieves eventual consistency by breaking the transaction into a series of smaller steps, each handled by a different service. This avoids distributed locks and can scale well in highly distributed environments.</t>
+    </r>
+  </si>
+  <si>
+    <t>Why Use the Saga Pattern</t>
+  </si>
+  <si>
+    <t>In distributed systems, especially those built using microservices, achieving atomic transactions (where either all operations succeed or none do) can be challenging because:
+ - Microservices often have independent databases.
+ - Network failures and service unavailability can result in partial failures.
+ - Distributed locks are hard to manage and do not scale well.
+ - The Saga pattern resolves this by turning a large transaction into a series of smaller, atomic transactions, each local to a service. If a failure occurs, the system performs compensating transactions to undo any changes made by previous steps.</t>
+  </si>
+  <si>
+    <t>The Saga Execution Coordinator</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - The Saga Execution Coordinator is the central component to implement a Saga flow. It contains a Saga log that captures the sequence of events of a distributed transaction.
+ - For any failure, the SEC component inspects the Saga log to identify the impacted components and the sequence in which the compensating transactions should run.
+ - It can then identify the transactions successfully rolled back, which ones are pending, and can take appropriate actions.</t>
+  </si>
+  <si>
+    <t>Types of Saga Implementations</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Choreography-based Saga (Event-driven):
+ - In this approach, each service involved in the Saga </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>listens for events and performs its transaction in response</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. After completing its part of the transaction, it publishes an event that triggers the next service in the workflow.
+ - Benefits: 
+  + </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Decentralized</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: There is no central coordinator, and </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>services independently</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> manage their part of the transaction.
+  + </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Easy to add new services</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: New services can be added to the transaction simply by subscribing to events.
+ - Drawbacks:
+  + Complex coordination: With many services and events, the system can become difficult to reason about.
+  + Event loops: Complex event-driven systems can lead to cyclical dependencies, resulting in event loops or inconsistent states.
+  + Compensating actions: Every service must manage and implement its compensating transaction, increasing complexity.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Orchestration-based Saga:
+ - In this approach, a central orchestrator coordinates the entire Saga. The </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>orchestrator tells each service what operation to perform and handles the flow of the transaction</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>. It also manages compensating transactions in case of failures.
+ - Benefits:
+  + Centralized control: The orchestrator manages the entire workflow, making it easier to handle complex transaction logic.
+  + Clear failure handling: If a step fails, the orchestrator can immediately trigger compensating actions.
+ - Drawbacks:
+  + Single point of failure: The orchestrator becomes a critical component. If it fails, the Saga can break.
+  + Tight coupling: The orchestrator must know about all the services involved in the transaction, which can lead to tight coupling between the services and the orchestrator.</t>
+    </r>
+  </si>
+  <si>
+    <t>Key Components of the Saga Pattern</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Atomic Transactions: Each step of a Saga is a local transaction that is atomic (it either completes successfully or fails without side effects).
+ - Compensating Transactions: These are the rollback operations that undo the work of a previously completed step if a failure occurs.
+ - Eventual Consistency: Sagas don’t guarantee immediate consistency but ensure that the system reaches a consistent state eventually.
+ - Asynchronous Communication: Sagas often rely on asynchronous messaging systems (e.g., Kafka, RabbitMQ) to propagate events between services, ensuring that the system remains responsive.</t>
+  </si>
+  <si>
+    <t>Compensating Transactions</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - One of the core principles of the Saga pattern is that each service must be capable of rolling back its changes if something goes wrong. This is achieved through compensating transactions, which are the "undo" steps for each local transaction.
+ - Compensating transactions can vary in complexity:
+  + Simple compensations: Releasing reserved resources, such as unlocking inventory or rolling back account balances.
+  + Complex compensations: If a service made external API calls or performed side effects (e.g., sending emails), compensating actions may involve more complex logic.</t>
+  </si>
+  <si>
+    <t>Error Handling and Recovery</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Timeouts: If a service doesn’t respond within a given time, the Saga needs to assume that something went wrong and trigger compensating actions.
+ - Retries: Temporary failures (e.g., network issues) might require the orchestrator or services to retry the transaction step.
+ - Idempotency: To ensure safe retries, every transaction step and compensating transaction must be idempotent, meaning that repeating the operation will have the same effect as performing it once.</t>
+  </si>
+  <si>
+    <t>Saga Pattern in Microservices</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Decentralization: Microservices are independent, and the Saga pattern enables each service to manage its own local transactions and rollback logic.
+ - Loose coupling: By using events or an orchestrator, services are loosely coupled, allowing for easier scaling and maintenance.
+ - Scalability: The Saga pattern is scalable as it avoids distributed locks, which can become a bottleneck in traditional distributed transactions.</t>
+  </si>
+  <si>
+    <t>Eventual Consistency in Sagas</t>
+  </si>
+  <si>
+    <t>The Saga pattern provides eventual consistency, which means that while the system might temporarily be in an inconsistent state (e.g., an order is created, but payment hasn’t been processed yet), it will eventually converge to a consistent state. This is acceptable in many modern applications, where strong consistency is not a strict requirement for every operation (e.g., e-commerce systems, where slight delays in consistency don’t affect user experience).</t>
+  </si>
+  <si>
+    <t>Issues and considerations</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Consider the following points when implementing the Saga pattern:
+ - The Saga pattern may </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>initially be challenging</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(thách thức khi bắt đầu), as it requires a new way of thinking on how to coordinate a transaction and maintain data consistency for a business process spanning multiple microservices.
+ - The Saga pattern is particularly hard to debug, and the </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>complexity grows as participants increase</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.
+ - Data can't be rolled back, because saga participants commit changes to their local databases.
+ - The implementation must be capable of handling a set of potential transient failures, and provide idempotence for reducing side-effects and ensuring data consistency. Idempotence means that the same operation can be repeated multiple times without changing the initial result. For more information, see the guidance on ensuring idempotence when processing messages and updating state together.
+ - It's best to implement observability to monitor and track the saga workflow.
+ - The lack of participant data isolation imposes durability challenges. The saga implementation must include countermeasures to reduce anomalies.
+ - Compensating transactions don't always work.</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">The following </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>anomalies</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(điều bất thường) can happen without proper measures:
+ - Lost updates, when one saga writes without reading changes made by another saga.
+ - Dirty reads, when a transaction or a saga reads updates made by a saga that has not yet completed those updates.
+ - Fuzzy/nonrepeatable reads, when different saga steps read different data because a data update occurs between the reads.</t>
+    </r>
+  </si>
+  <si>
+    <t>Suggested countermeasures to reduce or prevent anomalies include:
+ - Semantic lock, an application-level lock where a saga's compensable transaction uses a semaphore to indicate an update is in progress.
+ - Commutative updates that can be executed in any order and produce the same result.
+ - Pessimistic view: It's possible for one saga to read dirty data, while another saga is running a compensable transaction to roll back the operation. Pessimistic view reorders the saga so the underlying data updates in a      retryable transaction, which eliminates the possibility of a dirty read.
+ - Reread value verifies that data is unchanged, and then updates the record. If the record has changed, the steps abort and the saga may restart.
+ - A version file records the operations on a record as they arrive, and then executes them in the correct order.
+ - By value uses each request's business risk to dynamically select the concurrency mechanism. Low-risk requests favor sagas, while high-risk requests favor distributed transactions.</t>
+  </si>
+  <si>
+    <t>Overview</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> - In the </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sprawling landscape</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(bối cảnh rộng lớn) of microservices, the Outbox Pattern </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>emerges</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(xuất hiện) as a </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>paragon</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(chuẩn mực) of </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>order</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> and </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>consistency</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.</t>
+    </r>
+  </si>
+  <si>
+    <t>Outbox Pattern in Microservices</t>
+  </si>
+  <si>
+    <r>
+      <t>Goals</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:
+ - First, the Outbox Pattern defines temporary storage (outbox table) where microservices log their outgoing data changes. This pattern serializes the data, preparing it for transmission.
+ - Then, it sends the serialized records from the outbox table to other services or external systems. Throughout this operation, the pattern ensures data consistency and reliability.
+ - If a network problem or service downtime prevents immediate data dispatch, it holds onto the data to avoid loss. When technicians fix these issues, the pattern sends the data correctly.
+ - At its core, Outbox Pattern isn’t just a pattern. It stands as a mechanism for resilience and consistency in microservices. As systems expand and complexity increases, relying on strategies like the Outbox Pattern becomes favorable and necessary.
+</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Architecture</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">:
+ - Whenever a business transaction unfolds within a microservice, it makes the required changes within a database transaction. Rather than forging a direct link with external services such as RabbitMQ, EventHub, or Kafka, </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>we store all the events (table changes) in the outbox table in the same database that the microservice uses</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.
+ - A background service consistently checks the outbox table and relays the archived events to a pre-chosen message broker or event-streaming platform.
+ - Transitioning further, the services subscribed to the message broker get notified about the events and react according to their business rules.</t>
+    </r>
+  </si>
+  <si>
+    <t>Two-phase commit (2PC) is a standardized protocol that ensures atomicity, consistency, isolation and durability (ACID) of a transaction; it is an atomic commitment protocol for distributed systems.</t>
+  </si>
+  <si>
+    <t>How does two-phase commit work?</t>
+  </si>
+  <si>
+    <t>Phase 1 (the prepare phase):
+ - The protocol ensures all resource managers have saved the transaction’s updates to stable storage. Every server that is required to commit writes its data records in a log. If a server is unsuccessful in doing so, then it responds with a failure message; if it is successful, then it sends an OK message.</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="36">
+  <fonts count="37">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2839,14 +3524,6 @@
       <color theme="1"/>
       <name val="Arial"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="10"/>
@@ -2885,14 +3562,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF9C0006"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
@@ -2949,15 +3618,40 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -2972,41 +3666,9 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3018,24 +3680,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -3049,13 +3696,28 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
@@ -3063,6 +3725,22 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <u/>
       <sz val="11"/>
       <color theme="1"/>
@@ -3129,7 +3807,133 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3141,67 +3945,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3213,91 +3969,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
+        <fgColor rgb="FFFFCC99"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -3363,6 +4041,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -3382,6 +4075,21 @@
     </border>
     <border>
       <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
       <right style="thin">
@@ -3396,17 +4104,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
       </top>
       <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -3428,173 +4132,147 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="16" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="16" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="22" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="10" borderId="11" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="12" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="32" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="33" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="16" borderId="12" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="10" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="7" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="16" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -3602,32 +4280,59 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="48" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="48" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="48"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -3636,21 +4341,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="48" applyFont="1"/>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" xfId="33" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="48" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="4" borderId="0" xfId="33" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="0" xfId="23" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="0" xfId="23" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="48" applyFont="1"/>
@@ -3672,14 +4374,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="14" fillId="4" borderId="0" xfId="33" applyFont="1" applyAlignment="1">
@@ -4198,199 +4900,199 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="12.75" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="9.14" style="37"/>
-    <col min="2" max="2" width="39.5733333333333" style="37" customWidth="1"/>
-    <col min="3" max="3" width="95.5733333333333" style="37" customWidth="1"/>
-    <col min="4" max="4" width="60.7133333333333" style="37" customWidth="1"/>
-    <col min="5" max="5" width="58.8533333333333" style="37" customWidth="1"/>
-    <col min="6" max="6" width="50" style="37" customWidth="1"/>
-    <col min="7" max="7" width="49.7133333333333" style="37" customWidth="1"/>
-    <col min="8" max="16384" width="9.14" style="37"/>
+    <col min="1" max="1" width="9.14" style="45"/>
+    <col min="2" max="2" width="39.5733333333333" style="45" customWidth="1"/>
+    <col min="3" max="3" width="95.5733333333333" style="45" customWidth="1"/>
+    <col min="4" max="4" width="60.7133333333333" style="45" customWidth="1"/>
+    <col min="5" max="5" width="58.8533333333333" style="45" customWidth="1"/>
+    <col min="6" max="6" width="50" style="45" customWidth="1"/>
+    <col min="7" max="7" width="49.7133333333333" style="45" customWidth="1"/>
+    <col min="8" max="16384" width="9.14" style="45"/>
   </cols>
   <sheetData>
     <row r="1" ht="76.5" spans="1:3">
-      <c r="A1" s="37">
+      <c r="A1" s="45">
         <v>1</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="45" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="41" t="s">
+      <c r="C1" s="49" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" ht="63.75" spans="1:3">
-      <c r="A2" s="37">
+      <c r="A2" s="45">
         <v>2</v>
       </c>
-      <c r="B2" s="37" t="s">
+      <c r="B2" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="41" t="s">
+      <c r="C2" s="49" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" ht="38.25" spans="1:3">
-      <c r="A3" s="37">
+      <c r="A3" s="45">
         <v>3</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="47" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="41" t="s">
+      <c r="C3" s="49" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" ht="38.25" spans="1:3">
-      <c r="A4" s="37">
+      <c r="A4" s="45">
         <v>4</v>
       </c>
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="45" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="42" t="s">
+      <c r="C4" s="50" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" ht="178.5" spans="1:3">
-      <c r="A5" s="37">
+      <c r="A5" s="45">
         <v>5</v>
       </c>
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="24" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" ht="25.5" spans="1:3">
-      <c r="A6" s="37">
+      <c r="A6" s="45">
         <v>6</v>
       </c>
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="45" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="42" t="s">
+      <c r="C6" s="50" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" ht="229.5" spans="1:3">
-      <c r="A7" s="37">
+      <c r="A7" s="45">
         <v>7</v>
       </c>
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="38" t="s">
+      <c r="C7" s="46" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" ht="245.25" customHeight="1" spans="1:3">
-      <c r="A8" s="37">
+      <c r="A8" s="45">
         <v>8</v>
       </c>
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="45" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="38" t="s">
+      <c r="C8" s="46" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" ht="223.5" customHeight="1" spans="1:3">
-      <c r="A9" s="37">
+      <c r="A9" s="45">
         <v>9</v>
       </c>
-      <c r="B9" s="37" t="s">
+      <c r="B9" s="45" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="41" t="s">
+      <c r="C9" s="49" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" ht="204" spans="1:4">
-      <c r="A10" s="37">
+      <c r="A10" s="45">
         <v>10</v>
       </c>
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="45" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="C10" s="24" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="40" t="s">
+      <c r="D10" s="48" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" ht="25.5" spans="2:3">
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="45" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="15" t="s">
+      <c r="C11" s="24" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" ht="102" spans="2:3">
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="15" t="s">
+      <c r="C12" s="24" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" ht="140.25" spans="2:3">
-      <c r="B13" s="37" t="s">
+      <c r="B13" s="45" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="15" t="s">
+      <c r="C13" s="24" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" ht="288.75" customHeight="1" spans="2:7">
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="45" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="15" t="s">
+      <c r="C14" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="38" t="s">
+      <c r="D14" s="46" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="15" t="s">
+      <c r="E14" s="24" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="15" t="s">
+      <c r="F14" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="15" t="s">
+      <c r="G14" s="24" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" ht="38.25" spans="2:3">
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="45" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="15" t="s">
+      <c r="C15" s="24" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" ht="240.75" customHeight="1" spans="2:2">
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="45" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" ht="153" spans="2:3">
-      <c r="B17" s="37" t="s">
+      <c r="B17" s="45" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="38" t="s">
+      <c r="C17" s="46" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="18" ht="153" spans="2:3">
-      <c r="B18" s="37" t="s">
+      <c r="B18" s="45" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="38" t="s">
+      <c r="C18" s="46" t="s">
         <v>39</v>
       </c>
     </row>
@@ -4419,12 +5121,12 @@
   </cols>
   <sheetData>
     <row r="1" ht="89.25" spans="4:4">
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="1" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="2" ht="350" customHeight="1" spans="4:4">
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="17" t="s">
         <v>195</v>
       </c>
     </row>
@@ -4451,57 +5153,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="11" t="s">
         <v>196</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="B1" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="C1" s="3" t="s">
+      <c r="C1" s="13" t="s">
         <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="14" t="s">
         <v>199</v>
       </c>
-      <c r="B2" s="5"/>
-      <c r="C2" s="4"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="14"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="1" t="s">
+      <c r="A3" s="11" t="s">
         <v>200</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="1"/>
+      <c r="B3" s="15"/>
+      <c r="C3" s="11"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="4" t="s">
+      <c r="A4" s="14" t="s">
         <v>201</v>
       </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="4"/>
+      <c r="B4" s="15"/>
+      <c r="C4" s="14"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="1" t="s">
+      <c r="A5" s="11" t="s">
         <v>202</v>
       </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="1"/>
+      <c r="B5" s="15"/>
+      <c r="C5" s="11"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="4" t="s">
+      <c r="A6" s="14" t="s">
         <v>203</v>
       </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="4"/>
+      <c r="B6" s="15"/>
+      <c r="C6" s="14"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="1" t="s">
+      <c r="A7" s="11" t="s">
         <v>204</v>
       </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="1"/>
+      <c r="B7" s="16"/>
+      <c r="C7" s="11"/>
     </row>
     <row r="8" customFormat="1"/>
     <row r="9" customFormat="1"/>
@@ -4573,14 +5275,123 @@
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="12.1" style="8" customWidth="1"/>
+    <col min="2" max="2" width="168" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="267.75" spans="1:2">
+      <c r="A1" s="8" t="s">
+        <v>211</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="2" ht="76.5" spans="1:2">
+      <c r="A2" s="8" t="s">
+        <v>213</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" ht="38.25" spans="1:2">
+      <c r="A3" s="8" t="s">
+        <v>215</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" ht="127.5" spans="1:2">
+      <c r="A4" s="8" t="s">
+        <v>217</v>
+      </c>
+      <c r="B4" s="9" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="5" ht="114.75" spans="2:2">
+      <c r="B5" s="9" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="6" ht="51" spans="1:2">
+      <c r="A6" s="8" t="s">
+        <v>220</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="7" ht="63.75" spans="1:2">
+      <c r="A7" s="8" t="s">
+        <v>222</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="8" ht="38.25" spans="1:2">
+      <c r="A8" s="8" t="s">
+        <v>224</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="9" ht="38.25" spans="1:2">
+      <c r="A9" s="8" t="s">
+        <v>226</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="10" ht="38.25" spans="1:2">
+      <c r="A10" s="8" t="s">
+        <v>228</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="11" ht="127.5" spans="1:2">
+      <c r="A11" s="10" t="s">
+        <v>230</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="12" ht="51" spans="1:2">
+      <c r="A12" s="10"/>
+      <c r="B12" s="9" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="13" ht="102" spans="1:2">
+      <c r="A13" s="10"/>
+      <c r="B13" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A11:A13"/>
+  </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="A11:A13" r:id="rId1" display="Issues and considerations"/>
+  </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -4589,14 +5400,35 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1"/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
-  <sheetData/>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="13" style="4" customWidth="1"/>
+    <col min="2" max="2" width="160.3" style="5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" s="4" t="s">
+        <v>234</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="2" ht="153" spans="1:2">
+      <c r="A2" s="4" t="s">
+        <v>236</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>237</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -4623,12 +5455,48 @@
   <sheetPr/>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H28" sqref="H28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
   <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelRow="3" outlineLevelCol="1"/>
+  <cols>
+    <col min="2" max="2" width="149.5" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" ht="25.5" spans="2:2">
+      <c r="B1" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="3" ht="51" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>239</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="4" spans="2:2">
+      <c r="B4" s="3"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -4650,298 +5518,298 @@
   </cols>
   <sheetData>
     <row r="1" ht="89.25" spans="1:2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="38" t="s">
         <v>40</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="2" ht="89.25" spans="1:2">
-      <c r="A2" s="30"/>
-      <c r="B2" s="31" t="s">
+      <c r="A2" s="38"/>
+      <c r="B2" s="39" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="3" ht="102" spans="1:2">
-      <c r="A3" s="30"/>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="38"/>
+      <c r="B3" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="4" ht="63.75" spans="1:2">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="38" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="5" ht="63.75" spans="1:2">
-      <c r="A5" s="30"/>
-      <c r="B5" s="31" t="s">
+      <c r="A5" s="38"/>
+      <c r="B5" s="39" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="30"/>
-      <c r="B6" s="31" t="s">
+      <c r="A6" s="38"/>
+      <c r="B6" s="39" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="7" ht="38.25" spans="1:2">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="38" t="s">
         <v>48</v>
       </c>
-      <c r="B7" s="31" t="s">
+      <c r="B7" s="39" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="8" ht="38.25" spans="1:2">
-      <c r="A8" s="30"/>
-      <c r="B8" s="31" t="s">
+      <c r="A8" s="38"/>
+      <c r="B8" s="39" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="30"/>
-      <c r="B9" s="31" t="s">
+      <c r="A9" s="38"/>
+      <c r="B9" s="39" t="s">
         <v>51</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="30"/>
-      <c r="B10" s="31" t="s">
+      <c r="A10" s="38"/>
+      <c r="B10" s="39" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="30"/>
-      <c r="B11" s="31" t="s">
+      <c r="A11" s="38"/>
+      <c r="B11" s="39" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="12" ht="51" spans="1:2">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="38" t="s">
         <v>54</v>
       </c>
-      <c r="B12" s="31" t="s">
+      <c r="B12" s="39" t="s">
         <v>55</v>
       </c>
     </row>
     <row r="13" ht="63.75" spans="1:2">
-      <c r="A13" s="30"/>
-      <c r="B13" s="31" t="s">
+      <c r="A13" s="38"/>
+      <c r="B13" s="39" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="14" ht="127.5" spans="1:2">
-      <c r="A14" s="30"/>
-      <c r="B14" s="31" t="s">
+      <c r="A14" s="38"/>
+      <c r="B14" s="39" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="30"/>
-      <c r="B15" s="31" t="s">
+      <c r="A15" s="38"/>
+      <c r="B15" s="39" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="30"/>
-      <c r="B16" s="31" t="s">
+      <c r="A16" s="38"/>
+      <c r="B16" s="39" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="17" ht="102" spans="1:2">
-      <c r="A17" s="30"/>
-      <c r="B17" s="31" t="s">
+      <c r="A17" s="38"/>
+      <c r="B17" s="39" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="18" ht="38.25" spans="1:2">
-      <c r="A18" s="30"/>
-      <c r="B18" s="31" t="s">
+      <c r="A18" s="38"/>
+      <c r="B18" s="39" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="30"/>
-      <c r="B19" s="31" t="s">
+      <c r="A19" s="38"/>
+      <c r="B19" s="39" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="30"/>
-      <c r="B20" s="32" t="s">
+      <c r="A20" s="38"/>
+      <c r="B20" s="40" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="21" ht="165.75" spans="1:2">
-      <c r="A21" s="33" t="s">
+      <c r="A21" s="41" t="s">
         <v>64</v>
       </c>
-      <c r="B21" s="31" t="s">
+      <c r="B21" s="39" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="22" ht="242.25" spans="1:2">
-      <c r="A22" s="33"/>
-      <c r="B22" s="31" t="s">
+      <c r="A22" s="41"/>
+      <c r="B22" s="39" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="23" ht="153" spans="1:2">
-      <c r="A23" s="33"/>
-      <c r="B23" s="31" t="s">
+      <c r="A23" s="41"/>
+      <c r="B23" s="39" t="s">
         <v>67</v>
       </c>
     </row>
     <row r="24" ht="38.25" spans="1:2">
-      <c r="A24" s="33"/>
-      <c r="B24" s="31" t="s">
+      <c r="A24" s="41"/>
+      <c r="B24" s="39" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="25" ht="25.5" spans="1:2">
-      <c r="A25" s="33"/>
-      <c r="B25" s="31" t="s">
+      <c r="A25" s="41"/>
+      <c r="B25" s="39" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="26" ht="51" spans="1:2">
-      <c r="A26" s="33"/>
-      <c r="B26" s="31" t="s">
+      <c r="A26" s="41"/>
+      <c r="B26" s="39" t="s">
         <v>70</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="33"/>
-      <c r="B27" s="31" t="s">
+      <c r="A27" s="41"/>
+      <c r="B27" s="39" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="33"/>
-      <c r="B28" s="32" t="s">
+      <c r="A28" s="41"/>
+      <c r="B28" s="40" t="s">
         <v>72</v>
       </c>
     </row>
     <row r="29" ht="38.25" spans="1:2">
-      <c r="A29" s="34" t="s">
+      <c r="A29" s="42" t="s">
         <v>73</v>
       </c>
-      <c r="B29" s="31" t="s">
+      <c r="B29" s="39" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="30"/>
-      <c r="B30" s="31" t="s">
+      <c r="A30" s="38"/>
+      <c r="B30" s="39" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="30"/>
-      <c r="B31" s="31" t="s">
+      <c r="A31" s="38"/>
+      <c r="B31" s="39" t="s">
         <v>76</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="30"/>
-      <c r="B32" s="31" t="s">
+      <c r="A32" s="38"/>
+      <c r="B32" s="39" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="30"/>
-      <c r="B33" s="31" t="s">
+      <c r="A33" s="38"/>
+      <c r="B33" s="39" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="34" ht="51" spans="1:2">
-      <c r="A34" s="33" t="s">
+      <c r="A34" s="41" t="s">
         <v>79</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="1" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="35" ht="38.25" spans="1:2">
-      <c r="A35" s="30"/>
-      <c r="B35" s="7" t="s">
+      <c r="A35" s="38"/>
+      <c r="B35" s="1" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="36" ht="51" spans="1:2">
-      <c r="A36" s="30"/>
-      <c r="B36" s="7" t="s">
+      <c r="A36" s="38"/>
+      <c r="B36" s="1" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="37" ht="51" spans="1:2">
-      <c r="A37" s="30"/>
-      <c r="B37" s="7" t="s">
+      <c r="A37" s="38"/>
+      <c r="B37" s="1" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="38" ht="25.5" spans="1:2">
-      <c r="A38" s="30" t="s">
+      <c r="A38" s="38" t="s">
         <v>84</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="1" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="39" ht="76.5" spans="1:2">
-      <c r="A39" s="30"/>
-      <c r="B39" s="7" t="s">
+      <c r="A39" s="38"/>
+      <c r="B39" s="1" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="40" ht="25.5" spans="1:2">
-      <c r="A40" s="30"/>
-      <c r="B40" s="7" t="s">
+      <c r="A40" s="38"/>
+      <c r="B40" s="1" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="41" ht="25.5" spans="1:2">
-      <c r="A41" s="30"/>
-      <c r="B41" s="7" t="s">
+      <c r="A41" s="38"/>
+      <c r="B41" s="1" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="30"/>
-      <c r="B42" s="7" t="s">
+      <c r="A42" s="38"/>
+      <c r="B42" s="1" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="43" ht="25.5" spans="1:2">
-      <c r="A43" s="30"/>
-      <c r="B43" s="7" t="s">
+      <c r="A43" s="38"/>
+      <c r="B43" s="1" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="30"/>
-      <c r="B44" s="7"/>
+      <c r="A44" s="38"/>
+      <c r="B44" s="1"/>
     </row>
     <row r="45" ht="26.25" customHeight="1" spans="1:2">
-      <c r="A45" s="35" t="s">
+      <c r="A45" s="43" t="s">
         <v>91</v>
       </c>
-      <c r="B45" s="35"/>
+      <c r="B45" s="43"/>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="35"/>
-      <c r="B46" s="35"/>
+      <c r="A46" s="43"/>
+      <c r="B46" s="43"/>
     </row>
     <row r="47" ht="51" spans="1:2">
-      <c r="A47" s="30" t="s">
+      <c r="A47" s="38" t="s">
         <v>92</v>
       </c>
-      <c r="B47" s="36" t="s">
+      <c r="B47" s="44" t="s">
         <v>93</v>
       </c>
     </row>
@@ -4978,201 +5846,201 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="55.8533333333333" style="22" customWidth="1"/>
-    <col min="2" max="2" width="54.14" style="23" customWidth="1"/>
-    <col min="3" max="3" width="101.713333333333" style="24" customWidth="1"/>
+    <col min="1" max="1" width="55.8533333333333" style="30" customWidth="1"/>
+    <col min="2" max="2" width="54.14" style="31" customWidth="1"/>
+    <col min="3" max="3" width="101.713333333333" style="32" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" spans="1:1">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="33" t="s">
         <v>94</v>
       </c>
     </row>
     <row r="2" ht="12.75" spans="1:3">
-      <c r="A2" s="25"/>
-      <c r="B2" s="26"/>
-      <c r="C2" s="27"/>
+      <c r="A2" s="33"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="35"/>
     </row>
     <row r="3" ht="12.75" spans="1:2">
-      <c r="A3" s="25"/>
-      <c r="B3" s="26"/>
+      <c r="A3" s="33"/>
+      <c r="B3" s="34"/>
     </row>
     <row r="4" ht="12.75" spans="1:2">
-      <c r="A4" s="25"/>
-      <c r="B4" s="26"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="34"/>
     </row>
     <row r="5" ht="12.75" spans="1:2">
-      <c r="A5" s="25"/>
-      <c r="B5" s="26"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="34"/>
     </row>
     <row r="6" ht="12.75" spans="1:2">
-      <c r="A6" s="25"/>
-      <c r="B6" s="26"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="34"/>
     </row>
     <row r="7" ht="12.75" spans="1:2">
-      <c r="A7" s="25"/>
-      <c r="B7" s="26"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="34"/>
     </row>
     <row r="8" ht="12.75" spans="1:2">
-      <c r="A8" s="25"/>
-      <c r="B8" s="26"/>
+      <c r="A8" s="33"/>
+      <c r="B8" s="34"/>
     </row>
     <row r="9" ht="12.75" spans="1:2">
-      <c r="A9" s="25"/>
-      <c r="B9" s="26"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="34"/>
     </row>
     <row r="10" ht="12.75" spans="1:2">
-      <c r="A10" s="25"/>
-      <c r="B10" s="26"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="34"/>
     </row>
     <row r="11" ht="12.75" spans="1:2">
-      <c r="A11" s="25"/>
-      <c r="B11" s="26"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="34"/>
     </row>
     <row r="12" ht="12.75" spans="1:2">
-      <c r="A12" s="25"/>
-      <c r="B12" s="26"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="34"/>
     </row>
     <row r="13" ht="12.75" spans="1:2">
-      <c r="A13" s="25"/>
-      <c r="B13" s="26"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="34"/>
     </row>
     <row r="14" ht="12.75" spans="1:2">
-      <c r="A14" s="25"/>
-      <c r="B14" s="26"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="34"/>
     </row>
     <row r="15" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A15" s="25"/>
-      <c r="B15" s="26"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="34"/>
     </row>
     <row r="16" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A16" s="25"/>
-      <c r="B16" s="26"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="34"/>
     </row>
     <row r="17" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A17" s="25"/>
-      <c r="B17" s="26"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="34"/>
     </row>
     <row r="18" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A18" s="25"/>
-      <c r="B18" s="26"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="34"/>
     </row>
     <row r="19" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A19" s="25"/>
-      <c r="B19" s="26"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="34"/>
     </row>
     <row r="20" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A20" s="25"/>
-      <c r="B20" s="26"/>
+      <c r="A20" s="33"/>
+      <c r="B20" s="34"/>
     </row>
     <row r="21" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A21" s="25"/>
-      <c r="B21" s="26"/>
+      <c r="A21" s="33"/>
+      <c r="B21" s="34"/>
     </row>
     <row r="22" ht="17.25" spans="1:2">
-      <c r="A22" s="25"/>
-      <c r="B22" s="26"/>
+      <c r="A22" s="33"/>
+      <c r="B22" s="34"/>
     </row>
     <row r="23" ht="17.25" spans="1:2">
-      <c r="A23" s="25"/>
-      <c r="B23" s="26"/>
+      <c r="A23" s="33"/>
+      <c r="B23" s="34"/>
     </row>
     <row r="24" ht="17.25" spans="1:2">
-      <c r="A24" s="25"/>
-      <c r="B24" s="28"/>
+      <c r="A24" s="33"/>
+      <c r="B24" s="36"/>
     </row>
     <row r="26" ht="17.25" spans="1:2">
-      <c r="A26" s="25" t="s">
+      <c r="A26" s="33" t="s">
         <v>95</v>
       </c>
-      <c r="B26" s="23" t="s">
+      <c r="B26" s="31" t="s">
         <v>96</v>
       </c>
     </row>
     <row r="27" ht="17.25" spans="1:2">
-      <c r="A27" s="25"/>
-      <c r="B27" s="23" t="s">
+      <c r="A27" s="33"/>
+      <c r="B27" s="31" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="28" ht="17.25" spans="1:2">
-      <c r="A28" s="25"/>
-      <c r="B28" s="23" t="s">
+      <c r="A28" s="33"/>
+      <c r="B28" s="31" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="25"/>
+      <c r="A29" s="33"/>
     </row>
     <row r="30" ht="12.75" spans="1:3">
-      <c r="A30" s="25" t="s">
+      <c r="A30" s="33" t="s">
         <v>99</v>
       </c>
-      <c r="B30" s="23" t="s">
+      <c r="B30" s="31" t="s">
         <v>100</v>
       </c>
-      <c r="C30" s="24" t="s">
+      <c r="C30" s="32" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="31" ht="12.75" spans="1:3">
-      <c r="A31" s="25"/>
-      <c r="C31" s="24" t="s">
+      <c r="A31" s="33"/>
+      <c r="C31" s="32" t="s">
         <v>102</v>
       </c>
     </row>
     <row r="32" ht="12.75" spans="1:3">
-      <c r="A32" s="25"/>
-      <c r="C32" s="24" t="s">
+      <c r="A32" s="33"/>
+      <c r="C32" s="32" t="s">
         <v>103</v>
       </c>
     </row>
     <row r="33" ht="12.75" spans="1:3">
-      <c r="A33" s="25"/>
-      <c r="C33" s="24" t="s">
+      <c r="A33" s="33"/>
+      <c r="C33" s="32" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="35" ht="114.75" spans="1:3">
-      <c r="A35" s="25" t="s">
+      <c r="A35" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="B35" s="23" t="s">
+      <c r="B35" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="C35" s="43" t="s">
+      <c r="C35" s="51" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="36" ht="89.25" spans="1:3">
-      <c r="A36" s="25"/>
-      <c r="B36" s="23" t="s">
+      <c r="A36" s="33"/>
+      <c r="B36" s="31" t="s">
         <v>108</v>
       </c>
-      <c r="C36" s="43" t="s">
+      <c r="C36" s="51" t="s">
         <v>109</v>
       </c>
     </row>
     <row r="37" ht="76.5" spans="1:3">
-      <c r="A37" s="25"/>
-      <c r="B37" s="23" t="s">
+      <c r="A37" s="33"/>
+      <c r="B37" s="31" t="s">
         <v>110</v>
       </c>
-      <c r="C37" s="29" t="s">
+      <c r="C37" s="37" t="s">
         <v>111</v>
       </c>
     </row>
     <row r="38" ht="51" spans="1:3">
-      <c r="A38" s="25"/>
-      <c r="B38" s="23" t="s">
+      <c r="A38" s="33"/>
+      <c r="B38" s="31" t="s">
         <v>112</v>
       </c>
-      <c r="C38" s="29" t="s">
+      <c r="C38" s="37" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="25" t="s">
+      <c r="A40" s="33" t="s">
         <v>114</v>
       </c>
     </row>
@@ -5203,291 +6071,291 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="32" style="15" customWidth="1"/>
-    <col min="2" max="2" width="109" style="15" customWidth="1"/>
+    <col min="1" max="1" width="32" style="24" customWidth="1"/>
+    <col min="2" max="2" width="109" style="24" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="127.5" spans="1:3">
-      <c r="A1" s="16" t="s">
+      <c r="A1" s="25" t="s">
         <v>115</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="50" t="s">
         <v>116</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="26" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="2" ht="200.25" customHeight="1" spans="1:2">
-      <c r="A2" s="15" t="s">
+      <c r="A2" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="24" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="3" ht="102" spans="1:2">
-      <c r="A3" s="15" t="s">
+      <c r="A3" s="24" t="s">
         <v>120</v>
       </c>
-      <c r="B3" s="15" t="s">
+      <c r="B3" s="24" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="4" ht="25.5" spans="1:2">
-      <c r="A4" s="15" t="s">
+      <c r="A4" s="24" t="s">
         <v>122</v>
       </c>
-      <c r="B4" s="42" t="s">
+      <c r="B4" s="50" t="s">
         <v>123</v>
       </c>
     </row>
     <row r="5" ht="25.5" spans="1:2">
-      <c r="A5" s="15" t="s">
+      <c r="A5" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="24" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="6" ht="38.25" spans="1:1">
-      <c r="A6" s="15" t="s">
+      <c r="A6" s="24" t="s">
         <v>126</v>
       </c>
     </row>
     <row r="7" ht="38.25" spans="1:2">
-      <c r="A7" s="15" t="s">
+      <c r="A7" s="24" t="s">
         <v>127</v>
       </c>
-      <c r="B7" s="15" t="s">
+      <c r="B7" s="24" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="8" ht="114.75" spans="1:2">
-      <c r="A8" s="15" t="s">
+      <c r="A8" s="24" t="s">
         <v>129</v>
       </c>
-      <c r="B8" s="15" t="s">
+      <c r="B8" s="24" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="12" ht="51" spans="1:2">
-      <c r="A12" s="15" t="s">
+      <c r="A12" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="24" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="13" ht="51" spans="1:2">
-      <c r="A13" s="15" t="s">
+      <c r="A13" s="24" t="s">
         <v>133</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="24" t="s">
         <v>134</v>
       </c>
     </row>
     <row r="14" ht="89.25" spans="1:2">
-      <c r="A14" s="15" t="s">
+      <c r="A14" s="24" t="s">
         <v>135</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="24" t="s">
         <v>136</v>
       </c>
     </row>
     <row r="15" ht="102" spans="1:2">
-      <c r="A15" s="15" t="s">
+      <c r="A15" s="24" t="s">
         <v>137</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="24" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="15" t="s">
+      <c r="A16" s="24" t="s">
         <v>139</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="24" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="17" ht="178.5" spans="1:2">
-      <c r="A17" s="15" t="s">
+      <c r="A17" s="24" t="s">
         <v>141</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="24" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="18" ht="25.5" spans="1:2">
-      <c r="A18" s="15" t="s">
+      <c r="A18" s="24" t="s">
         <v>143</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="24" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="19" ht="280.5" spans="1:2">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="24" t="s">
         <v>145</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="24" t="s">
         <v>146</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="15" t="s">
+      <c r="A20" s="24" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="15" t="s">
+      <c r="A22" s="24" t="s">
         <v>148</v>
       </c>
     </row>
     <row r="23" spans="2:2">
-      <c r="B23" s="18"/>
+      <c r="B23" s="27"/>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="15" t="s">
+      <c r="A25" s="24" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="15" t="s">
+      <c r="A28" s="24" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="15" t="s">
+      <c r="A31" s="24" t="s">
         <v>151</v>
       </c>
-      <c r="B31" s="15" t="s">
+      <c r="B31" s="24" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="33" ht="38.25" spans="1:2">
-      <c r="A33" s="15" t="s">
+      <c r="A33" s="24" t="s">
         <v>153</v>
       </c>
-      <c r="B33" s="15" t="s">
+      <c r="B33" s="24" t="s">
         <v>154</v>
       </c>
     </row>
     <row r="34" ht="114.75" spans="1:2">
-      <c r="A34" s="15" t="s">
+      <c r="A34" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="B34" s="15" t="s">
+      <c r="B34" s="24" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="15" t="s">
+      <c r="A36" s="24" t="s">
         <v>157</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="15" t="s">
+      <c r="A38" s="24" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="15" t="s">
+      <c r="A40" s="24" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="15" t="s">
+      <c r="A42" s="24" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="15" t="s">
+      <c r="A44" s="24" t="s">
         <v>161</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="15" t="s">
+      <c r="A46" s="24" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="15" t="s">
+      <c r="A48" s="24" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="15" t="s">
+      <c r="A50" s="24" t="s">
         <v>164</v>
       </c>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="15" t="s">
+      <c r="A52" s="24" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="19" t="s">
+      <c r="A54" s="28" t="s">
         <v>166</v>
       </c>
-      <c r="B54" s="15" t="s">
+      <c r="B54" s="24" t="s">
         <v>167</v>
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="19"/>
-      <c r="B55" s="15" t="s">
+      <c r="A55" s="28"/>
+      <c r="B55" s="24" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="19"/>
-      <c r="B56" s="15" t="s">
+      <c r="A56" s="28"/>
+      <c r="B56" s="24" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="58" ht="25.5" spans="1:2">
-      <c r="A58" s="20" t="s">
+      <c r="A58" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="B58" s="15" t="s">
+      <c r="B58" s="24" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="20"/>
-      <c r="B59" s="21" t="s">
+      <c r="A59" s="8"/>
+      <c r="B59" s="29" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="60" spans="1:2">
-      <c r="A60" s="20"/>
-      <c r="B60" s="21" t="s">
+      <c r="A60" s="8"/>
+      <c r="B60" s="29" t="s">
         <v>173</v>
       </c>
     </row>
     <row r="61" spans="1:2">
-      <c r="A61" s="20"/>
-      <c r="B61" s="21" t="s">
+      <c r="A61" s="8"/>
+      <c r="B61" s="29" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="62" spans="1:2">
-      <c r="A62" s="20"/>
-      <c r="B62" s="21" t="s">
+      <c r="A62" s="8"/>
+      <c r="B62" s="29" t="s">
         <v>175</v>
       </c>
     </row>
     <row r="63" spans="1:2">
-      <c r="A63" s="20"/>
-      <c r="B63" s="21" t="s">
+      <c r="A63" s="8"/>
+      <c r="B63" s="29" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="20"/>
-      <c r="B64" s="21" t="s">
+      <c r="A64" s="8"/>
+      <c r="B64" s="29" t="s">
         <v>177</v>
       </c>
     </row>
@@ -5515,77 +6383,77 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21.75" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="47" style="9" customWidth="1"/>
-    <col min="2" max="2" width="125" style="10" customWidth="1"/>
-    <col min="3" max="3" width="60" style="11" customWidth="1"/>
-    <col min="4" max="16384" width="9.14" style="11"/>
+    <col min="1" max="1" width="47" style="18" customWidth="1"/>
+    <col min="2" max="2" width="125" style="19" customWidth="1"/>
+    <col min="3" max="3" width="60" style="20" customWidth="1"/>
+    <col min="4" max="16384" width="9.14" style="20"/>
   </cols>
   <sheetData>
     <row r="1" ht="120.75" spans="1:2">
-      <c r="A1" s="9" t="s">
+      <c r="A1" s="18" t="s">
         <v>178</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="B1" s="21" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="2" ht="138" spans="2:2">
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="21" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="3" ht="172.5" spans="1:3">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="18" t="s">
         <v>181</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="21" t="s">
         <v>182</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="22" t="s">
         <v>183</v>
       </c>
     </row>
     <row r="4" ht="103.5" spans="1:2">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="18" t="s">
         <v>184</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="21" t="s">
         <v>185</v>
       </c>
     </row>
     <row r="5" ht="65.25" spans="1:2">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="23" t="s">
         <v>186</v>
       </c>
-      <c r="B5" s="12"/>
+      <c r="B5" s="21"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="18" t="s">
         <v>187</v>
       </c>
-      <c r="B6" s="12"/>
+      <c r="B6" s="21"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="9" t="s">
+      <c r="A7" s="18" t="s">
         <v>188</v>
       </c>
-      <c r="B7" s="12"/>
+      <c r="B7" s="21"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="9" t="s">
+      <c r="A8" s="18" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="9" ht="34.5" spans="1:2">
-      <c r="A9" s="9" t="s">
+      <c r="A9" s="18" t="s">
         <v>190</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="21" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="9" t="s">
+      <c r="A10" s="18" t="s">
         <v>192</v>
       </c>
     </row>
@@ -5648,7 +6516,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="76.5" spans="3:3">
-      <c r="C1" s="8" t="s">
+      <c r="C1" s="17" t="s">
         <v>193</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[DSA][Overview][Data structure and Algorithm in Java book]
</commit_message>
<xml_diff>
--- a/System/Documents.xlsx
+++ b/System/Documents.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="13530" firstSheet="13" activeTab="19"/>
+    <workbookView windowWidth="28695" windowHeight="13530" firstSheet="14" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="Trang_tính1" sheetId="1" state="hidden" r:id="rId1"/>
@@ -27,13 +27,14 @@
     <sheet name="KAFKA" sheetId="36" r:id="rId18"/>
     <sheet name="Two phases commit" sheetId="37" r:id="rId19"/>
     <sheet name="Designing_Data_Intensive_Applic" sheetId="40" r:id="rId20"/>
+    <sheet name="Headfirst Design Pattern" sheetId="41" r:id="rId21"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="487" uniqueCount="485">
   <si>
     <t>Kiến Trúc về Microservice</t>
   </si>
@@ -10280,6 +10281,65 @@
 Reliable, Scalable, and Maintainable Applications</t>
   </si>
   <si>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> - Many applications today are </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>data-intensive</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, as opposed to </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>compute-intensive.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Raw CPU power is rarely a limiting factor for these applications—bigger problems are usually the amount of data, the complexity of data, and the speed at which it is changing.</t>
+    </r>
+  </si>
+  <si>
+    <t>Thinking About Data Systems</t>
+  </si>
+  <si>
     <t>Chapter 2.
 Data Models and Query Languages</t>
   </si>
@@ -10330,6 +10390,48 @@
   <si>
     <t>Chapter 12.
 The Future of Data Systems</t>
+  </si>
+  <si>
+    <t>1. Welcome to Design Pattern</t>
+  </si>
+  <si>
+    <t>2. Observer Pattern</t>
+  </si>
+  <si>
+    <t>3. Decorator Pattern</t>
+  </si>
+  <si>
+    <t>4. Factory Pattern</t>
+  </si>
+  <si>
+    <t>5. Singleton Pattern</t>
+  </si>
+  <si>
+    <t>6. Command Pattern</t>
+  </si>
+  <si>
+    <t>7. Adapter and Facade Pattern</t>
+  </si>
+  <si>
+    <t>8. Template Method Pattern</t>
+  </si>
+  <si>
+    <t>9. Iterator and Composite Pattern</t>
+  </si>
+  <si>
+    <t>10. State Pattern</t>
+  </si>
+  <si>
+    <t>11. Proxy Pattern</t>
+  </si>
+  <si>
+    <t>12. Compound patterns</t>
+  </si>
+  <si>
+    <t>13. Patterns in the Real World</t>
+  </si>
+  <si>
+    <t>14. Leftover Pattern</t>
   </si>
 </sst>
 </file>
@@ -10337,10 +10439,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="45">
     <font>
@@ -10503,6 +10605,14 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF800080"/>
@@ -10512,23 +10622,45 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="13"/>
+      <sz val="15"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
-      <sz val="18"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -10544,38 +10676,8 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -10596,22 +10698,15 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <i/>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -10622,6 +10717,22 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <i/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -10670,15 +10781,6 @@
     </font>
     <font>
       <b/>
-      <i/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
@@ -10718,6 +10820,30 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -10730,13 +10856,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10748,7 +10886,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10760,13 +10904,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10778,43 +10952,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10826,7 +10970,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10838,49 +10982,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -10956,7 +11058,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -10965,7 +11067,7 @@
       <right/>
       <top/>
       <bottom style="medium">
-        <color theme="4"/>
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -11032,15 +11134,6 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top style="thin">
         <color theme="4"/>
       </top>
@@ -11049,120 +11142,129 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="30" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="37" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="34" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="36" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="10" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="21" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="14" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="10" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="28" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -11171,19 +11273,19 @@
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="11" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="24" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -11191,7 +11293,7 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="72">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -11200,31 +11302,19 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -11309,9 +11399,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="48" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -12113,199 +12200,199 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="12.75" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="9.14" style="68"/>
-    <col min="2" max="2" width="39.5733333333333" style="68" customWidth="1"/>
-    <col min="3" max="3" width="95.5733333333333" style="68" customWidth="1"/>
-    <col min="4" max="4" width="60.7133333333333" style="68" customWidth="1"/>
-    <col min="5" max="5" width="58.8533333333333" style="68" customWidth="1"/>
-    <col min="6" max="6" width="50" style="68" customWidth="1"/>
-    <col min="7" max="7" width="49.7133333333333" style="68" customWidth="1"/>
-    <col min="8" max="16384" width="9.14" style="68"/>
+    <col min="1" max="1" width="9.14" style="63"/>
+    <col min="2" max="2" width="39.5733333333333" style="63" customWidth="1"/>
+    <col min="3" max="3" width="95.5733333333333" style="63" customWidth="1"/>
+    <col min="4" max="4" width="60.7133333333333" style="63" customWidth="1"/>
+    <col min="5" max="5" width="58.8533333333333" style="63" customWidth="1"/>
+    <col min="6" max="6" width="50" style="63" customWidth="1"/>
+    <col min="7" max="7" width="49.7133333333333" style="63" customWidth="1"/>
+    <col min="8" max="16384" width="9.14" style="63"/>
   </cols>
   <sheetData>
     <row r="1" ht="76.5" spans="1:3">
-      <c r="A1" s="68">
+      <c r="A1" s="63">
         <v>1</v>
       </c>
-      <c r="B1" s="68" t="s">
+      <c r="B1" s="63" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="67" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" ht="63.75" spans="1:3">
-      <c r="A2" s="68">
+      <c r="A2" s="63">
         <v>2</v>
       </c>
-      <c r="B2" s="68" t="s">
+      <c r="B2" s="63" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="72" t="s">
+      <c r="C2" s="67" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" ht="38.25" spans="1:3">
-      <c r="A3" s="68">
+      <c r="A3" s="63">
         <v>3</v>
       </c>
-      <c r="B3" s="70" t="s">
+      <c r="B3" s="65" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="72" t="s">
+      <c r="C3" s="67" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" ht="38.25" spans="1:3">
-      <c r="A4" s="68">
+      <c r="A4" s="63">
         <v>4</v>
       </c>
-      <c r="B4" s="68" t="s">
+      <c r="B4" s="63" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="73" t="s">
+      <c r="C4" s="68" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" ht="178.5" spans="1:3">
-      <c r="A5" s="68">
+      <c r="A5" s="63">
         <v>5</v>
       </c>
-      <c r="B5" s="68" t="s">
+      <c r="B5" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="27" t="s">
+      <c r="C5" s="23" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="6" ht="25.5" spans="1:3">
-      <c r="A6" s="68">
+      <c r="A6" s="63">
         <v>6</v>
       </c>
-      <c r="B6" s="68" t="s">
+      <c r="B6" s="63" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="73" t="s">
+      <c r="C6" s="68" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" ht="229.5" spans="1:3">
-      <c r="A7" s="68">
+      <c r="A7" s="63">
         <v>7</v>
       </c>
-      <c r="B7" s="68" t="s">
+      <c r="B7" s="63" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="69" t="s">
+      <c r="C7" s="64" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" ht="245.25" customHeight="1" spans="1:3">
-      <c r="A8" s="68">
+      <c r="A8" s="63">
         <v>8</v>
       </c>
-      <c r="B8" s="68" t="s">
+      <c r="B8" s="63" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="69" t="s">
+      <c r="C8" s="64" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" ht="223.5" customHeight="1" spans="1:3">
-      <c r="A9" s="68">
+      <c r="A9" s="63">
         <v>9</v>
       </c>
-      <c r="B9" s="68" t="s">
+      <c r="B9" s="63" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="72" t="s">
+      <c r="C9" s="67" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" ht="204" spans="1:4">
-      <c r="A10" s="68">
+      <c r="A10" s="63">
         <v>10</v>
       </c>
-      <c r="B10" s="68" t="s">
+      <c r="B10" s="63" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="27" t="s">
+      <c r="C10" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="71" t="s">
+      <c r="D10" s="66" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" ht="25.5" spans="2:3">
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="63" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="27" t="s">
+      <c r="C11" s="23" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="12" ht="102" spans="2:3">
-      <c r="B12" s="68" t="s">
+      <c r="B12" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="27" t="s">
+      <c r="C12" s="23" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="13" ht="140.25" spans="2:3">
-      <c r="B13" s="68" t="s">
+      <c r="B13" s="63" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="27" t="s">
+      <c r="C13" s="23" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="14" ht="288.75" customHeight="1" spans="2:7">
-      <c r="B14" s="68" t="s">
+      <c r="B14" s="63" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="27" t="s">
+      <c r="C14" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="69" t="s">
+      <c r="D14" s="64" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="27" t="s">
+      <c r="E14" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="27" t="s">
+      <c r="F14" s="23" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="27" t="s">
+      <c r="G14" s="23" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="15" ht="38.25" spans="2:3">
-      <c r="B15" s="68" t="s">
+      <c r="B15" s="63" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="27" t="s">
+      <c r="C15" s="23" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" ht="240.75" customHeight="1" spans="2:2">
-      <c r="B16" s="68" t="s">
+      <c r="B16" s="63" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" ht="153" spans="2:3">
-      <c r="B17" s="68" t="s">
+      <c r="B17" s="63" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="69" t="s">
+      <c r="C17" s="64" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="18" ht="153" spans="2:3">
-      <c r="B18" s="68" t="s">
+      <c r="B18" s="63" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="69" t="s">
+      <c r="C18" s="64" t="s">
         <v>39</v>
       </c>
     </row>
@@ -12334,7 +12421,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="76.5" spans="3:3">
-      <c r="C1" s="20" t="s">
+      <c r="C1" s="16" t="s">
         <v>406</v>
       </c>
     </row>
@@ -12375,12 +12462,12 @@
   </cols>
   <sheetData>
     <row r="1" ht="89.25" spans="4:4">
-      <c r="D1" s="7" t="s">
+      <c r="D1" s="6" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="2" ht="350" customHeight="1" spans="4:4">
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="16" t="s">
         <v>408</v>
       </c>
     </row>
@@ -12407,57 +12494,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="10" t="s">
         <v>409</v>
       </c>
-      <c r="B1" s="15" t="s">
+      <c r="B1" s="11" t="s">
         <v>410</v>
       </c>
-      <c r="C1" s="16" t="s">
+      <c r="C1" s="12" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="13" t="s">
         <v>412</v>
       </c>
-      <c r="B2" s="18"/>
-      <c r="C2" s="17"/>
+      <c r="B2" s="14"/>
+      <c r="C2" s="13"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="10" t="s">
         <v>413</v>
       </c>
-      <c r="B3" s="18"/>
-      <c r="C3" s="14"/>
+      <c r="B3" s="14"/>
+      <c r="C3" s="10"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="13" t="s">
         <v>414</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="17"/>
+      <c r="B4" s="14"/>
+      <c r="C4" s="13"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="10" t="s">
         <v>415</v>
       </c>
-      <c r="B5" s="18"/>
-      <c r="C5" s="14"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="10"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="13" t="s">
         <v>416</v>
       </c>
-      <c r="B6" s="18"/>
-      <c r="C6" s="17"/>
+      <c r="B6" s="14"/>
+      <c r="C6" s="13"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="10" t="s">
         <v>417</v>
       </c>
-      <c r="B7" s="19"/>
-      <c r="C7" s="14"/>
+      <c r="B7" s="15"/>
+      <c r="C7" s="10"/>
     </row>
     <row r="8" customFormat="1"/>
     <row r="9" customFormat="1"/>
@@ -12537,104 +12624,104 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="12.1" style="10" customWidth="1"/>
-    <col min="2" max="2" width="168" style="8" customWidth="1"/>
+    <col min="1" max="1" width="12.1" style="7" customWidth="1"/>
+    <col min="2" max="2" width="168" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="267.75" spans="1:2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
         <v>424</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="5" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="2" ht="76.5" spans="1:2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="7" t="s">
         <v>426</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="3" t="s">
         <v>427</v>
       </c>
     </row>
     <row r="3" ht="38.25" spans="1:2">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="7" t="s">
         <v>428</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="3" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="4" ht="127.5" spans="1:2">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="7" t="s">
         <v>430</v>
       </c>
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="5" t="s">
         <v>431</v>
       </c>
     </row>
     <row r="5" ht="114.75" spans="2:2">
-      <c r="B5" s="11" t="s">
+      <c r="B5" s="5" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="6" ht="51" spans="1:2">
-      <c r="A6" s="10" t="s">
+      <c r="A6" s="7" t="s">
         <v>433</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="3" t="s">
         <v>434</v>
       </c>
     </row>
     <row r="7" ht="63.75" spans="1:2">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="7" t="s">
         <v>435</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="3" t="s">
         <v>436</v>
       </c>
     </row>
     <row r="8" ht="38.25" spans="1:2">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="7" t="s">
         <v>437</v>
       </c>
-      <c r="B8" s="8" t="s">
+      <c r="B8" s="3" t="s">
         <v>438</v>
       </c>
     </row>
     <row r="9" ht="38.25" spans="1:2">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="7" t="s">
         <v>439</v>
       </c>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="3" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="10" ht="38.25" spans="1:2">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="7" t="s">
         <v>441</v>
       </c>
-      <c r="B10" s="8" t="s">
+      <c r="B10" s="3" t="s">
         <v>442</v>
       </c>
     </row>
     <row r="11" ht="127.5" spans="1:2">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="9" t="s">
         <v>443</v>
       </c>
-      <c r="B11" s="11" t="s">
+      <c r="B11" s="5" t="s">
         <v>444</v>
       </c>
     </row>
     <row r="12" ht="51" spans="1:2">
-      <c r="A12" s="13"/>
-      <c r="B12" s="11" t="s">
+      <c r="A12" s="9"/>
+      <c r="B12" s="5" t="s">
         <v>445</v>
       </c>
     </row>
     <row r="13" ht="102" spans="1:2">
-      <c r="A13" s="13"/>
-      <c r="B13" s="8" t="s">
+      <c r="A13" s="9"/>
+      <c r="B13" s="3" t="s">
         <v>446</v>
       </c>
     </row>
@@ -12662,23 +12749,23 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="13" style="10" customWidth="1"/>
-    <col min="2" max="2" width="160.3" style="8" customWidth="1"/>
+    <col min="1" max="1" width="13" style="7" customWidth="1"/>
+    <col min="2" max="2" width="160.3" style="3" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="7" t="s">
         <v>447</v>
       </c>
-      <c r="B1" s="11" t="s">
+      <c r="B1" s="5" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="2" ht="153" spans="1:2">
-      <c r="A2" s="10" t="s">
+      <c r="A2" s="7" t="s">
         <v>449</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="8" t="s">
         <v>450</v>
       </c>
     </row>
@@ -12735,20 +12822,20 @@
   </cols>
   <sheetData>
     <row r="1" ht="25.5" spans="2:2">
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>451</v>
       </c>
     </row>
     <row r="3" ht="51" spans="1:2">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>452</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="3" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="4" spans="2:2">
-      <c r="B4" s="9"/>
+      <c r="B4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -12767,132 +12854,132 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85333333333333" defaultRowHeight="21.75" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="17" style="26" customWidth="1"/>
-    <col min="2" max="2" width="15.8533333333333" style="57" customWidth="1"/>
-    <col min="3" max="3" width="13.8533333333333" style="58" customWidth="1"/>
-    <col min="4" max="4" width="156.14" style="59" customWidth="1"/>
+    <col min="1" max="1" width="17" style="22" customWidth="1"/>
+    <col min="2" max="2" width="15.8533333333333" style="52" customWidth="1"/>
+    <col min="3" max="3" width="13.8533333333333" style="53" customWidth="1"/>
+    <col min="4" max="4" width="156.14" style="54" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="90" customHeight="1" spans="2:4">
-      <c r="B1" s="57" t="s">
+      <c r="B1" s="52" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="60" t="s">
+      <c r="C1" s="55" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="61"/>
+      <c r="D1" s="56"/>
     </row>
     <row r="2" ht="57" customHeight="1" spans="3:4">
-      <c r="C2" s="62" t="s">
+      <c r="C2" s="57" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="63"/>
+      <c r="D2" s="58"/>
     </row>
     <row r="3" ht="151" customHeight="1" spans="1:4">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="57" t="s">
+      <c r="B3" s="52" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="64" t="s">
+      <c r="C3" s="59" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="61"/>
+      <c r="D3" s="56"/>
     </row>
     <row r="4" ht="66" customHeight="1" spans="2:4">
-      <c r="B4" s="57" t="s">
+      <c r="B4" s="52" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="60" t="s">
+      <c r="C4" s="55" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="61"/>
+      <c r="D4" s="56"/>
     </row>
     <row r="5" ht="114" customHeight="1" spans="2:4">
-      <c r="B5" s="57" t="s">
+      <c r="B5" s="52" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="60" t="s">
+      <c r="C5" s="55" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="61"/>
+      <c r="D5" s="56"/>
     </row>
     <row r="6" ht="33.95" customHeight="1" spans="2:5">
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="66" t="s">
+      <c r="C6" s="61" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="61" t="s">
+      <c r="D6" s="56" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="8"/>
+      <c r="E6" s="3"/>
     </row>
     <row r="7" ht="45" customHeight="1" spans="2:3">
-      <c r="B7" s="57" t="s">
+      <c r="B7" s="52" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="60" t="s">
+      <c r="C7" s="55" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="8" ht="30" customHeight="1" spans="2:3">
-      <c r="B8" s="57" t="s">
+      <c r="B8" s="52" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="64" t="s">
+      <c r="C8" s="59" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="9" ht="25.5" spans="1:4">
-      <c r="A9" s="26" t="s">
+      <c r="A9" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="57" t="s">
+      <c r="B9" s="52" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="49" t="s">
+      <c r="C9" s="44" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="67" t="s">
+      <c r="D9" s="62" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="10" ht="25.5" spans="3:4">
-      <c r="C10" s="49" t="s">
+      <c r="C10" s="44" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="61" t="s">
+      <c r="D10" s="56" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="11" ht="38.25" spans="3:4">
-      <c r="C11" s="49" t="s">
+      <c r="C11" s="44" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="67" t="s">
+      <c r="D11" s="62" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="12" spans="2:4">
-      <c r="B12" s="49" t="s">
+      <c r="B12" s="44" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="61" t="s">
+      <c r="C12" s="56" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="61"/>
+      <c r="D12" s="56"/>
     </row>
     <row r="13" ht="308" customHeight="1" spans="2:4">
-      <c r="B13" s="57" t="s">
+      <c r="B13" s="52" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="64" t="s">
+      <c r="C13" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="61"/>
+      <c r="D13" s="56"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -12921,133 +13008,96 @@
   <sheetPr/>
   <dimension ref="A1:E54"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="24" outlineLevelCol="4"/>
   <cols>
     <col min="1" max="1" width="26.8" style="1" customWidth="1"/>
     <col min="2" max="2" width="25.6" style="2" customWidth="1"/>
-    <col min="3" max="4" width="8.8" style="3"/>
-    <col min="5" max="5" width="110.7" style="3" customWidth="1"/>
+    <col min="3" max="3" width="8.8" style="3"/>
+    <col min="4" max="4" width="8.8" style="4"/>
+    <col min="5" max="5" width="110.7" style="4" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="72" spans="1:5">
-      <c r="A1" s="4" t="s">
+    <row r="1" ht="32" customHeight="1" spans="1:3">
+      <c r="A1" s="1" t="s">
         <v>454</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
         <v>455</v>
       </c>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-    </row>
-    <row r="2" spans="1:2">
-      <c r="A2" s="4"/>
-      <c r="B2" s="5"/>
-    </row>
-    <row r="3" ht="30" customHeight="1" spans="1:2">
-      <c r="A3" s="4"/>
-      <c r="B3" s="5"/>
-    </row>
-    <row r="4" ht="34" customHeight="1" spans="1:2">
-      <c r="A4" s="4"/>
-      <c r="B4" s="5"/>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="4"/>
-      <c r="B5" s="5"/>
-    </row>
-    <row r="6" ht="54" spans="1:2">
-      <c r="A6" s="4"/>
+      <c r="C1" s="5" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="2" ht="51" spans="3:3">
+      <c r="C2" s="3" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="3" ht="30" customHeight="1"/>
+    <row r="4" ht="34" customHeight="1"/>
+    <row r="6" spans="2:2">
       <c r="B6" s="2" t="s">
-        <v>456</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1">
-      <c r="A7" s="4"/>
-    </row>
-    <row r="8" spans="1:1">
-      <c r="A8" s="4"/>
-    </row>
-    <row r="9" spans="1:1">
-      <c r="A9" s="4"/>
-    </row>
-    <row r="10" ht="36" spans="1:2">
-      <c r="A10" s="4"/>
+        <v>458</v>
+      </c>
+    </row>
+    <row r="10" spans="2:2">
       <c r="B10" s="2" t="s">
-        <v>457</v>
-      </c>
-    </row>
-    <row r="11" spans="1:1">
-      <c r="A11" s="4"/>
-    </row>
-    <row r="12" spans="1:1">
-      <c r="A12" s="4"/>
-    </row>
-    <row r="13" spans="1:1">
-      <c r="A13" s="4"/>
-    </row>
-    <row r="14" ht="36" spans="1:2">
-      <c r="A14" s="4"/>
+        <v>459</v>
+      </c>
+    </row>
+    <row r="14" spans="2:2">
       <c r="B14" s="2" t="s">
-        <v>458</v>
-      </c>
-    </row>
-    <row r="15" spans="1:1">
-      <c r="A15" s="4"/>
-    </row>
-    <row r="16" spans="1:1">
-      <c r="A16" s="4"/>
-    </row>
-    <row r="17" ht="36" spans="1:2">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="17" ht="12.75" spans="1:2">
       <c r="A17" s="1" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>460</v>
-      </c>
-    </row>
-    <row r="19" ht="48"/>
-    <row r="22" ht="36" spans="2:2">
+        <v>462</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2">
       <c r="B22" s="2" t="s">
-        <v>461</v>
-      </c>
-    </row>
-    <row r="28" ht="36" spans="2:2">
+        <v>463</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2">
       <c r="B28" s="2" t="s">
-        <v>462</v>
-      </c>
-    </row>
-    <row r="32" ht="54" spans="2:2">
+        <v>464</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2">
       <c r="B32" s="2" t="s">
-        <v>463</v>
-      </c>
-    </row>
-    <row r="37" ht="54" spans="2:2">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="37" spans="2:2">
       <c r="B37" s="2" t="s">
-        <v>464</v>
-      </c>
-    </row>
-    <row r="42" ht="36" spans="1:2">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="42" ht="12.75" spans="1:2">
       <c r="A42" s="1" t="s">
-        <v>465</v>
+        <v>467</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="43" ht="48"/>
-    <row r="46" ht="36" spans="2:2">
+        <v>468</v>
+      </c>
+    </row>
+    <row r="46" spans="2:2">
       <c r="B46" s="2" t="s">
-        <v>467</v>
-      </c>
-    </row>
-    <row r="50" ht="54" spans="2:2">
+        <v>469</v>
+      </c>
+    </row>
+    <row r="50" spans="2:2">
       <c r="B50" s="2" t="s">
-        <v>468</v>
+        <v>470</v>
       </c>
     </row>
   </sheetData>
@@ -13074,6 +13124,96 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75"/>
+  <cols>
+    <col min="1" max="1" width="25.6" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" t="s">
+        <v>472</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>475</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>476</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" t="s">
+        <v>477</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" t="s">
+        <v>479</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" t="s">
+        <v>480</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" t="s">
+        <v>481</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1">
+      <c r="A12" t="s">
+        <v>482</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1">
+      <c r="A13" t="s">
+        <v>483</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1">
+      <c r="A14" t="s">
+        <v>484</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
@@ -13085,1197 +13225,1197 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="20.5" style="48" customWidth="1"/>
-    <col min="2" max="2" width="14.5733333333333" style="49" customWidth="1"/>
-    <col min="3" max="3" width="15.7133333333333" style="49" customWidth="1"/>
-    <col min="4" max="4" width="167.106666666667" style="23" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="23"/>
+    <col min="1" max="1" width="20.5" style="1" customWidth="1"/>
+    <col min="2" max="2" width="14.5733333333333" style="44" customWidth="1"/>
+    <col min="3" max="3" width="15.7133333333333" style="44" customWidth="1"/>
+    <col min="4" max="4" width="167.106666666667" style="19" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="19"/>
   </cols>
   <sheetData>
-    <row r="1" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A1" s="50" t="s">
+    <row r="1" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A1" s="45" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="9" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="49" t="s">
+      <c r="C1" s="44" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="11"/>
-    </row>
-    <row r="2" s="23" customFormat="1" ht="357" spans="1:4">
-      <c r="A2" s="51"/>
-      <c r="B2" s="13"/>
-      <c r="C2" s="49" t="s">
+      <c r="D1" s="5"/>
+    </row>
+    <row r="2" s="19" customFormat="1" ht="357" spans="1:4">
+      <c r="A2" s="46"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="44" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="11" t="s">
+      <c r="D2" s="5" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" s="23" customFormat="1" ht="89.25" spans="1:4">
-      <c r="A3" s="51"/>
-      <c r="B3" s="52" t="s">
+    <row r="3" s="19" customFormat="1" ht="89.25" spans="1:4">
+      <c r="A3" s="46"/>
+      <c r="B3" s="47" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="49" t="s">
+      <c r="C3" s="44" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="5" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="4" s="23" customFormat="1" ht="76.5" spans="1:4">
-      <c r="A4" s="51"/>
-      <c r="B4" s="52"/>
-      <c r="C4" s="49" t="s">
+    <row r="4" s="19" customFormat="1" ht="76.5" spans="1:4">
+      <c r="A4" s="46"/>
+      <c r="B4" s="47"/>
+      <c r="C4" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="11" t="s">
+      <c r="D4" s="5" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" s="23" customFormat="1" ht="229.5" spans="1:4">
-      <c r="A5" s="51"/>
-      <c r="B5" s="52"/>
-      <c r="C5" s="49" t="s">
+    <row r="5" s="19" customFormat="1" ht="229.5" spans="1:4">
+      <c r="A5" s="46"/>
+      <c r="B5" s="47"/>
+      <c r="C5" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="5" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" s="23" customFormat="1" ht="63.75" spans="1:4">
-      <c r="A6" s="51"/>
-      <c r="B6" s="52"/>
-      <c r="C6" s="49" t="s">
+    <row r="6" s="19" customFormat="1" ht="63.75" spans="1:4">
+      <c r="A6" s="46"/>
+      <c r="B6" s="47"/>
+      <c r="C6" s="44" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="11" t="s">
+      <c r="D6" s="5" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="7" s="23" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A7" s="51"/>
-      <c r="B7" s="52"/>
-      <c r="C7" s="49" t="s">
+    <row r="7" s="19" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A7" s="46"/>
+      <c r="B7" s="47"/>
+      <c r="C7" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="D7" s="11" t="s">
+      <c r="D7" s="5" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="8" s="23" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A8" s="51"/>
-      <c r="B8" s="52"/>
-      <c r="C8" s="49" t="s">
+    <row r="8" s="19" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A8" s="46"/>
+      <c r="B8" s="47"/>
+      <c r="C8" s="44" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="11" t="s">
+      <c r="D8" s="5" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A9" s="51"/>
-      <c r="B9" s="52"/>
-      <c r="C9" s="49" t="s">
+    <row r="9" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A9" s="46"/>
+      <c r="B9" s="47"/>
+      <c r="C9" s="44" t="s">
         <v>87</v>
       </c>
-      <c r="D9" s="11"/>
-    </row>
-    <row r="10" s="23" customFormat="1" ht="216.75" spans="1:4">
-      <c r="A10" s="51"/>
-      <c r="B10" s="52"/>
-      <c r="C10" s="49" t="s">
+      <c r="D9" s="5"/>
+    </row>
+    <row r="10" s="19" customFormat="1" ht="216.75" spans="1:4">
+      <c r="A10" s="46"/>
+      <c r="B10" s="47"/>
+      <c r="C10" s="44" t="s">
         <v>88</v>
       </c>
-      <c r="D10" s="11" t="s">
+      <c r="D10" s="5" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="11" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A11" s="51"/>
-      <c r="B11" s="52"/>
-      <c r="C11" s="49" t="s">
+    <row r="11" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A11" s="46"/>
+      <c r="B11" s="47"/>
+      <c r="C11" s="44" t="s">
         <v>90</v>
       </c>
-      <c r="D11" s="11"/>
-    </row>
-    <row r="12" s="23" customFormat="1" ht="12.75" spans="1:3">
-      <c r="A12" s="51"/>
-      <c r="B12" s="52"/>
-      <c r="C12" s="49" t="s">
+      <c r="D11" s="5"/>
+    </row>
+    <row r="12" s="19" customFormat="1" ht="12.75" spans="1:3">
+      <c r="A12" s="46"/>
+      <c r="B12" s="47"/>
+      <c r="C12" s="44" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="13" s="23" customFormat="1" ht="107.25" customHeight="1" spans="1:4">
-      <c r="A13" s="51"/>
-      <c r="B13" s="52" t="s">
+    <row r="13" s="19" customFormat="1" ht="107.25" customHeight="1" spans="1:4">
+      <c r="A13" s="46"/>
+      <c r="B13" s="47" t="s">
         <v>92</v>
       </c>
-      <c r="C13" s="11" t="s">
+      <c r="C13" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="D13" s="11"/>
-    </row>
-    <row r="14" s="23" customFormat="1" ht="89.25" spans="1:4">
-      <c r="A14" s="51"/>
-      <c r="B14" s="52"/>
-      <c r="C14" s="49" t="s">
+      <c r="D13" s="5"/>
+    </row>
+    <row r="14" s="19" customFormat="1" ht="89.25" spans="1:4">
+      <c r="A14" s="46"/>
+      <c r="B14" s="47"/>
+      <c r="C14" s="44" t="s">
         <v>94</v>
       </c>
-      <c r="D14" s="11" t="s">
+      <c r="D14" s="5" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="15" s="23" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A15" s="51"/>
-      <c r="B15" s="52"/>
-      <c r="C15" s="49" t="s">
+    <row r="15" s="19" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A15" s="46"/>
+      <c r="B15" s="47"/>
+      <c r="C15" s="44" t="s">
         <v>96</v>
       </c>
-      <c r="D15" s="11" t="s">
+      <c r="D15" s="5" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="16" s="23" customFormat="1" ht="89.25" spans="1:4">
-      <c r="A16" s="51"/>
-      <c r="B16" s="52"/>
-      <c r="C16" s="49"/>
-      <c r="D16" s="11" t="s">
+    <row r="16" s="19" customFormat="1" ht="89.25" spans="1:4">
+      <c r="A16" s="46"/>
+      <c r="B16" s="47"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="5" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="17" s="23" customFormat="1" ht="63.75" spans="1:4">
-      <c r="A17" s="51"/>
-      <c r="B17" s="52"/>
-      <c r="C17" s="49"/>
-      <c r="D17" s="11" t="s">
+    <row r="17" s="19" customFormat="1" ht="63.75" spans="1:4">
+      <c r="A17" s="46"/>
+      <c r="B17" s="47"/>
+      <c r="C17" s="44"/>
+      <c r="D17" s="5" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="18" s="23" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A18" s="51"/>
-      <c r="B18" s="52"/>
-      <c r="C18" s="49"/>
-      <c r="D18" s="11" t="s">
+    <row r="18" s="19" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A18" s="46"/>
+      <c r="B18" s="47"/>
+      <c r="C18" s="44"/>
+      <c r="D18" s="5" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="19" s="23" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A19" s="51"/>
-      <c r="B19" s="52"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="11" t="s">
+    <row r="19" s="19" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A19" s="46"/>
+      <c r="B19" s="47"/>
+      <c r="C19" s="44"/>
+      <c r="D19" s="5" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="20" s="23" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A20" s="51"/>
-      <c r="B20" s="52"/>
-      <c r="C20" s="49"/>
-      <c r="D20" s="11" t="s">
+    <row r="20" s="19" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A20" s="46"/>
+      <c r="B20" s="47"/>
+      <c r="C20" s="44"/>
+      <c r="D20" s="5" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="21" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A21" s="51"/>
-      <c r="B21" s="52"/>
-      <c r="C21" s="49"/>
-      <c r="D21" s="11" t="s">
+    <row r="21" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A21" s="46"/>
+      <c r="B21" s="47"/>
+      <c r="C21" s="44"/>
+      <c r="D21" s="5" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="22" s="23" customFormat="1" ht="76.5" spans="1:4">
-      <c r="A22" s="51"/>
-      <c r="B22" s="52"/>
-      <c r="C22" s="49" t="s">
+    <row r="22" s="19" customFormat="1" ht="76.5" spans="1:4">
+      <c r="A22" s="46"/>
+      <c r="B22" s="47"/>
+      <c r="C22" s="44" t="s">
         <v>104</v>
       </c>
-      <c r="D22" s="11" t="s">
+      <c r="D22" s="5" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="23" s="23" customFormat="1" ht="76.5" spans="1:4">
-      <c r="A23" s="51"/>
-      <c r="B23" s="52"/>
-      <c r="C23" s="49"/>
-      <c r="D23" s="11" t="s">
+    <row r="23" s="19" customFormat="1" ht="76.5" spans="1:4">
+      <c r="A23" s="46"/>
+      <c r="B23" s="47"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="5" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="24" s="23" customFormat="1" ht="89.25" spans="1:4">
-      <c r="A24" s="51"/>
-      <c r="B24" s="52"/>
-      <c r="C24" s="49"/>
-      <c r="D24" s="11" t="s">
+    <row r="24" s="19" customFormat="1" ht="89.25" spans="1:4">
+      <c r="A24" s="46"/>
+      <c r="B24" s="47"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="5" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="25" s="23" customFormat="1" ht="63.75" spans="1:4">
-      <c r="A25" s="51"/>
-      <c r="B25" s="52"/>
-      <c r="C25" s="49"/>
-      <c r="D25" s="11" t="s">
+    <row r="25" s="19" customFormat="1" ht="63.75" spans="1:4">
+      <c r="A25" s="46"/>
+      <c r="B25" s="47"/>
+      <c r="C25" s="44"/>
+      <c r="D25" s="5" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="26" s="23" customFormat="1" ht="89.25" spans="1:4">
-      <c r="A26" s="51"/>
-      <c r="B26" s="52"/>
-      <c r="C26" s="49"/>
-      <c r="D26" s="11" t="s">
+    <row r="26" s="19" customFormat="1" ht="89.25" spans="1:4">
+      <c r="A26" s="46"/>
+      <c r="B26" s="47"/>
+      <c r="C26" s="44"/>
+      <c r="D26" s="5" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="27" s="23" customFormat="1" ht="165.75" spans="1:4">
-      <c r="A27" s="51"/>
-      <c r="B27" s="52"/>
-      <c r="C27" s="49"/>
-      <c r="D27" s="11" t="s">
+    <row r="27" s="19" customFormat="1" ht="165.75" spans="1:4">
+      <c r="A27" s="46"/>
+      <c r="B27" s="47"/>
+      <c r="C27" s="44"/>
+      <c r="D27" s="5" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="28" s="23" customFormat="1" ht="89.25" spans="1:4">
-      <c r="A28" s="51"/>
-      <c r="B28" s="52"/>
-      <c r="C28" s="49"/>
-      <c r="D28" s="11" t="s">
+    <row r="28" s="19" customFormat="1" ht="89.25" spans="1:4">
+      <c r="A28" s="46"/>
+      <c r="B28" s="47"/>
+      <c r="C28" s="44"/>
+      <c r="D28" s="5" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="29" s="23" customFormat="1" ht="153" spans="1:4">
-      <c r="A29" s="51"/>
-      <c r="B29" s="52"/>
-      <c r="C29" s="49"/>
-      <c r="D29" s="11" t="s">
+    <row r="29" s="19" customFormat="1" ht="153" spans="1:4">
+      <c r="A29" s="46"/>
+      <c r="B29" s="47"/>
+      <c r="C29" s="44"/>
+      <c r="D29" s="5" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="30" s="23" customFormat="1" ht="89.25" spans="1:4">
-      <c r="A30" s="51"/>
-      <c r="B30" s="52"/>
-      <c r="C30" s="49"/>
-      <c r="D30" s="11" t="s">
+    <row r="30" s="19" customFormat="1" ht="89.25" spans="1:4">
+      <c r="A30" s="46"/>
+      <c r="B30" s="47"/>
+      <c r="C30" s="44"/>
+      <c r="D30" s="5" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="31" s="23" customFormat="1" ht="140.25" spans="1:4">
-      <c r="A31" s="51"/>
-      <c r="B31" s="52"/>
-      <c r="C31" s="49"/>
-      <c r="D31" s="11" t="s">
+    <row r="31" s="19" customFormat="1" ht="140.25" spans="1:4">
+      <c r="A31" s="46"/>
+      <c r="B31" s="47"/>
+      <c r="C31" s="44"/>
+      <c r="D31" s="5" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="32" s="23" customFormat="1" ht="89.25" spans="1:4">
-      <c r="A32" s="51"/>
-      <c r="B32" s="52"/>
-      <c r="C32" s="49"/>
-      <c r="D32" s="11" t="s">
+    <row r="32" s="19" customFormat="1" ht="89.25" spans="1:4">
+      <c r="A32" s="46"/>
+      <c r="B32" s="47"/>
+      <c r="C32" s="44"/>
+      <c r="D32" s="5" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="33" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A33" s="51"/>
-      <c r="B33" s="52"/>
-      <c r="C33" s="49"/>
-      <c r="D33" s="11" t="s">
+    <row r="33" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A33" s="46"/>
+      <c r="B33" s="47"/>
+      <c r="C33" s="44"/>
+      <c r="D33" s="5" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="34" s="23" customFormat="1" ht="89.25" spans="1:4">
-      <c r="A34" s="51"/>
-      <c r="B34" s="52"/>
-      <c r="C34" s="49"/>
-      <c r="D34" s="20" t="s">
+    <row r="34" s="19" customFormat="1" ht="89.25" spans="1:4">
+      <c r="A34" s="46"/>
+      <c r="B34" s="47"/>
+      <c r="C34" s="44"/>
+      <c r="D34" s="16" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="35" s="23" customFormat="1" ht="369.75" spans="1:4">
-      <c r="A35" s="51"/>
-      <c r="B35" s="52"/>
-      <c r="C35" s="49"/>
-      <c r="D35" s="11" t="s">
+    <row r="35" s="19" customFormat="1" ht="369.75" spans="1:4">
+      <c r="A35" s="46"/>
+      <c r="B35" s="47"/>
+      <c r="C35" s="44"/>
+      <c r="D35" s="5" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="36" s="23" customFormat="1" ht="357" spans="1:4">
-      <c r="A36" s="51"/>
-      <c r="B36" s="52"/>
-      <c r="C36" s="49"/>
-      <c r="D36" s="11" t="s">
+    <row r="36" s="19" customFormat="1" ht="357" spans="1:4">
+      <c r="A36" s="46"/>
+      <c r="B36" s="47"/>
+      <c r="C36" s="44"/>
+      <c r="D36" s="5" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="37" s="23" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A37" s="51"/>
-      <c r="B37" s="52"/>
-      <c r="C37" s="49"/>
-      <c r="D37" s="11" t="s">
+    <row r="37" s="19" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A37" s="46"/>
+      <c r="B37" s="47"/>
+      <c r="C37" s="44"/>
+      <c r="D37" s="5" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="38" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A38" s="51"/>
-      <c r="B38" s="52"/>
-      <c r="C38" s="49"/>
-      <c r="D38" s="11" t="s">
+    <row r="38" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A38" s="46"/>
+      <c r="B38" s="47"/>
+      <c r="C38" s="44"/>
+      <c r="D38" s="5" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="39" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A39" s="51"/>
-      <c r="B39" s="52"/>
-      <c r="C39" s="49"/>
-      <c r="D39" s="11" t="s">
+    <row r="39" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A39" s="46"/>
+      <c r="B39" s="47"/>
+      <c r="C39" s="44"/>
+      <c r="D39" s="5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="40" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A40" s="51"/>
-      <c r="B40" s="52"/>
-      <c r="C40" s="49"/>
-      <c r="D40" s="11" t="s">
+    <row r="40" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A40" s="46"/>
+      <c r="B40" s="47"/>
+      <c r="C40" s="44"/>
+      <c r="D40" s="5" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="41" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A41" s="51"/>
-      <c r="B41" s="52"/>
-      <c r="C41" s="49" t="s">
+    <row r="41" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A41" s="46"/>
+      <c r="B41" s="47"/>
+      <c r="C41" s="44" t="s">
         <v>124</v>
       </c>
-      <c r="D41" s="11"/>
-    </row>
-    <row r="42" s="23" customFormat="1" ht="89.25" spans="1:4">
-      <c r="A42" s="51"/>
-      <c r="B42" s="52"/>
-      <c r="C42" s="49" t="s">
+      <c r="D41" s="5"/>
+    </row>
+    <row r="42" s="19" customFormat="1" ht="89.25" spans="1:4">
+      <c r="A42" s="46"/>
+      <c r="B42" s="47"/>
+      <c r="C42" s="44" t="s">
         <v>125</v>
       </c>
-      <c r="D42" s="11" t="s">
+      <c r="D42" s="5" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="43" s="23" customFormat="1" ht="114.75" spans="1:4">
-      <c r="A43" s="51"/>
-      <c r="B43" s="13" t="s">
+    <row r="43" s="19" customFormat="1" ht="114.75" spans="1:4">
+      <c r="A43" s="46"/>
+      <c r="B43" s="9" t="s">
         <v>127</v>
       </c>
-      <c r="C43" s="52" t="s">
+      <c r="C43" s="47" t="s">
         <v>128</v>
       </c>
-      <c r="D43" s="11" t="s">
+      <c r="D43" s="5" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="44" s="23" customFormat="1" ht="395.25" spans="1:4">
-      <c r="A44" s="51"/>
-      <c r="B44" s="13"/>
-      <c r="C44" s="52"/>
-      <c r="D44" s="11" t="s">
+    <row r="44" s="19" customFormat="1" ht="395.25" spans="1:4">
+      <c r="A44" s="46"/>
+      <c r="B44" s="9"/>
+      <c r="C44" s="47"/>
+      <c r="D44" s="5" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="45" s="23" customFormat="1" ht="409.5" spans="1:4">
-      <c r="A45" s="51"/>
-      <c r="B45" s="13"/>
-      <c r="C45" s="52"/>
-      <c r="D45" s="11" t="s">
+    <row r="45" s="19" customFormat="1" ht="409.5" spans="1:4">
+      <c r="A45" s="46"/>
+      <c r="B45" s="9"/>
+      <c r="C45" s="47"/>
+      <c r="D45" s="5" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="46" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A46" s="51"/>
-      <c r="B46" s="13"/>
-      <c r="C46" s="52"/>
-      <c r="D46" s="11" t="s">
+    <row r="46" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A46" s="46"/>
+      <c r="B46" s="9"/>
+      <c r="C46" s="47"/>
+      <c r="D46" s="5" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="47" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A47" s="51"/>
-      <c r="B47" s="13"/>
-      <c r="C47" s="52"/>
-      <c r="D47" s="11" t="s">
+    <row r="47" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A47" s="46"/>
+      <c r="B47" s="9"/>
+      <c r="C47" s="47"/>
+      <c r="D47" s="5" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="48" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A48" s="51"/>
-      <c r="B48" s="13"/>
-      <c r="C48" s="52"/>
-      <c r="D48" s="11" t="s">
+    <row r="48" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A48" s="46"/>
+      <c r="B48" s="9"/>
+      <c r="C48" s="47"/>
+      <c r="D48" s="5" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="49" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A49" s="51"/>
-      <c r="B49" s="13"/>
-      <c r="C49" s="52"/>
-      <c r="D49" s="11" t="s">
+    <row r="49" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A49" s="46"/>
+      <c r="B49" s="9"/>
+      <c r="C49" s="47"/>
+      <c r="D49" s="5" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="50" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A50" s="51"/>
-      <c r="B50" s="13"/>
-      <c r="C50" s="52"/>
-      <c r="D50" s="11" t="s">
+    <row r="50" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A50" s="46"/>
+      <c r="B50" s="9"/>
+      <c r="C50" s="47"/>
+      <c r="D50" s="5" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="51" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A51" s="51"/>
-      <c r="B51" s="13"/>
-      <c r="C51" s="45" t="s">
+    <row r="51" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A51" s="46"/>
+      <c r="B51" s="9"/>
+      <c r="C51" s="41" t="s">
         <v>137</v>
       </c>
-      <c r="D51" s="11" t="s">
+      <c r="D51" s="5" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="52" s="23" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A52" s="51"/>
-      <c r="B52" s="13"/>
-      <c r="C52" s="45"/>
-      <c r="D52" s="11" t="s">
+    <row r="52" s="19" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A52" s="46"/>
+      <c r="B52" s="9"/>
+      <c r="C52" s="41"/>
+      <c r="D52" s="5" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="53" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A53" s="51"/>
-      <c r="B53" s="13"/>
-      <c r="C53" s="45"/>
-      <c r="D53" s="11" t="s">
+    <row r="53" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A53" s="46"/>
+      <c r="B53" s="9"/>
+      <c r="C53" s="41"/>
+      <c r="D53" s="5" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="54" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A54" s="51"/>
-      <c r="B54" s="13"/>
-      <c r="C54" s="45"/>
-      <c r="D54" s="11" t="s">
+    <row r="54" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A54" s="46"/>
+      <c r="B54" s="9"/>
+      <c r="C54" s="41"/>
+      <c r="D54" s="5" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="55" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A55" s="51"/>
-      <c r="B55" s="13"/>
-      <c r="C55" s="45"/>
-      <c r="D55" s="11" t="s">
+    <row r="55" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A55" s="46"/>
+      <c r="B55" s="9"/>
+      <c r="C55" s="41"/>
+      <c r="D55" s="5" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="56" s="23" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A56" s="51"/>
-      <c r="B56" s="13"/>
-      <c r="C56" s="49" t="s">
+    <row r="56" s="19" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A56" s="46"/>
+      <c r="B56" s="9"/>
+      <c r="C56" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="D56" s="11"/>
-    </row>
-    <row r="57" s="23" customFormat="1" ht="409.5" spans="1:4">
-      <c r="A57" s="51"/>
-      <c r="B57" s="13"/>
-      <c r="C57" s="52" t="s">
+      <c r="D56" s="5"/>
+    </row>
+    <row r="57" s="19" customFormat="1" ht="409.5" spans="1:4">
+      <c r="A57" s="46"/>
+      <c r="B57" s="9"/>
+      <c r="C57" s="47" t="s">
         <v>144</v>
       </c>
-      <c r="D57" s="20" t="s">
+      <c r="D57" s="16" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="58" s="23" customFormat="1" ht="51" spans="1:4">
-      <c r="A58" s="51"/>
-      <c r="B58" s="13"/>
-      <c r="C58" s="52"/>
-      <c r="D58" s="11" t="s">
+    <row r="58" s="19" customFormat="1" ht="51" spans="1:4">
+      <c r="A58" s="46"/>
+      <c r="B58" s="9"/>
+      <c r="C58" s="47"/>
+      <c r="D58" s="5" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="59" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A59" s="51"/>
-      <c r="B59" s="13"/>
-      <c r="C59" s="52"/>
-      <c r="D59" s="11" t="s">
+    <row r="59" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A59" s="46"/>
+      <c r="B59" s="9"/>
+      <c r="C59" s="47"/>
+      <c r="D59" s="5" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="60" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A60" s="51"/>
-      <c r="B60" s="13"/>
-      <c r="C60" s="52"/>
-      <c r="D60" s="11" t="s">
+    <row r="60" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A60" s="46"/>
+      <c r="B60" s="9"/>
+      <c r="C60" s="47"/>
+      <c r="D60" s="5" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="61" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A61" s="51"/>
-      <c r="B61" s="13"/>
-      <c r="C61" s="49" t="s">
+    <row r="61" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A61" s="46"/>
+      <c r="B61" s="9"/>
+      <c r="C61" s="44" t="s">
         <v>149</v>
       </c>
-      <c r="D61" s="11" t="s">
+      <c r="D61" s="5" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="62" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A62" s="51"/>
-      <c r="B62" s="13"/>
-      <c r="C62" s="49"/>
-      <c r="D62" s="11" t="s">
+    <row r="62" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A62" s="46"/>
+      <c r="B62" s="9"/>
+      <c r="C62" s="44"/>
+      <c r="D62" s="5" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="63" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A63" s="51"/>
-      <c r="B63" s="13"/>
-      <c r="C63" s="49"/>
-      <c r="D63" s="11" t="s">
+    <row r="63" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A63" s="46"/>
+      <c r="B63" s="9"/>
+      <c r="C63" s="44"/>
+      <c r="D63" s="5" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="64" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A64" s="51"/>
-      <c r="B64" s="13"/>
-      <c r="C64" s="49"/>
-      <c r="D64" s="11" t="s">
+    <row r="64" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A64" s="46"/>
+      <c r="B64" s="9"/>
+      <c r="C64" s="44"/>
+      <c r="D64" s="5" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="65" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A65" s="51"/>
-      <c r="B65" s="13"/>
-      <c r="C65" s="49"/>
-      <c r="D65" s="11" t="s">
+    <row r="65" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A65" s="46"/>
+      <c r="B65" s="9"/>
+      <c r="C65" s="44"/>
+      <c r="D65" s="5" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="66" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A66" s="51"/>
-      <c r="B66" s="13"/>
-      <c r="C66" s="49"/>
-      <c r="D66" s="11" t="s">
+    <row r="66" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A66" s="46"/>
+      <c r="B66" s="9"/>
+      <c r="C66" s="44"/>
+      <c r="D66" s="5" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="67" s="23" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A67" s="51"/>
-      <c r="B67" s="13"/>
-      <c r="C67" s="49" t="s">
+    <row r="67" s="19" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A67" s="46"/>
+      <c r="B67" s="9"/>
+      <c r="C67" s="44" t="s">
         <v>155</v>
       </c>
-      <c r="D67" s="11" t="s">
+      <c r="D67" s="5" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="68" s="23" customFormat="1" ht="51" spans="1:4">
-      <c r="A68" s="51"/>
-      <c r="B68" s="13"/>
-      <c r="C68" s="49"/>
-      <c r="D68" s="11" t="s">
+    <row r="68" s="19" customFormat="1" ht="51" spans="1:4">
+      <c r="A68" s="46"/>
+      <c r="B68" s="9"/>
+      <c r="C68" s="44"/>
+      <c r="D68" s="5" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="69" s="23" customFormat="1" ht="51" spans="1:4">
-      <c r="A69" s="51"/>
-      <c r="B69" s="13"/>
-      <c r="C69" s="49"/>
-      <c r="D69" s="11" t="s">
+    <row r="69" s="19" customFormat="1" ht="51" spans="1:4">
+      <c r="A69" s="46"/>
+      <c r="B69" s="9"/>
+      <c r="C69" s="44"/>
+      <c r="D69" s="5" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="70" s="23" customFormat="1" ht="63.75" spans="1:4">
-      <c r="A70" s="51"/>
-      <c r="B70" s="13"/>
-      <c r="C70" s="49"/>
-      <c r="D70" s="11" t="s">
+    <row r="70" s="19" customFormat="1" ht="63.75" spans="1:4">
+      <c r="A70" s="46"/>
+      <c r="B70" s="9"/>
+      <c r="C70" s="44"/>
+      <c r="D70" s="5" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="71" s="23" customFormat="1" ht="63.75" spans="1:4">
-      <c r="A71" s="51"/>
-      <c r="B71" s="13"/>
-      <c r="C71" s="49"/>
-      <c r="D71" s="11" t="s">
+    <row r="71" s="19" customFormat="1" ht="63.75" spans="1:4">
+      <c r="A71" s="46"/>
+      <c r="B71" s="9"/>
+      <c r="C71" s="44"/>
+      <c r="D71" s="5" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="72" s="23" customFormat="1" ht="51" spans="1:4">
-      <c r="A72" s="51"/>
-      <c r="B72" s="13"/>
-      <c r="C72" s="49"/>
-      <c r="D72" s="11" t="s">
+    <row r="72" s="19" customFormat="1" ht="51" spans="1:4">
+      <c r="A72" s="46"/>
+      <c r="B72" s="9"/>
+      <c r="C72" s="44"/>
+      <c r="D72" s="5" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="73" s="23" customFormat="1" ht="51" spans="1:4">
-      <c r="A73" s="51"/>
-      <c r="B73" s="13"/>
-      <c r="C73" s="49"/>
-      <c r="D73" s="11" t="s">
+    <row r="73" s="19" customFormat="1" ht="51" spans="1:4">
+      <c r="A73" s="46"/>
+      <c r="B73" s="9"/>
+      <c r="C73" s="44"/>
+      <c r="D73" s="5" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="74" s="23" customFormat="1" ht="63.75" spans="1:4">
-      <c r="A74" s="51"/>
-      <c r="B74" s="13"/>
-      <c r="C74" s="49"/>
-      <c r="D74" s="11" t="s">
+    <row r="74" s="19" customFormat="1" ht="63.75" spans="1:4">
+      <c r="A74" s="46"/>
+      <c r="B74" s="9"/>
+      <c r="C74" s="44"/>
+      <c r="D74" s="5" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="75" s="23" customFormat="1" ht="63.75" spans="1:4">
-      <c r="A75" s="51"/>
-      <c r="B75" s="13"/>
-      <c r="C75" s="49"/>
-      <c r="D75" s="11" t="s">
+    <row r="75" s="19" customFormat="1" ht="63.75" spans="1:4">
+      <c r="A75" s="46"/>
+      <c r="B75" s="9"/>
+      <c r="C75" s="44"/>
+      <c r="D75" s="5" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="76" s="23" customFormat="1" ht="51" spans="1:4">
-      <c r="A76" s="51"/>
-      <c r="B76" s="13"/>
-      <c r="C76" s="49"/>
-      <c r="D76" s="11" t="s">
+    <row r="76" s="19" customFormat="1" ht="51" spans="1:4">
+      <c r="A76" s="46"/>
+      <c r="B76" s="9"/>
+      <c r="C76" s="44"/>
+      <c r="D76" s="5" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="77" s="23" customFormat="1" ht="153" spans="1:4">
-      <c r="A77" s="51"/>
-      <c r="B77" s="13"/>
-      <c r="C77" s="49"/>
-      <c r="D77" s="11" t="s">
+    <row r="77" s="19" customFormat="1" ht="153" spans="1:4">
+      <c r="A77" s="46"/>
+      <c r="B77" s="9"/>
+      <c r="C77" s="44"/>
+      <c r="D77" s="5" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="78" s="23" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A78" s="51"/>
-      <c r="B78" s="13"/>
-      <c r="C78" s="49"/>
-      <c r="D78" s="11" t="s">
+    <row r="78" s="19" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A78" s="46"/>
+      <c r="B78" s="9"/>
+      <c r="C78" s="44"/>
+      <c r="D78" s="5" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="79" s="23" customFormat="1" ht="114.75" spans="1:4">
-      <c r="A79" s="51"/>
-      <c r="B79" s="13"/>
-      <c r="C79" s="49" t="s">
+    <row r="79" s="19" customFormat="1" ht="114.75" spans="1:4">
+      <c r="A79" s="46"/>
+      <c r="B79" s="9"/>
+      <c r="C79" s="44" t="s">
         <v>168</v>
       </c>
-      <c r="D79" s="11" t="s">
+      <c r="D79" s="5" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="80" s="23" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A80" s="51"/>
-      <c r="B80" s="13"/>
-      <c r="C80" s="45" t="s">
+    <row r="80" s="19" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A80" s="46"/>
+      <c r="B80" s="9"/>
+      <c r="C80" s="41" t="s">
         <v>170</v>
       </c>
-      <c r="D80" s="11" t="s">
+      <c r="D80" s="5" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="81" s="23" customFormat="1" ht="165.75" spans="1:4">
-      <c r="A81" s="51"/>
-      <c r="B81" s="13"/>
-      <c r="C81" s="45"/>
-      <c r="D81" s="20" t="s">
+    <row r="81" s="19" customFormat="1" ht="165.75" spans="1:4">
+      <c r="A81" s="46"/>
+      <c r="B81" s="9"/>
+      <c r="C81" s="41"/>
+      <c r="D81" s="16" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="82" s="23" customFormat="1" ht="102" spans="1:4">
-      <c r="A82" s="51"/>
-      <c r="B82" s="13"/>
-      <c r="C82" s="45"/>
-      <c r="D82" s="20" t="s">
+    <row r="82" s="19" customFormat="1" ht="102" spans="1:4">
+      <c r="A82" s="46"/>
+      <c r="B82" s="9"/>
+      <c r="C82" s="41"/>
+      <c r="D82" s="16" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="83" s="23" customFormat="1" ht="51" spans="1:4">
-      <c r="A83" s="51"/>
-      <c r="B83" s="13"/>
-      <c r="C83" s="45"/>
-      <c r="D83" s="20" t="s">
+    <row r="83" s="19" customFormat="1" ht="51" spans="1:4">
+      <c r="A83" s="46"/>
+      <c r="B83" s="9"/>
+      <c r="C83" s="41"/>
+      <c r="D83" s="16" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="84" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A84" s="51"/>
-      <c r="B84" s="13"/>
-      <c r="C84" s="52" t="s">
+    <row r="84" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A84" s="46"/>
+      <c r="B84" s="9"/>
+      <c r="C84" s="47" t="s">
         <v>175</v>
       </c>
-      <c r="D84" s="20" t="s">
+      <c r="D84" s="16" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="85" s="23" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A85" s="51"/>
-      <c r="B85" s="13" t="s">
+    <row r="85" s="19" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A85" s="46"/>
+      <c r="B85" s="9" t="s">
         <v>177</v>
       </c>
-      <c r="C85" s="52"/>
-      <c r="D85" s="20"/>
-    </row>
-    <row r="86" s="23" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A86" s="51"/>
-      <c r="B86" s="13" t="s">
+      <c r="C85" s="47"/>
+      <c r="D85" s="16"/>
+    </row>
+    <row r="86" s="19" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A86" s="46"/>
+      <c r="B86" s="9" t="s">
         <v>178</v>
       </c>
-      <c r="C86" s="52"/>
-      <c r="D86" s="20"/>
-    </row>
-    <row r="87" s="23" customFormat="1" ht="51" spans="1:4">
-      <c r="A87" s="51"/>
-      <c r="B87" s="13" t="s">
+      <c r="C86" s="47"/>
+      <c r="D86" s="16"/>
+    </row>
+    <row r="87" s="19" customFormat="1" ht="51" spans="1:4">
+      <c r="A87" s="46"/>
+      <c r="B87" s="9" t="s">
         <v>179</v>
       </c>
-      <c r="C87" s="52"/>
-      <c r="D87" s="20"/>
-    </row>
-    <row r="88" s="23" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A88" s="51"/>
-      <c r="B88" s="13" t="s">
+      <c r="C87" s="47"/>
+      <c r="D87" s="16"/>
+    </row>
+    <row r="88" s="19" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A88" s="46"/>
+      <c r="B88" s="9" t="s">
         <v>180</v>
       </c>
-      <c r="C88" s="52"/>
-      <c r="D88" s="20"/>
-    </row>
-    <row r="89" s="23" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A89" s="51"/>
-      <c r="B89" s="13" t="s">
+      <c r="C88" s="47"/>
+      <c r="D88" s="16"/>
+    </row>
+    <row r="89" s="19" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A89" s="46"/>
+      <c r="B89" s="9" t="s">
         <v>181</v>
       </c>
-      <c r="C89" s="52"/>
-      <c r="D89" s="20"/>
-    </row>
-    <row r="90" s="23" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A90" s="51"/>
-      <c r="B90" s="13" t="s">
+      <c r="C89" s="47"/>
+      <c r="D89" s="16"/>
+    </row>
+    <row r="90" s="19" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A90" s="46"/>
+      <c r="B90" s="9" t="s">
         <v>182</v>
       </c>
-      <c r="C90" s="52"/>
-      <c r="D90" s="20"/>
-    </row>
-    <row r="91" s="23" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A91" s="51"/>
-      <c r="B91" s="13" t="s">
+      <c r="C90" s="47"/>
+      <c r="D90" s="16"/>
+    </row>
+    <row r="91" s="19" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A91" s="46"/>
+      <c r="B91" s="9" t="s">
         <v>183</v>
       </c>
-      <c r="C91" s="52"/>
-      <c r="D91" s="20"/>
-    </row>
-    <row r="92" s="23" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A92" s="51"/>
-      <c r="B92" s="13" t="s">
+      <c r="C91" s="47"/>
+      <c r="D91" s="16"/>
+    </row>
+    <row r="92" s="19" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A92" s="46"/>
+      <c r="B92" s="9" t="s">
         <v>184</v>
       </c>
-      <c r="C92" s="52"/>
-      <c r="D92" s="20"/>
-    </row>
-    <row r="93" s="23" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A93" s="51"/>
-      <c r="B93" s="53" t="s">
+      <c r="C92" s="47"/>
+      <c r="D92" s="16"/>
+    </row>
+    <row r="93" s="19" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A93" s="46"/>
+      <c r="B93" s="48" t="s">
         <v>185</v>
       </c>
-      <c r="C93" s="52"/>
-      <c r="D93" s="20"/>
-    </row>
-    <row r="94" s="23" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A94" s="51"/>
-      <c r="B94" s="13" t="s">
+      <c r="C93" s="47"/>
+      <c r="D93" s="16"/>
+    </row>
+    <row r="94" s="19" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A94" s="46"/>
+      <c r="B94" s="9" t="s">
         <v>186</v>
       </c>
-      <c r="C94" s="52"/>
-      <c r="D94" s="20"/>
-    </row>
-    <row r="95" s="23" customFormat="1" ht="51" spans="1:4">
-      <c r="A95" s="51"/>
-      <c r="B95" s="53" t="s">
+      <c r="C94" s="47"/>
+      <c r="D94" s="16"/>
+    </row>
+    <row r="95" s="19" customFormat="1" ht="51" spans="1:4">
+      <c r="A95" s="46"/>
+      <c r="B95" s="48" t="s">
         <v>187</v>
       </c>
-      <c r="C95" s="52"/>
-      <c r="D95" s="20"/>
-    </row>
-    <row r="96" s="23" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A96" s="51"/>
-      <c r="B96" s="53" t="s">
+      <c r="C95" s="47"/>
+      <c r="D95" s="16"/>
+    </row>
+    <row r="96" s="19" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A96" s="46"/>
+      <c r="B96" s="48" t="s">
         <v>188</v>
       </c>
-      <c r="C96" s="52"/>
-      <c r="D96" s="20"/>
-    </row>
-    <row r="97" s="23" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A97" s="51"/>
-      <c r="B97" s="53" t="s">
+      <c r="C96" s="47"/>
+      <c r="D96" s="16"/>
+    </row>
+    <row r="97" s="19" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A97" s="46"/>
+      <c r="B97" s="48" t="s">
         <v>189</v>
       </c>
-      <c r="C97" s="52"/>
-      <c r="D97" s="20"/>
-    </row>
-    <row r="98" s="23" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A98" s="51"/>
-      <c r="B98" s="53" t="s">
+      <c r="C97" s="47"/>
+      <c r="D97" s="16"/>
+    </row>
+    <row r="98" s="19" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A98" s="46"/>
+      <c r="B98" s="48" t="s">
         <v>190</v>
       </c>
-      <c r="C98" s="52"/>
-      <c r="D98" s="20"/>
-    </row>
-    <row r="99" s="23" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A99" s="51"/>
-      <c r="B99" s="53" t="s">
+      <c r="C98" s="47"/>
+      <c r="D98" s="16"/>
+    </row>
+    <row r="99" s="19" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A99" s="46"/>
+      <c r="B99" s="48" t="s">
         <v>191</v>
       </c>
-      <c r="C99" s="52"/>
-      <c r="D99" s="20"/>
-    </row>
-    <row r="100" s="23" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A100" s="51"/>
-      <c r="B100" s="13" t="s">
+      <c r="C99" s="47"/>
+      <c r="D99" s="16"/>
+    </row>
+    <row r="100" s="19" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A100" s="46"/>
+      <c r="B100" s="9" t="s">
         <v>192</v>
       </c>
-      <c r="C100" s="52"/>
-      <c r="D100" s="20"/>
-    </row>
-    <row r="101" s="23" customFormat="1" ht="51" spans="1:4">
-      <c r="A101" s="51"/>
-      <c r="B101" s="13" t="s">
+      <c r="C100" s="47"/>
+      <c r="D100" s="16"/>
+    </row>
+    <row r="101" s="19" customFormat="1" ht="51" spans="1:4">
+      <c r="A101" s="46"/>
+      <c r="B101" s="9" t="s">
         <v>193</v>
       </c>
-      <c r="C101" s="52"/>
-      <c r="D101" s="20"/>
-    </row>
-    <row r="102" s="23" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A102" s="51"/>
-      <c r="B102" s="53" t="s">
+      <c r="C101" s="47"/>
+      <c r="D101" s="16"/>
+    </row>
+    <row r="102" s="19" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A102" s="46"/>
+      <c r="B102" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="C102" s="52"/>
-      <c r="D102" s="20"/>
-    </row>
-    <row r="103" s="23" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A103" s="51"/>
-      <c r="B103" s="13" t="s">
+      <c r="C102" s="47"/>
+      <c r="D102" s="16"/>
+    </row>
+    <row r="103" s="19" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A103" s="46"/>
+      <c r="B103" s="9" t="s">
         <v>195</v>
       </c>
-      <c r="C103" s="52"/>
-      <c r="D103" s="20"/>
-    </row>
-    <row r="104" s="23" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A104" s="51"/>
-      <c r="B104" s="13" t="s">
+      <c r="C103" s="47"/>
+      <c r="D103" s="16"/>
+    </row>
+    <row r="104" s="19" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A104" s="46"/>
+      <c r="B104" s="9" t="s">
         <v>196</v>
       </c>
-      <c r="C104" s="52"/>
-      <c r="D104" s="20"/>
-    </row>
-    <row r="105" s="23" customFormat="1" ht="153" spans="1:4">
-      <c r="A105" s="51"/>
-      <c r="B105" s="54" t="s">
+      <c r="C104" s="47"/>
+      <c r="D104" s="16"/>
+    </row>
+    <row r="105" s="19" customFormat="1" ht="153" spans="1:4">
+      <c r="A105" s="46"/>
+      <c r="B105" s="49" t="s">
         <v>197</v>
       </c>
-      <c r="C105" s="49" t="s">
+      <c r="C105" s="44" t="s">
         <v>198</v>
       </c>
-      <c r="D105" s="11" t="s">
+      <c r="D105" s="5" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="106" s="23" customFormat="1" ht="51" spans="1:4">
-      <c r="A106" s="51"/>
-      <c r="B106" s="54"/>
-      <c r="C106" s="49" t="s">
+    <row r="106" s="19" customFormat="1" ht="51" spans="1:4">
+      <c r="A106" s="46"/>
+      <c r="B106" s="49"/>
+      <c r="C106" s="44" t="s">
         <v>200</v>
       </c>
-      <c r="D106" s="11" t="s">
+      <c r="D106" s="5" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="107" s="23" customFormat="1" ht="306" spans="1:4">
-      <c r="A107" s="51"/>
-      <c r="B107" s="54"/>
-      <c r="C107" s="49" t="s">
+    <row r="107" s="19" customFormat="1" ht="306" spans="1:4">
+      <c r="A107" s="46"/>
+      <c r="B107" s="49"/>
+      <c r="C107" s="44" t="s">
         <v>202</v>
       </c>
-      <c r="D107" s="20" t="s">
+      <c r="D107" s="16" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="108" s="23" customFormat="1" ht="229.5" spans="1:4">
-      <c r="A108" s="51"/>
-      <c r="B108" s="54"/>
-      <c r="C108" s="49"/>
-      <c r="D108" s="20" t="s">
+    <row r="108" s="19" customFormat="1" ht="229.5" spans="1:4">
+      <c r="A108" s="46"/>
+      <c r="B108" s="49"/>
+      <c r="C108" s="44"/>
+      <c r="D108" s="16" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="109" s="23" customFormat="1" ht="242.25" spans="1:4">
-      <c r="A109" s="51"/>
-      <c r="B109" s="54"/>
-      <c r="C109" s="49" t="s">
+    <row r="109" s="19" customFormat="1" ht="242.25" spans="1:4">
+      <c r="A109" s="46"/>
+      <c r="B109" s="49"/>
+      <c r="C109" s="44" t="s">
         <v>205</v>
       </c>
-      <c r="D109" s="20" t="s">
+      <c r="D109" s="16" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="110" s="23" customFormat="1" ht="216.75" spans="1:4">
-      <c r="A110" s="51"/>
-      <c r="B110" s="54"/>
-      <c r="C110" s="49" t="s">
+    <row r="110" s="19" customFormat="1" ht="216.75" spans="1:4">
+      <c r="A110" s="46"/>
+      <c r="B110" s="49"/>
+      <c r="C110" s="44" t="s">
         <v>207</v>
       </c>
-      <c r="D110" s="20" t="s">
+      <c r="D110" s="16" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="111" s="23" customFormat="1" ht="369.75" spans="1:4">
-      <c r="A111" s="51"/>
-      <c r="B111" s="54"/>
-      <c r="C111" s="49"/>
-      <c r="D111" s="20" t="s">
+    <row r="111" s="19" customFormat="1" ht="369.75" spans="1:4">
+      <c r="A111" s="46"/>
+      <c r="B111" s="49"/>
+      <c r="C111" s="44"/>
+      <c r="D111" s="16" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="112" s="23" customFormat="1" ht="382.5" spans="1:4">
-      <c r="A112" s="51"/>
-      <c r="B112" s="54"/>
-      <c r="C112" s="49" t="s">
+    <row r="112" s="19" customFormat="1" ht="382.5" spans="1:4">
+      <c r="A112" s="46"/>
+      <c r="B112" s="49"/>
+      <c r="C112" s="44" t="s">
         <v>210</v>
       </c>
-      <c r="D112" s="20" t="s">
+      <c r="D112" s="16" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="113" s="23" customFormat="1" ht="255" spans="1:4">
-      <c r="A113" s="51"/>
-      <c r="B113" s="55"/>
-      <c r="C113" s="49" t="s">
+    <row r="113" s="19" customFormat="1" ht="255" spans="1:4">
+      <c r="A113" s="46"/>
+      <c r="B113" s="50"/>
+      <c r="C113" s="44" t="s">
         <v>212</v>
       </c>
-      <c r="D113" s="11" t="s">
+      <c r="D113" s="5" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="114" s="23" customFormat="1" ht="165.75" spans="1:4">
-      <c r="A114" s="51"/>
-      <c r="B114" s="55"/>
-      <c r="C114" s="49" t="s">
+    <row r="114" s="19" customFormat="1" ht="165.75" spans="1:4">
+      <c r="A114" s="46"/>
+      <c r="B114" s="50"/>
+      <c r="C114" s="44" t="s">
         <v>214</v>
       </c>
-      <c r="D114" s="11" t="s">
+      <c r="D114" s="5" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="115" s="23" customFormat="1" ht="89.25" spans="1:4">
-      <c r="A115" s="51"/>
-      <c r="B115" s="55"/>
-      <c r="C115" s="49" t="s">
+    <row r="115" s="19" customFormat="1" ht="89.25" spans="1:4">
+      <c r="A115" s="46"/>
+      <c r="B115" s="50"/>
+      <c r="C115" s="44" t="s">
         <v>216</v>
       </c>
-      <c r="D115" s="11" t="s">
+      <c r="D115" s="5" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="116" s="23" customFormat="1" ht="89.25" spans="1:4">
-      <c r="A116" s="51"/>
-      <c r="B116" s="55"/>
-      <c r="C116" s="49"/>
-      <c r="D116" s="11" t="s">
+    <row r="116" s="19" customFormat="1" ht="89.25" spans="1:4">
+      <c r="A116" s="46"/>
+      <c r="B116" s="50"/>
+      <c r="C116" s="44"/>
+      <c r="D116" s="5" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="117" s="23" customFormat="1" ht="63.75" spans="1:4">
-      <c r="A117" s="51"/>
-      <c r="B117" s="55"/>
-      <c r="C117" s="49" t="s">
+    <row r="117" s="19" customFormat="1" ht="63.75" spans="1:4">
+      <c r="A117" s="46"/>
+      <c r="B117" s="50"/>
+      <c r="C117" s="44" t="s">
         <v>219</v>
       </c>
-      <c r="D117" s="11" t="s">
+      <c r="D117" s="5" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="118" s="23" customFormat="1" ht="274.5" customHeight="1" spans="1:4">
-      <c r="A118" s="51"/>
-      <c r="B118" s="49" t="s">
+    <row r="118" s="19" customFormat="1" ht="274.5" customHeight="1" spans="1:4">
+      <c r="A118" s="46"/>
+      <c r="B118" s="44" t="s">
         <v>221</v>
       </c>
-      <c r="C118" s="11" t="s">
+      <c r="C118" s="5" t="s">
         <v>222</v>
       </c>
-      <c r="D118" s="11"/>
-    </row>
-    <row r="119" s="23" customFormat="1" ht="243.75" customHeight="1" spans="1:4">
-      <c r="A119" s="51"/>
-      <c r="B119" s="49"/>
-      <c r="C119" s="11" t="s">
+      <c r="D118" s="5"/>
+    </row>
+    <row r="119" s="19" customFormat="1" ht="243.75" customHeight="1" spans="1:4">
+      <c r="A119" s="46"/>
+      <c r="B119" s="44"/>
+      <c r="C119" s="5" t="s">
         <v>223</v>
       </c>
-      <c r="D119" s="11"/>
-    </row>
-    <row r="120" s="23" customFormat="1" ht="391.5" customHeight="1" spans="1:4">
-      <c r="A120" s="51"/>
-      <c r="B120" s="49" t="s">
+      <c r="D119" s="5"/>
+    </row>
+    <row r="120" s="19" customFormat="1" ht="391.5" customHeight="1" spans="1:4">
+      <c r="A120" s="46"/>
+      <c r="B120" s="44" t="s">
         <v>224</v>
       </c>
-      <c r="C120" s="11" t="s">
+      <c r="C120" s="5" t="s">
         <v>225</v>
       </c>
-      <c r="D120" s="11"/>
-    </row>
-    <row r="121" s="23" customFormat="1" ht="231" customHeight="1" spans="1:4">
-      <c r="A121" s="51"/>
-      <c r="B121" s="49"/>
-      <c r="C121" s="11" t="s">
+      <c r="D120" s="5"/>
+    </row>
+    <row r="121" s="19" customFormat="1" ht="231" customHeight="1" spans="1:4">
+      <c r="A121" s="46"/>
+      <c r="B121" s="44"/>
+      <c r="C121" s="5" t="s">
         <v>226</v>
       </c>
-      <c r="D121" s="11"/>
-    </row>
-    <row r="122" s="23" customFormat="1" ht="45" customHeight="1" spans="1:4">
-      <c r="A122" s="56" t="s">
+      <c r="D121" s="5"/>
+    </row>
+    <row r="122" s="19" customFormat="1" ht="45" customHeight="1" spans="1:4">
+      <c r="A122" s="51" t="s">
         <v>227</v>
       </c>
-      <c r="B122" s="49" t="s">
+      <c r="B122" s="44" t="s">
         <v>228</v>
       </c>
-      <c r="C122" s="11" t="s">
+      <c r="C122" s="5" t="s">
         <v>229</v>
       </c>
-      <c r="D122" s="11"/>
-    </row>
-    <row r="123" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A123" s="51"/>
-      <c r="B123" s="49" t="s">
+      <c r="D122" s="5"/>
+    </row>
+    <row r="123" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A123" s="46"/>
+      <c r="B123" s="44" t="s">
         <v>230</v>
       </c>
-      <c r="C123" s="49" t="s">
+      <c r="C123" s="44" t="s">
         <v>231</v>
       </c>
-      <c r="D123" s="11" t="s">
+      <c r="D123" s="5" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="124" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A124" s="51"/>
-      <c r="B124" s="49"/>
-      <c r="C124" s="49" t="s">
+    <row r="124" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A124" s="46"/>
+      <c r="B124" s="44"/>
+      <c r="C124" s="44" t="s">
         <v>233</v>
       </c>
-      <c r="D124" s="11" t="s">
+      <c r="D124" s="5" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="125" s="23" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A125" s="51"/>
-      <c r="B125" s="49"/>
-      <c r="C125" s="49" t="s">
+    <row r="125" s="19" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A125" s="46"/>
+      <c r="B125" s="44"/>
+      <c r="C125" s="44" t="s">
         <v>235</v>
       </c>
-      <c r="D125" s="11" t="s">
+      <c r="D125" s="5" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="126" s="23" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A126" s="51"/>
-      <c r="B126" s="49"/>
-      <c r="C126" s="49" t="s">
+    <row r="126" s="19" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A126" s="46"/>
+      <c r="B126" s="44"/>
+      <c r="C126" s="44" t="s">
         <v>237</v>
       </c>
-      <c r="D126" s="11" t="s">
+      <c r="D126" s="5" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="127" s="23" customFormat="1" ht="51" spans="1:4">
-      <c r="A127" s="51"/>
-      <c r="B127" s="49" t="s">
+    <row r="127" s="19" customFormat="1" ht="51" spans="1:4">
+      <c r="A127" s="46"/>
+      <c r="B127" s="44" t="s">
         <v>239</v>
       </c>
-      <c r="C127" s="49" t="s">
+      <c r="C127" s="44" t="s">
         <v>240</v>
       </c>
-      <c r="D127" s="11" t="s">
+      <c r="D127" s="5" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="128" s="23" customFormat="1" ht="51" spans="1:4">
-      <c r="A128" s="51"/>
-      <c r="B128" s="49"/>
-      <c r="C128" s="49" t="s">
+    <row r="128" s="19" customFormat="1" ht="51" spans="1:4">
+      <c r="A128" s="46"/>
+      <c r="B128" s="44"/>
+      <c r="C128" s="44" t="s">
         <v>242</v>
       </c>
-      <c r="D128" s="11" t="s">
+      <c r="D128" s="5" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="129" s="23" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A129" s="51"/>
-      <c r="B129" s="49"/>
-      <c r="C129" s="11" t="s">
+    <row r="129" s="19" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A129" s="46"/>
+      <c r="B129" s="44"/>
+      <c r="C129" s="5" t="s">
         <v>244</v>
       </c>
-      <c r="D129" s="11"/>
-    </row>
-    <row r="130" s="23" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A130" s="51"/>
-      <c r="B130" s="49"/>
-      <c r="C130" s="11" t="s">
+      <c r="D129" s="5"/>
+    </row>
+    <row r="130" s="19" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A130" s="46"/>
+      <c r="B130" s="44"/>
+      <c r="C130" s="5" t="s">
         <v>245</v>
       </c>
-      <c r="D130" s="11"/>
-    </row>
-    <row r="131" s="23" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A131" s="51"/>
-      <c r="B131" s="49"/>
-      <c r="C131" s="11" t="s">
+      <c r="D130" s="5"/>
+    </row>
+    <row r="131" s="19" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A131" s="46"/>
+      <c r="B131" s="44"/>
+      <c r="C131" s="5" t="s">
         <v>246</v>
       </c>
-      <c r="D131" s="11"/>
-    </row>
-    <row r="132" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A132" s="51"/>
-      <c r="B132" s="49"/>
-      <c r="C132" s="11" t="s">
+      <c r="D131" s="5"/>
+    </row>
+    <row r="132" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A132" s="46"/>
+      <c r="B132" s="44"/>
+      <c r="C132" s="5" t="s">
         <v>247</v>
       </c>
-      <c r="D132" s="11"/>
-    </row>
-    <row r="133" s="23" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A133" s="51"/>
-      <c r="B133" s="49" t="s">
+      <c r="D132" s="5"/>
+    </row>
+    <row r="133" s="19" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A133" s="46"/>
+      <c r="B133" s="44" t="s">
         <v>248</v>
       </c>
-      <c r="C133" s="11" t="s">
+      <c r="C133" s="5" t="s">
         <v>249</v>
       </c>
-      <c r="D133" s="11"/>
-    </row>
-    <row r="134" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A134" s="51"/>
-      <c r="B134" s="49"/>
-      <c r="C134" s="11" t="s">
+      <c r="D133" s="5"/>
+    </row>
+    <row r="134" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A134" s="46"/>
+      <c r="B134" s="44"/>
+      <c r="C134" s="5" t="s">
         <v>250</v>
       </c>
-      <c r="D134" s="11"/>
-    </row>
-    <row r="135" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A135" s="51"/>
-      <c r="B135" s="49"/>
-      <c r="C135" s="11" t="s">
+      <c r="D134" s="5"/>
+    </row>
+    <row r="135" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A135" s="46"/>
+      <c r="B135" s="44"/>
+      <c r="C135" s="5" t="s">
         <v>251</v>
       </c>
-      <c r="D135" s="11"/>
-    </row>
-    <row r="136" s="23" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A136" s="51"/>
-      <c r="B136" s="49" t="s">
+      <c r="D135" s="5"/>
+    </row>
+    <row r="136" s="19" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A136" s="46"/>
+      <c r="B136" s="44" t="s">
         <v>252</v>
       </c>
-      <c r="C136" s="11"/>
-      <c r="D136" s="11"/>
+      <c r="C136" s="5"/>
+      <c r="D136" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="30">
@@ -14363,298 +14503,298 @@
   </cols>
   <sheetData>
     <row r="1" ht="89.25" spans="1:2">
-      <c r="A1" s="41" t="s">
+      <c r="A1" s="37" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="2" ht="89.25" spans="1:2">
-      <c r="A2" s="41"/>
-      <c r="B2" s="42" t="s">
+      <c r="A2" s="37"/>
+      <c r="B2" s="38" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="3" ht="102" spans="1:2">
-      <c r="A3" s="41"/>
-      <c r="B3" s="7" t="s">
+      <c r="A3" s="37"/>
+      <c r="B3" s="6" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="4" ht="63.75" spans="1:2">
-      <c r="A4" s="41" t="s">
+      <c r="A4" s="37" t="s">
         <v>257</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="6" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="5" ht="63.75" spans="1:2">
-      <c r="A5" s="41"/>
-      <c r="B5" s="42" t="s">
+      <c r="A5" s="37"/>
+      <c r="B5" s="38" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="41"/>
-      <c r="B6" s="42" t="s">
+      <c r="A6" s="37"/>
+      <c r="B6" s="38" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="7" ht="38.25" spans="1:2">
-      <c r="A7" s="41" t="s">
+      <c r="A7" s="37" t="s">
         <v>261</v>
       </c>
-      <c r="B7" s="42" t="s">
+      <c r="B7" s="38" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="8" ht="38.25" spans="1:2">
-      <c r="A8" s="41"/>
-      <c r="B8" s="42" t="s">
+      <c r="A8" s="37"/>
+      <c r="B8" s="38" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="41"/>
-      <c r="B9" s="42" t="s">
+      <c r="A9" s="37"/>
+      <c r="B9" s="38" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="41"/>
-      <c r="B10" s="42" t="s">
+      <c r="A10" s="37"/>
+      <c r="B10" s="38" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="41"/>
-      <c r="B11" s="42" t="s">
+      <c r="A11" s="37"/>
+      <c r="B11" s="38" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="12" ht="51" spans="1:2">
-      <c r="A12" s="41" t="s">
+      <c r="A12" s="37" t="s">
         <v>267</v>
       </c>
-      <c r="B12" s="42" t="s">
+      <c r="B12" s="38" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="13" ht="63.75" spans="1:2">
-      <c r="A13" s="41"/>
-      <c r="B13" s="42" t="s">
+      <c r="A13" s="37"/>
+      <c r="B13" s="38" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="14" ht="127.5" spans="1:2">
-      <c r="A14" s="41"/>
-      <c r="B14" s="42" t="s">
+      <c r="A14" s="37"/>
+      <c r="B14" s="38" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="41"/>
-      <c r="B15" s="42" t="s">
+      <c r="A15" s="37"/>
+      <c r="B15" s="38" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="41"/>
-      <c r="B16" s="42" t="s">
+      <c r="A16" s="37"/>
+      <c r="B16" s="38" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="17" ht="102" spans="1:2">
-      <c r="A17" s="41"/>
-      <c r="B17" s="42" t="s">
+      <c r="A17" s="37"/>
+      <c r="B17" s="38" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="18" ht="38.25" spans="1:2">
-      <c r="A18" s="41"/>
-      <c r="B18" s="42" t="s">
+      <c r="A18" s="37"/>
+      <c r="B18" s="38" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="41"/>
-      <c r="B19" s="42" t="s">
+      <c r="A19" s="37"/>
+      <c r="B19" s="38" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="41"/>
-      <c r="B20" s="43" t="s">
+      <c r="A20" s="37"/>
+      <c r="B20" s="39" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="21" ht="165.75" spans="1:2">
-      <c r="A21" s="44" t="s">
+      <c r="A21" s="40" t="s">
         <v>277</v>
       </c>
-      <c r="B21" s="42" t="s">
+      <c r="B21" s="38" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="22" ht="242.25" spans="1:2">
-      <c r="A22" s="44"/>
-      <c r="B22" s="42" t="s">
+      <c r="A22" s="40"/>
+      <c r="B22" s="38" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="23" ht="153" spans="1:2">
-      <c r="A23" s="44"/>
-      <c r="B23" s="42" t="s">
+      <c r="A23" s="40"/>
+      <c r="B23" s="38" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="24" ht="38.25" spans="1:2">
-      <c r="A24" s="44"/>
-      <c r="B24" s="42" t="s">
+      <c r="A24" s="40"/>
+      <c r="B24" s="38" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="25" ht="25.5" spans="1:2">
-      <c r="A25" s="44"/>
-      <c r="B25" s="42" t="s">
+      <c r="A25" s="40"/>
+      <c r="B25" s="38" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="26" ht="51" spans="1:2">
-      <c r="A26" s="44"/>
-      <c r="B26" s="42" t="s">
+      <c r="A26" s="40"/>
+      <c r="B26" s="38" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="44"/>
-      <c r="B27" s="42" t="s">
+      <c r="A27" s="40"/>
+      <c r="B27" s="38" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="44"/>
-      <c r="B28" s="43" t="s">
+      <c r="A28" s="40"/>
+      <c r="B28" s="39" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="29" ht="38.25" spans="1:2">
-      <c r="A29" s="45" t="s">
+      <c r="A29" s="41" t="s">
         <v>286</v>
       </c>
-      <c r="B29" s="42" t="s">
+      <c r="B29" s="38" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="41"/>
-      <c r="B30" s="42" t="s">
+      <c r="A30" s="37"/>
+      <c r="B30" s="38" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="41"/>
-      <c r="B31" s="42" t="s">
+      <c r="A31" s="37"/>
+      <c r="B31" s="38" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="41"/>
-      <c r="B32" s="42" t="s">
+      <c r="A32" s="37"/>
+      <c r="B32" s="38" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="41"/>
-      <c r="B33" s="42" t="s">
+      <c r="A33" s="37"/>
+      <c r="B33" s="38" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="34" ht="51" spans="1:2">
-      <c r="A34" s="44" t="s">
+      <c r="A34" s="40" t="s">
         <v>292</v>
       </c>
-      <c r="B34" s="7" t="s">
+      <c r="B34" s="6" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="35" ht="38.25" spans="1:2">
-      <c r="A35" s="41"/>
-      <c r="B35" s="7" t="s">
+      <c r="A35" s="37"/>
+      <c r="B35" s="6" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="36" ht="51" spans="1:2">
-      <c r="A36" s="41"/>
-      <c r="B36" s="7" t="s">
+      <c r="A36" s="37"/>
+      <c r="B36" s="6" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="37" ht="51" spans="1:2">
-      <c r="A37" s="41"/>
-      <c r="B37" s="7" t="s">
+      <c r="A37" s="37"/>
+      <c r="B37" s="6" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="38" ht="25.5" spans="1:2">
-      <c r="A38" s="41" t="s">
+      <c r="A38" s="37" t="s">
         <v>297</v>
       </c>
-      <c r="B38" s="7" t="s">
+      <c r="B38" s="6" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="39" ht="76.5" spans="1:2">
-      <c r="A39" s="41"/>
-      <c r="B39" s="7" t="s">
+      <c r="A39" s="37"/>
+      <c r="B39" s="6" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="40" ht="25.5" spans="1:2">
-      <c r="A40" s="41"/>
-      <c r="B40" s="7" t="s">
+      <c r="A40" s="37"/>
+      <c r="B40" s="6" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="41" ht="25.5" spans="1:2">
-      <c r="A41" s="41"/>
-      <c r="B41" s="7" t="s">
+      <c r="A41" s="37"/>
+      <c r="B41" s="6" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="41"/>
-      <c r="B42" s="7" t="s">
+      <c r="A42" s="37"/>
+      <c r="B42" s="6" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="43" ht="25.5" spans="1:2">
-      <c r="A43" s="41"/>
-      <c r="B43" s="7" t="s">
+      <c r="A43" s="37"/>
+      <c r="B43" s="6" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="41"/>
-      <c r="B44" s="7"/>
+      <c r="A44" s="37"/>
+      <c r="B44" s="6"/>
     </row>
     <row r="45" ht="26.25" customHeight="1" spans="1:2">
-      <c r="A45" s="46" t="s">
+      <c r="A45" s="42" t="s">
         <v>304</v>
       </c>
-      <c r="B45" s="46"/>
+      <c r="B45" s="42"/>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="46"/>
-      <c r="B46" s="46"/>
+      <c r="A46" s="42"/>
+      <c r="B46" s="42"/>
     </row>
     <row r="47" ht="51" spans="1:2">
-      <c r="A47" s="41" t="s">
+      <c r="A47" s="37" t="s">
         <v>305</v>
       </c>
-      <c r="B47" s="47" t="s">
+      <c r="B47" s="43" t="s">
         <v>306</v>
       </c>
     </row>
@@ -14691,201 +14831,201 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="55.8533333333333" style="33" customWidth="1"/>
-    <col min="2" max="2" width="54.14" style="34" customWidth="1"/>
-    <col min="3" max="3" width="101.713333333333" style="35" customWidth="1"/>
+    <col min="1" max="1" width="55.8533333333333" style="29" customWidth="1"/>
+    <col min="2" max="2" width="54.14" style="30" customWidth="1"/>
+    <col min="3" max="3" width="101.713333333333" style="31" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" spans="1:1">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="32" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="2" ht="12.75" spans="1:3">
-      <c r="A2" s="36"/>
-      <c r="B2" s="37"/>
-      <c r="C2" s="38"/>
+      <c r="A2" s="32"/>
+      <c r="B2" s="33"/>
+      <c r="C2" s="34"/>
     </row>
     <row r="3" ht="12.75" spans="1:2">
-      <c r="A3" s="36"/>
-      <c r="B3" s="37"/>
+      <c r="A3" s="32"/>
+      <c r="B3" s="33"/>
     </row>
     <row r="4" ht="12.75" spans="1:2">
-      <c r="A4" s="36"/>
-      <c r="B4" s="37"/>
+      <c r="A4" s="32"/>
+      <c r="B4" s="33"/>
     </row>
     <row r="5" ht="12.75" spans="1:2">
-      <c r="A5" s="36"/>
-      <c r="B5" s="37"/>
+      <c r="A5" s="32"/>
+      <c r="B5" s="33"/>
     </row>
     <row r="6" ht="12.75" spans="1:2">
-      <c r="A6" s="36"/>
-      <c r="B6" s="37"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="33"/>
     </row>
     <row r="7" ht="12.75" spans="1:2">
-      <c r="A7" s="36"/>
-      <c r="B7" s="37"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="33"/>
     </row>
     <row r="8" ht="12.75" spans="1:2">
-      <c r="A8" s="36"/>
-      <c r="B8" s="37"/>
+      <c r="A8" s="32"/>
+      <c r="B8" s="33"/>
     </row>
     <row r="9" ht="12.75" spans="1:2">
-      <c r="A9" s="36"/>
-      <c r="B9" s="37"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="33"/>
     </row>
     <row r="10" ht="12.75" spans="1:2">
-      <c r="A10" s="36"/>
-      <c r="B10" s="37"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="33"/>
     </row>
     <row r="11" ht="12.75" spans="1:2">
-      <c r="A11" s="36"/>
-      <c r="B11" s="37"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="33"/>
     </row>
     <row r="12" ht="12.75" spans="1:2">
-      <c r="A12" s="36"/>
-      <c r="B12" s="37"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="33"/>
     </row>
     <row r="13" ht="12.75" spans="1:2">
-      <c r="A13" s="36"/>
-      <c r="B13" s="37"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="33"/>
     </row>
     <row r="14" ht="12.75" spans="1:2">
-      <c r="A14" s="36"/>
-      <c r="B14" s="37"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="33"/>
     </row>
     <row r="15" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A15" s="36"/>
-      <c r="B15" s="37"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="33"/>
     </row>
     <row r="16" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A16" s="36"/>
-      <c r="B16" s="37"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="33"/>
     </row>
     <row r="17" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A17" s="36"/>
-      <c r="B17" s="37"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="33"/>
     </row>
     <row r="18" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A18" s="36"/>
-      <c r="B18" s="37"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="33"/>
     </row>
     <row r="19" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A19" s="36"/>
-      <c r="B19" s="37"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="33"/>
     </row>
     <row r="20" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A20" s="36"/>
-      <c r="B20" s="37"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="33"/>
     </row>
     <row r="21" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A21" s="36"/>
-      <c r="B21" s="37"/>
+      <c r="A21" s="32"/>
+      <c r="B21" s="33"/>
     </row>
     <row r="22" ht="17.25" spans="1:2">
-      <c r="A22" s="36"/>
-      <c r="B22" s="37"/>
+      <c r="A22" s="32"/>
+      <c r="B22" s="33"/>
     </row>
     <row r="23" ht="17.25" spans="1:2">
-      <c r="A23" s="36"/>
-      <c r="B23" s="37"/>
+      <c r="A23" s="32"/>
+      <c r="B23" s="33"/>
     </row>
     <row r="24" ht="17.25" spans="1:2">
-      <c r="A24" s="36"/>
-      <c r="B24" s="39"/>
+      <c r="A24" s="32"/>
+      <c r="B24" s="35"/>
     </row>
     <row r="26" ht="17.25" spans="1:2">
-      <c r="A26" s="36" t="s">
+      <c r="A26" s="32" t="s">
         <v>308</v>
       </c>
-      <c r="B26" s="34" t="s">
+      <c r="B26" s="30" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="27" ht="17.25" spans="1:2">
-      <c r="A27" s="36"/>
-      <c r="B27" s="34" t="s">
+      <c r="A27" s="32"/>
+      <c r="B27" s="30" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="28" ht="17.25" spans="1:2">
-      <c r="A28" s="36"/>
-      <c r="B28" s="34" t="s">
+      <c r="A28" s="32"/>
+      <c r="B28" s="30" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="36"/>
+      <c r="A29" s="32"/>
     </row>
     <row r="30" ht="12.75" spans="1:3">
-      <c r="A30" s="36" t="s">
+      <c r="A30" s="32" t="s">
         <v>312</v>
       </c>
-      <c r="B30" s="34" t="s">
+      <c r="B30" s="30" t="s">
         <v>313</v>
       </c>
-      <c r="C30" s="35" t="s">
+      <c r="C30" s="31" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="31" ht="12.75" spans="1:3">
-      <c r="A31" s="36"/>
-      <c r="C31" s="35" t="s">
+      <c r="A31" s="32"/>
+      <c r="C31" s="31" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="32" ht="12.75" spans="1:3">
-      <c r="A32" s="36"/>
-      <c r="C32" s="35" t="s">
+      <c r="A32" s="32"/>
+      <c r="C32" s="31" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="33" ht="12.75" spans="1:3">
-      <c r="A33" s="36"/>
-      <c r="C33" s="35" t="s">
+      <c r="A33" s="32"/>
+      <c r="C33" s="31" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="35" ht="114.75" spans="1:3">
-      <c r="A35" s="36" t="s">
+      <c r="A35" s="32" t="s">
         <v>318</v>
       </c>
-      <c r="B35" s="34" t="s">
+      <c r="B35" s="30" t="s">
         <v>319</v>
       </c>
-      <c r="C35" s="74" t="s">
+      <c r="C35" s="69" t="s">
         <v>320</v>
       </c>
     </row>
     <row r="36" ht="89.25" spans="1:3">
-      <c r="A36" s="36"/>
-      <c r="B36" s="34" t="s">
+      <c r="A36" s="32"/>
+      <c r="B36" s="30" t="s">
         <v>321</v>
       </c>
-      <c r="C36" s="74" t="s">
+      <c r="C36" s="69" t="s">
         <v>322</v>
       </c>
     </row>
     <row r="37" ht="76.5" spans="1:3">
-      <c r="A37" s="36"/>
-      <c r="B37" s="34" t="s">
+      <c r="A37" s="32"/>
+      <c r="B37" s="30" t="s">
         <v>323</v>
       </c>
-      <c r="C37" s="40" t="s">
+      <c r="C37" s="36" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="38" ht="51" spans="1:3">
-      <c r="A38" s="36"/>
-      <c r="B38" s="34" t="s">
+      <c r="A38" s="32"/>
+      <c r="B38" s="30" t="s">
         <v>325</v>
       </c>
-      <c r="C38" s="40" t="s">
+      <c r="C38" s="36" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="36" t="s">
+      <c r="A40" s="32" t="s">
         <v>327</v>
       </c>
     </row>
@@ -14916,291 +15056,291 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="32" style="27" customWidth="1"/>
-    <col min="2" max="2" width="109" style="27" customWidth="1"/>
+    <col min="1" max="1" width="32" style="23" customWidth="1"/>
+    <col min="2" max="2" width="109" style="23" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="127.5" spans="1:3">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="24" t="s">
         <v>328</v>
       </c>
-      <c r="B1" s="73" t="s">
+      <c r="B1" s="68" t="s">
         <v>329</v>
       </c>
-      <c r="C1" s="29" t="s">
+      <c r="C1" s="25" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="2" ht="200.25" customHeight="1" spans="1:2">
-      <c r="A2" s="27" t="s">
+      <c r="A2" s="23" t="s">
         <v>331</v>
       </c>
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="23" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="3" ht="102" spans="1:2">
-      <c r="A3" s="27" t="s">
+      <c r="A3" s="23" t="s">
         <v>333</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="23" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="4" ht="25.5" spans="1:2">
-      <c r="A4" s="27" t="s">
+      <c r="A4" s="23" t="s">
         <v>335</v>
       </c>
-      <c r="B4" s="73" t="s">
+      <c r="B4" s="68" t="s">
         <v>336</v>
       </c>
     </row>
     <row r="5" ht="25.5" spans="1:2">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="23" t="s">
         <v>337</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="B5" s="23" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="6" ht="38.25" spans="1:1">
-      <c r="A6" s="27" t="s">
+      <c r="A6" s="23" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="7" ht="38.25" spans="1:2">
-      <c r="A7" s="27" t="s">
+      <c r="A7" s="23" t="s">
         <v>340</v>
       </c>
-      <c r="B7" s="27" t="s">
+      <c r="B7" s="23" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="8" ht="114.75" spans="1:2">
-      <c r="A8" s="27" t="s">
+      <c r="A8" s="23" t="s">
         <v>342</v>
       </c>
-      <c r="B8" s="27" t="s">
+      <c r="B8" s="23" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="12" ht="51" spans="1:2">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="23" t="s">
         <v>344</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="23" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="13" ht="51" spans="1:2">
-      <c r="A13" s="27" t="s">
+      <c r="A13" s="23" t="s">
         <v>346</v>
       </c>
-      <c r="B13" s="27" t="s">
+      <c r="B13" s="23" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="14" ht="89.25" spans="1:2">
-      <c r="A14" s="27" t="s">
+      <c r="A14" s="23" t="s">
         <v>348</v>
       </c>
-      <c r="B14" s="27" t="s">
+      <c r="B14" s="23" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="15" ht="102" spans="1:2">
-      <c r="A15" s="27" t="s">
+      <c r="A15" s="23" t="s">
         <v>350</v>
       </c>
-      <c r="B15" s="27" t="s">
+      <c r="B15" s="23" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="27" t="s">
+      <c r="A16" s="23" t="s">
         <v>352</v>
       </c>
-      <c r="B16" s="27" t="s">
+      <c r="B16" s="23" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="17" ht="178.5" spans="1:2">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="23" t="s">
         <v>354</v>
       </c>
-      <c r="B17" s="27" t="s">
+      <c r="B17" s="23" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="18" ht="25.5" spans="1:2">
-      <c r="A18" s="27" t="s">
+      <c r="A18" s="23" t="s">
         <v>356</v>
       </c>
-      <c r="B18" s="27" t="s">
+      <c r="B18" s="23" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="19" ht="280.5" spans="1:2">
-      <c r="A19" s="27" t="s">
+      <c r="A19" s="23" t="s">
         <v>358</v>
       </c>
-      <c r="B19" s="27" t="s">
+      <c r="B19" s="23" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="27" t="s">
+      <c r="A20" s="23" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="27" t="s">
+      <c r="A22" s="23" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="23" spans="2:2">
-      <c r="B23" s="30"/>
+      <c r="B23" s="26"/>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="27" t="s">
+      <c r="A25" s="23" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="27" t="s">
+      <c r="A28" s="23" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="27" t="s">
+      <c r="A31" s="23" t="s">
         <v>364</v>
       </c>
-      <c r="B31" s="27" t="s">
+      <c r="B31" s="23" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="33" ht="38.25" spans="1:2">
-      <c r="A33" s="27" t="s">
+      <c r="A33" s="23" t="s">
         <v>366</v>
       </c>
-      <c r="B33" s="27" t="s">
+      <c r="B33" s="23" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="34" ht="114.75" spans="1:2">
-      <c r="A34" s="27" t="s">
+      <c r="A34" s="23" t="s">
         <v>368</v>
       </c>
-      <c r="B34" s="27" t="s">
+      <c r="B34" s="23" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="27" t="s">
+      <c r="A36" s="23" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="27" t="s">
+      <c r="A38" s="23" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="27" t="s">
+      <c r="A40" s="23" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="27" t="s">
+      <c r="A42" s="23" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="27" t="s">
+      <c r="A44" s="23" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="27" t="s">
+      <c r="A46" s="23" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="27" t="s">
+      <c r="A48" s="23" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="27" t="s">
+      <c r="A50" s="23" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="27" t="s">
+      <c r="A52" s="23" t="s">
         <v>378</v>
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="31" t="s">
+      <c r="A54" s="27" t="s">
         <v>379</v>
       </c>
-      <c r="B54" s="27" t="s">
+      <c r="B54" s="23" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="31"/>
-      <c r="B55" s="27" t="s">
+      <c r="A55" s="27"/>
+      <c r="B55" s="23" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="31"/>
-      <c r="B56" s="27" t="s">
+      <c r="A56" s="27"/>
+      <c r="B56" s="23" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="58" ht="25.5" spans="1:2">
-      <c r="A58" s="10" t="s">
+      <c r="A58" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="B58" s="27" t="s">
+      <c r="B58" s="23" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="10"/>
-      <c r="B59" s="32" t="s">
+      <c r="A59" s="7"/>
+      <c r="B59" s="28" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="60" spans="1:2">
-      <c r="A60" s="10"/>
-      <c r="B60" s="32" t="s">
+      <c r="A60" s="7"/>
+      <c r="B60" s="28" t="s">
         <v>386</v>
       </c>
     </row>
     <row r="61" spans="1:2">
-      <c r="A61" s="10"/>
-      <c r="B61" s="32" t="s">
+      <c r="A61" s="7"/>
+      <c r="B61" s="28" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="62" spans="1:2">
-      <c r="A62" s="10"/>
-      <c r="B62" s="32" t="s">
+      <c r="A62" s="7"/>
+      <c r="B62" s="28" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="63" spans="1:2">
-      <c r="A63" s="10"/>
-      <c r="B63" s="32" t="s">
+      <c r="A63" s="7"/>
+      <c r="B63" s="28" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="10"/>
-      <c r="B64" s="32" t="s">
+      <c r="A64" s="7"/>
+      <c r="B64" s="28" t="s">
         <v>390</v>
       </c>
     </row>
@@ -15228,77 +15368,77 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21.75" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="47" style="21" customWidth="1"/>
-    <col min="2" max="2" width="125" style="22" customWidth="1"/>
-    <col min="3" max="3" width="60" style="23" customWidth="1"/>
-    <col min="4" max="16384" width="9.14" style="23"/>
+    <col min="1" max="1" width="47" style="17" customWidth="1"/>
+    <col min="2" max="2" width="125" style="18" customWidth="1"/>
+    <col min="3" max="3" width="60" style="19" customWidth="1"/>
+    <col min="4" max="16384" width="9.14" style="19"/>
   </cols>
   <sheetData>
     <row r="1" ht="120.75" spans="1:2">
-      <c r="A1" s="21" t="s">
+      <c r="A1" s="17" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="24" t="s">
+      <c r="B1" s="20" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="2" ht="138" spans="2:2">
-      <c r="B2" s="24" t="s">
+      <c r="B2" s="20" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="3" ht="172.5" spans="1:3">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="17" t="s">
         <v>394</v>
       </c>
-      <c r="B3" s="24" t="s">
+      <c r="B3" s="20" t="s">
         <v>395</v>
       </c>
-      <c r="C3" s="25" t="s">
+      <c r="C3" s="21" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="4" ht="103.5" spans="1:2">
-      <c r="A4" s="21" t="s">
+      <c r="A4" s="17" t="s">
         <v>397</v>
       </c>
-      <c r="B4" s="24" t="s">
+      <c r="B4" s="20" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="5" ht="65.25" spans="1:2">
-      <c r="A5" s="26" t="s">
+      <c r="A5" s="22" t="s">
         <v>399</v>
       </c>
-      <c r="B5" s="24"/>
+      <c r="B5" s="20"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="21" t="s">
+      <c r="A6" s="17" t="s">
         <v>400</v>
       </c>
-      <c r="B6" s="24"/>
+      <c r="B6" s="20"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="21" t="s">
+      <c r="A7" s="17" t="s">
         <v>401</v>
       </c>
-      <c r="B7" s="24"/>
+      <c r="B7" s="20"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="21" t="s">
+      <c r="A8" s="17" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="9" ht="34.5" spans="1:2">
-      <c r="A9" s="21" t="s">
+      <c r="A9" s="17" t="s">
         <v>403</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="20" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="21" t="s">
+      <c r="A10" s="17" t="s">
         <v>405</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[feat][design_pattern][Application in strategy design pattern]
</commit_message>
<xml_diff>
--- a/System/Documents.xlsx
+++ b/System/Documents.xlsx
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="498">
   <si>
     <t>Kiến Trúc về Microservice</t>
   </si>
@@ -10396,6 +10396,14 @@
   </si>
   <si>
     <r>
+      <rPr>
+        <b/>
+        <sz val="22"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
       <t xml:space="preserve">Welcome to Design Pattern
 </t>
     </r>
@@ -10632,20 +10640,132 @@
     </r>
   </si>
   <si>
-    <r>
-      <t>The Strategy Pattern</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">:
- - Defines a family of algorithms, encapsulates each one, and makes them interchangeable. Strategy lets the algorithm vary independently from clients that use it.
+    <t xml:space="preserve">The Strategy Pattern
  </t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Defines a </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>family of algorithms</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>encapsulates</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> each one, and makes them </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>interchangeable</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">. Strategy lets the algorithm vary independently from clients that use it:
+ - The Context: maintains a reference to one of the concrete strategies and communicates with this object only via the strategy interface
+ - The Strategy interface: Is common to all concrete strategies. It declares a method the context uses to execute a strategy.
+ - The Concrete Strategies: implement different </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>variations</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(biến thể) of an algorithm the context uses.
+ - The context calls the execution method on the linked strategy object each time it needs to run the algorithm. The context doesn’t know what type of strategy it works with or how the algorithm is executed.
+ - The Client: Creates a specific strategy object and passes it to the context. The context exposes a setter which lets clients replace the strategy associated with the context at runtime.
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Applicability: Use the Strategy Design pattern when
+ - Different </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>variants</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(biến thể) of an algorithm within an object and be able to switch algorithms during runtime.
+ - Have a lot of similar classes that only differ in the way they execute some behavior.
+ - 
+ - </t>
     </r>
   </si>
   <si>
@@ -10736,7 +10856,7 @@
     <t>It feels a little weird to have a class that’s just a behavior. Aren’t classes supposed to represent things? Aren’t classes supposed to have both state(instance variables) AND behavior(methods)?</t>
   </si>
   <si>
-    <t xml:space="preserve"> - In an OO system, yes, classes represent things that generally have both state (instance variables) and methods. And in this case, the thing happens to be a behavior. 
+    <t xml:space="preserve"> - In an OO system, classes represent things that generally have both state (instance variables) and methods. And in this case, the thing happens to be a behavior. 
  - But even a behavior can still have state and methods; a flying behavior might have instance variables representing the attributes for the flying (wing beats per minute, max altitude, speed, etc.) behavior.</t>
   </si>
   <si>
@@ -10784,10 +10904,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="47">
     <font>
@@ -10959,14 +11079,14 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -10974,7 +11094,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -10989,26 +11109,33 @@
     </font>
     <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <sz val="15"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -11019,9 +11146,17 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
+      <i/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -11037,7 +11172,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -11051,7 +11186,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -11059,22 +11194,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -11180,7 +11300,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -11192,7 +11318,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -11204,25 +11336,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -11234,13 +11348,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -11252,73 +11384,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -11336,19 +11408,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFFFFFCC"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -11423,15 +11543,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -11447,6 +11558,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF3F3F3F"/>
       </left>
@@ -11458,17 +11578,6 @@
       </top>
       <bottom style="thin">
         <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -11511,108 +11620,140 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="25" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="37" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="38" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="34" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="13" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="38" fillId="0" borderId="12" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="9" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="11" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="32" borderId="12" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="32" borderId="11" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="11" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="9" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="9" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="37" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="27" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -11621,31 +11762,10 @@
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="15" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="28" borderId="10" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -11675,6 +11795,15 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -11772,9 +11901,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="33" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -11819,12 +11945,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -12636,7 +12756,7 @@
       <c r="B5" s="68" t="s">
         <v>8</v>
       </c>
-      <c r="C5" s="30" t="s">
+      <c r="C5" s="33" t="s">
         <v>9</v>
       </c>
     </row>
@@ -12691,7 +12811,7 @@
       <c r="B10" s="68" t="s">
         <v>18</v>
       </c>
-      <c r="C10" s="30" t="s">
+      <c r="C10" s="33" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="71" t="s">
@@ -12702,7 +12822,7 @@
       <c r="B11" s="68" t="s">
         <v>21</v>
       </c>
-      <c r="C11" s="30" t="s">
+      <c r="C11" s="33" t="s">
         <v>22</v>
       </c>
     </row>
@@ -12710,7 +12830,7 @@
       <c r="B12" s="68" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="30" t="s">
+      <c r="C12" s="33" t="s">
         <v>24</v>
       </c>
     </row>
@@ -12718,7 +12838,7 @@
       <c r="B13" s="68" t="s">
         <v>25</v>
       </c>
-      <c r="C13" s="30" t="s">
+      <c r="C13" s="33" t="s">
         <v>26</v>
       </c>
     </row>
@@ -12726,19 +12846,19 @@
       <c r="B14" s="68" t="s">
         <v>27</v>
       </c>
-      <c r="C14" s="30" t="s">
+      <c r="C14" s="33" t="s">
         <v>28</v>
       </c>
       <c r="D14" s="69" t="s">
         <v>29</v>
       </c>
-      <c r="E14" s="30" t="s">
+      <c r="E14" s="33" t="s">
         <v>30</v>
       </c>
-      <c r="F14" s="30" t="s">
+      <c r="F14" s="33" t="s">
         <v>31</v>
       </c>
-      <c r="G14" s="30" t="s">
+      <c r="G14" s="33" t="s">
         <v>32</v>
       </c>
     </row>
@@ -12746,7 +12866,7 @@
       <c r="B15" s="68" t="s">
         <v>33</v>
       </c>
-      <c r="C15" s="30" t="s">
+      <c r="C15" s="33" t="s">
         <v>34</v>
       </c>
     </row>
@@ -12796,7 +12916,7 @@
   </cols>
   <sheetData>
     <row r="1" ht="76.5" spans="3:3">
-      <c r="C1" s="23" t="s">
+      <c r="C1" s="26" t="s">
         <v>406</v>
       </c>
     </row>
@@ -12837,12 +12957,12 @@
   </cols>
   <sheetData>
     <row r="1" ht="89.25" spans="4:4">
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="16" t="s">
         <v>407</v>
       </c>
     </row>
     <row r="2" ht="350" customHeight="1" spans="4:4">
-      <c r="D2" s="23" t="s">
+      <c r="D2" s="26" t="s">
         <v>408</v>
       </c>
     </row>
@@ -12869,57 +12989,57 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
-      <c r="A1" s="17" t="s">
+      <c r="A1" s="20" t="s">
         <v>409</v>
       </c>
-      <c r="B1" s="18" t="s">
+      <c r="B1" s="21" t="s">
         <v>410</v>
       </c>
-      <c r="C1" s="19" t="s">
+      <c r="C1" s="22" t="s">
         <v>411</v>
       </c>
     </row>
     <row r="2" spans="1:3">
-      <c r="A2" s="20" t="s">
+      <c r="A2" s="23" t="s">
         <v>412</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="20"/>
+      <c r="B2" s="24"/>
+      <c r="C2" s="23"/>
     </row>
     <row r="3" spans="1:3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="20" t="s">
         <v>413</v>
       </c>
-      <c r="B3" s="21"/>
-      <c r="C3" s="17"/>
+      <c r="B3" s="24"/>
+      <c r="C3" s="20"/>
     </row>
     <row r="4" spans="1:3">
-      <c r="A4" s="20" t="s">
+      <c r="A4" s="23" t="s">
         <v>414</v>
       </c>
-      <c r="B4" s="21"/>
-      <c r="C4" s="20"/>
+      <c r="B4" s="24"/>
+      <c r="C4" s="23"/>
     </row>
     <row r="5" spans="1:3">
-      <c r="A5" s="17" t="s">
+      <c r="A5" s="20" t="s">
         <v>415</v>
       </c>
-      <c r="B5" s="21"/>
-      <c r="C5" s="17"/>
+      <c r="B5" s="24"/>
+      <c r="C5" s="20"/>
     </row>
     <row r="6" spans="1:3">
-      <c r="A6" s="20" t="s">
+      <c r="A6" s="23" t="s">
         <v>416</v>
       </c>
-      <c r="B6" s="21"/>
-      <c r="C6" s="20"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="23"/>
     </row>
     <row r="7" spans="1:3">
-      <c r="A7" s="17" t="s">
+      <c r="A7" s="20" t="s">
         <v>417</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="17"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="20"/>
     </row>
     <row r="8" customFormat="1"/>
     <row r="9" customFormat="1"/>
@@ -12999,104 +13119,104 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="12.1" style="14" customWidth="1"/>
-    <col min="2" max="2" width="168" style="11" customWidth="1"/>
+    <col min="1" max="1" width="12.1" style="17" customWidth="1"/>
+    <col min="2" max="2" width="168" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="267.75" spans="1:2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="17" t="s">
         <v>424</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="12" t="s">
         <v>425</v>
       </c>
     </row>
     <row r="2" ht="76.5" spans="1:2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="17" t="s">
         <v>426</v>
       </c>
-      <c r="B2" s="11" t="s">
+      <c r="B2" s="14" t="s">
         <v>427</v>
       </c>
     </row>
     <row r="3" ht="38.25" spans="1:2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="17" t="s">
         <v>428</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="14" t="s">
         <v>429</v>
       </c>
     </row>
     <row r="4" ht="127.5" spans="1:2">
-      <c r="A4" s="14" t="s">
+      <c r="A4" s="17" t="s">
         <v>430</v>
       </c>
-      <c r="B4" s="9" t="s">
+      <c r="B4" s="12" t="s">
         <v>431</v>
       </c>
     </row>
     <row r="5" ht="114.75" spans="2:2">
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="12" t="s">
         <v>432</v>
       </c>
     </row>
     <row r="6" ht="51" spans="1:2">
-      <c r="A6" s="14" t="s">
+      <c r="A6" s="17" t="s">
         <v>433</v>
       </c>
-      <c r="B6" s="11" t="s">
+      <c r="B6" s="14" t="s">
         <v>434</v>
       </c>
     </row>
     <row r="7" ht="63.75" spans="1:2">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="17" t="s">
         <v>435</v>
       </c>
-      <c r="B7" s="11" t="s">
+      <c r="B7" s="14" t="s">
         <v>436</v>
       </c>
     </row>
     <row r="8" ht="38.25" spans="1:2">
-      <c r="A8" s="14" t="s">
+      <c r="A8" s="17" t="s">
         <v>437</v>
       </c>
-      <c r="B8" s="11" t="s">
+      <c r="B8" s="14" t="s">
         <v>438</v>
       </c>
     </row>
     <row r="9" ht="38.25" spans="1:2">
-      <c r="A9" s="14" t="s">
+      <c r="A9" s="17" t="s">
         <v>439</v>
       </c>
-      <c r="B9" s="11" t="s">
+      <c r="B9" s="14" t="s">
         <v>440</v>
       </c>
     </row>
     <row r="10" ht="38.25" spans="1:2">
-      <c r="A10" s="14" t="s">
+      <c r="A10" s="17" t="s">
         <v>441</v>
       </c>
-      <c r="B10" s="11" t="s">
+      <c r="B10" s="14" t="s">
         <v>442</v>
       </c>
     </row>
     <row r="11" ht="127.5" spans="1:2">
-      <c r="A11" s="16" t="s">
+      <c r="A11" s="19" t="s">
         <v>443</v>
       </c>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="12" t="s">
         <v>444</v>
       </c>
     </row>
     <row r="12" ht="51" spans="1:2">
-      <c r="A12" s="16"/>
-      <c r="B12" s="9" t="s">
+      <c r="A12" s="19"/>
+      <c r="B12" s="12" t="s">
         <v>445</v>
       </c>
     </row>
     <row r="13" ht="102" spans="1:2">
-      <c r="A13" s="16"/>
-      <c r="B13" s="11" t="s">
+      <c r="A13" s="19"/>
+      <c r="B13" s="14" t="s">
         <v>446</v>
       </c>
     </row>
@@ -13124,23 +13244,23 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="12.75" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="13" style="14" customWidth="1"/>
-    <col min="2" max="2" width="160.3" style="11" customWidth="1"/>
+    <col min="1" max="1" width="13" style="17" customWidth="1"/>
+    <col min="2" max="2" width="160.3" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
-      <c r="A1" s="14" t="s">
+      <c r="A1" s="17" t="s">
         <v>447</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="12" t="s">
         <v>448</v>
       </c>
     </row>
     <row r="2" ht="153" spans="1:2">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="17" t="s">
         <v>449</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="18" t="s">
         <v>450</v>
       </c>
     </row>
@@ -13197,20 +13317,20 @@
   </cols>
   <sheetData>
     <row r="1" ht="25.5" spans="2:2">
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="16" t="s">
         <v>451</v>
       </c>
     </row>
     <row r="3" ht="51" spans="1:2">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="16" t="s">
         <v>452</v>
       </c>
-      <c r="B3" s="11" t="s">
+      <c r="B3" s="14" t="s">
         <v>453</v>
       </c>
     </row>
     <row r="4" spans="2:2">
-      <c r="B4" s="12"/>
+      <c r="B4" s="15"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -13229,56 +13349,56 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85333333333333" defaultRowHeight="21.75" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="17" style="29" customWidth="1"/>
-    <col min="2" max="2" width="15.8533333333333" style="59" customWidth="1"/>
-    <col min="3" max="3" width="13.8533333333333" style="60" customWidth="1"/>
-    <col min="4" max="4" width="156.14" style="61" customWidth="1"/>
+    <col min="1" max="1" width="17" style="32" customWidth="1"/>
+    <col min="2" max="2" width="15.8533333333333" style="61" customWidth="1"/>
+    <col min="3" max="3" width="13.8533333333333" style="62" customWidth="1"/>
+    <col min="4" max="4" width="156.14" style="63" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="90" customHeight="1" spans="2:4">
-      <c r="B1" s="59" t="s">
+      <c r="B1" s="61" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="62" t="s">
+      <c r="C1" s="64" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="63"/>
+      <c r="D1" s="65"/>
     </row>
     <row r="2" ht="57" customHeight="1" spans="3:4">
-      <c r="C2" s="64" t="s">
+      <c r="C2" s="10" t="s">
         <v>42</v>
       </c>
       <c r="D2" s="6"/>
     </row>
     <row r="3" ht="151" customHeight="1" spans="1:4">
-      <c r="A3" s="29" t="s">
+      <c r="A3" s="32" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="59" t="s">
+      <c r="B3" s="61" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="65" t="s">
+      <c r="C3" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="63"/>
+      <c r="D3" s="65"/>
     </row>
     <row r="4" ht="66" customHeight="1" spans="2:4">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="61" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="62" t="s">
+      <c r="C4" s="64" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="63"/>
+      <c r="D4" s="65"/>
     </row>
     <row r="5" ht="114" customHeight="1" spans="2:4">
-      <c r="B5" s="59" t="s">
+      <c r="B5" s="61" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="62" t="s">
+      <c r="C5" s="64" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="63"/>
+      <c r="D5" s="65"/>
     </row>
     <row r="6" ht="33.95" customHeight="1" spans="2:5">
       <c r="B6" s="66" t="s">
@@ -13287,35 +13407,35 @@
       <c r="C6" s="67" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="63" t="s">
+      <c r="D6" s="65" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="11"/>
+      <c r="E6" s="14"/>
     </row>
     <row r="7" ht="45" customHeight="1" spans="2:3">
-      <c r="B7" s="59" t="s">
+      <c r="B7" s="61" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="62" t="s">
+      <c r="C7" s="64" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="8" ht="30" customHeight="1" spans="2:3">
-      <c r="B8" s="59" t="s">
+      <c r="B8" s="61" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="65" t="s">
+      <c r="C8" s="9" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="9" ht="25.5" spans="1:4">
-      <c r="A9" s="29" t="s">
+      <c r="A9" s="32" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="59" t="s">
+      <c r="B9" s="61" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="51" t="s">
+      <c r="C9" s="53" t="s">
         <v>59</v>
       </c>
       <c r="D9" s="7" t="s">
@@ -13323,15 +13443,15 @@
       </c>
     </row>
     <row r="10" ht="25.5" spans="3:4">
-      <c r="C10" s="51" t="s">
+      <c r="C10" s="53" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="63" t="s">
+      <c r="D10" s="65" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="11" ht="38.25" spans="3:4">
-      <c r="C11" s="51" t="s">
+      <c r="C11" s="53" t="s">
         <v>63</v>
       </c>
       <c r="D11" s="7" t="s">
@@ -13339,22 +13459,22 @@
       </c>
     </row>
     <row r="12" spans="2:4">
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="53" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="63" t="s">
+      <c r="C12" s="65" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="63"/>
+      <c r="D12" s="65"/>
     </row>
     <row r="13" ht="308" customHeight="1" spans="2:4">
-      <c r="B13" s="59" t="s">
+      <c r="B13" s="61" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="65" t="s">
+      <c r="C13" s="9" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="63"/>
+      <c r="D13" s="65"/>
     </row>
   </sheetData>
   <mergeCells count="14">
@@ -13389,26 +13509,26 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="24" outlineLevelCol="4"/>
   <cols>
-    <col min="1" max="1" width="26.8" style="10" customWidth="1"/>
+    <col min="1" max="1" width="26.8" style="13" customWidth="1"/>
     <col min="2" max="2" width="25.6" style="5" customWidth="1"/>
-    <col min="3" max="3" width="8.8" style="11"/>
-    <col min="4" max="4" width="8.8" style="12"/>
-    <col min="5" max="5" width="110.7" style="12" customWidth="1"/>
+    <col min="3" max="3" width="8.8" style="14"/>
+    <col min="4" max="4" width="8.8" style="15"/>
+    <col min="5" max="5" width="110.7" style="15" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="32" customHeight="1" spans="1:3">
-      <c r="A1" s="10" t="s">
+      <c r="A1" s="13" t="s">
         <v>454</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>455</v>
       </c>
-      <c r="C1" s="9" t="s">
+      <c r="C1" s="12" t="s">
         <v>456</v>
       </c>
     </row>
     <row r="2" ht="51" spans="3:3">
-      <c r="C2" s="11" t="s">
+      <c r="C2" s="14" t="s">
         <v>457</v>
       </c>
     </row>
@@ -13430,7 +13550,7 @@
       </c>
     </row>
     <row r="17" ht="12.75" spans="1:2">
-      <c r="A17" s="10" t="s">
+      <c r="A17" s="13" t="s">
         <v>461</v>
       </c>
       <c r="B17" s="5" t="s">
@@ -13458,7 +13578,7 @@
       </c>
     </row>
     <row r="42" ht="12.75" spans="1:2">
-      <c r="A42" s="10" t="s">
+      <c r="A42" s="13" t="s">
         <v>467</v>
       </c>
       <c r="B42" s="5" t="s">
@@ -13502,10 +13622,10 @@
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D20"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8" defaultRowHeight="26.25" outlineLevelCol="3"/>
@@ -13552,99 +13672,132 @@
       </c>
       <c r="D4" s="7"/>
     </row>
-    <row r="5" ht="36" customHeight="1" spans="1:4">
+    <row r="5" ht="127.5" spans="1:4">
       <c r="A5" s="4"/>
       <c r="B5" s="5"/>
-      <c r="C5" s="6" t="s">
+      <c r="C5" s="8" t="s">
         <v>477</v>
       </c>
-      <c r="D5" s="7"/>
-    </row>
-    <row r="6" ht="66" customHeight="1" spans="1:4">
+      <c r="D5" s="9" t="s">
+        <v>478</v>
+      </c>
+    </row>
+    <row r="6" ht="63.75" spans="1:4">
       <c r="A6" s="4"/>
-      <c r="B6" s="5" t="s">
-        <v>478</v>
-      </c>
-      <c r="C6" s="8" t="s">
+      <c r="B6" s="5"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="7" t="s">
         <v>479</v>
       </c>
-      <c r="D6" s="7" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="7" ht="90" customHeight="1" spans="1:4">
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="4"/>
       <c r="B7" s="5"/>
-      <c r="C7" s="9" t="s">
+      <c r="C7" s="8"/>
+      <c r="D7" s="7"/>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" s="4"/>
+      <c r="B8" s="5"/>
+      <c r="C8" s="8"/>
+      <c r="D8" s="7"/>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="4"/>
+      <c r="B9" s="5"/>
+      <c r="C9" s="8"/>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" s="4"/>
+      <c r="B10" s="5"/>
+      <c r="C10" s="10"/>
+      <c r="D10" s="7"/>
+    </row>
+    <row r="11" ht="66" customHeight="1" spans="1:4">
+      <c r="A11" s="4"/>
+      <c r="B11" s="5" t="s">
+        <v>480</v>
+      </c>
+      <c r="C11" s="11" t="s">
         <v>481</v>
       </c>
-      <c r="D7" s="7" t="s">
+      <c r="D11" s="7" t="s">
         <v>482</v>
       </c>
     </row>
-    <row r="8" ht="52.5" spans="1:1">
-      <c r="A8" s="1" t="s">
+    <row r="12" ht="90" customHeight="1" spans="1:4">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="12" t="s">
         <v>483</v>
       </c>
-    </row>
-    <row r="9" ht="52.5" spans="1:1">
-      <c r="A9" s="1" t="s">
+      <c r="D12" s="7" t="s">
         <v>484</v>
-      </c>
-    </row>
-    <row r="10" ht="52.5" spans="1:1">
-      <c r="A10" s="1" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="11" ht="52.5" spans="1:1">
-      <c r="A11" s="1" t="s">
-        <v>486</v>
-      </c>
-    </row>
-    <row r="12" ht="52.5" spans="1:1">
-      <c r="A12" s="1" t="s">
-        <v>487</v>
       </c>
     </row>
     <row r="13" ht="52.5" spans="1:1">
       <c r="A13" s="1" t="s">
-        <v>488</v>
+        <v>485</v>
       </c>
     </row>
     <row r="14" ht="52.5" spans="1:1">
       <c r="A14" s="1" t="s">
-        <v>489</v>
-      </c>
-    </row>
-    <row r="15" ht="78.75" spans="1:1">
+        <v>486</v>
+      </c>
+    </row>
+    <row r="15" ht="52.5" spans="1:1">
       <c r="A15" s="1" t="s">
-        <v>490</v>
+        <v>487</v>
       </c>
     </row>
     <row r="16" ht="52.5" spans="1:1">
       <c r="A16" s="1" t="s">
-        <v>491</v>
+        <v>488</v>
       </c>
     </row>
     <row r="17" ht="52.5" spans="1:1">
       <c r="A17" s="1" t="s">
-        <v>492</v>
+        <v>489</v>
       </c>
     </row>
     <row r="18" ht="52.5" spans="1:1">
       <c r="A18" s="1" t="s">
-        <v>493</v>
+        <v>490</v>
       </c>
     </row>
     <row r="19" ht="52.5" spans="1:1">
       <c r="A19" s="1" t="s">
+        <v>491</v>
+      </c>
+    </row>
+    <row r="20" ht="78.75" spans="1:1">
+      <c r="A20" s="1" t="s">
+        <v>492</v>
+      </c>
+    </row>
+    <row r="21" ht="52.5" spans="1:1">
+      <c r="A21" s="1" t="s">
+        <v>493</v>
+      </c>
+    </row>
+    <row r="22" ht="52.5" spans="1:1">
+      <c r="A22" s="1" t="s">
         <v>494</v>
       </c>
     </row>
-    <row r="20" ht="52.5" spans="1:1">
-      <c r="A20" s="1" t="s">
+    <row r="23" ht="52.5" spans="1:1">
+      <c r="A23" s="1" t="s">
         <v>495</v>
+      </c>
+    </row>
+    <row r="24" ht="52.5" spans="1:1">
+      <c r="A24" s="1" t="s">
+        <v>496</v>
+      </c>
+    </row>
+    <row r="25" ht="52.5" spans="1:1">
+      <c r="A25" s="1" t="s">
+        <v>497</v>
       </c>
     </row>
   </sheetData>
@@ -13653,10 +13806,10 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="A2:A7"/>
-    <mergeCell ref="B2:B5"/>
-    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="A2:A12"/>
+    <mergeCell ref="B2:B10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C5:C10"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -13674,1197 +13827,1197 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="20.5" style="10" customWidth="1"/>
-    <col min="2" max="2" width="14.5733333333333" style="51" customWidth="1"/>
-    <col min="3" max="3" width="15.7133333333333" style="51" customWidth="1"/>
-    <col min="4" max="4" width="167.106666666667" style="26" customWidth="1"/>
-    <col min="5" max="16384" width="9" style="26"/>
+    <col min="1" max="1" width="20.5" style="13" customWidth="1"/>
+    <col min="2" max="2" width="14.5733333333333" style="53" customWidth="1"/>
+    <col min="3" max="3" width="15.7133333333333" style="53" customWidth="1"/>
+    <col min="4" max="4" width="167.106666666667" style="29" customWidth="1"/>
+    <col min="5" max="16384" width="9" style="29"/>
   </cols>
   <sheetData>
-    <row r="1" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A1" s="52" t="s">
+    <row r="1" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A1" s="54" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="16" t="s">
+      <c r="B1" s="19" t="s">
         <v>70</v>
       </c>
-      <c r="C1" s="51" t="s">
+      <c r="C1" s="53" t="s">
         <v>71</v>
       </c>
-      <c r="D1" s="9"/>
-    </row>
-    <row r="2" s="26" customFormat="1" ht="357" spans="1:4">
-      <c r="A2" s="53"/>
-      <c r="B2" s="16"/>
-      <c r="C2" s="51" t="s">
+      <c r="D1" s="12"/>
+    </row>
+    <row r="2" s="29" customFormat="1" ht="357" spans="1:4">
+      <c r="A2" s="55"/>
+      <c r="B2" s="19"/>
+      <c r="C2" s="53" t="s">
         <v>72</v>
       </c>
-      <c r="D2" s="9" t="s">
+      <c r="D2" s="12" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="3" s="26" customFormat="1" ht="89.25" spans="1:4">
-      <c r="A3" s="53"/>
-      <c r="B3" s="54" t="s">
+    <row r="3" s="29" customFormat="1" ht="89.25" spans="1:4">
+      <c r="A3" s="55"/>
+      <c r="B3" s="56" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="51" t="s">
+      <c r="C3" s="53" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="12" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="4" s="26" customFormat="1" ht="76.5" spans="1:4">
-      <c r="A4" s="53"/>
-      <c r="B4" s="54"/>
-      <c r="C4" s="51" t="s">
+    <row r="4" s="29" customFormat="1" ht="76.5" spans="1:4">
+      <c r="A4" s="55"/>
+      <c r="B4" s="56"/>
+      <c r="C4" s="53" t="s">
         <v>77</v>
       </c>
-      <c r="D4" s="9" t="s">
+      <c r="D4" s="12" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="5" s="26" customFormat="1" ht="229.5" spans="1:4">
-      <c r="A5" s="53"/>
-      <c r="B5" s="54"/>
-      <c r="C5" s="51" t="s">
+    <row r="5" s="29" customFormat="1" ht="229.5" spans="1:4">
+      <c r="A5" s="55"/>
+      <c r="B5" s="56"/>
+      <c r="C5" s="53" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="9" t="s">
+      <c r="D5" s="12" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="6" s="26" customFormat="1" ht="63.75" spans="1:4">
-      <c r="A6" s="53"/>
-      <c r="B6" s="54"/>
-      <c r="C6" s="51" t="s">
+    <row r="6" s="29" customFormat="1" ht="63.75" spans="1:4">
+      <c r="A6" s="55"/>
+      <c r="B6" s="56"/>
+      <c r="C6" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="D6" s="9" t="s">
+      <c r="D6" s="12" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="7" s="26" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A7" s="53"/>
-      <c r="B7" s="54"/>
-      <c r="C7" s="51" t="s">
+    <row r="7" s="29" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A7" s="55"/>
+      <c r="B7" s="56"/>
+      <c r="C7" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="D7" s="9" t="s">
+      <c r="D7" s="12" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="8" s="26" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A8" s="53"/>
-      <c r="B8" s="54"/>
-      <c r="C8" s="51" t="s">
+    <row r="8" s="29" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A8" s="55"/>
+      <c r="B8" s="56"/>
+      <c r="C8" s="53" t="s">
         <v>85</v>
       </c>
-      <c r="D8" s="9" t="s">
+      <c r="D8" s="12" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="9" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A9" s="53"/>
-      <c r="B9" s="54"/>
-      <c r="C9" s="51" t="s">
+    <row r="9" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A9" s="55"/>
+      <c r="B9" s="56"/>
+      <c r="C9" s="53" t="s">
         <v>87</v>
       </c>
-      <c r="D9" s="9"/>
-    </row>
-    <row r="10" s="26" customFormat="1" ht="216.75" spans="1:4">
-      <c r="A10" s="53"/>
-      <c r="B10" s="54"/>
-      <c r="C10" s="51" t="s">
+      <c r="D9" s="12"/>
+    </row>
+    <row r="10" s="29" customFormat="1" ht="216.75" spans="1:4">
+      <c r="A10" s="55"/>
+      <c r="B10" s="56"/>
+      <c r="C10" s="53" t="s">
         <v>88</v>
       </c>
-      <c r="D10" s="9" t="s">
+      <c r="D10" s="12" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="11" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A11" s="53"/>
-      <c r="B11" s="54"/>
-      <c r="C11" s="51" t="s">
+    <row r="11" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A11" s="55"/>
+      <c r="B11" s="56"/>
+      <c r="C11" s="53" t="s">
         <v>90</v>
       </c>
-      <c r="D11" s="9"/>
-    </row>
-    <row r="12" s="26" customFormat="1" ht="12.75" spans="1:3">
-      <c r="A12" s="53"/>
-      <c r="B12" s="54"/>
-      <c r="C12" s="51" t="s">
+      <c r="D11" s="12"/>
+    </row>
+    <row r="12" s="29" customFormat="1" ht="12.75" spans="1:3">
+      <c r="A12" s="55"/>
+      <c r="B12" s="56"/>
+      <c r="C12" s="53" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="13" s="26" customFormat="1" ht="107.25" customHeight="1" spans="1:4">
-      <c r="A13" s="53"/>
-      <c r="B13" s="54" t="s">
+    <row r="13" s="29" customFormat="1" ht="107.25" customHeight="1" spans="1:4">
+      <c r="A13" s="55"/>
+      <c r="B13" s="56" t="s">
         <v>92</v>
       </c>
-      <c r="C13" s="9" t="s">
+      <c r="C13" s="12" t="s">
         <v>93</v>
       </c>
-      <c r="D13" s="9"/>
-    </row>
-    <row r="14" s="26" customFormat="1" ht="89.25" spans="1:4">
-      <c r="A14" s="53"/>
-      <c r="B14" s="54"/>
-      <c r="C14" s="51" t="s">
+      <c r="D13" s="12"/>
+    </row>
+    <row r="14" s="29" customFormat="1" ht="89.25" spans="1:4">
+      <c r="A14" s="55"/>
+      <c r="B14" s="56"/>
+      <c r="C14" s="53" t="s">
         <v>94</v>
       </c>
-      <c r="D14" s="9" t="s">
+      <c r="D14" s="12" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="15" s="26" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A15" s="53"/>
-      <c r="B15" s="54"/>
-      <c r="C15" s="51" t="s">
+    <row r="15" s="29" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A15" s="55"/>
+      <c r="B15" s="56"/>
+      <c r="C15" s="53" t="s">
         <v>96</v>
       </c>
-      <c r="D15" s="9" t="s">
+      <c r="D15" s="12" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="16" s="26" customFormat="1" ht="89.25" spans="1:4">
-      <c r="A16" s="53"/>
-      <c r="B16" s="54"/>
-      <c r="C16" s="51"/>
-      <c r="D16" s="9" t="s">
+    <row r="16" s="29" customFormat="1" ht="89.25" spans="1:4">
+      <c r="A16" s="55"/>
+      <c r="B16" s="56"/>
+      <c r="C16" s="53"/>
+      <c r="D16" s="12" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="17" s="26" customFormat="1" ht="63.75" spans="1:4">
-      <c r="A17" s="53"/>
-      <c r="B17" s="54"/>
-      <c r="C17" s="51"/>
-      <c r="D17" s="9" t="s">
+    <row r="17" s="29" customFormat="1" ht="63.75" spans="1:4">
+      <c r="A17" s="55"/>
+      <c r="B17" s="56"/>
+      <c r="C17" s="53"/>
+      <c r="D17" s="12" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="18" s="26" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A18" s="53"/>
-      <c r="B18" s="54"/>
-      <c r="C18" s="51"/>
-      <c r="D18" s="9" t="s">
+    <row r="18" s="29" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A18" s="55"/>
+      <c r="B18" s="56"/>
+      <c r="C18" s="53"/>
+      <c r="D18" s="12" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="19" s="26" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A19" s="53"/>
-      <c r="B19" s="54"/>
-      <c r="C19" s="51"/>
-      <c r="D19" s="9" t="s">
+    <row r="19" s="29" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A19" s="55"/>
+      <c r="B19" s="56"/>
+      <c r="C19" s="53"/>
+      <c r="D19" s="12" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="20" s="26" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A20" s="53"/>
-      <c r="B20" s="54"/>
-      <c r="C20" s="51"/>
-      <c r="D20" s="9" t="s">
+    <row r="20" s="29" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A20" s="55"/>
+      <c r="B20" s="56"/>
+      <c r="C20" s="53"/>
+      <c r="D20" s="12" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="21" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A21" s="53"/>
-      <c r="B21" s="54"/>
-      <c r="C21" s="51"/>
-      <c r="D21" s="9" t="s">
+    <row r="21" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A21" s="55"/>
+      <c r="B21" s="56"/>
+      <c r="C21" s="53"/>
+      <c r="D21" s="12" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="22" s="26" customFormat="1" ht="76.5" spans="1:4">
-      <c r="A22" s="53"/>
-      <c r="B22" s="54"/>
-      <c r="C22" s="51" t="s">
+    <row r="22" s="29" customFormat="1" ht="76.5" spans="1:4">
+      <c r="A22" s="55"/>
+      <c r="B22" s="56"/>
+      <c r="C22" s="53" t="s">
         <v>104</v>
       </c>
-      <c r="D22" s="9" t="s">
+      <c r="D22" s="12" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="23" s="26" customFormat="1" ht="76.5" spans="1:4">
-      <c r="A23" s="53"/>
-      <c r="B23" s="54"/>
-      <c r="C23" s="51"/>
-      <c r="D23" s="9" t="s">
+    <row r="23" s="29" customFormat="1" ht="76.5" spans="1:4">
+      <c r="A23" s="55"/>
+      <c r="B23" s="56"/>
+      <c r="C23" s="53"/>
+      <c r="D23" s="12" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="24" s="26" customFormat="1" ht="89.25" spans="1:4">
-      <c r="A24" s="53"/>
-      <c r="B24" s="54"/>
-      <c r="C24" s="51"/>
-      <c r="D24" s="9" t="s">
+    <row r="24" s="29" customFormat="1" ht="89.25" spans="1:4">
+      <c r="A24" s="55"/>
+      <c r="B24" s="56"/>
+      <c r="C24" s="53"/>
+      <c r="D24" s="12" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="25" s="26" customFormat="1" ht="63.75" spans="1:4">
-      <c r="A25" s="53"/>
-      <c r="B25" s="54"/>
-      <c r="C25" s="51"/>
-      <c r="D25" s="9" t="s">
+    <row r="25" s="29" customFormat="1" ht="63.75" spans="1:4">
+      <c r="A25" s="55"/>
+      <c r="B25" s="56"/>
+      <c r="C25" s="53"/>
+      <c r="D25" s="12" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="26" s="26" customFormat="1" ht="89.25" spans="1:4">
-      <c r="A26" s="53"/>
-      <c r="B26" s="54"/>
-      <c r="C26" s="51"/>
-      <c r="D26" s="9" t="s">
+    <row r="26" s="29" customFormat="1" ht="89.25" spans="1:4">
+      <c r="A26" s="55"/>
+      <c r="B26" s="56"/>
+      <c r="C26" s="53"/>
+      <c r="D26" s="12" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="27" s="26" customFormat="1" ht="165.75" spans="1:4">
-      <c r="A27" s="53"/>
-      <c r="B27" s="54"/>
-      <c r="C27" s="51"/>
-      <c r="D27" s="9" t="s">
+    <row r="27" s="29" customFormat="1" ht="165.75" spans="1:4">
+      <c r="A27" s="55"/>
+      <c r="B27" s="56"/>
+      <c r="C27" s="53"/>
+      <c r="D27" s="12" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="28" s="26" customFormat="1" ht="89.25" spans="1:4">
-      <c r="A28" s="53"/>
-      <c r="B28" s="54"/>
-      <c r="C28" s="51"/>
-      <c r="D28" s="9" t="s">
+    <row r="28" s="29" customFormat="1" ht="89.25" spans="1:4">
+      <c r="A28" s="55"/>
+      <c r="B28" s="56"/>
+      <c r="C28" s="53"/>
+      <c r="D28" s="12" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="29" s="26" customFormat="1" ht="153" spans="1:4">
-      <c r="A29" s="53"/>
-      <c r="B29" s="54"/>
-      <c r="C29" s="51"/>
-      <c r="D29" s="9" t="s">
+    <row r="29" s="29" customFormat="1" ht="153" spans="1:4">
+      <c r="A29" s="55"/>
+      <c r="B29" s="56"/>
+      <c r="C29" s="53"/>
+      <c r="D29" s="12" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="30" s="26" customFormat="1" ht="89.25" spans="1:4">
-      <c r="A30" s="53"/>
-      <c r="B30" s="54"/>
-      <c r="C30" s="51"/>
-      <c r="D30" s="9" t="s">
+    <row r="30" s="29" customFormat="1" ht="89.25" spans="1:4">
+      <c r="A30" s="55"/>
+      <c r="B30" s="56"/>
+      <c r="C30" s="53"/>
+      <c r="D30" s="12" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="31" s="26" customFormat="1" ht="140.25" spans="1:4">
-      <c r="A31" s="53"/>
-      <c r="B31" s="54"/>
-      <c r="C31" s="51"/>
-      <c r="D31" s="9" t="s">
+    <row r="31" s="29" customFormat="1" ht="140.25" spans="1:4">
+      <c r="A31" s="55"/>
+      <c r="B31" s="56"/>
+      <c r="C31" s="53"/>
+      <c r="D31" s="12" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="32" s="26" customFormat="1" ht="89.25" spans="1:4">
-      <c r="A32" s="53"/>
-      <c r="B32" s="54"/>
-      <c r="C32" s="51"/>
-      <c r="D32" s="9" t="s">
+    <row r="32" s="29" customFormat="1" ht="89.25" spans="1:4">
+      <c r="A32" s="55"/>
+      <c r="B32" s="56"/>
+      <c r="C32" s="53"/>
+      <c r="D32" s="12" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="33" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A33" s="53"/>
-      <c r="B33" s="54"/>
-      <c r="C33" s="51"/>
-      <c r="D33" s="9" t="s">
+    <row r="33" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A33" s="55"/>
+      <c r="B33" s="56"/>
+      <c r="C33" s="53"/>
+      <c r="D33" s="12" t="s">
         <v>116</v>
       </c>
     </row>
-    <row r="34" s="26" customFormat="1" ht="89.25" spans="1:4">
-      <c r="A34" s="53"/>
-      <c r="B34" s="54"/>
-      <c r="C34" s="51"/>
-      <c r="D34" s="23" t="s">
+    <row r="34" s="29" customFormat="1" ht="89.25" spans="1:4">
+      <c r="A34" s="55"/>
+      <c r="B34" s="56"/>
+      <c r="C34" s="53"/>
+      <c r="D34" s="26" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="35" s="26" customFormat="1" ht="369.75" spans="1:4">
-      <c r="A35" s="53"/>
-      <c r="B35" s="54"/>
-      <c r="C35" s="51"/>
-      <c r="D35" s="9" t="s">
+    <row r="35" s="29" customFormat="1" ht="369.75" spans="1:4">
+      <c r="A35" s="55"/>
+      <c r="B35" s="56"/>
+      <c r="C35" s="53"/>
+      <c r="D35" s="12" t="s">
         <v>118</v>
       </c>
     </row>
-    <row r="36" s="26" customFormat="1" ht="357" spans="1:4">
-      <c r="A36" s="53"/>
-      <c r="B36" s="54"/>
-      <c r="C36" s="51"/>
-      <c r="D36" s="9" t="s">
+    <row r="36" s="29" customFormat="1" ht="357" spans="1:4">
+      <c r="A36" s="55"/>
+      <c r="B36" s="56"/>
+      <c r="C36" s="53"/>
+      <c r="D36" s="12" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="37" s="26" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A37" s="53"/>
-      <c r="B37" s="54"/>
-      <c r="C37" s="51"/>
-      <c r="D37" s="9" t="s">
+    <row r="37" s="29" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A37" s="55"/>
+      <c r="B37" s="56"/>
+      <c r="C37" s="53"/>
+      <c r="D37" s="12" t="s">
         <v>120</v>
       </c>
     </row>
-    <row r="38" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A38" s="53"/>
-      <c r="B38" s="54"/>
-      <c r="C38" s="51"/>
-      <c r="D38" s="9" t="s">
+    <row r="38" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A38" s="55"/>
+      <c r="B38" s="56"/>
+      <c r="C38" s="53"/>
+      <c r="D38" s="12" t="s">
         <v>121</v>
       </c>
     </row>
-    <row r="39" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A39" s="53"/>
-      <c r="B39" s="54"/>
-      <c r="C39" s="51"/>
-      <c r="D39" s="9" t="s">
+    <row r="39" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A39" s="55"/>
+      <c r="B39" s="56"/>
+      <c r="C39" s="53"/>
+      <c r="D39" s="12" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="40" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A40" s="53"/>
-      <c r="B40" s="54"/>
-      <c r="C40" s="51"/>
-      <c r="D40" s="9" t="s">
+    <row r="40" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A40" s="55"/>
+      <c r="B40" s="56"/>
+      <c r="C40" s="53"/>
+      <c r="D40" s="12" t="s">
         <v>123</v>
       </c>
     </row>
-    <row r="41" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A41" s="53"/>
-      <c r="B41" s="54"/>
-      <c r="C41" s="51" t="s">
+    <row r="41" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A41" s="55"/>
+      <c r="B41" s="56"/>
+      <c r="C41" s="53" t="s">
         <v>124</v>
       </c>
-      <c r="D41" s="9"/>
-    </row>
-    <row r="42" s="26" customFormat="1" ht="89.25" spans="1:4">
-      <c r="A42" s="53"/>
-      <c r="B42" s="54"/>
-      <c r="C42" s="51" t="s">
+      <c r="D41" s="12"/>
+    </row>
+    <row r="42" s="29" customFormat="1" ht="89.25" spans="1:4">
+      <c r="A42" s="55"/>
+      <c r="B42" s="56"/>
+      <c r="C42" s="53" t="s">
         <v>125</v>
       </c>
-      <c r="D42" s="9" t="s">
+      <c r="D42" s="12" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="43" s="26" customFormat="1" ht="114.75" spans="1:4">
-      <c r="A43" s="53"/>
-      <c r="B43" s="16" t="s">
+    <row r="43" s="29" customFormat="1" ht="114.75" spans="1:4">
+      <c r="A43" s="55"/>
+      <c r="B43" s="19" t="s">
         <v>127</v>
       </c>
-      <c r="C43" s="54" t="s">
+      <c r="C43" s="56" t="s">
         <v>128</v>
       </c>
-      <c r="D43" s="9" t="s">
+      <c r="D43" s="12" t="s">
         <v>129</v>
       </c>
     </row>
-    <row r="44" s="26" customFormat="1" ht="395.25" spans="1:4">
-      <c r="A44" s="53"/>
-      <c r="B44" s="16"/>
-      <c r="C44" s="54"/>
-      <c r="D44" s="9" t="s">
+    <row r="44" s="29" customFormat="1" ht="395.25" spans="1:4">
+      <c r="A44" s="55"/>
+      <c r="B44" s="19"/>
+      <c r="C44" s="56"/>
+      <c r="D44" s="12" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="45" s="26" customFormat="1" ht="409.5" spans="1:4">
-      <c r="A45" s="53"/>
-      <c r="B45" s="16"/>
-      <c r="C45" s="54"/>
-      <c r="D45" s="9" t="s">
+    <row r="45" s="29" customFormat="1" ht="409.5" spans="1:4">
+      <c r="A45" s="55"/>
+      <c r="B45" s="19"/>
+      <c r="C45" s="56"/>
+      <c r="D45" s="12" t="s">
         <v>131</v>
       </c>
     </row>
-    <row r="46" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A46" s="53"/>
-      <c r="B46" s="16"/>
-      <c r="C46" s="54"/>
-      <c r="D46" s="9" t="s">
+    <row r="46" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A46" s="55"/>
+      <c r="B46" s="19"/>
+      <c r="C46" s="56"/>
+      <c r="D46" s="12" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="47" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A47" s="53"/>
-      <c r="B47" s="16"/>
-      <c r="C47" s="54"/>
-      <c r="D47" s="9" t="s">
+    <row r="47" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A47" s="55"/>
+      <c r="B47" s="19"/>
+      <c r="C47" s="56"/>
+      <c r="D47" s="12" t="s">
         <v>133</v>
       </c>
     </row>
-    <row r="48" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A48" s="53"/>
-      <c r="B48" s="16"/>
-      <c r="C48" s="54"/>
-      <c r="D48" s="9" t="s">
+    <row r="48" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A48" s="55"/>
+      <c r="B48" s="19"/>
+      <c r="C48" s="56"/>
+      <c r="D48" s="12" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="49" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A49" s="53"/>
-      <c r="B49" s="16"/>
-      <c r="C49" s="54"/>
-      <c r="D49" s="9" t="s">
+    <row r="49" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A49" s="55"/>
+      <c r="B49" s="19"/>
+      <c r="C49" s="56"/>
+      <c r="D49" s="12" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="50" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A50" s="53"/>
-      <c r="B50" s="16"/>
-      <c r="C50" s="54"/>
-      <c r="D50" s="9" t="s">
+    <row r="50" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A50" s="55"/>
+      <c r="B50" s="19"/>
+      <c r="C50" s="56"/>
+      <c r="D50" s="12" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="51" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A51" s="53"/>
-      <c r="B51" s="16"/>
-      <c r="C51" s="48" t="s">
+    <row r="51" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A51" s="55"/>
+      <c r="B51" s="19"/>
+      <c r="C51" s="8" t="s">
         <v>137</v>
       </c>
-      <c r="D51" s="9" t="s">
+      <c r="D51" s="12" t="s">
         <v>138</v>
       </c>
     </row>
-    <row r="52" s="26" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A52" s="53"/>
-      <c r="B52" s="16"/>
-      <c r="C52" s="48"/>
-      <c r="D52" s="9" t="s">
+    <row r="52" s="29" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A52" s="55"/>
+      <c r="B52" s="19"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="12" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="53" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A53" s="53"/>
-      <c r="B53" s="16"/>
-      <c r="C53" s="48"/>
-      <c r="D53" s="9" t="s">
+    <row r="53" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A53" s="55"/>
+      <c r="B53" s="19"/>
+      <c r="C53" s="8"/>
+      <c r="D53" s="12" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="54" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A54" s="53"/>
-      <c r="B54" s="16"/>
-      <c r="C54" s="48"/>
-      <c r="D54" s="9" t="s">
+    <row r="54" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A54" s="55"/>
+      <c r="B54" s="19"/>
+      <c r="C54" s="8"/>
+      <c r="D54" s="12" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="55" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A55" s="53"/>
-      <c r="B55" s="16"/>
-      <c r="C55" s="48"/>
-      <c r="D55" s="9" t="s">
+    <row r="55" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A55" s="55"/>
+      <c r="B55" s="19"/>
+      <c r="C55" s="8"/>
+      <c r="D55" s="12" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="56" s="26" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A56" s="53"/>
-      <c r="B56" s="16"/>
-      <c r="C56" s="51" t="s">
+    <row r="56" s="29" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A56" s="55"/>
+      <c r="B56" s="19"/>
+      <c r="C56" s="53" t="s">
         <v>143</v>
       </c>
-      <c r="D56" s="9"/>
-    </row>
-    <row r="57" s="26" customFormat="1" ht="409.5" spans="1:4">
-      <c r="A57" s="53"/>
-      <c r="B57" s="16"/>
-      <c r="C57" s="54" t="s">
+      <c r="D56" s="12"/>
+    </row>
+    <row r="57" s="29" customFormat="1" ht="409.5" spans="1:4">
+      <c r="A57" s="55"/>
+      <c r="B57" s="19"/>
+      <c r="C57" s="56" t="s">
         <v>144</v>
       </c>
-      <c r="D57" s="23" t="s">
+      <c r="D57" s="26" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="58" s="26" customFormat="1" ht="51" spans="1:4">
-      <c r="A58" s="53"/>
-      <c r="B58" s="16"/>
-      <c r="C58" s="54"/>
-      <c r="D58" s="9" t="s">
+    <row r="58" s="29" customFormat="1" ht="51" spans="1:4">
+      <c r="A58" s="55"/>
+      <c r="B58" s="19"/>
+      <c r="C58" s="56"/>
+      <c r="D58" s="12" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="59" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A59" s="53"/>
-      <c r="B59" s="16"/>
-      <c r="C59" s="54"/>
-      <c r="D59" s="9" t="s">
+    <row r="59" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A59" s="55"/>
+      <c r="B59" s="19"/>
+      <c r="C59" s="56"/>
+      <c r="D59" s="12" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="60" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A60" s="53"/>
-      <c r="B60" s="16"/>
-      <c r="C60" s="54"/>
-      <c r="D60" s="9" t="s">
+    <row r="60" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A60" s="55"/>
+      <c r="B60" s="19"/>
+      <c r="C60" s="56"/>
+      <c r="D60" s="12" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="61" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A61" s="53"/>
-      <c r="B61" s="16"/>
-      <c r="C61" s="51" t="s">
+    <row r="61" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A61" s="55"/>
+      <c r="B61" s="19"/>
+      <c r="C61" s="53" t="s">
         <v>149</v>
       </c>
-      <c r="D61" s="9" t="s">
+      <c r="D61" s="12" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="62" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A62" s="53"/>
-      <c r="B62" s="16"/>
-      <c r="C62" s="51"/>
-      <c r="D62" s="9" t="s">
+    <row r="62" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A62" s="55"/>
+      <c r="B62" s="19"/>
+      <c r="C62" s="53"/>
+      <c r="D62" s="12" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="63" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A63" s="53"/>
-      <c r="B63" s="16"/>
-      <c r="C63" s="51"/>
-      <c r="D63" s="9" t="s">
+    <row r="63" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A63" s="55"/>
+      <c r="B63" s="19"/>
+      <c r="C63" s="53"/>
+      <c r="D63" s="12" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="64" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A64" s="53"/>
-      <c r="B64" s="16"/>
-      <c r="C64" s="51"/>
-      <c r="D64" s="9" t="s">
+    <row r="64" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A64" s="55"/>
+      <c r="B64" s="19"/>
+      <c r="C64" s="53"/>
+      <c r="D64" s="12" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="65" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A65" s="53"/>
-      <c r="B65" s="16"/>
-      <c r="C65" s="51"/>
-      <c r="D65" s="9" t="s">
+    <row r="65" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A65" s="55"/>
+      <c r="B65" s="19"/>
+      <c r="C65" s="53"/>
+      <c r="D65" s="12" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="66" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A66" s="53"/>
-      <c r="B66" s="16"/>
-      <c r="C66" s="51"/>
-      <c r="D66" s="9" t="s">
+    <row r="66" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A66" s="55"/>
+      <c r="B66" s="19"/>
+      <c r="C66" s="53"/>
+      <c r="D66" s="12" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="67" s="26" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A67" s="53"/>
-      <c r="B67" s="16"/>
-      <c r="C67" s="51" t="s">
+    <row r="67" s="29" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A67" s="55"/>
+      <c r="B67" s="19"/>
+      <c r="C67" s="53" t="s">
         <v>155</v>
       </c>
-      <c r="D67" s="9" t="s">
+      <c r="D67" s="12" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="68" s="26" customFormat="1" ht="51" spans="1:4">
-      <c r="A68" s="53"/>
-      <c r="B68" s="16"/>
-      <c r="C68" s="51"/>
-      <c r="D68" s="9" t="s">
+    <row r="68" s="29" customFormat="1" ht="51" spans="1:4">
+      <c r="A68" s="55"/>
+      <c r="B68" s="19"/>
+      <c r="C68" s="53"/>
+      <c r="D68" s="12" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="69" s="26" customFormat="1" ht="51" spans="1:4">
-      <c r="A69" s="53"/>
-      <c r="B69" s="16"/>
-      <c r="C69" s="51"/>
-      <c r="D69" s="9" t="s">
+    <row r="69" s="29" customFormat="1" ht="51" spans="1:4">
+      <c r="A69" s="55"/>
+      <c r="B69" s="19"/>
+      <c r="C69" s="53"/>
+      <c r="D69" s="12" t="s">
         <v>158</v>
       </c>
     </row>
-    <row r="70" s="26" customFormat="1" ht="63.75" spans="1:4">
-      <c r="A70" s="53"/>
-      <c r="B70" s="16"/>
-      <c r="C70" s="51"/>
-      <c r="D70" s="9" t="s">
+    <row r="70" s="29" customFormat="1" ht="63.75" spans="1:4">
+      <c r="A70" s="55"/>
+      <c r="B70" s="19"/>
+      <c r="C70" s="53"/>
+      <c r="D70" s="12" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="71" s="26" customFormat="1" ht="63.75" spans="1:4">
-      <c r="A71" s="53"/>
-      <c r="B71" s="16"/>
-      <c r="C71" s="51"/>
-      <c r="D71" s="9" t="s">
+    <row r="71" s="29" customFormat="1" ht="63.75" spans="1:4">
+      <c r="A71" s="55"/>
+      <c r="B71" s="19"/>
+      <c r="C71" s="53"/>
+      <c r="D71" s="12" t="s">
         <v>160</v>
       </c>
     </row>
-    <row r="72" s="26" customFormat="1" ht="51" spans="1:4">
-      <c r="A72" s="53"/>
-      <c r="B72" s="16"/>
-      <c r="C72" s="51"/>
-      <c r="D72" s="9" t="s">
+    <row r="72" s="29" customFormat="1" ht="51" spans="1:4">
+      <c r="A72" s="55"/>
+      <c r="B72" s="19"/>
+      <c r="C72" s="53"/>
+      <c r="D72" s="12" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="73" s="26" customFormat="1" ht="51" spans="1:4">
-      <c r="A73" s="53"/>
-      <c r="B73" s="16"/>
-      <c r="C73" s="51"/>
-      <c r="D73" s="9" t="s">
+    <row r="73" s="29" customFormat="1" ht="51" spans="1:4">
+      <c r="A73" s="55"/>
+      <c r="B73" s="19"/>
+      <c r="C73" s="53"/>
+      <c r="D73" s="12" t="s">
         <v>162</v>
       </c>
     </row>
-    <row r="74" s="26" customFormat="1" ht="63.75" spans="1:4">
-      <c r="A74" s="53"/>
-      <c r="B74" s="16"/>
-      <c r="C74" s="51"/>
-      <c r="D74" s="9" t="s">
+    <row r="74" s="29" customFormat="1" ht="63.75" spans="1:4">
+      <c r="A74" s="55"/>
+      <c r="B74" s="19"/>
+      <c r="C74" s="53"/>
+      <c r="D74" s="12" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="75" s="26" customFormat="1" ht="63.75" spans="1:4">
-      <c r="A75" s="53"/>
-      <c r="B75" s="16"/>
-      <c r="C75" s="51"/>
-      <c r="D75" s="9" t="s">
+    <row r="75" s="29" customFormat="1" ht="63.75" spans="1:4">
+      <c r="A75" s="55"/>
+      <c r="B75" s="19"/>
+      <c r="C75" s="53"/>
+      <c r="D75" s="12" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="76" s="26" customFormat="1" ht="51" spans="1:4">
-      <c r="A76" s="53"/>
-      <c r="B76" s="16"/>
-      <c r="C76" s="51"/>
-      <c r="D76" s="9" t="s">
+    <row r="76" s="29" customFormat="1" ht="51" spans="1:4">
+      <c r="A76" s="55"/>
+      <c r="B76" s="19"/>
+      <c r="C76" s="53"/>
+      <c r="D76" s="12" t="s">
         <v>165</v>
       </c>
     </row>
-    <row r="77" s="26" customFormat="1" ht="153" spans="1:4">
-      <c r="A77" s="53"/>
-      <c r="B77" s="16"/>
-      <c r="C77" s="51"/>
-      <c r="D77" s="9" t="s">
+    <row r="77" s="29" customFormat="1" ht="153" spans="1:4">
+      <c r="A77" s="55"/>
+      <c r="B77" s="19"/>
+      <c r="C77" s="53"/>
+      <c r="D77" s="12" t="s">
         <v>166</v>
       </c>
     </row>
-    <row r="78" s="26" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A78" s="53"/>
-      <c r="B78" s="16"/>
-      <c r="C78" s="51"/>
-      <c r="D78" s="9" t="s">
+    <row r="78" s="29" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A78" s="55"/>
+      <c r="B78" s="19"/>
+      <c r="C78" s="53"/>
+      <c r="D78" s="12" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="79" s="26" customFormat="1" ht="114.75" spans="1:4">
-      <c r="A79" s="53"/>
-      <c r="B79" s="16"/>
-      <c r="C79" s="51" t="s">
+    <row r="79" s="29" customFormat="1" ht="114.75" spans="1:4">
+      <c r="A79" s="55"/>
+      <c r="B79" s="19"/>
+      <c r="C79" s="53" t="s">
         <v>168</v>
       </c>
-      <c r="D79" s="9" t="s">
+      <c r="D79" s="12" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="80" s="26" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A80" s="53"/>
-      <c r="B80" s="16"/>
-      <c r="C80" s="48" t="s">
+    <row r="80" s="29" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A80" s="55"/>
+      <c r="B80" s="19"/>
+      <c r="C80" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="D80" s="9" t="s">
+      <c r="D80" s="12" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="81" s="26" customFormat="1" ht="165.75" spans="1:4">
-      <c r="A81" s="53"/>
-      <c r="B81" s="16"/>
-      <c r="C81" s="48"/>
-      <c r="D81" s="23" t="s">
+    <row r="81" s="29" customFormat="1" ht="165.75" spans="1:4">
+      <c r="A81" s="55"/>
+      <c r="B81" s="19"/>
+      <c r="C81" s="8"/>
+      <c r="D81" s="26" t="s">
         <v>172</v>
       </c>
     </row>
-    <row r="82" s="26" customFormat="1" ht="102" spans="1:4">
-      <c r="A82" s="53"/>
-      <c r="B82" s="16"/>
-      <c r="C82" s="48"/>
-      <c r="D82" s="23" t="s">
+    <row r="82" s="29" customFormat="1" ht="102" spans="1:4">
+      <c r="A82" s="55"/>
+      <c r="B82" s="19"/>
+      <c r="C82" s="8"/>
+      <c r="D82" s="26" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="83" s="26" customFormat="1" ht="51" spans="1:4">
-      <c r="A83" s="53"/>
-      <c r="B83" s="16"/>
-      <c r="C83" s="48"/>
-      <c r="D83" s="23" t="s">
+    <row r="83" s="29" customFormat="1" ht="51" spans="1:4">
+      <c r="A83" s="55"/>
+      <c r="B83" s="19"/>
+      <c r="C83" s="8"/>
+      <c r="D83" s="26" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="84" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A84" s="53"/>
-      <c r="B84" s="16"/>
-      <c r="C84" s="54" t="s">
+    <row r="84" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A84" s="55"/>
+      <c r="B84" s="19"/>
+      <c r="C84" s="56" t="s">
         <v>175</v>
       </c>
-      <c r="D84" s="23" t="s">
+      <c r="D84" s="26" t="s">
         <v>176</v>
       </c>
     </row>
-    <row r="85" s="26" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A85" s="53"/>
-      <c r="B85" s="16" t="s">
+    <row r="85" s="29" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A85" s="55"/>
+      <c r="B85" s="19" t="s">
         <v>177</v>
       </c>
-      <c r="C85" s="54"/>
-      <c r="D85" s="23"/>
-    </row>
-    <row r="86" s="26" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A86" s="53"/>
-      <c r="B86" s="16" t="s">
+      <c r="C85" s="56"/>
+      <c r="D85" s="26"/>
+    </row>
+    <row r="86" s="29" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A86" s="55"/>
+      <c r="B86" s="19" t="s">
         <v>178</v>
       </c>
-      <c r="C86" s="54"/>
-      <c r="D86" s="23"/>
-    </row>
-    <row r="87" s="26" customFormat="1" ht="51" spans="1:4">
-      <c r="A87" s="53"/>
-      <c r="B87" s="16" t="s">
+      <c r="C86" s="56"/>
+      <c r="D86" s="26"/>
+    </row>
+    <row r="87" s="29" customFormat="1" ht="51" spans="1:4">
+      <c r="A87" s="55"/>
+      <c r="B87" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="C87" s="54"/>
-      <c r="D87" s="23"/>
-    </row>
-    <row r="88" s="26" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A88" s="53"/>
-      <c r="B88" s="16" t="s">
+      <c r="C87" s="56"/>
+      <c r="D87" s="26"/>
+    </row>
+    <row r="88" s="29" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A88" s="55"/>
+      <c r="B88" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="C88" s="54"/>
-      <c r="D88" s="23"/>
-    </row>
-    <row r="89" s="26" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A89" s="53"/>
-      <c r="B89" s="16" t="s">
+      <c r="C88" s="56"/>
+      <c r="D88" s="26"/>
+    </row>
+    <row r="89" s="29" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A89" s="55"/>
+      <c r="B89" s="19" t="s">
         <v>181</v>
       </c>
-      <c r="C89" s="54"/>
-      <c r="D89" s="23"/>
-    </row>
-    <row r="90" s="26" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A90" s="53"/>
-      <c r="B90" s="16" t="s">
+      <c r="C89" s="56"/>
+      <c r="D89" s="26"/>
+    </row>
+    <row r="90" s="29" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A90" s="55"/>
+      <c r="B90" s="19" t="s">
         <v>182</v>
       </c>
-      <c r="C90" s="54"/>
-      <c r="D90" s="23"/>
-    </row>
-    <row r="91" s="26" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A91" s="53"/>
-      <c r="B91" s="16" t="s">
+      <c r="C90" s="56"/>
+      <c r="D90" s="26"/>
+    </row>
+    <row r="91" s="29" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A91" s="55"/>
+      <c r="B91" s="19" t="s">
         <v>183</v>
       </c>
-      <c r="C91" s="54"/>
-      <c r="D91" s="23"/>
-    </row>
-    <row r="92" s="26" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A92" s="53"/>
-      <c r="B92" s="16" t="s">
+      <c r="C91" s="56"/>
+      <c r="D91" s="26"/>
+    </row>
+    <row r="92" s="29" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A92" s="55"/>
+      <c r="B92" s="19" t="s">
         <v>184</v>
       </c>
-      <c r="C92" s="54"/>
-      <c r="D92" s="23"/>
-    </row>
-    <row r="93" s="26" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A93" s="53"/>
-      <c r="B93" s="55" t="s">
+      <c r="C92" s="56"/>
+      <c r="D92" s="26"/>
+    </row>
+    <row r="93" s="29" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A93" s="55"/>
+      <c r="B93" s="57" t="s">
         <v>185</v>
       </c>
-      <c r="C93" s="54"/>
-      <c r="D93" s="23"/>
-    </row>
-    <row r="94" s="26" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A94" s="53"/>
-      <c r="B94" s="16" t="s">
+      <c r="C93" s="56"/>
+      <c r="D93" s="26"/>
+    </row>
+    <row r="94" s="29" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A94" s="55"/>
+      <c r="B94" s="19" t="s">
         <v>186</v>
       </c>
-      <c r="C94" s="54"/>
-      <c r="D94" s="23"/>
-    </row>
-    <row r="95" s="26" customFormat="1" ht="51" spans="1:4">
-      <c r="A95" s="53"/>
-      <c r="B95" s="55" t="s">
+      <c r="C94" s="56"/>
+      <c r="D94" s="26"/>
+    </row>
+    <row r="95" s="29" customFormat="1" ht="51" spans="1:4">
+      <c r="A95" s="55"/>
+      <c r="B95" s="57" t="s">
         <v>187</v>
       </c>
-      <c r="C95" s="54"/>
-      <c r="D95" s="23"/>
-    </row>
-    <row r="96" s="26" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A96" s="53"/>
-      <c r="B96" s="55" t="s">
+      <c r="C95" s="56"/>
+      <c r="D95" s="26"/>
+    </row>
+    <row r="96" s="29" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A96" s="55"/>
+      <c r="B96" s="57" t="s">
         <v>188</v>
       </c>
-      <c r="C96" s="54"/>
-      <c r="D96" s="23"/>
-    </row>
-    <row r="97" s="26" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A97" s="53"/>
-      <c r="B97" s="55" t="s">
+      <c r="C96" s="56"/>
+      <c r="D96" s="26"/>
+    </row>
+    <row r="97" s="29" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A97" s="55"/>
+      <c r="B97" s="57" t="s">
         <v>189</v>
       </c>
-      <c r="C97" s="54"/>
-      <c r="D97" s="23"/>
-    </row>
-    <row r="98" s="26" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A98" s="53"/>
-      <c r="B98" s="55" t="s">
+      <c r="C97" s="56"/>
+      <c r="D97" s="26"/>
+    </row>
+    <row r="98" s="29" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A98" s="55"/>
+      <c r="B98" s="57" t="s">
         <v>190</v>
       </c>
-      <c r="C98" s="54"/>
-      <c r="D98" s="23"/>
-    </row>
-    <row r="99" s="26" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A99" s="53"/>
-      <c r="B99" s="55" t="s">
+      <c r="C98" s="56"/>
+      <c r="D98" s="26"/>
+    </row>
+    <row r="99" s="29" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A99" s="55"/>
+      <c r="B99" s="57" t="s">
         <v>191</v>
       </c>
-      <c r="C99" s="54"/>
-      <c r="D99" s="23"/>
-    </row>
-    <row r="100" s="26" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A100" s="53"/>
-      <c r="B100" s="16" t="s">
+      <c r="C99" s="56"/>
+      <c r="D99" s="26"/>
+    </row>
+    <row r="100" s="29" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A100" s="55"/>
+      <c r="B100" s="19" t="s">
         <v>192</v>
       </c>
-      <c r="C100" s="54"/>
-      <c r="D100" s="23"/>
-    </row>
-    <row r="101" s="26" customFormat="1" ht="51" spans="1:4">
-      <c r="A101" s="53"/>
-      <c r="B101" s="16" t="s">
+      <c r="C100" s="56"/>
+      <c r="D100" s="26"/>
+    </row>
+    <row r="101" s="29" customFormat="1" ht="51" spans="1:4">
+      <c r="A101" s="55"/>
+      <c r="B101" s="19" t="s">
         <v>193</v>
       </c>
-      <c r="C101" s="54"/>
-      <c r="D101" s="23"/>
-    </row>
-    <row r="102" s="26" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A102" s="53"/>
-      <c r="B102" s="55" t="s">
+      <c r="C101" s="56"/>
+      <c r="D101" s="26"/>
+    </row>
+    <row r="102" s="29" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A102" s="55"/>
+      <c r="B102" s="57" t="s">
         <v>194</v>
       </c>
-      <c r="C102" s="54"/>
-      <c r="D102" s="23"/>
-    </row>
-    <row r="103" s="26" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A103" s="53"/>
-      <c r="B103" s="16" t="s">
+      <c r="C102" s="56"/>
+      <c r="D102" s="26"/>
+    </row>
+    <row r="103" s="29" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A103" s="55"/>
+      <c r="B103" s="19" t="s">
         <v>195</v>
       </c>
-      <c r="C103" s="54"/>
-      <c r="D103" s="23"/>
-    </row>
-    <row r="104" s="26" customFormat="1" ht="38.25" spans="1:4">
-      <c r="A104" s="53"/>
-      <c r="B104" s="16" t="s">
+      <c r="C103" s="56"/>
+      <c r="D103" s="26"/>
+    </row>
+    <row r="104" s="29" customFormat="1" ht="38.25" spans="1:4">
+      <c r="A104" s="55"/>
+      <c r="B104" s="19" t="s">
         <v>196</v>
       </c>
-      <c r="C104" s="54"/>
-      <c r="D104" s="23"/>
-    </row>
-    <row r="105" s="26" customFormat="1" ht="153" spans="1:4">
-      <c r="A105" s="53"/>
-      <c r="B105" s="56" t="s">
+      <c r="C104" s="56"/>
+      <c r="D104" s="26"/>
+    </row>
+    <row r="105" s="29" customFormat="1" ht="153" spans="1:4">
+      <c r="A105" s="55"/>
+      <c r="B105" s="58" t="s">
         <v>197</v>
       </c>
-      <c r="C105" s="51" t="s">
+      <c r="C105" s="53" t="s">
         <v>198</v>
       </c>
-      <c r="D105" s="9" t="s">
+      <c r="D105" s="12" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="106" s="26" customFormat="1" ht="51" spans="1:4">
-      <c r="A106" s="53"/>
-      <c r="B106" s="56"/>
-      <c r="C106" s="51" t="s">
+    <row r="106" s="29" customFormat="1" ht="51" spans="1:4">
+      <c r="A106" s="55"/>
+      <c r="B106" s="58"/>
+      <c r="C106" s="53" t="s">
         <v>200</v>
       </c>
-      <c r="D106" s="9" t="s">
+      <c r="D106" s="12" t="s">
         <v>201</v>
       </c>
     </row>
-    <row r="107" s="26" customFormat="1" ht="306" spans="1:4">
-      <c r="A107" s="53"/>
-      <c r="B107" s="56"/>
-      <c r="C107" s="51" t="s">
+    <row r="107" s="29" customFormat="1" ht="306" spans="1:4">
+      <c r="A107" s="55"/>
+      <c r="B107" s="58"/>
+      <c r="C107" s="53" t="s">
         <v>202</v>
       </c>
-      <c r="D107" s="23" t="s">
+      <c r="D107" s="26" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="108" s="26" customFormat="1" ht="229.5" spans="1:4">
-      <c r="A108" s="53"/>
-      <c r="B108" s="56"/>
-      <c r="C108" s="51"/>
-      <c r="D108" s="23" t="s">
+    <row r="108" s="29" customFormat="1" ht="229.5" spans="1:4">
+      <c r="A108" s="55"/>
+      <c r="B108" s="58"/>
+      <c r="C108" s="53"/>
+      <c r="D108" s="26" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="109" s="26" customFormat="1" ht="242.25" spans="1:4">
-      <c r="A109" s="53"/>
-      <c r="B109" s="56"/>
-      <c r="C109" s="51" t="s">
+    <row r="109" s="29" customFormat="1" ht="242.25" spans="1:4">
+      <c r="A109" s="55"/>
+      <c r="B109" s="58"/>
+      <c r="C109" s="53" t="s">
         <v>205</v>
       </c>
-      <c r="D109" s="23" t="s">
+      <c r="D109" s="26" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="110" s="26" customFormat="1" ht="216.75" spans="1:4">
-      <c r="A110" s="53"/>
-      <c r="B110" s="56"/>
-      <c r="C110" s="51" t="s">
+    <row r="110" s="29" customFormat="1" ht="216.75" spans="1:4">
+      <c r="A110" s="55"/>
+      <c r="B110" s="58"/>
+      <c r="C110" s="53" t="s">
         <v>207</v>
       </c>
-      <c r="D110" s="23" t="s">
+      <c r="D110" s="26" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="111" s="26" customFormat="1" ht="369.75" spans="1:4">
-      <c r="A111" s="53"/>
-      <c r="B111" s="56"/>
-      <c r="C111" s="51"/>
-      <c r="D111" s="23" t="s">
+    <row r="111" s="29" customFormat="1" ht="369.75" spans="1:4">
+      <c r="A111" s="55"/>
+      <c r="B111" s="58"/>
+      <c r="C111" s="53"/>
+      <c r="D111" s="26" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="112" s="26" customFormat="1" ht="382.5" spans="1:4">
-      <c r="A112" s="53"/>
-      <c r="B112" s="56"/>
-      <c r="C112" s="51" t="s">
+    <row r="112" s="29" customFormat="1" ht="382.5" spans="1:4">
+      <c r="A112" s="55"/>
+      <c r="B112" s="58"/>
+      <c r="C112" s="53" t="s">
         <v>210</v>
       </c>
-      <c r="D112" s="23" t="s">
+      <c r="D112" s="26" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="113" s="26" customFormat="1" ht="255" spans="1:4">
-      <c r="A113" s="53"/>
-      <c r="B113" s="57"/>
-      <c r="C113" s="51" t="s">
+    <row r="113" s="29" customFormat="1" ht="255" spans="1:4">
+      <c r="A113" s="55"/>
+      <c r="B113" s="59"/>
+      <c r="C113" s="53" t="s">
         <v>212</v>
       </c>
-      <c r="D113" s="9" t="s">
+      <c r="D113" s="12" t="s">
         <v>213</v>
       </c>
     </row>
-    <row r="114" s="26" customFormat="1" ht="165.75" spans="1:4">
-      <c r="A114" s="53"/>
-      <c r="B114" s="57"/>
-      <c r="C114" s="51" t="s">
+    <row r="114" s="29" customFormat="1" ht="165.75" spans="1:4">
+      <c r="A114" s="55"/>
+      <c r="B114" s="59"/>
+      <c r="C114" s="53" t="s">
         <v>214</v>
       </c>
-      <c r="D114" s="9" t="s">
+      <c r="D114" s="12" t="s">
         <v>215</v>
       </c>
     </row>
-    <row r="115" s="26" customFormat="1" ht="89.25" spans="1:4">
-      <c r="A115" s="53"/>
-      <c r="B115" s="57"/>
-      <c r="C115" s="51" t="s">
+    <row r="115" s="29" customFormat="1" ht="89.25" spans="1:4">
+      <c r="A115" s="55"/>
+      <c r="B115" s="59"/>
+      <c r="C115" s="53" t="s">
         <v>216</v>
       </c>
-      <c r="D115" s="9" t="s">
+      <c r="D115" s="12" t="s">
         <v>217</v>
       </c>
     </row>
-    <row r="116" s="26" customFormat="1" ht="89.25" spans="1:4">
-      <c r="A116" s="53"/>
-      <c r="B116" s="57"/>
-      <c r="C116" s="51"/>
-      <c r="D116" s="9" t="s">
+    <row r="116" s="29" customFormat="1" ht="89.25" spans="1:4">
+      <c r="A116" s="55"/>
+      <c r="B116" s="59"/>
+      <c r="C116" s="53"/>
+      <c r="D116" s="12" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="117" s="26" customFormat="1" ht="63.75" spans="1:4">
-      <c r="A117" s="53"/>
-      <c r="B117" s="57"/>
-      <c r="C117" s="51" t="s">
+    <row r="117" s="29" customFormat="1" ht="63.75" spans="1:4">
+      <c r="A117" s="55"/>
+      <c r="B117" s="59"/>
+      <c r="C117" s="53" t="s">
         <v>219</v>
       </c>
-      <c r="D117" s="9" t="s">
+      <c r="D117" s="12" t="s">
         <v>220</v>
       </c>
     </row>
-    <row r="118" s="26" customFormat="1" ht="274.5" customHeight="1" spans="1:4">
-      <c r="A118" s="53"/>
-      <c r="B118" s="51" t="s">
+    <row r="118" s="29" customFormat="1" ht="274.5" customHeight="1" spans="1:4">
+      <c r="A118" s="55"/>
+      <c r="B118" s="53" t="s">
         <v>221</v>
       </c>
-      <c r="C118" s="9" t="s">
+      <c r="C118" s="12" t="s">
         <v>222</v>
       </c>
-      <c r="D118" s="9"/>
-    </row>
-    <row r="119" s="26" customFormat="1" ht="243.75" customHeight="1" spans="1:4">
-      <c r="A119" s="53"/>
-      <c r="B119" s="51"/>
-      <c r="C119" s="9" t="s">
+      <c r="D118" s="12"/>
+    </row>
+    <row r="119" s="29" customFormat="1" ht="243.75" customHeight="1" spans="1:4">
+      <c r="A119" s="55"/>
+      <c r="B119" s="53"/>
+      <c r="C119" s="12" t="s">
         <v>223</v>
       </c>
-      <c r="D119" s="9"/>
-    </row>
-    <row r="120" s="26" customFormat="1" ht="391.5" customHeight="1" spans="1:4">
-      <c r="A120" s="53"/>
-      <c r="B120" s="51" t="s">
+      <c r="D119" s="12"/>
+    </row>
+    <row r="120" s="29" customFormat="1" ht="391.5" customHeight="1" spans="1:4">
+      <c r="A120" s="55"/>
+      <c r="B120" s="53" t="s">
         <v>224</v>
       </c>
-      <c r="C120" s="9" t="s">
+      <c r="C120" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="D120" s="9"/>
-    </row>
-    <row r="121" s="26" customFormat="1" ht="231" customHeight="1" spans="1:4">
-      <c r="A121" s="53"/>
-      <c r="B121" s="51"/>
-      <c r="C121" s="9" t="s">
+      <c r="D120" s="12"/>
+    </row>
+    <row r="121" s="29" customFormat="1" ht="231" customHeight="1" spans="1:4">
+      <c r="A121" s="55"/>
+      <c r="B121" s="53"/>
+      <c r="C121" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="D121" s="9"/>
-    </row>
-    <row r="122" s="26" customFormat="1" ht="45" customHeight="1" spans="1:4">
-      <c r="A122" s="58" t="s">
+      <c r="D121" s="12"/>
+    </row>
+    <row r="122" s="29" customFormat="1" ht="45" customHeight="1" spans="1:4">
+      <c r="A122" s="60" t="s">
         <v>227</v>
       </c>
-      <c r="B122" s="51" t="s">
+      <c r="B122" s="53" t="s">
         <v>228</v>
       </c>
-      <c r="C122" s="9" t="s">
+      <c r="C122" s="12" t="s">
         <v>229</v>
       </c>
-      <c r="D122" s="9"/>
-    </row>
-    <row r="123" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A123" s="53"/>
-      <c r="B123" s="51" t="s">
+      <c r="D122" s="12"/>
+    </row>
+    <row r="123" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A123" s="55"/>
+      <c r="B123" s="53" t="s">
         <v>230</v>
       </c>
-      <c r="C123" s="51" t="s">
+      <c r="C123" s="53" t="s">
         <v>231</v>
       </c>
-      <c r="D123" s="9" t="s">
+      <c r="D123" s="12" t="s">
         <v>232</v>
       </c>
     </row>
-    <row r="124" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A124" s="53"/>
-      <c r="B124" s="51"/>
-      <c r="C124" s="51" t="s">
+    <row r="124" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A124" s="55"/>
+      <c r="B124" s="53"/>
+      <c r="C124" s="53" t="s">
         <v>233</v>
       </c>
-      <c r="D124" s="9" t="s">
+      <c r="D124" s="12" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="125" s="26" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A125" s="53"/>
-      <c r="B125" s="51"/>
-      <c r="C125" s="51" t="s">
+    <row r="125" s="29" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A125" s="55"/>
+      <c r="B125" s="53"/>
+      <c r="C125" s="53" t="s">
         <v>235</v>
       </c>
-      <c r="D125" s="9" t="s">
+      <c r="D125" s="12" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="126" s="26" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A126" s="53"/>
-      <c r="B126" s="51"/>
-      <c r="C126" s="51" t="s">
+    <row r="126" s="29" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A126" s="55"/>
+      <c r="B126" s="53"/>
+      <c r="C126" s="53" t="s">
         <v>237</v>
       </c>
-      <c r="D126" s="9" t="s">
+      <c r="D126" s="12" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="127" s="26" customFormat="1" ht="51" spans="1:4">
-      <c r="A127" s="53"/>
-      <c r="B127" s="51" t="s">
+    <row r="127" s="29" customFormat="1" ht="51" spans="1:4">
+      <c r="A127" s="55"/>
+      <c r="B127" s="53" t="s">
         <v>239</v>
       </c>
-      <c r="C127" s="51" t="s">
+      <c r="C127" s="53" t="s">
         <v>240</v>
       </c>
-      <c r="D127" s="9" t="s">
+      <c r="D127" s="12" t="s">
         <v>241</v>
       </c>
     </row>
-    <row r="128" s="26" customFormat="1" ht="51" spans="1:4">
-      <c r="A128" s="53"/>
-      <c r="B128" s="51"/>
-      <c r="C128" s="51" t="s">
+    <row r="128" s="29" customFormat="1" ht="51" spans="1:4">
+      <c r="A128" s="55"/>
+      <c r="B128" s="53"/>
+      <c r="C128" s="53" t="s">
         <v>242</v>
       </c>
-      <c r="D128" s="9" t="s">
+      <c r="D128" s="12" t="s">
         <v>243</v>
       </c>
     </row>
-    <row r="129" s="26" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A129" s="53"/>
-      <c r="B129" s="51"/>
-      <c r="C129" s="9" t="s">
+    <row r="129" s="29" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A129" s="55"/>
+      <c r="B129" s="53"/>
+      <c r="C129" s="12" t="s">
         <v>244</v>
       </c>
-      <c r="D129" s="9"/>
-    </row>
-    <row r="130" s="26" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A130" s="53"/>
-      <c r="B130" s="51"/>
-      <c r="C130" s="9" t="s">
+      <c r="D129" s="12"/>
+    </row>
+    <row r="130" s="29" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A130" s="55"/>
+      <c r="B130" s="53"/>
+      <c r="C130" s="12" t="s">
         <v>245</v>
       </c>
-      <c r="D130" s="9"/>
-    </row>
-    <row r="131" s="26" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A131" s="53"/>
-      <c r="B131" s="51"/>
-      <c r="C131" s="9" t="s">
+      <c r="D130" s="12"/>
+    </row>
+    <row r="131" s="29" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A131" s="55"/>
+      <c r="B131" s="53"/>
+      <c r="C131" s="12" t="s">
         <v>246</v>
       </c>
-      <c r="D131" s="9"/>
-    </row>
-    <row r="132" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A132" s="53"/>
-      <c r="B132" s="51"/>
-      <c r="C132" s="9" t="s">
+      <c r="D131" s="12"/>
+    </row>
+    <row r="132" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A132" s="55"/>
+      <c r="B132" s="53"/>
+      <c r="C132" s="12" t="s">
         <v>247</v>
       </c>
-      <c r="D132" s="9"/>
-    </row>
-    <row r="133" s="26" customFormat="1" ht="25.5" spans="1:4">
-      <c r="A133" s="53"/>
-      <c r="B133" s="51" t="s">
+      <c r="D132" s="12"/>
+    </row>
+    <row r="133" s="29" customFormat="1" ht="25.5" spans="1:4">
+      <c r="A133" s="55"/>
+      <c r="B133" s="53" t="s">
         <v>248</v>
       </c>
-      <c r="C133" s="9" t="s">
+      <c r="C133" s="12" t="s">
         <v>249</v>
       </c>
-      <c r="D133" s="9"/>
-    </row>
-    <row r="134" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A134" s="53"/>
-      <c r="B134" s="51"/>
-      <c r="C134" s="9" t="s">
+      <c r="D133" s="12"/>
+    </row>
+    <row r="134" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A134" s="55"/>
+      <c r="B134" s="53"/>
+      <c r="C134" s="12" t="s">
         <v>250</v>
       </c>
-      <c r="D134" s="9"/>
-    </row>
-    <row r="135" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A135" s="53"/>
-      <c r="B135" s="51"/>
-      <c r="C135" s="9" t="s">
+      <c r="D134" s="12"/>
+    </row>
+    <row r="135" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A135" s="55"/>
+      <c r="B135" s="53"/>
+      <c r="C135" s="12" t="s">
         <v>251</v>
       </c>
-      <c r="D135" s="9"/>
-    </row>
-    <row r="136" s="26" customFormat="1" ht="12.75" spans="1:4">
-      <c r="A136" s="53"/>
-      <c r="B136" s="51" t="s">
+      <c r="D135" s="12"/>
+    </row>
+    <row r="136" s="29" customFormat="1" ht="12.75" spans="1:4">
+      <c r="A136" s="55"/>
+      <c r="B136" s="53" t="s">
         <v>252</v>
       </c>
-      <c r="C136" s="9"/>
-      <c r="D136" s="9"/>
+      <c r="C136" s="12"/>
+      <c r="D136" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="30">
@@ -14952,298 +15105,298 @@
   </cols>
   <sheetData>
     <row r="1" ht="89.25" spans="1:2">
-      <c r="A1" s="44" t="s">
+      <c r="A1" s="47" t="s">
         <v>253</v>
       </c>
-      <c r="B1" s="13" t="s">
+      <c r="B1" s="16" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="2" ht="89.25" spans="1:2">
-      <c r="A2" s="44"/>
-      <c r="B2" s="45" t="s">
+      <c r="A2" s="47"/>
+      <c r="B2" s="48" t="s">
         <v>255</v>
       </c>
     </row>
     <row r="3" ht="102" spans="1:2">
-      <c r="A3" s="44"/>
-      <c r="B3" s="13" t="s">
+      <c r="A3" s="47"/>
+      <c r="B3" s="16" t="s">
         <v>256</v>
       </c>
     </row>
     <row r="4" ht="63.75" spans="1:2">
-      <c r="A4" s="44" t="s">
+      <c r="A4" s="47" t="s">
         <v>257</v>
       </c>
-      <c r="B4" s="13" t="s">
+      <c r="B4" s="16" t="s">
         <v>258</v>
       </c>
     </row>
     <row r="5" ht="63.75" spans="1:2">
-      <c r="A5" s="44"/>
-      <c r="B5" s="45" t="s">
+      <c r="A5" s="47"/>
+      <c r="B5" s="48" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="44"/>
-      <c r="B6" s="45" t="s">
+      <c r="A6" s="47"/>
+      <c r="B6" s="48" t="s">
         <v>260</v>
       </c>
     </row>
     <row r="7" ht="38.25" spans="1:2">
-      <c r="A7" s="44" t="s">
+      <c r="A7" s="47" t="s">
         <v>261</v>
       </c>
-      <c r="B7" s="45" t="s">
+      <c r="B7" s="48" t="s">
         <v>262</v>
       </c>
     </row>
     <row r="8" ht="38.25" spans="1:2">
-      <c r="A8" s="44"/>
-      <c r="B8" s="45" t="s">
+      <c r="A8" s="47"/>
+      <c r="B8" s="48" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="9" spans="1:2">
-      <c r="A9" s="44"/>
-      <c r="B9" s="45" t="s">
+      <c r="A9" s="47"/>
+      <c r="B9" s="48" t="s">
         <v>264</v>
       </c>
     </row>
     <row r="10" spans="1:2">
-      <c r="A10" s="44"/>
-      <c r="B10" s="45" t="s">
+      <c r="A10" s="47"/>
+      <c r="B10" s="48" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="11" spans="1:2">
-      <c r="A11" s="44"/>
-      <c r="B11" s="45" t="s">
+      <c r="A11" s="47"/>
+      <c r="B11" s="48" t="s">
         <v>266</v>
       </c>
     </row>
     <row r="12" ht="51" spans="1:2">
-      <c r="A12" s="44" t="s">
+      <c r="A12" s="47" t="s">
         <v>267</v>
       </c>
-      <c r="B12" s="45" t="s">
+      <c r="B12" s="48" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="13" ht="63.75" spans="1:2">
-      <c r="A13" s="44"/>
-      <c r="B13" s="45" t="s">
+      <c r="A13" s="47"/>
+      <c r="B13" s="48" t="s">
         <v>269</v>
       </c>
     </row>
     <row r="14" ht="127.5" spans="1:2">
-      <c r="A14" s="44"/>
-      <c r="B14" s="45" t="s">
+      <c r="A14" s="47"/>
+      <c r="B14" s="48" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="15" spans="1:2">
-      <c r="A15" s="44"/>
-      <c r="B15" s="45" t="s">
+      <c r="A15" s="47"/>
+      <c r="B15" s="48" t="s">
         <v>271</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="44"/>
-      <c r="B16" s="45" t="s">
+      <c r="A16" s="47"/>
+      <c r="B16" s="48" t="s">
         <v>272</v>
       </c>
     </row>
     <row r="17" ht="102" spans="1:2">
-      <c r="A17" s="44"/>
-      <c r="B17" s="45" t="s">
+      <c r="A17" s="47"/>
+      <c r="B17" s="48" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="18" ht="38.25" spans="1:2">
-      <c r="A18" s="44"/>
-      <c r="B18" s="45" t="s">
+      <c r="A18" s="47"/>
+      <c r="B18" s="48" t="s">
         <v>274</v>
       </c>
     </row>
     <row r="19" spans="1:2">
-      <c r="A19" s="44"/>
-      <c r="B19" s="45" t="s">
+      <c r="A19" s="47"/>
+      <c r="B19" s="48" t="s">
         <v>275</v>
       </c>
     </row>
     <row r="20" spans="1:2">
-      <c r="A20" s="44"/>
-      <c r="B20" s="46" t="s">
+      <c r="A20" s="47"/>
+      <c r="B20" s="49" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="21" ht="165.75" spans="1:2">
-      <c r="A21" s="47" t="s">
+      <c r="A21" s="50" t="s">
         <v>277</v>
       </c>
-      <c r="B21" s="45" t="s">
+      <c r="B21" s="48" t="s">
         <v>278</v>
       </c>
     </row>
     <row r="22" ht="242.25" spans="1:2">
-      <c r="A22" s="47"/>
-      <c r="B22" s="45" t="s">
+      <c r="A22" s="50"/>
+      <c r="B22" s="48" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="23" ht="153" spans="1:2">
-      <c r="A23" s="47"/>
-      <c r="B23" s="45" t="s">
+      <c r="A23" s="50"/>
+      <c r="B23" s="48" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="24" ht="38.25" spans="1:2">
-      <c r="A24" s="47"/>
-      <c r="B24" s="45" t="s">
+      <c r="A24" s="50"/>
+      <c r="B24" s="48" t="s">
         <v>281</v>
       </c>
     </row>
     <row r="25" ht="25.5" spans="1:2">
-      <c r="A25" s="47"/>
-      <c r="B25" s="45" t="s">
+      <c r="A25" s="50"/>
+      <c r="B25" s="48" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="26" ht="51" spans="1:2">
-      <c r="A26" s="47"/>
-      <c r="B26" s="45" t="s">
+      <c r="A26" s="50"/>
+      <c r="B26" s="48" t="s">
         <v>283</v>
       </c>
     </row>
     <row r="27" spans="1:2">
-      <c r="A27" s="47"/>
-      <c r="B27" s="45" t="s">
+      <c r="A27" s="50"/>
+      <c r="B27" s="48" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="28" spans="1:2">
-      <c r="A28" s="47"/>
-      <c r="B28" s="46" t="s">
+      <c r="A28" s="50"/>
+      <c r="B28" s="49" t="s">
         <v>285</v>
       </c>
     </row>
     <row r="29" ht="38.25" spans="1:2">
-      <c r="A29" s="48" t="s">
+      <c r="A29" s="8" t="s">
         <v>286</v>
       </c>
-      <c r="B29" s="45" t="s">
+      <c r="B29" s="48" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="30" spans="1:2">
-      <c r="A30" s="44"/>
-      <c r="B30" s="45" t="s">
+      <c r="A30" s="47"/>
+      <c r="B30" s="48" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="44"/>
-      <c r="B31" s="45" t="s">
+      <c r="A31" s="47"/>
+      <c r="B31" s="48" t="s">
         <v>289</v>
       </c>
     </row>
     <row r="32" spans="1:2">
-      <c r="A32" s="44"/>
-      <c r="B32" s="45" t="s">
+      <c r="A32" s="47"/>
+      <c r="B32" s="48" t="s">
         <v>290</v>
       </c>
     </row>
     <row r="33" spans="1:2">
-      <c r="A33" s="44"/>
-      <c r="B33" s="45" t="s">
+      <c r="A33" s="47"/>
+      <c r="B33" s="48" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="34" ht="51" spans="1:2">
-      <c r="A34" s="47" t="s">
+      <c r="A34" s="50" t="s">
         <v>292</v>
       </c>
-      <c r="B34" s="13" t="s">
+      <c r="B34" s="16" t="s">
         <v>293</v>
       </c>
     </row>
     <row r="35" ht="38.25" spans="1:2">
-      <c r="A35" s="44"/>
-      <c r="B35" s="13" t="s">
+      <c r="A35" s="47"/>
+      <c r="B35" s="16" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="36" ht="51" spans="1:2">
-      <c r="A36" s="44"/>
-      <c r="B36" s="13" t="s">
+      <c r="A36" s="47"/>
+      <c r="B36" s="16" t="s">
         <v>295</v>
       </c>
     </row>
     <row r="37" ht="51" spans="1:2">
-      <c r="A37" s="44"/>
-      <c r="B37" s="13" t="s">
+      <c r="A37" s="47"/>
+      <c r="B37" s="16" t="s">
         <v>296</v>
       </c>
     </row>
     <row r="38" ht="25.5" spans="1:2">
-      <c r="A38" s="44" t="s">
+      <c r="A38" s="47" t="s">
         <v>297</v>
       </c>
-      <c r="B38" s="13" t="s">
+      <c r="B38" s="16" t="s">
         <v>298</v>
       </c>
     </row>
     <row r="39" ht="76.5" spans="1:2">
-      <c r="A39" s="44"/>
-      <c r="B39" s="13" t="s">
+      <c r="A39" s="47"/>
+      <c r="B39" s="16" t="s">
         <v>299</v>
       </c>
     </row>
     <row r="40" ht="25.5" spans="1:2">
-      <c r="A40" s="44"/>
-      <c r="B40" s="13" t="s">
+      <c r="A40" s="47"/>
+      <c r="B40" s="16" t="s">
         <v>300</v>
       </c>
     </row>
     <row r="41" ht="25.5" spans="1:2">
-      <c r="A41" s="44"/>
-      <c r="B41" s="13" t="s">
+      <c r="A41" s="47"/>
+      <c r="B41" s="16" t="s">
         <v>301</v>
       </c>
     </row>
     <row r="42" spans="1:2">
-      <c r="A42" s="44"/>
-      <c r="B42" s="13" t="s">
+      <c r="A42" s="47"/>
+      <c r="B42" s="16" t="s">
         <v>302</v>
       </c>
     </row>
     <row r="43" ht="25.5" spans="1:2">
-      <c r="A43" s="44"/>
-      <c r="B43" s="13" t="s">
+      <c r="A43" s="47"/>
+      <c r="B43" s="16" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="44" spans="1:2">
-      <c r="A44" s="44"/>
-      <c r="B44" s="13"/>
+      <c r="A44" s="47"/>
+      <c r="B44" s="16"/>
     </row>
     <row r="45" ht="26.25" customHeight="1" spans="1:2">
-      <c r="A45" s="49" t="s">
+      <c r="A45" s="51" t="s">
         <v>304</v>
       </c>
-      <c r="B45" s="49"/>
+      <c r="B45" s="51"/>
     </row>
     <row r="46" spans="1:2">
-      <c r="A46" s="49"/>
-      <c r="B46" s="49"/>
+      <c r="A46" s="51"/>
+      <c r="B46" s="51"/>
     </row>
     <row r="47" ht="51" spans="1:2">
-      <c r="A47" s="44" t="s">
+      <c r="A47" s="47" t="s">
         <v>305</v>
       </c>
-      <c r="B47" s="50" t="s">
+      <c r="B47" s="52" t="s">
         <v>306</v>
       </c>
     </row>
@@ -15280,166 +15433,166 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="24" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="55.8533333333333" style="36" customWidth="1"/>
-    <col min="2" max="2" width="54.14" style="37" customWidth="1"/>
-    <col min="3" max="3" width="101.713333333333" style="38" customWidth="1"/>
+    <col min="1" max="1" width="55.8533333333333" style="39" customWidth="1"/>
+    <col min="2" max="2" width="54.14" style="40" customWidth="1"/>
+    <col min="3" max="3" width="101.713333333333" style="41" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="12.75" spans="1:1">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="42" t="s">
         <v>307</v>
       </c>
     </row>
     <row r="2" ht="12.75" spans="1:3">
-      <c r="A2" s="39"/>
-      <c r="B2" s="40"/>
-      <c r="C2" s="41"/>
+      <c r="A2" s="42"/>
+      <c r="B2" s="43"/>
+      <c r="C2" s="44"/>
     </row>
     <row r="3" ht="12.75" spans="1:2">
-      <c r="A3" s="39"/>
-      <c r="B3" s="40"/>
+      <c r="A3" s="42"/>
+      <c r="B3" s="43"/>
     </row>
     <row r="4" ht="12.75" spans="1:2">
-      <c r="A4" s="39"/>
-      <c r="B4" s="40"/>
+      <c r="A4" s="42"/>
+      <c r="B4" s="43"/>
     </row>
     <row r="5" ht="12.75" spans="1:2">
-      <c r="A5" s="39"/>
-      <c r="B5" s="40"/>
+      <c r="A5" s="42"/>
+      <c r="B5" s="43"/>
     </row>
     <row r="6" ht="12.75" spans="1:2">
-      <c r="A6" s="39"/>
-      <c r="B6" s="40"/>
+      <c r="A6" s="42"/>
+      <c r="B6" s="43"/>
     </row>
     <row r="7" ht="12.75" spans="1:2">
-      <c r="A7" s="39"/>
-      <c r="B7" s="40"/>
+      <c r="A7" s="42"/>
+      <c r="B7" s="43"/>
     </row>
     <row r="8" ht="12.75" spans="1:2">
-      <c r="A8" s="39"/>
-      <c r="B8" s="40"/>
+      <c r="A8" s="42"/>
+      <c r="B8" s="43"/>
     </row>
     <row r="9" ht="12.75" spans="1:2">
-      <c r="A9" s="39"/>
-      <c r="B9" s="40"/>
+      <c r="A9" s="42"/>
+      <c r="B9" s="43"/>
     </row>
     <row r="10" ht="12.75" spans="1:2">
-      <c r="A10" s="39"/>
-      <c r="B10" s="40"/>
+      <c r="A10" s="42"/>
+      <c r="B10" s="43"/>
     </row>
     <row r="11" ht="12.75" spans="1:2">
-      <c r="A11" s="39"/>
-      <c r="B11" s="40"/>
+      <c r="A11" s="42"/>
+      <c r="B11" s="43"/>
     </row>
     <row r="12" ht="12.75" spans="1:2">
-      <c r="A12" s="39"/>
-      <c r="B12" s="40"/>
+      <c r="A12" s="42"/>
+      <c r="B12" s="43"/>
     </row>
     <row r="13" ht="12.75" spans="1:2">
-      <c r="A13" s="39"/>
-      <c r="B13" s="40"/>
+      <c r="A13" s="42"/>
+      <c r="B13" s="43"/>
     </row>
     <row r="14" ht="12.75" spans="1:2">
-      <c r="A14" s="39"/>
-      <c r="B14" s="40"/>
+      <c r="A14" s="42"/>
+      <c r="B14" s="43"/>
     </row>
     <row r="15" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A15" s="39"/>
-      <c r="B15" s="40"/>
+      <c r="A15" s="42"/>
+      <c r="B15" s="43"/>
     </row>
     <row r="16" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A16" s="39"/>
-      <c r="B16" s="40"/>
+      <c r="A16" s="42"/>
+      <c r="B16" s="43"/>
     </row>
     <row r="17" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A17" s="39"/>
-      <c r="B17" s="40"/>
+      <c r="A17" s="42"/>
+      <c r="B17" s="43"/>
     </row>
     <row r="18" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A18" s="39"/>
-      <c r="B18" s="40"/>
+      <c r="A18" s="42"/>
+      <c r="B18" s="43"/>
     </row>
     <row r="19" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A19" s="39"/>
-      <c r="B19" s="40"/>
+      <c r="A19" s="42"/>
+      <c r="B19" s="43"/>
     </row>
     <row r="20" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A20" s="39"/>
-      <c r="B20" s="40"/>
+      <c r="A20" s="42"/>
+      <c r="B20" s="43"/>
     </row>
     <row r="21" ht="18.75" customHeight="1" spans="1:2">
-      <c r="A21" s="39"/>
-      <c r="B21" s="40"/>
+      <c r="A21" s="42"/>
+      <c r="B21" s="43"/>
     </row>
     <row r="22" ht="17.25" spans="1:2">
-      <c r="A22" s="39"/>
-      <c r="B22" s="40"/>
+      <c r="A22" s="42"/>
+      <c r="B22" s="43"/>
     </row>
     <row r="23" ht="17.25" spans="1:2">
-      <c r="A23" s="39"/>
-      <c r="B23" s="40"/>
+      <c r="A23" s="42"/>
+      <c r="B23" s="43"/>
     </row>
     <row r="24" ht="17.25" spans="1:2">
-      <c r="A24" s="39"/>
-      <c r="B24" s="42"/>
+      <c r="A24" s="42"/>
+      <c r="B24" s="45"/>
     </row>
     <row r="26" ht="17.25" spans="1:2">
-      <c r="A26" s="39" t="s">
+      <c r="A26" s="42" t="s">
         <v>308</v>
       </c>
-      <c r="B26" s="37" t="s">
+      <c r="B26" s="40" t="s">
         <v>309</v>
       </c>
     </row>
     <row r="27" ht="17.25" spans="1:2">
-      <c r="A27" s="39"/>
-      <c r="B27" s="37" t="s">
+      <c r="A27" s="42"/>
+      <c r="B27" s="40" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="28" ht="17.25" spans="1:2">
-      <c r="A28" s="39"/>
-      <c r="B28" s="37" t="s">
+      <c r="A28" s="42"/>
+      <c r="B28" s="40" t="s">
         <v>311</v>
       </c>
     </row>
     <row r="29" spans="1:1">
-      <c r="A29" s="39"/>
+      <c r="A29" s="42"/>
     </row>
     <row r="30" ht="12.75" spans="1:3">
-      <c r="A30" s="39" t="s">
+      <c r="A30" s="42" t="s">
         <v>312</v>
       </c>
-      <c r="B30" s="37" t="s">
+      <c r="B30" s="40" t="s">
         <v>313</v>
       </c>
-      <c r="C30" s="38" t="s">
+      <c r="C30" s="41" t="s">
         <v>314</v>
       </c>
     </row>
     <row r="31" ht="12.75" spans="1:3">
-      <c r="A31" s="39"/>
-      <c r="C31" s="38" t="s">
+      <c r="A31" s="42"/>
+      <c r="C31" s="41" t="s">
         <v>315</v>
       </c>
     </row>
     <row r="32" ht="12.75" spans="1:3">
-      <c r="A32" s="39"/>
-      <c r="C32" s="38" t="s">
+      <c r="A32" s="42"/>
+      <c r="C32" s="41" t="s">
         <v>316</v>
       </c>
     </row>
     <row r="33" ht="12.75" spans="1:3">
-      <c r="A33" s="39"/>
-      <c r="C33" s="38" t="s">
+      <c r="A33" s="42"/>
+      <c r="C33" s="41" t="s">
         <v>317</v>
       </c>
     </row>
     <row r="35" ht="114.75" spans="1:3">
-      <c r="A35" s="39" t="s">
+      <c r="A35" s="42" t="s">
         <v>318</v>
       </c>
-      <c r="B35" s="37" t="s">
+      <c r="B35" s="40" t="s">
         <v>319</v>
       </c>
       <c r="C35" s="74" t="s">
@@ -15447,8 +15600,8 @@
       </c>
     </row>
     <row r="36" ht="89.25" spans="1:3">
-      <c r="A36" s="39"/>
-      <c r="B36" s="37" t="s">
+      <c r="A36" s="42"/>
+      <c r="B36" s="40" t="s">
         <v>321</v>
       </c>
       <c r="C36" s="74" t="s">
@@ -15456,25 +15609,25 @@
       </c>
     </row>
     <row r="37" ht="76.5" spans="1:3">
-      <c r="A37" s="39"/>
-      <c r="B37" s="37" t="s">
+      <c r="A37" s="42"/>
+      <c r="B37" s="40" t="s">
         <v>323</v>
       </c>
-      <c r="C37" s="43" t="s">
+      <c r="C37" s="46" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="38" ht="51" spans="1:3">
-      <c r="A38" s="39"/>
-      <c r="B38" s="37" t="s">
+      <c r="A38" s="42"/>
+      <c r="B38" s="40" t="s">
         <v>325</v>
       </c>
-      <c r="C38" s="43" t="s">
+      <c r="C38" s="46" t="s">
         <v>326</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="39" t="s">
+      <c r="A40" s="42" t="s">
         <v>327</v>
       </c>
     </row>
@@ -15505,39 +15658,39 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="12.75" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="32" style="30" customWidth="1"/>
-    <col min="2" max="2" width="109" style="30" customWidth="1"/>
+    <col min="1" max="1" width="32" style="33" customWidth="1"/>
+    <col min="2" max="2" width="109" style="33" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="127.5" spans="1:3">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="34" t="s">
         <v>328</v>
       </c>
       <c r="B1" s="73" t="s">
         <v>329</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="35" t="s">
         <v>330</v>
       </c>
     </row>
     <row r="2" ht="200.25" customHeight="1" spans="1:2">
-      <c r="A2" s="30" t="s">
+      <c r="A2" s="33" t="s">
         <v>331</v>
       </c>
-      <c r="B2" s="30" t="s">
+      <c r="B2" s="33" t="s">
         <v>332</v>
       </c>
     </row>
     <row r="3" ht="102" spans="1:2">
-      <c r="A3" s="30" t="s">
+      <c r="A3" s="33" t="s">
         <v>333</v>
       </c>
-      <c r="B3" s="30" t="s">
+      <c r="B3" s="33" t="s">
         <v>334</v>
       </c>
     </row>
     <row r="4" ht="25.5" spans="1:2">
-      <c r="A4" s="30" t="s">
+      <c r="A4" s="33" t="s">
         <v>335</v>
       </c>
       <c r="B4" s="73" t="s">
@@ -15545,251 +15698,251 @@
       </c>
     </row>
     <row r="5" ht="25.5" spans="1:2">
-      <c r="A5" s="30" t="s">
+      <c r="A5" s="33" t="s">
         <v>337</v>
       </c>
-      <c r="B5" s="30" t="s">
+      <c r="B5" s="33" t="s">
         <v>338</v>
       </c>
     </row>
     <row r="6" ht="38.25" spans="1:1">
-      <c r="A6" s="30" t="s">
+      <c r="A6" s="33" t="s">
         <v>339</v>
       </c>
     </row>
     <row r="7" ht="38.25" spans="1:2">
-      <c r="A7" s="30" t="s">
+      <c r="A7" s="33" t="s">
         <v>340</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="33" t="s">
         <v>341</v>
       </c>
     </row>
     <row r="8" ht="114.75" spans="1:2">
-      <c r="A8" s="30" t="s">
+      <c r="A8" s="33" t="s">
         <v>342</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="33" t="s">
         <v>343</v>
       </c>
     </row>
     <row r="12" ht="51" spans="1:2">
-      <c r="A12" s="30" t="s">
+      <c r="A12" s="33" t="s">
         <v>344</v>
       </c>
-      <c r="B12" s="30" t="s">
+      <c r="B12" s="33" t="s">
         <v>345</v>
       </c>
     </row>
     <row r="13" ht="51" spans="1:2">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="33" t="s">
         <v>346</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="33" t="s">
         <v>347</v>
       </c>
     </row>
     <row r="14" ht="89.25" spans="1:2">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="33" t="s">
         <v>348</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="33" t="s">
         <v>349</v>
       </c>
     </row>
     <row r="15" ht="102" spans="1:2">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="33" t="s">
         <v>350</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="33" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="16" spans="1:2">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="33" t="s">
         <v>352</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="33" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="17" ht="178.5" spans="1:2">
-      <c r="A17" s="30" t="s">
+      <c r="A17" s="33" t="s">
         <v>354</v>
       </c>
-      <c r="B17" s="30" t="s">
+      <c r="B17" s="33" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="18" ht="25.5" spans="1:2">
-      <c r="A18" s="30" t="s">
+      <c r="A18" s="33" t="s">
         <v>356</v>
       </c>
-      <c r="B18" s="30" t="s">
+      <c r="B18" s="33" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="19" ht="280.5" spans="1:2">
-      <c r="A19" s="30" t="s">
+      <c r="A19" s="33" t="s">
         <v>358</v>
       </c>
-      <c r="B19" s="30" t="s">
+      <c r="B19" s="33" t="s">
         <v>359</v>
       </c>
     </row>
     <row r="20" spans="1:1">
-      <c r="A20" s="30" t="s">
+      <c r="A20" s="33" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="22" spans="1:1">
-      <c r="A22" s="30" t="s">
+      <c r="A22" s="33" t="s">
         <v>361</v>
       </c>
     </row>
     <row r="23" spans="2:2">
-      <c r="B23" s="33"/>
+      <c r="B23" s="36"/>
     </row>
     <row r="25" spans="1:1">
-      <c r="A25" s="30" t="s">
+      <c r="A25" s="33" t="s">
         <v>362</v>
       </c>
     </row>
     <row r="28" spans="1:1">
-      <c r="A28" s="30" t="s">
+      <c r="A28" s="33" t="s">
         <v>363</v>
       </c>
     </row>
     <row r="31" spans="1:2">
-      <c r="A31" s="30" t="s">
+      <c r="A31" s="33" t="s">
         <v>364</v>
       </c>
-      <c r="B31" s="30" t="s">
+      <c r="B31" s="33" t="s">
         <v>365</v>
       </c>
     </row>
     <row r="33" ht="38.25" spans="1:2">
-      <c r="A33" s="30" t="s">
+      <c r="A33" s="33" t="s">
         <v>366</v>
       </c>
-      <c r="B33" s="30" t="s">
+      <c r="B33" s="33" t="s">
         <v>367</v>
       </c>
     </row>
     <row r="34" ht="114.75" spans="1:2">
-      <c r="A34" s="30" t="s">
+      <c r="A34" s="33" t="s">
         <v>368</v>
       </c>
-      <c r="B34" s="30" t="s">
+      <c r="B34" s="33" t="s">
         <v>369</v>
       </c>
     </row>
     <row r="36" spans="1:1">
-      <c r="A36" s="30" t="s">
+      <c r="A36" s="33" t="s">
         <v>370</v>
       </c>
     </row>
     <row r="38" spans="1:1">
-      <c r="A38" s="30" t="s">
+      <c r="A38" s="33" t="s">
         <v>371</v>
       </c>
     </row>
     <row r="40" spans="1:1">
-      <c r="A40" s="30" t="s">
+      <c r="A40" s="33" t="s">
         <v>372</v>
       </c>
     </row>
     <row r="42" spans="1:1">
-      <c r="A42" s="30" t="s">
+      <c r="A42" s="33" t="s">
         <v>373</v>
       </c>
     </row>
     <row r="44" spans="1:1">
-      <c r="A44" s="30" t="s">
+      <c r="A44" s="33" t="s">
         <v>374</v>
       </c>
     </row>
     <row r="46" spans="1:1">
-      <c r="A46" s="30" t="s">
+      <c r="A46" s="33" t="s">
         <v>375</v>
       </c>
     </row>
     <row r="48" spans="1:1">
-      <c r="A48" s="30" t="s">
+      <c r="A48" s="33" t="s">
         <v>376</v>
       </c>
     </row>
     <row r="50" spans="1:1">
-      <c r="A50" s="30" t="s">
+      <c r="A50" s="33" t="s">
         <v>377</v>
       </c>
     </row>
     <row r="52" spans="1:1">
-      <c r="A52" s="30" t="s">
+      <c r="A52" s="33" t="s">
         <v>378</v>
       </c>
     </row>
     <row r="54" spans="1:2">
-      <c r="A54" s="34" t="s">
+      <c r="A54" s="37" t="s">
         <v>379</v>
       </c>
-      <c r="B54" s="30" t="s">
+      <c r="B54" s="33" t="s">
         <v>380</v>
       </c>
     </row>
     <row r="55" spans="1:2">
-      <c r="A55" s="34"/>
-      <c r="B55" s="30" t="s">
+      <c r="A55" s="37"/>
+      <c r="B55" s="33" t="s">
         <v>381</v>
       </c>
     </row>
     <row r="56" spans="1:2">
-      <c r="A56" s="34"/>
-      <c r="B56" s="30" t="s">
+      <c r="A56" s="37"/>
+      <c r="B56" s="33" t="s">
         <v>382</v>
       </c>
     </row>
     <row r="58" ht="25.5" spans="1:2">
-      <c r="A58" s="14" t="s">
+      <c r="A58" s="17" t="s">
         <v>383</v>
       </c>
-      <c r="B58" s="30" t="s">
+      <c r="B58" s="33" t="s">
         <v>384</v>
       </c>
     </row>
     <row r="59" spans="1:2">
-      <c r="A59" s="14"/>
-      <c r="B59" s="35" t="s">
+      <c r="A59" s="17"/>
+      <c r="B59" s="38" t="s">
         <v>385</v>
       </c>
     </row>
     <row r="60" spans="1:2">
-      <c r="A60" s="14"/>
-      <c r="B60" s="35" t="s">
+      <c r="A60" s="17"/>
+      <c r="B60" s="38" t="s">
         <v>386</v>
       </c>
     </row>
     <row r="61" spans="1:2">
-      <c r="A61" s="14"/>
-      <c r="B61" s="35" t="s">
+      <c r="A61" s="17"/>
+      <c r="B61" s="38" t="s">
         <v>387</v>
       </c>
     </row>
     <row r="62" spans="1:2">
-      <c r="A62" s="14"/>
-      <c r="B62" s="35" t="s">
+      <c r="A62" s="17"/>
+      <c r="B62" s="38" t="s">
         <v>388</v>
       </c>
     </row>
     <row r="63" spans="1:2">
-      <c r="A63" s="14"/>
-      <c r="B63" s="35" t="s">
+      <c r="A63" s="17"/>
+      <c r="B63" s="38" t="s">
         <v>389</v>
       </c>
     </row>
     <row r="64" spans="1:2">
-      <c r="A64" s="14"/>
-      <c r="B64" s="35" t="s">
+      <c r="A64" s="17"/>
+      <c r="B64" s="38" t="s">
         <v>390</v>
       </c>
     </row>
@@ -15817,77 +15970,77 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="21.75" outlineLevelCol="2"/>
   <cols>
-    <col min="1" max="1" width="47" style="24" customWidth="1"/>
-    <col min="2" max="2" width="125" style="25" customWidth="1"/>
-    <col min="3" max="3" width="60" style="26" customWidth="1"/>
-    <col min="4" max="16384" width="9.14" style="26"/>
+    <col min="1" max="1" width="47" style="27" customWidth="1"/>
+    <col min="2" max="2" width="125" style="28" customWidth="1"/>
+    <col min="3" max="3" width="60" style="29" customWidth="1"/>
+    <col min="4" max="16384" width="9.14" style="29"/>
   </cols>
   <sheetData>
     <row r="1" ht="120.75" spans="1:2">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="27" t="s">
         <v>391</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="30" t="s">
         <v>392</v>
       </c>
     </row>
     <row r="2" ht="138" spans="2:2">
-      <c r="B2" s="27" t="s">
+      <c r="B2" s="30" t="s">
         <v>393</v>
       </c>
     </row>
     <row r="3" ht="172.5" spans="1:3">
-      <c r="A3" s="24" t="s">
+      <c r="A3" s="27" t="s">
         <v>394</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="30" t="s">
         <v>395</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="31" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="4" ht="103.5" spans="1:2">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="27" t="s">
         <v>397</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="B4" s="30" t="s">
         <v>398</v>
       </c>
     </row>
     <row r="5" ht="65.25" spans="1:2">
-      <c r="A5" s="29" t="s">
+      <c r="A5" s="32" t="s">
         <v>399</v>
       </c>
-      <c r="B5" s="27"/>
+      <c r="B5" s="30"/>
     </row>
     <row r="6" spans="1:2">
-      <c r="A6" s="24" t="s">
+      <c r="A6" s="27" t="s">
         <v>400</v>
       </c>
-      <c r="B6" s="27"/>
+      <c r="B6" s="30"/>
     </row>
     <row r="7" spans="1:2">
-      <c r="A7" s="24" t="s">
+      <c r="A7" s="27" t="s">
         <v>401</v>
       </c>
-      <c r="B7" s="27"/>
+      <c r="B7" s="30"/>
     </row>
     <row r="8" spans="1:1">
-      <c r="A8" s="24" t="s">
+      <c r="A8" s="27" t="s">
         <v>402</v>
       </c>
     </row>
     <row r="9" ht="34.5" spans="1:2">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="27" t="s">
         <v>403</v>
       </c>
-      <c r="B9" s="27" t="s">
+      <c r="B9" s="30" t="s">
         <v>404</v>
       </c>
     </row>
     <row r="10" spans="1:1">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="27" t="s">
         <v>405</v>
       </c>
     </row>

</xml_diff>

<commit_message>
[feat][OOAD][greate software in 3 steps]
</commit_message>
<xml_diff>
--- a/System/Documents.xlsx
+++ b/System/Documents.xlsx
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="490" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="500" uniqueCount="496">
   <si>
     <t>Kiến Trúc về Microservice</t>
   </si>
@@ -661,7 +661,7 @@
     </r>
   </si>
   <si>
-    <t>Greate software</t>
+    <t>Greate Software</t>
   </si>
   <si>
     <t>What does great software mean:
@@ -673,21 +673,110 @@
  - Greate software is well-designed, well-coded and easy to maintain, reuse and extend.</t>
   </si>
   <si>
-    <r>
-      <t>Greate software in 3 easy steps</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>:
- 1. Make sure your software does what the customer wants it to do. This is where getting good requirements and doing some analysis comes in.
- 2. Apply basic OO principles to add flexibility. 
- 3. Strive(cố gắng) for a maintainable, reusable design: It's time to apply patterns and principles to make sure your software is ready to use for years to come.</t>
+    <t>Greate software in 3 steps</t>
+  </si>
+  <si>
+    <t xml:space="preserve">statisfy customer
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Win your customer over.
+ - Make sure your software does what the customer wants it to do. This is where getting good requirements and doing some analysis comes in.</t>
+  </si>
+  <si>
+    <t>Apply basic OO principles to add flexibility</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> - Once your software works, you can look for any duplicate code or bad class design that might have </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>slipped in</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>(để lọt vào), and make sure you're using good OO programming techniques.</t>
+    </r>
+  </si>
+  <si>
+    <t>Strive(cố gắng) for a maintainable, reusable design</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - It's time to apply patterns and principles to make sure your software is ready to use for years to come.</t>
+  </si>
+  <si>
+    <t>Object</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> - Objects are very particular about their jobs. Each object is interested in doing its job, and only its job, to the best of its ability.
+ - Objects should do what their names indicate.
+ - Each object should represent a single concept.
+ - Unused properties are a dead giveaway.</t>
+  </si>
+  <si>
+    <t>Encapsulation</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve"> - Encapsulation is also about breaking your app into </t>
+    </r>
+    <r>
+      <rPr>
+        <u/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>logical parts</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">(các phần hợp lý), and then keeping those </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>parts separate</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <charset val="134"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>.
+ - The idea behind encapsulation is to protect information in one part of your application from the other parts of your application.
+ - The power of encapsulation by breaking up the different parts of your app, you can change one part without having to change all the other parts.</t>
     </r>
   </si>
   <si>
@@ -728,13 +817,6 @@
   </si>
   <si>
     <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <charset val="134"/>
-        <scheme val="minor"/>
-      </rPr>
       <t xml:space="preserve"> - Requirement: it's a specific thing your system has to do to work correctly.
    + specific thing: A requirement is usually a single thing(một điều duy nhất), and you can test that thing to make sure you've actually fullilled the requirement.
    + system: Is complete app or project you're working on. Is everything needed to meet a customer's goals.
@@ -790,9 +872,6 @@
   </si>
   <si>
     <t>OO Principles</t>
-  </si>
-  <si>
-    <t>Encapsulation</t>
   </si>
   <si>
     <t xml:space="preserve"> - The idea behind encapsulation is to protect information in one part of your application from the other part of your application
@@ -11146,8 +11225,8 @@
   <numFmts count="4">
     <numFmt numFmtId="176" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
   <fonts count="46">
     <font>
@@ -11315,8 +11394,16 @@
       <charset val="134"/>
     </font>
     <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color theme="0"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -11329,11 +11416,11 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
       <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -11353,13 +11440,6 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
       <sz val="11"/>
       <color theme="3"/>
@@ -11368,54 +11448,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -11432,6 +11466,51 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -11525,7 +11604,121 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -11537,31 +11730,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -11573,49 +11742,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -11627,73 +11766,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -11704,6 +11783,24 @@
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -11724,27 +11821,26 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
         <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color rgb="FFFF8001"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
       </bottom>
       <diagonal/>
     </border>
@@ -11764,17 +11860,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
       </bottom>
       <diagonal/>
     </border>
@@ -11793,152 +11883,141 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="27" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="32" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="36" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="12" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="37" fillId="22" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="35" fillId="26" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="37" fillId="12" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="31" fillId="22" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="35" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="8" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="32" fillId="25" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="29" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -11946,7 +12025,7 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -12108,16 +12187,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -12869,65 +12945,65 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14" defaultRowHeight="12.75" outlineLevelCol="6"/>
   <cols>
-    <col min="1" max="1" width="9.14" style="65"/>
-    <col min="2" max="2" width="39.5733333333333" style="65" customWidth="1"/>
-    <col min="3" max="3" width="95.5733333333333" style="65" customWidth="1"/>
-    <col min="4" max="4" width="60.7133333333333" style="65" customWidth="1"/>
-    <col min="5" max="5" width="58.8533333333333" style="65" customWidth="1"/>
-    <col min="6" max="6" width="50" style="65" customWidth="1"/>
-    <col min="7" max="7" width="49.7133333333333" style="65" customWidth="1"/>
-    <col min="8" max="16384" width="9.14" style="65"/>
+    <col min="1" max="1" width="9.14" style="64"/>
+    <col min="2" max="2" width="39.5733333333333" style="64" customWidth="1"/>
+    <col min="3" max="3" width="95.5733333333333" style="64" customWidth="1"/>
+    <col min="4" max="4" width="60.7133333333333" style="64" customWidth="1"/>
+    <col min="5" max="5" width="58.8533333333333" style="64" customWidth="1"/>
+    <col min="6" max="6" width="50" style="64" customWidth="1"/>
+    <col min="7" max="7" width="49.7133333333333" style="64" customWidth="1"/>
+    <col min="8" max="16384" width="9.14" style="64"/>
   </cols>
   <sheetData>
     <row r="1" ht="76.5" spans="1:3">
-      <c r="A1" s="65">
+      <c r="A1" s="64">
         <v>1</v>
       </c>
-      <c r="B1" s="65" t="s">
+      <c r="B1" s="64" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="69" t="s">
+      <c r="C1" s="68" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" ht="63.75" spans="1:3">
-      <c r="A2" s="65">
+      <c r="A2" s="64">
         <v>2</v>
       </c>
-      <c r="B2" s="65" t="s">
+      <c r="B2" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="69" t="s">
+      <c r="C2" s="68" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" ht="38.25" spans="1:3">
-      <c r="A3" s="65">
+      <c r="A3" s="64">
         <v>3</v>
       </c>
-      <c r="B3" s="67" t="s">
+      <c r="B3" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="69" t="s">
+      <c r="C3" s="68" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" ht="38.25" spans="1:3">
-      <c r="A4" s="65">
+      <c r="A4" s="64">
         <v>4</v>
       </c>
-      <c r="B4" s="65" t="s">
+      <c r="B4" s="64" t="s">
         <v>6</v>
       </c>
-      <c r="C4" s="70" t="s">
+      <c r="C4" s="69" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" ht="178.5" spans="1:3">
-      <c r="A5" s="65">
+      <c r="A5" s="64">
         <v>5</v>
       </c>
-      <c r="B5" s="65" t="s">
+      <c r="B5" s="64" t="s">
         <v>8</v>
       </c>
       <c r="C5" s="21" t="s">
@@ -12935,65 +13011,65 @@
       </c>
     </row>
     <row r="6" ht="25.5" spans="1:3">
-      <c r="A6" s="65">
+      <c r="A6" s="64">
         <v>6</v>
       </c>
-      <c r="B6" s="65" t="s">
+      <c r="B6" s="64" t="s">
         <v>10</v>
       </c>
-      <c r="C6" s="70" t="s">
+      <c r="C6" s="69" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="7" ht="229.5" spans="1:3">
-      <c r="A7" s="65">
+      <c r="A7" s="64">
         <v>7</v>
       </c>
-      <c r="B7" s="65" t="s">
+      <c r="B7" s="64" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="66" t="s">
+      <c r="C7" s="65" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="8" ht="245.25" customHeight="1" spans="1:3">
-      <c r="A8" s="65">
+      <c r="A8" s="64">
         <v>8</v>
       </c>
-      <c r="B8" s="65" t="s">
+      <c r="B8" s="64" t="s">
         <v>14</v>
       </c>
-      <c r="C8" s="66" t="s">
+      <c r="C8" s="65" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="9" ht="223.5" customHeight="1" spans="1:3">
-      <c r="A9" s="65">
+      <c r="A9" s="64">
         <v>9</v>
       </c>
-      <c r="B9" s="65" t="s">
+      <c r="B9" s="64" t="s">
         <v>16</v>
       </c>
-      <c r="C9" s="69" t="s">
+      <c r="C9" s="68" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="10" ht="204" spans="1:4">
-      <c r="A10" s="65">
+      <c r="A10" s="64">
         <v>10</v>
       </c>
-      <c r="B10" s="65" t="s">
+      <c r="B10" s="64" t="s">
         <v>18</v>
       </c>
       <c r="C10" s="21" t="s">
         <v>19</v>
       </c>
-      <c r="D10" s="68" t="s">
+      <c r="D10" s="67" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="11" ht="25.5" spans="2:3">
-      <c r="B11" s="65" t="s">
+      <c r="B11" s="64" t="s">
         <v>21</v>
       </c>
       <c r="C11" s="21" t="s">
@@ -13001,7 +13077,7 @@
       </c>
     </row>
     <row r="12" ht="102" spans="2:3">
-      <c r="B12" s="65" t="s">
+      <c r="B12" s="64" t="s">
         <v>23</v>
       </c>
       <c r="C12" s="21" t="s">
@@ -13009,7 +13085,7 @@
       </c>
     </row>
     <row r="13" ht="140.25" spans="2:3">
-      <c r="B13" s="65" t="s">
+      <c r="B13" s="64" t="s">
         <v>25</v>
       </c>
       <c r="C13" s="21" t="s">
@@ -13017,13 +13093,13 @@
       </c>
     </row>
     <row r="14" ht="288.75" customHeight="1" spans="2:7">
-      <c r="B14" s="65" t="s">
+      <c r="B14" s="64" t="s">
         <v>27</v>
       </c>
       <c r="C14" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="D14" s="66" t="s">
+      <c r="D14" s="65" t="s">
         <v>29</v>
       </c>
       <c r="E14" s="21" t="s">
@@ -13037,7 +13113,7 @@
       </c>
     </row>
     <row r="15" ht="38.25" spans="2:3">
-      <c r="B15" s="65" t="s">
+      <c r="B15" s="64" t="s">
         <v>33</v>
       </c>
       <c r="C15" s="21" t="s">
@@ -13045,23 +13121,23 @@
       </c>
     </row>
     <row r="16" ht="240.75" customHeight="1" spans="2:2">
-      <c r="B16" s="65" t="s">
+      <c r="B16" s="64" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="17" ht="153" spans="2:3">
-      <c r="B17" s="65" t="s">
+      <c r="B17" s="64" t="s">
         <v>36</v>
       </c>
-      <c r="C17" s="66" t="s">
+      <c r="C17" s="65" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="18" ht="153" spans="2:3">
-      <c r="B18" s="65" t="s">
+      <c r="B18" s="64" t="s">
         <v>38</v>
       </c>
-      <c r="C18" s="66" t="s">
+      <c r="C18" s="65" t="s">
         <v>39</v>
       </c>
     </row>
@@ -13092,18 +13168,18 @@
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" s="17" t="s">
-        <v>411</v>
+        <v>420</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>412</v>
+        <v>421</v>
       </c>
     </row>
     <row r="2" ht="153" spans="1:2">
       <c r="A2" s="17" t="s">
-        <v>413</v>
+        <v>422</v>
       </c>
       <c r="B2" s="19" t="s">
-        <v>414</v>
+        <v>423</v>
       </c>
     </row>
   </sheetData>
@@ -13131,70 +13207,70 @@
   <sheetData>
     <row r="1" ht="120.75" spans="1:2">
       <c r="A1" s="11" t="s">
-        <v>415</v>
+        <v>424</v>
       </c>
       <c r="B1" s="14" t="s">
-        <v>416</v>
+        <v>425</v>
       </c>
     </row>
     <row r="2" ht="138" spans="2:2">
       <c r="B2" s="14" t="s">
-        <v>417</v>
+        <v>426</v>
       </c>
     </row>
     <row r="3" ht="172.5" spans="1:3">
       <c r="A3" s="11" t="s">
-        <v>418</v>
+        <v>427</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>419</v>
+        <v>428</v>
       </c>
       <c r="C3" s="15" t="s">
-        <v>420</v>
+        <v>429</v>
       </c>
     </row>
     <row r="4" ht="103.5" spans="1:2">
       <c r="A4" s="11" t="s">
-        <v>421</v>
+        <v>430</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>422</v>
+        <v>431</v>
       </c>
     </row>
     <row r="5" ht="65.25" spans="1:2">
       <c r="A5" s="16" t="s">
-        <v>423</v>
+        <v>432</v>
       </c>
       <c r="B5" s="14"/>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="11" t="s">
-        <v>424</v>
+        <v>433</v>
       </c>
       <c r="B6" s="14"/>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="11" t="s">
-        <v>425</v>
+        <v>434</v>
       </c>
       <c r="B7" s="14"/>
     </row>
     <row r="8" spans="1:1">
       <c r="A8" s="11" t="s">
-        <v>426</v>
+        <v>435</v>
       </c>
     </row>
     <row r="9" ht="34.5" spans="1:2">
       <c r="A9" s="11" t="s">
-        <v>427</v>
+        <v>436</v>
       </c>
       <c r="B9" s="14" t="s">
-        <v>428</v>
+        <v>437</v>
       </c>
     </row>
     <row r="10" spans="1:1">
       <c r="A10" s="11" t="s">
-        <v>429</v>
+        <v>438</v>
       </c>
     </row>
   </sheetData>
@@ -13226,276 +13302,276 @@
   <sheetData>
     <row r="1" ht="89.25" spans="1:2">
       <c r="A1" s="4" t="s">
-        <v>430</v>
+        <v>439</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>431</v>
+        <v>440</v>
       </c>
     </row>
     <row r="2" ht="89.25" spans="1:2">
       <c r="A2" s="4"/>
       <c r="B2" s="5" t="s">
-        <v>432</v>
+        <v>441</v>
       </c>
     </row>
     <row r="3" ht="102" spans="1:2">
       <c r="A3" s="4"/>
       <c r="B3" s="1" t="s">
-        <v>433</v>
+        <v>442</v>
       </c>
     </row>
     <row r="4" ht="63.75" spans="1:2">
       <c r="A4" s="4" t="s">
-        <v>434</v>
+        <v>443</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>435</v>
+        <v>444</v>
       </c>
     </row>
     <row r="5" ht="63.75" spans="1:2">
       <c r="A5" s="4"/>
       <c r="B5" s="5" t="s">
-        <v>436</v>
+        <v>445</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="4"/>
       <c r="B6" s="5" t="s">
-        <v>437</v>
+        <v>446</v>
       </c>
     </row>
     <row r="7" ht="38.25" spans="1:2">
       <c r="A7" s="4" t="s">
-        <v>438</v>
+        <v>447</v>
       </c>
       <c r="B7" s="5" t="s">
-        <v>439</v>
+        <v>448</v>
       </c>
     </row>
     <row r="8" ht="38.25" spans="1:2">
       <c r="A8" s="4"/>
       <c r="B8" s="5" t="s">
-        <v>440</v>
+        <v>449</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="4"/>
       <c r="B9" s="5" t="s">
-        <v>441</v>
+        <v>450</v>
       </c>
     </row>
     <row r="10" spans="1:2">
       <c r="A10" s="4"/>
       <c r="B10" s="5" t="s">
-        <v>442</v>
+        <v>451</v>
       </c>
     </row>
     <row r="11" spans="1:2">
       <c r="A11" s="4"/>
       <c r="B11" s="5" t="s">
-        <v>443</v>
+        <v>452</v>
       </c>
     </row>
     <row r="12" ht="51" spans="1:2">
       <c r="A12" s="4" t="s">
-        <v>444</v>
+        <v>453</v>
       </c>
       <c r="B12" s="5" t="s">
-        <v>445</v>
+        <v>454</v>
       </c>
     </row>
     <row r="13" ht="63.75" spans="1:2">
       <c r="A13" s="4"/>
       <c r="B13" s="5" t="s">
-        <v>446</v>
+        <v>455</v>
       </c>
     </row>
     <row r="14" ht="127.5" spans="1:2">
       <c r="A14" s="4"/>
       <c r="B14" s="5" t="s">
-        <v>447</v>
+        <v>456</v>
       </c>
     </row>
     <row r="15" spans="1:2">
       <c r="A15" s="4"/>
       <c r="B15" s="5" t="s">
-        <v>448</v>
+        <v>457</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="4"/>
       <c r="B16" s="5" t="s">
-        <v>449</v>
+        <v>458</v>
       </c>
     </row>
     <row r="17" ht="102" spans="1:2">
       <c r="A17" s="4"/>
       <c r="B17" s="5" t="s">
-        <v>450</v>
+        <v>459</v>
       </c>
     </row>
     <row r="18" ht="38.25" spans="1:2">
       <c r="A18" s="4"/>
       <c r="B18" s="5" t="s">
-        <v>451</v>
+        <v>460</v>
       </c>
     </row>
     <row r="19" spans="1:2">
       <c r="A19" s="4"/>
       <c r="B19" s="5" t="s">
-        <v>452</v>
+        <v>461</v>
       </c>
     </row>
     <row r="20" spans="1:2">
       <c r="A20" s="4"/>
       <c r="B20" s="6" t="s">
-        <v>453</v>
+        <v>462</v>
       </c>
     </row>
     <row r="21" ht="165.75" spans="1:2">
       <c r="A21" s="7" t="s">
-        <v>454</v>
+        <v>463</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>455</v>
+        <v>464</v>
       </c>
     </row>
     <row r="22" ht="242.25" spans="1:2">
       <c r="A22" s="7"/>
       <c r="B22" s="5" t="s">
-        <v>456</v>
+        <v>465</v>
       </c>
     </row>
     <row r="23" ht="153" spans="1:2">
       <c r="A23" s="7"/>
       <c r="B23" s="5" t="s">
-        <v>457</v>
+        <v>466</v>
       </c>
     </row>
     <row r="24" ht="38.25" spans="1:2">
       <c r="A24" s="7"/>
       <c r="B24" s="5" t="s">
-        <v>458</v>
+        <v>467</v>
       </c>
     </row>
     <row r="25" ht="25.5" spans="1:2">
       <c r="A25" s="7"/>
       <c r="B25" s="5" t="s">
-        <v>459</v>
+        <v>468</v>
       </c>
     </row>
     <row r="26" ht="51" spans="1:2">
       <c r="A26" s="7"/>
       <c r="B26" s="5" t="s">
-        <v>460</v>
+        <v>469</v>
       </c>
     </row>
     <row r="27" spans="1:2">
       <c r="A27" s="7"/>
       <c r="B27" s="5" t="s">
-        <v>461</v>
+        <v>470</v>
       </c>
     </row>
     <row r="28" spans="1:2">
       <c r="A28" s="7"/>
       <c r="B28" s="6" t="s">
-        <v>462</v>
+        <v>471</v>
       </c>
     </row>
     <row r="29" ht="38.25" spans="1:2">
       <c r="A29" s="8" t="s">
-        <v>463</v>
+        <v>472</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>464</v>
+        <v>473</v>
       </c>
     </row>
     <row r="30" spans="1:2">
       <c r="A30" s="4"/>
       <c r="B30" s="5" t="s">
-        <v>465</v>
+        <v>474</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="4"/>
       <c r="B31" s="5" t="s">
-        <v>466</v>
+        <v>475</v>
       </c>
     </row>
     <row r="32" spans="1:2">
       <c r="A32" s="4"/>
       <c r="B32" s="5" t="s">
-        <v>467</v>
+        <v>476</v>
       </c>
     </row>
     <row r="33" spans="1:2">
       <c r="A33" s="4"/>
       <c r="B33" s="5" t="s">
-        <v>468</v>
+        <v>477</v>
       </c>
     </row>
     <row r="34" ht="51" spans="1:2">
       <c r="A34" s="7" t="s">
-        <v>469</v>
+        <v>478</v>
       </c>
       <c r="B34" s="1" t="s">
-        <v>470</v>
+        <v>479</v>
       </c>
     </row>
     <row r="35" ht="38.25" spans="1:2">
       <c r="A35" s="4"/>
       <c r="B35" s="1" t="s">
-        <v>471</v>
+        <v>480</v>
       </c>
     </row>
     <row r="36" ht="51" spans="1:2">
       <c r="A36" s="4"/>
       <c r="B36" s="1" t="s">
-        <v>472</v>
+        <v>481</v>
       </c>
     </row>
     <row r="37" ht="51" spans="1:2">
       <c r="A37" s="4"/>
       <c r="B37" s="1" t="s">
-        <v>473</v>
+        <v>482</v>
       </c>
     </row>
     <row r="38" ht="25.5" spans="1:2">
       <c r="A38" s="4" t="s">
-        <v>474</v>
+        <v>483</v>
       </c>
       <c r="B38" s="1" t="s">
-        <v>475</v>
+        <v>484</v>
       </c>
     </row>
     <row r="39" ht="76.5" spans="1:2">
       <c r="A39" s="4"/>
       <c r="B39" s="1" t="s">
-        <v>476</v>
+        <v>485</v>
       </c>
     </row>
     <row r="40" ht="25.5" spans="1:2">
       <c r="A40" s="4"/>
       <c r="B40" s="1" t="s">
-        <v>477</v>
+        <v>486</v>
       </c>
     </row>
     <row r="41" ht="25.5" spans="1:2">
       <c r="A41" s="4"/>
       <c r="B41" s="1" t="s">
-        <v>478</v>
+        <v>487</v>
       </c>
     </row>
     <row r="42" spans="1:2">
       <c r="A42" s="4"/>
       <c r="B42" s="1" t="s">
-        <v>479</v>
+        <v>488</v>
       </c>
     </row>
     <row r="43" ht="25.5" spans="1:2">
       <c r="A43" s="4"/>
       <c r="B43" s="1" t="s">
-        <v>480</v>
+        <v>489</v>
       </c>
     </row>
     <row r="44" spans="1:2">
@@ -13504,7 +13580,7 @@
     </row>
     <row r="45" ht="26.25" customHeight="1" spans="1:2">
       <c r="A45" s="9" t="s">
-        <v>481</v>
+        <v>490</v>
       </c>
       <c r="B45" s="9"/>
     </row>
@@ -13514,10 +13590,10 @@
     </row>
     <row r="47" ht="51" spans="1:2">
       <c r="A47" s="4" t="s">
-        <v>482</v>
+        <v>491</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>483</v>
+        <v>492</v>
       </c>
     </row>
   </sheetData>
@@ -13654,15 +13730,15 @@
   <sheetData>
     <row r="1" ht="25.5" spans="2:2">
       <c r="B1" s="1" t="s">
-        <v>484</v>
+        <v>493</v>
       </c>
     </row>
     <row r="3" ht="51" spans="1:2">
       <c r="A3" s="1" t="s">
-        <v>485</v>
+        <v>494</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>486</v>
+        <v>495</v>
       </c>
     </row>
     <row r="4" spans="2:2">
@@ -13677,10 +13753,10 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:E14"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:D4"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85333333333333" defaultRowHeight="21.75" outlineLevelCol="4"/>
@@ -13691,143 +13767,192 @@
     <col min="4" max="4" width="156.14" style="58" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" ht="96" customHeight="1" spans="2:4">
-      <c r="B1" s="56" t="s">
+    <row r="1" ht="96" customHeight="1" spans="1:4">
+      <c r="A1" s="16" t="s">
         <v>40</v>
       </c>
-      <c r="C1" s="59" t="s">
+      <c r="B1" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="60"/>
-    </row>
-    <row r="2" ht="57" customHeight="1" spans="3:4">
-      <c r="C2" s="61" t="s">
+      <c r="C1" s="2"/>
+      <c r="D1" s="2"/>
+    </row>
+    <row r="2" ht="96" customHeight="1" spans="2:4">
+      <c r="B2" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="D2" s="51"/>
-    </row>
-    <row r="3" ht="151" customHeight="1" spans="1:4">
-      <c r="A3" s="16" t="s">
+      <c r="C2" s="17" t="s">
         <v>43</v>
       </c>
-      <c r="B3" s="56" t="s">
+      <c r="D2" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C3" s="62" t="s">
+    </row>
+    <row r="3" ht="68" customHeight="1" spans="2:4">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17" t="s">
         <v>45</v>
       </c>
-      <c r="D3" s="60"/>
-    </row>
-    <row r="4" ht="66" customHeight="1" spans="2:4">
-      <c r="B4" s="56" t="s">
+      <c r="D3" s="18" t="s">
         <v>46</v>
       </c>
-      <c r="C4" s="59" t="s">
+    </row>
+    <row r="4" ht="57" customHeight="1" spans="2:4">
+      <c r="B4" s="17"/>
+      <c r="C4" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="D4" s="60"/>
-    </row>
-    <row r="5" ht="114" customHeight="1" spans="2:4">
+      <c r="D4" s="18" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="5" ht="57" customHeight="1" spans="2:4">
       <c r="B5" s="56" t="s">
-        <v>48</v>
-      </c>
-      <c r="C5" s="59" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="60"/>
-    </row>
-    <row r="6" ht="33.95" customHeight="1" spans="2:5">
-      <c r="B6" s="63" t="s">
+      <c r="C5" s="18" t="s">
         <v>50</v>
       </c>
-      <c r="C6" s="64" t="s">
+      <c r="D5" s="18"/>
+    </row>
+    <row r="6" ht="57" customHeight="1" spans="2:4">
+      <c r="B6" s="56" t="s">
         <v>51</v>
       </c>
-      <c r="D6" s="60" t="s">
+      <c r="C6" s="18" t="s">
         <v>52</v>
       </c>
-      <c r="E6" s="2"/>
-    </row>
-    <row r="7" ht="45" customHeight="1" spans="2:3">
-      <c r="B7" s="56" t="s">
+      <c r="D6" s="18"/>
+    </row>
+    <row r="7" ht="57" customHeight="1" spans="3:4">
+      <c r="C7" s="18"/>
+      <c r="D7" s="18"/>
+    </row>
+    <row r="8" ht="151" customHeight="1" spans="1:4">
+      <c r="A8" s="16" t="s">
         <v>53</v>
       </c>
-      <c r="C7" s="59" t="s">
+      <c r="B8" s="56" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="8" ht="30" customHeight="1" spans="2:3">
-      <c r="B8" s="56" t="s">
+      <c r="C8" s="59" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="62" t="s">
+      <c r="D8" s="60"/>
+    </row>
+    <row r="9" ht="66" customHeight="1" spans="2:4">
+      <c r="B9" s="56" t="s">
         <v>56</v>
       </c>
-    </row>
-    <row r="9" ht="25.5" spans="1:4">
-      <c r="A9" s="16" t="s">
+      <c r="C9" s="61" t="s">
         <v>57</v>
       </c>
-      <c r="B9" s="56" t="s">
+      <c r="D9" s="60"/>
+    </row>
+    <row r="10" ht="114" customHeight="1" spans="2:4">
+      <c r="B10" s="56" t="s">
         <v>58</v>
       </c>
-      <c r="C9" s="37" t="s">
+      <c r="C10" s="61" t="s">
         <v>59</v>
       </c>
-      <c r="D9" s="53" t="s">
+      <c r="D10" s="60"/>
+    </row>
+    <row r="11" ht="33.95" customHeight="1" spans="2:5">
+      <c r="B11" s="62" t="s">
         <v>60</v>
       </c>
-    </row>
-    <row r="10" ht="25.5" spans="3:4">
-      <c r="C10" s="37" t="s">
+      <c r="C11" s="63" t="s">
+        <v>51</v>
+      </c>
+      <c r="D11" s="60" t="s">
         <v>61</v>
       </c>
-      <c r="D10" s="60" t="s">
+      <c r="E11" s="2"/>
+    </row>
+    <row r="12" ht="45" customHeight="1" spans="2:3">
+      <c r="B12" s="56" t="s">
         <v>62</v>
       </c>
-    </row>
-    <row r="11" ht="38.25" spans="3:4">
-      <c r="C11" s="37" t="s">
+      <c r="C12" s="61" t="s">
         <v>63</v>
       </c>
-      <c r="D11" s="53" t="s">
+    </row>
+    <row r="13" ht="30" customHeight="1" spans="2:3">
+      <c r="B13" s="56" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="12" ht="30" customHeight="1" spans="2:4">
-      <c r="B12" s="37" t="s">
+      <c r="C13" s="59" t="s">
         <v>65</v>
       </c>
-      <c r="C12" s="60" t="s">
+    </row>
+    <row r="14" ht="25.5" spans="1:4">
+      <c r="A14" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="D12" s="60"/>
-    </row>
-    <row r="13" ht="308" customHeight="1" spans="2:4">
-      <c r="B13" s="56" t="s">
+      <c r="B14" s="56" t="s">
         <v>67</v>
       </c>
-      <c r="C13" s="62" t="s">
+      <c r="C14" s="37" t="s">
         <v>68</v>
       </c>
-      <c r="D13" s="60"/>
+      <c r="D14" s="53" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="15" ht="25.5" spans="3:4">
+      <c r="C15" s="37" t="s">
+        <v>70</v>
+      </c>
+      <c r="D15" s="60" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="16" ht="38.25" spans="3:4">
+      <c r="C16" s="37" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="53" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="17" ht="30" customHeight="1" spans="2:4">
+      <c r="B17" s="37" t="s">
+        <v>74</v>
+      </c>
+      <c r="C17" s="60" t="s">
+        <v>75</v>
+      </c>
+      <c r="D17" s="60"/>
+    </row>
+    <row r="18" ht="308" customHeight="1" spans="2:4">
+      <c r="B18" s="56" t="s">
+        <v>76</v>
+      </c>
+      <c r="C18" s="59" t="s">
+        <v>77</v>
+      </c>
+      <c r="D18" s="60"/>
     </row>
   </sheetData>
-  <mergeCells count="14">
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="C3:D3"/>
-    <mergeCell ref="C4:D4"/>
+  <mergeCells count="17">
+    <mergeCell ref="B1:D1"/>
     <mergeCell ref="C5:D5"/>
-    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="C6:D6"/>
     <mergeCell ref="C7:D7"/>
     <mergeCell ref="C8:D8"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C10:D10"/>
+    <mergeCell ref="D11:E11"/>
     <mergeCell ref="C12:D12"/>
     <mergeCell ref="C13:D13"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="A9:A14"/>
-    <mergeCell ref="B1:B2"/>
-    <mergeCell ref="B9:B11"/>
+    <mergeCell ref="C17:D17"/>
+    <mergeCell ref="C18:D18"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A14:A19"/>
+    <mergeCell ref="B2:B4"/>
+    <mergeCell ref="B14:B16"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -13854,10 +13979,10 @@
   <sheetData>
     <row r="1" ht="26.25" spans="1:5">
       <c r="A1" s="45" t="s">
-        <v>69</v>
+        <v>78</v>
       </c>
       <c r="B1" s="49" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C1" s="49"/>
       <c r="D1" s="49"/>
@@ -13865,30 +13990,30 @@
     </row>
     <row r="2" ht="55" customHeight="1" spans="2:5">
       <c r="B2" s="49" t="s">
-        <v>71</v>
+        <v>80</v>
       </c>
       <c r="C2" s="18" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="D2" s="18"/>
       <c r="E2" s="18"/>
     </row>
     <row r="3" ht="57" customHeight="1" spans="2:5">
       <c r="B3" s="49" t="s">
-        <v>50</v>
+        <v>60</v>
       </c>
       <c r="C3" s="18" t="s">
-        <v>73</v>
+        <v>82</v>
       </c>
       <c r="D3" s="18"/>
       <c r="E3" s="18"/>
     </row>
     <row r="4" ht="44" customHeight="1" spans="2:5">
       <c r="B4" s="49" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="C4" s="18" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="D4" s="18"/>
       <c r="E4" s="18"/>
@@ -13896,7 +14021,7 @@
     <row r="5" spans="2:5">
       <c r="B5" s="49"/>
       <c r="C5" s="18" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="D5" s="18"/>
       <c r="E5" s="18"/>
@@ -13909,13 +14034,13 @@
     </row>
     <row r="7" ht="87" customHeight="1" spans="2:5">
       <c r="B7" s="49" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="C7" s="50" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="D7" s="51" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="E7" s="53"/>
     </row>
@@ -13923,7 +14048,7 @@
       <c r="B8" s="49"/>
       <c r="C8" s="50"/>
       <c r="D8" s="51" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="E8" s="53"/>
     </row>
@@ -13931,36 +14056,36 @@
       <c r="B9" s="49"/>
       <c r="C9" s="50"/>
       <c r="D9" s="51" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="E9" s="53"/>
     </row>
     <row r="10" ht="66" customHeight="1" spans="2:5">
       <c r="B10" s="49"/>
       <c r="C10" s="50" t="s">
-        <v>82</v>
+        <v>91</v>
       </c>
       <c r="D10" s="52" t="s">
-        <v>83</v>
+        <v>92</v>
       </c>
       <c r="E10" s="53" t="s">
-        <v>84</v>
+        <v>93</v>
       </c>
     </row>
     <row r="11" ht="66" customHeight="1" spans="2:5">
       <c r="B11" s="49"/>
       <c r="C11" s="50"/>
       <c r="D11" s="18" t="s">
-        <v>85</v>
+        <v>94</v>
       </c>
       <c r="E11" s="53" t="s">
-        <v>86</v>
+        <v>95</v>
       </c>
     </row>
     <row r="12" ht="32" customHeight="1" spans="2:5">
       <c r="B12" s="49"/>
       <c r="C12" s="19" t="s">
-        <v>87</v>
+        <v>96</v>
       </c>
       <c r="D12" s="18"/>
       <c r="E12" s="18"/>
@@ -13968,29 +14093,29 @@
     <row r="13" ht="68" customHeight="1" spans="2:5">
       <c r="B13" s="49"/>
       <c r="C13" s="37" t="s">
-        <v>88</v>
+        <v>97</v>
       </c>
       <c r="D13" s="8"/>
       <c r="E13" s="18" t="s">
-        <v>89</v>
+        <v>98</v>
       </c>
     </row>
     <row r="14" ht="90" customHeight="1" spans="2:5">
       <c r="B14" s="49"/>
       <c r="C14" s="37" t="s">
-        <v>90</v>
+        <v>99</v>
       </c>
       <c r="D14" s="37"/>
       <c r="E14" s="55" t="s">
-        <v>91</v>
+        <v>100</v>
       </c>
     </row>
     <row r="15" ht="137" customHeight="1" spans="2:5">
       <c r="B15" s="49" t="s">
-        <v>92</v>
+        <v>101</v>
       </c>
       <c r="C15" s="53" t="s">
-        <v>93</v>
+        <v>102</v>
       </c>
       <c r="D15" s="53"/>
       <c r="E15" s="53"/>
@@ -13998,20 +14123,20 @@
     <row r="16" ht="137" customHeight="1" spans="2:5">
       <c r="B16" s="49"/>
       <c r="C16" s="37" t="s">
-        <v>94</v>
+        <v>103</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>95</v>
+        <v>104</v>
       </c>
       <c r="E16" s="18"/>
     </row>
     <row r="17" ht="35" customHeight="1" spans="2:5">
       <c r="B17" s="49"/>
       <c r="C17" s="37" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>96</v>
+        <v>105</v>
       </c>
       <c r="E17" s="18"/>
     </row>
@@ -14019,7 +14144,7 @@
       <c r="B18" s="49"/>
       <c r="C18" s="37"/>
       <c r="D18" s="18" t="s">
-        <v>97</v>
+        <v>106</v>
       </c>
       <c r="E18" s="18"/>
     </row>
@@ -14027,7 +14152,7 @@
       <c r="B19" s="49"/>
       <c r="C19" s="37"/>
       <c r="D19" s="18" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="E19" s="18"/>
     </row>
@@ -14035,23 +14160,23 @@
       <c r="B20" s="49"/>
       <c r="C20" s="37"/>
       <c r="D20" s="18" t="s">
-        <v>99</v>
+        <v>108</v>
       </c>
       <c r="E20" s="18"/>
     </row>
     <row r="21" ht="90" customHeight="1" spans="2:5">
       <c r="B21" s="49"/>
       <c r="C21" s="37" t="s">
-        <v>100</v>
+        <v>109</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>101</v>
+        <v>110</v>
       </c>
       <c r="E21" s="18"/>
     </row>
     <row r="22" spans="2:2">
       <c r="B22" s="49" t="s">
-        <v>102</v>
+        <v>111</v>
       </c>
     </row>
     <row r="23" spans="2:2">
@@ -14068,72 +14193,72 @@
     </row>
     <row r="27" ht="52.5" spans="2:2">
       <c r="B27" s="46" t="s">
-        <v>103</v>
+        <v>112</v>
       </c>
     </row>
     <row r="28" ht="52.5" spans="2:2">
       <c r="B28" s="46" t="s">
-        <v>104</v>
+        <v>113</v>
       </c>
     </row>
     <row r="29" ht="52.5" spans="2:2">
       <c r="B29" s="46" t="s">
-        <v>105</v>
+        <v>114</v>
       </c>
     </row>
     <row r="30" ht="52.5" spans="2:2">
       <c r="B30" s="46" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
     </row>
     <row r="31" ht="52.5" spans="2:2">
       <c r="B31" s="46" t="s">
-        <v>107</v>
+        <v>116</v>
       </c>
     </row>
     <row r="32" ht="78.75" spans="2:2">
       <c r="B32" s="46" t="s">
-        <v>108</v>
+        <v>117</v>
       </c>
     </row>
     <row r="33" ht="52.5" spans="2:2">
       <c r="B33" s="46" t="s">
-        <v>109</v>
+        <v>118</v>
       </c>
     </row>
     <row r="34" ht="52.5" spans="2:2">
       <c r="B34" s="46" t="s">
-        <v>110</v>
+        <v>119</v>
       </c>
     </row>
     <row r="35" ht="52.5" spans="2:2">
       <c r="B35" s="46" t="s">
-        <v>111</v>
+        <v>120</v>
       </c>
     </row>
     <row r="36" ht="52.5" spans="2:2">
       <c r="B36" s="46" t="s">
-        <v>112</v>
+        <v>121</v>
       </c>
     </row>
     <row r="37" ht="52.5" spans="2:2">
       <c r="B37" s="46" t="s">
-        <v>113</v>
+        <v>122</v>
       </c>
     </row>
     <row r="38" ht="12.75" spans="1:1">
       <c r="A38" s="45" t="s">
-        <v>114</v>
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:1">
       <c r="A43" s="45" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
     </row>
     <row r="44" ht="12.75" spans="1:1">
       <c r="A44" s="54" t="s">
-        <v>116</v>
+        <v>125</v>
       </c>
     </row>
     <row r="45" ht="12.75" spans="1:1">
@@ -14199,13 +14324,13 @@
   <sheetData>
     <row r="1" s="13" customFormat="1" ht="12.75" spans="1:4">
       <c r="A1" s="38" t="s">
-        <v>117</v>
+        <v>126</v>
       </c>
       <c r="B1" s="20" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="C1" s="37" t="s">
-        <v>119</v>
+        <v>128</v>
       </c>
       <c r="D1" s="18"/>
     </row>
@@ -14213,79 +14338,79 @@
       <c r="A2" s="39"/>
       <c r="B2" s="20"/>
       <c r="C2" s="37" t="s">
-        <v>120</v>
+        <v>129</v>
       </c>
       <c r="D2" s="18" t="s">
-        <v>121</v>
+        <v>130</v>
       </c>
     </row>
     <row r="3" s="13" customFormat="1" ht="89.25" spans="1:4">
       <c r="A3" s="39"/>
       <c r="B3" s="40" t="s">
-        <v>122</v>
+        <v>131</v>
       </c>
       <c r="C3" s="37" t="s">
-        <v>123</v>
+        <v>132</v>
       </c>
       <c r="D3" s="18" t="s">
-        <v>124</v>
+        <v>133</v>
       </c>
     </row>
     <row r="4" s="13" customFormat="1" ht="76.5" spans="1:4">
       <c r="A4" s="39"/>
       <c r="B4" s="40"/>
       <c r="C4" s="37" t="s">
-        <v>125</v>
+        <v>134</v>
       </c>
       <c r="D4" s="18" t="s">
-        <v>126</v>
+        <v>135</v>
       </c>
     </row>
     <row r="5" s="13" customFormat="1" ht="229.5" spans="1:4">
       <c r="A5" s="39"/>
       <c r="B5" s="40"/>
       <c r="C5" s="37" t="s">
-        <v>127</v>
+        <v>136</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>128</v>
+        <v>137</v>
       </c>
     </row>
     <row r="6" s="13" customFormat="1" ht="63.75" spans="1:4">
       <c r="A6" s="39"/>
       <c r="B6" s="40"/>
       <c r="C6" s="37" t="s">
-        <v>129</v>
+        <v>138</v>
       </c>
       <c r="D6" s="18" t="s">
-        <v>130</v>
+        <v>139</v>
       </c>
     </row>
     <row r="7" s="13" customFormat="1" ht="25.5" spans="1:4">
       <c r="A7" s="39"/>
       <c r="B7" s="40"/>
       <c r="C7" s="37" t="s">
-        <v>131</v>
+        <v>140</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
     </row>
     <row r="8" s="13" customFormat="1" ht="25.5" spans="1:4">
       <c r="A8" s="39"/>
       <c r="B8" s="40"/>
       <c r="C8" s="37" t="s">
-        <v>133</v>
+        <v>142</v>
       </c>
       <c r="D8" s="18" t="s">
-        <v>134</v>
+        <v>143</v>
       </c>
     </row>
     <row r="9" s="13" customFormat="1" ht="12.75" spans="1:4">
       <c r="A9" s="39"/>
       <c r="B9" s="40"/>
       <c r="C9" s="37" t="s">
-        <v>135</v>
+        <v>144</v>
       </c>
       <c r="D9" s="18"/>
     </row>
@@ -14293,17 +14418,17 @@
       <c r="A10" s="39"/>
       <c r="B10" s="40"/>
       <c r="C10" s="37" t="s">
-        <v>136</v>
+        <v>145</v>
       </c>
       <c r="D10" s="18" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" s="13" customFormat="1" ht="12.75" spans="1:4">
       <c r="A11" s="39"/>
       <c r="B11" s="40"/>
       <c r="C11" s="37" t="s">
-        <v>138</v>
+        <v>147</v>
       </c>
       <c r="D11" s="18"/>
     </row>
@@ -14311,16 +14436,16 @@
       <c r="A12" s="39"/>
       <c r="B12" s="40"/>
       <c r="C12" s="37" t="s">
-        <v>139</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" s="13" customFormat="1" ht="107.25" customHeight="1" spans="1:4">
       <c r="A13" s="39"/>
       <c r="B13" s="40" t="s">
-        <v>140</v>
+        <v>149</v>
       </c>
       <c r="C13" s="18" t="s">
-        <v>141</v>
+        <v>150</v>
       </c>
       <c r="D13" s="18"/>
     </row>
@@ -14328,20 +14453,20 @@
       <c r="A14" s="39"/>
       <c r="B14" s="40"/>
       <c r="C14" s="37" t="s">
-        <v>142</v>
+        <v>151</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>143</v>
+        <v>152</v>
       </c>
     </row>
     <row r="15" s="13" customFormat="1" ht="25.5" spans="1:4">
       <c r="A15" s="39"/>
       <c r="B15" s="40"/>
       <c r="C15" s="37" t="s">
-        <v>144</v>
+        <v>153</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>145</v>
+        <v>154</v>
       </c>
     </row>
     <row r="16" s="13" customFormat="1" ht="89.25" spans="1:4">
@@ -14349,7 +14474,7 @@
       <c r="B16" s="40"/>
       <c r="C16" s="37"/>
       <c r="D16" s="18" t="s">
-        <v>146</v>
+        <v>155</v>
       </c>
     </row>
     <row r="17" s="13" customFormat="1" ht="63.75" spans="1:4">
@@ -14357,7 +14482,7 @@
       <c r="B17" s="40"/>
       <c r="C17" s="37"/>
       <c r="D17" s="18" t="s">
-        <v>147</v>
+        <v>156</v>
       </c>
     </row>
     <row r="18" s="13" customFormat="1" ht="25.5" spans="1:4">
@@ -14365,7 +14490,7 @@
       <c r="B18" s="40"/>
       <c r="C18" s="37"/>
       <c r="D18" s="18" t="s">
-        <v>148</v>
+        <v>157</v>
       </c>
     </row>
     <row r="19" s="13" customFormat="1" ht="25.5" spans="1:4">
@@ -14373,7 +14498,7 @@
       <c r="B19" s="40"/>
       <c r="C19" s="37"/>
       <c r="D19" s="18" t="s">
-        <v>149</v>
+        <v>158</v>
       </c>
     </row>
     <row r="20" s="13" customFormat="1" ht="38.25" spans="1:4">
@@ -14381,7 +14506,7 @@
       <c r="B20" s="40"/>
       <c r="C20" s="37"/>
       <c r="D20" s="18" t="s">
-        <v>150</v>
+        <v>159</v>
       </c>
     </row>
     <row r="21" s="13" customFormat="1" ht="12.75" spans="1:4">
@@ -14389,17 +14514,17 @@
       <c r="B21" s="40"/>
       <c r="C21" s="37"/>
       <c r="D21" s="18" t="s">
-        <v>151</v>
+        <v>160</v>
       </c>
     </row>
     <row r="22" s="13" customFormat="1" ht="76.5" spans="1:4">
       <c r="A22" s="39"/>
       <c r="B22" s="40"/>
       <c r="C22" s="37" t="s">
-        <v>152</v>
+        <v>161</v>
       </c>
       <c r="D22" s="18" t="s">
-        <v>153</v>
+        <v>162</v>
       </c>
     </row>
     <row r="23" s="13" customFormat="1" ht="76.5" spans="1:4">
@@ -14407,7 +14532,7 @@
       <c r="B23" s="40"/>
       <c r="C23" s="37"/>
       <c r="D23" s="18" t="s">
-        <v>154</v>
+        <v>163</v>
       </c>
     </row>
     <row r="24" s="13" customFormat="1" ht="89.25" spans="1:4">
@@ -14415,7 +14540,7 @@
       <c r="B24" s="40"/>
       <c r="C24" s="37"/>
       <c r="D24" s="18" t="s">
-        <v>155</v>
+        <v>164</v>
       </c>
     </row>
     <row r="25" s="13" customFormat="1" ht="63.75" spans="1:4">
@@ -14423,7 +14548,7 @@
       <c r="B25" s="40"/>
       <c r="C25" s="37"/>
       <c r="D25" s="18" t="s">
-        <v>156</v>
+        <v>165</v>
       </c>
     </row>
     <row r="26" s="13" customFormat="1" ht="89.25" spans="1:4">
@@ -14431,7 +14556,7 @@
       <c r="B26" s="40"/>
       <c r="C26" s="37"/>
       <c r="D26" s="18" t="s">
-        <v>157</v>
+        <v>166</v>
       </c>
     </row>
     <row r="27" s="13" customFormat="1" ht="165.75" spans="1:4">
@@ -14439,7 +14564,7 @@
       <c r="B27" s="40"/>
       <c r="C27" s="37"/>
       <c r="D27" s="18" t="s">
-        <v>158</v>
+        <v>167</v>
       </c>
     </row>
     <row r="28" s="13" customFormat="1" ht="89.25" spans="1:4">
@@ -14447,7 +14572,7 @@
       <c r="B28" s="40"/>
       <c r="C28" s="37"/>
       <c r="D28" s="18" t="s">
-        <v>159</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" s="13" customFormat="1" ht="153" spans="1:4">
@@ -14455,7 +14580,7 @@
       <c r="B29" s="40"/>
       <c r="C29" s="37"/>
       <c r="D29" s="18" t="s">
-        <v>160</v>
+        <v>169</v>
       </c>
     </row>
     <row r="30" s="13" customFormat="1" ht="89.25" spans="1:4">
@@ -14463,7 +14588,7 @@
       <c r="B30" s="40"/>
       <c r="C30" s="37"/>
       <c r="D30" s="18" t="s">
-        <v>161</v>
+        <v>170</v>
       </c>
     </row>
     <row r="31" s="13" customFormat="1" ht="140.25" spans="1:4">
@@ -14471,7 +14596,7 @@
       <c r="B31" s="40"/>
       <c r="C31" s="37"/>
       <c r="D31" s="18" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
     </row>
     <row r="32" s="13" customFormat="1" ht="89.25" spans="1:4">
@@ -14479,7 +14604,7 @@
       <c r="B32" s="40"/>
       <c r="C32" s="37"/>
       <c r="D32" s="18" t="s">
-        <v>163</v>
+        <v>172</v>
       </c>
     </row>
     <row r="33" s="13" customFormat="1" ht="12.75" spans="1:4">
@@ -14487,7 +14612,7 @@
       <c r="B33" s="40"/>
       <c r="C33" s="37"/>
       <c r="D33" s="18" t="s">
-        <v>164</v>
+        <v>173</v>
       </c>
     </row>
     <row r="34" s="13" customFormat="1" ht="89.25" spans="1:4">
@@ -14495,7 +14620,7 @@
       <c r="B34" s="40"/>
       <c r="C34" s="37"/>
       <c r="D34" s="27" t="s">
-        <v>165</v>
+        <v>174</v>
       </c>
     </row>
     <row r="35" s="13" customFormat="1" ht="369.75" spans="1:4">
@@ -14503,7 +14628,7 @@
       <c r="B35" s="40"/>
       <c r="C35" s="37"/>
       <c r="D35" s="18" t="s">
-        <v>166</v>
+        <v>175</v>
       </c>
     </row>
     <row r="36" s="13" customFormat="1" ht="357" spans="1:4">
@@ -14511,7 +14636,7 @@
       <c r="B36" s="40"/>
       <c r="C36" s="37"/>
       <c r="D36" s="18" t="s">
-        <v>167</v>
+        <v>176</v>
       </c>
     </row>
     <row r="37" s="13" customFormat="1" ht="38.25" spans="1:4">
@@ -14519,7 +14644,7 @@
       <c r="B37" s="40"/>
       <c r="C37" s="37"/>
       <c r="D37" s="18" t="s">
-        <v>168</v>
+        <v>177</v>
       </c>
     </row>
     <row r="38" s="13" customFormat="1" ht="12.75" spans="1:4">
@@ -14527,7 +14652,7 @@
       <c r="B38" s="40"/>
       <c r="C38" s="37"/>
       <c r="D38" s="18" t="s">
-        <v>169</v>
+        <v>178</v>
       </c>
     </row>
     <row r="39" s="13" customFormat="1" ht="12.75" spans="1:4">
@@ -14535,7 +14660,7 @@
       <c r="B39" s="40"/>
       <c r="C39" s="37"/>
       <c r="D39" s="18" t="s">
-        <v>170</v>
+        <v>179</v>
       </c>
     </row>
     <row r="40" s="13" customFormat="1" ht="12.75" spans="1:4">
@@ -14543,14 +14668,14 @@
       <c r="B40" s="40"/>
       <c r="C40" s="37"/>
       <c r="D40" s="18" t="s">
-        <v>171</v>
+        <v>180</v>
       </c>
     </row>
     <row r="41" s="13" customFormat="1" ht="12.75" spans="1:4">
       <c r="A41" s="39"/>
       <c r="B41" s="40"/>
       <c r="C41" s="37" t="s">
-        <v>172</v>
+        <v>181</v>
       </c>
       <c r="D41" s="18"/>
     </row>
@@ -14558,22 +14683,22 @@
       <c r="A42" s="39"/>
       <c r="B42" s="40"/>
       <c r="C42" s="37" t="s">
-        <v>173</v>
+        <v>182</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>174</v>
+        <v>183</v>
       </c>
     </row>
     <row r="43" s="13" customFormat="1" ht="114.75" spans="1:4">
       <c r="A43" s="39"/>
       <c r="B43" s="20" t="s">
-        <v>175</v>
+        <v>184</v>
       </c>
       <c r="C43" s="40" t="s">
-        <v>176</v>
+        <v>185</v>
       </c>
       <c r="D43" s="18" t="s">
-        <v>177</v>
+        <v>186</v>
       </c>
     </row>
     <row r="44" s="13" customFormat="1" ht="395.25" spans="1:4">
@@ -14581,7 +14706,7 @@
       <c r="B44" s="20"/>
       <c r="C44" s="40"/>
       <c r="D44" s="18" t="s">
-        <v>178</v>
+        <v>187</v>
       </c>
     </row>
     <row r="45" s="13" customFormat="1" ht="409.5" spans="1:4">
@@ -14589,7 +14714,7 @@
       <c r="B45" s="20"/>
       <c r="C45" s="40"/>
       <c r="D45" s="18" t="s">
-        <v>179</v>
+        <v>188</v>
       </c>
     </row>
     <row r="46" s="13" customFormat="1" ht="12.75" spans="1:4">
@@ -14597,7 +14722,7 @@
       <c r="B46" s="20"/>
       <c r="C46" s="40"/>
       <c r="D46" s="18" t="s">
-        <v>180</v>
+        <v>189</v>
       </c>
     </row>
     <row r="47" s="13" customFormat="1" ht="12.75" spans="1:4">
@@ -14605,7 +14730,7 @@
       <c r="B47" s="20"/>
       <c r="C47" s="40"/>
       <c r="D47" s="18" t="s">
-        <v>181</v>
+        <v>190</v>
       </c>
     </row>
     <row r="48" s="13" customFormat="1" ht="12.75" spans="1:4">
@@ -14613,7 +14738,7 @@
       <c r="B48" s="20"/>
       <c r="C48" s="40"/>
       <c r="D48" s="18" t="s">
-        <v>182</v>
+        <v>191</v>
       </c>
     </row>
     <row r="49" s="13" customFormat="1" ht="12.75" spans="1:4">
@@ -14621,7 +14746,7 @@
       <c r="B49" s="20"/>
       <c r="C49" s="40"/>
       <c r="D49" s="18" t="s">
-        <v>183</v>
+        <v>192</v>
       </c>
     </row>
     <row r="50" s="13" customFormat="1" ht="12.75" spans="1:4">
@@ -14629,17 +14754,17 @@
       <c r="B50" s="20"/>
       <c r="C50" s="40"/>
       <c r="D50" s="18" t="s">
-        <v>184</v>
+        <v>193</v>
       </c>
     </row>
     <row r="51" s="13" customFormat="1" ht="12.75" spans="1:4">
       <c r="A51" s="39"/>
       <c r="B51" s="20"/>
       <c r="C51" s="8" t="s">
-        <v>185</v>
+        <v>194</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>186</v>
+        <v>195</v>
       </c>
     </row>
     <row r="52" s="13" customFormat="1" ht="25.5" spans="1:4">
@@ -14647,7 +14772,7 @@
       <c r="B52" s="20"/>
       <c r="C52" s="8"/>
       <c r="D52" s="18" t="s">
-        <v>187</v>
+        <v>196</v>
       </c>
     </row>
     <row r="53" s="13" customFormat="1" ht="12.75" spans="1:4">
@@ -14655,7 +14780,7 @@
       <c r="B53" s="20"/>
       <c r="C53" s="8"/>
       <c r="D53" s="18" t="s">
-        <v>188</v>
+        <v>197</v>
       </c>
     </row>
     <row r="54" s="13" customFormat="1" ht="12.75" spans="1:4">
@@ -14663,7 +14788,7 @@
       <c r="B54" s="20"/>
       <c r="C54" s="8"/>
       <c r="D54" s="18" t="s">
-        <v>189</v>
+        <v>198</v>
       </c>
     </row>
     <row r="55" s="13" customFormat="1" ht="12.75" spans="1:4">
@@ -14671,14 +14796,14 @@
       <c r="B55" s="20"/>
       <c r="C55" s="8"/>
       <c r="D55" s="18" t="s">
-        <v>190</v>
+        <v>199</v>
       </c>
     </row>
     <row r="56" s="13" customFormat="1" ht="25.5" spans="1:4">
       <c r="A56" s="39"/>
       <c r="B56" s="20"/>
       <c r="C56" s="37" t="s">
-        <v>191</v>
+        <v>200</v>
       </c>
       <c r="D56" s="18"/>
     </row>
@@ -14686,10 +14811,10 @@
       <c r="A57" s="39"/>
       <c r="B57" s="20"/>
       <c r="C57" s="40" t="s">
-        <v>192</v>
+        <v>201</v>
       </c>
       <c r="D57" s="27" t="s">
-        <v>193</v>
+        <v>202</v>
       </c>
     </row>
     <row r="58" s="13" customFormat="1" ht="51" spans="1:4">
@@ -14697,7 +14822,7 @@
       <c r="B58" s="20"/>
       <c r="C58" s="40"/>
       <c r="D58" s="18" t="s">
-        <v>194</v>
+        <v>203</v>
       </c>
     </row>
     <row r="59" s="13" customFormat="1" ht="12.75" spans="1:4">
@@ -14705,7 +14830,7 @@
       <c r="B59" s="20"/>
       <c r="C59" s="40"/>
       <c r="D59" s="18" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
     </row>
     <row r="60" s="13" customFormat="1" ht="12.75" spans="1:4">
@@ -14713,17 +14838,17 @@
       <c r="B60" s="20"/>
       <c r="C60" s="40"/>
       <c r="D60" s="18" t="s">
-        <v>196</v>
+        <v>205</v>
       </c>
     </row>
     <row r="61" s="13" customFormat="1" ht="12.75" spans="1:4">
       <c r="A61" s="39"/>
       <c r="B61" s="20"/>
       <c r="C61" s="37" t="s">
-        <v>197</v>
+        <v>206</v>
       </c>
       <c r="D61" s="18" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
     </row>
     <row r="62" s="13" customFormat="1" ht="12.75" spans="1:4">
@@ -14731,7 +14856,7 @@
       <c r="B62" s="20"/>
       <c r="C62" s="37"/>
       <c r="D62" s="18" t="s">
-        <v>199</v>
+        <v>208</v>
       </c>
     </row>
     <row r="63" s="13" customFormat="1" ht="12.75" spans="1:4">
@@ -14739,7 +14864,7 @@
       <c r="B63" s="20"/>
       <c r="C63" s="37"/>
       <c r="D63" s="18" t="s">
-        <v>200</v>
+        <v>209</v>
       </c>
     </row>
     <row r="64" s="13" customFormat="1" ht="12.75" spans="1:4">
@@ -14747,7 +14872,7 @@
       <c r="B64" s="20"/>
       <c r="C64" s="37"/>
       <c r="D64" s="18" t="s">
-        <v>201</v>
+        <v>210</v>
       </c>
     </row>
     <row r="65" s="13" customFormat="1" ht="12.75" spans="1:4">
@@ -14755,7 +14880,7 @@
       <c r="B65" s="20"/>
       <c r="C65" s="37"/>
       <c r="D65" s="18" t="s">
-        <v>202</v>
+        <v>211</v>
       </c>
     </row>
     <row r="66" s="13" customFormat="1" ht="12.75" spans="1:4">
@@ -14763,17 +14888,17 @@
       <c r="B66" s="20"/>
       <c r="C66" s="37"/>
       <c r="D66" s="18" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
     </row>
     <row r="67" s="13" customFormat="1" ht="38.25" spans="1:4">
       <c r="A67" s="39"/>
       <c r="B67" s="20"/>
       <c r="C67" s="37" t="s">
-        <v>203</v>
+        <v>212</v>
       </c>
       <c r="D67" s="18" t="s">
-        <v>204</v>
+        <v>213</v>
       </c>
     </row>
     <row r="68" s="13" customFormat="1" ht="51" spans="1:4">
@@ -14781,7 +14906,7 @@
       <c r="B68" s="20"/>
       <c r="C68" s="37"/>
       <c r="D68" s="18" t="s">
-        <v>205</v>
+        <v>214</v>
       </c>
     </row>
     <row r="69" s="13" customFormat="1" ht="51" spans="1:4">
@@ -14789,7 +14914,7 @@
       <c r="B69" s="20"/>
       <c r="C69" s="37"/>
       <c r="D69" s="18" t="s">
-        <v>206</v>
+        <v>215</v>
       </c>
     </row>
     <row r="70" s="13" customFormat="1" ht="63.75" spans="1:4">
@@ -14797,7 +14922,7 @@
       <c r="B70" s="20"/>
       <c r="C70" s="37"/>
       <c r="D70" s="18" t="s">
-        <v>207</v>
+        <v>216</v>
       </c>
     </row>
     <row r="71" s="13" customFormat="1" ht="63.75" spans="1:4">
@@ -14805,7 +14930,7 @@
       <c r="B71" s="20"/>
       <c r="C71" s="37"/>
       <c r="D71" s="18" t="s">
-        <v>208</v>
+        <v>217</v>
       </c>
     </row>
     <row r="72" s="13" customFormat="1" ht="51" spans="1:4">
@@ -14813,7 +14938,7 @@
       <c r="B72" s="20"/>
       <c r="C72" s="37"/>
       <c r="D72" s="18" t="s">
-        <v>209</v>
+        <v>218</v>
       </c>
     </row>
     <row r="73" s="13" customFormat="1" ht="51" spans="1:4">
@@ -14821,7 +14946,7 @@
       <c r="B73" s="20"/>
       <c r="C73" s="37"/>
       <c r="D73" s="18" t="s">
-        <v>210</v>
+        <v>219</v>
       </c>
     </row>
     <row r="74" s="13" customFormat="1" ht="63.75" spans="1:4">
@@ -14829,7 +14954,7 @@
       <c r="B74" s="20"/>
       <c r="C74" s="37"/>
       <c r="D74" s="18" t="s">
-        <v>211</v>
+        <v>220</v>
       </c>
     </row>
     <row r="75" s="13" customFormat="1" ht="63.75" spans="1:4">
@@ -14837,7 +14962,7 @@
       <c r="B75" s="20"/>
       <c r="C75" s="37"/>
       <c r="D75" s="18" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
     </row>
     <row r="76" s="13" customFormat="1" ht="51" spans="1:4">
@@ -14845,7 +14970,7 @@
       <c r="B76" s="20"/>
       <c r="C76" s="37"/>
       <c r="D76" s="18" t="s">
-        <v>213</v>
+        <v>222</v>
       </c>
     </row>
     <row r="77" s="13" customFormat="1" ht="153" spans="1:4">
@@ -14853,7 +14978,7 @@
       <c r="B77" s="20"/>
       <c r="C77" s="37"/>
       <c r="D77" s="18" t="s">
-        <v>214</v>
+        <v>223</v>
       </c>
     </row>
     <row r="78" s="13" customFormat="1" ht="38.25" spans="1:4">
@@ -14861,27 +14986,27 @@
       <c r="B78" s="20"/>
       <c r="C78" s="37"/>
       <c r="D78" s="18" t="s">
-        <v>215</v>
+        <v>224</v>
       </c>
     </row>
     <row r="79" s="13" customFormat="1" ht="114.75" spans="1:4">
       <c r="A79" s="39"/>
       <c r="B79" s="20"/>
       <c r="C79" s="37" t="s">
-        <v>216</v>
+        <v>225</v>
       </c>
       <c r="D79" s="18" t="s">
-        <v>217</v>
+        <v>226</v>
       </c>
     </row>
     <row r="80" s="13" customFormat="1" ht="38.25" spans="1:4">
       <c r="A80" s="39"/>
       <c r="B80" s="20"/>
       <c r="C80" s="8" t="s">
-        <v>218</v>
+        <v>227</v>
       </c>
       <c r="D80" s="18" t="s">
-        <v>219</v>
+        <v>228</v>
       </c>
     </row>
     <row r="81" s="13" customFormat="1" ht="165.75" spans="1:4">
@@ -14889,7 +15014,7 @@
       <c r="B81" s="20"/>
       <c r="C81" s="8"/>
       <c r="D81" s="27" t="s">
-        <v>220</v>
+        <v>229</v>
       </c>
     </row>
     <row r="82" s="13" customFormat="1" ht="102" spans="1:4">
@@ -14897,7 +15022,7 @@
       <c r="B82" s="20"/>
       <c r="C82" s="8"/>
       <c r="D82" s="27" t="s">
-        <v>221</v>
+        <v>230</v>
       </c>
     </row>
     <row r="83" s="13" customFormat="1" ht="51" spans="1:4">
@@ -14905,23 +15030,23 @@
       <c r="B83" s="20"/>
       <c r="C83" s="8"/>
       <c r="D83" s="27" t="s">
-        <v>222</v>
+        <v>231</v>
       </c>
     </row>
     <row r="84" s="13" customFormat="1" ht="12.75" spans="1:4">
       <c r="A84" s="39"/>
       <c r="B84" s="20"/>
       <c r="C84" s="40" t="s">
-        <v>223</v>
+        <v>232</v>
       </c>
       <c r="D84" s="27" t="s">
-        <v>224</v>
+        <v>233</v>
       </c>
     </row>
     <row r="85" s="13" customFormat="1" ht="38.25" spans="1:4">
       <c r="A85" s="39"/>
       <c r="B85" s="20" t="s">
-        <v>225</v>
+        <v>234</v>
       </c>
       <c r="C85" s="40"/>
       <c r="D85" s="27"/>
@@ -14929,7 +15054,7 @@
     <row r="86" s="13" customFormat="1" ht="25.5" spans="1:4">
       <c r="A86" s="39"/>
       <c r="B86" s="20" t="s">
-        <v>226</v>
+        <v>235</v>
       </c>
       <c r="C86" s="40"/>
       <c r="D86" s="27"/>
@@ -14937,7 +15062,7 @@
     <row r="87" s="13" customFormat="1" ht="51" spans="1:4">
       <c r="A87" s="39"/>
       <c r="B87" s="20" t="s">
-        <v>227</v>
+        <v>236</v>
       </c>
       <c r="C87" s="40"/>
       <c r="D87" s="27"/>
@@ -14945,7 +15070,7 @@
     <row r="88" s="13" customFormat="1" ht="25.5" spans="1:4">
       <c r="A88" s="39"/>
       <c r="B88" s="20" t="s">
-        <v>228</v>
+        <v>237</v>
       </c>
       <c r="C88" s="40"/>
       <c r="D88" s="27"/>
@@ -14953,7 +15078,7 @@
     <row r="89" s="13" customFormat="1" ht="25.5" spans="1:4">
       <c r="A89" s="39"/>
       <c r="B89" s="20" t="s">
-        <v>229</v>
+        <v>238</v>
       </c>
       <c r="C89" s="40"/>
       <c r="D89" s="27"/>
@@ -14961,7 +15086,7 @@
     <row r="90" s="13" customFormat="1" ht="38.25" spans="1:4">
       <c r="A90" s="39"/>
       <c r="B90" s="20" t="s">
-        <v>230</v>
+        <v>239</v>
       </c>
       <c r="C90" s="40"/>
       <c r="D90" s="27"/>
@@ -14969,7 +15094,7 @@
     <row r="91" s="13" customFormat="1" ht="38.25" spans="1:4">
       <c r="A91" s="39"/>
       <c r="B91" s="20" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="C91" s="40"/>
       <c r="D91" s="27"/>
@@ -14977,7 +15102,7 @@
     <row r="92" s="13" customFormat="1" ht="38.25" spans="1:4">
       <c r="A92" s="39"/>
       <c r="B92" s="20" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="C92" s="40"/>
       <c r="D92" s="27"/>
@@ -14985,7 +15110,7 @@
     <row r="93" s="13" customFormat="1" ht="38.25" spans="1:4">
       <c r="A93" s="39"/>
       <c r="B93" s="41" t="s">
-        <v>233</v>
+        <v>242</v>
       </c>
       <c r="C93" s="40"/>
       <c r="D93" s="27"/>
@@ -14993,7 +15118,7 @@
     <row r="94" s="13" customFormat="1" ht="38.25" spans="1:4">
       <c r="A94" s="39"/>
       <c r="B94" s="20" t="s">
-        <v>234</v>
+        <v>243</v>
       </c>
       <c r="C94" s="40"/>
       <c r="D94" s="27"/>
@@ -15001,7 +15126,7 @@
     <row r="95" s="13" customFormat="1" ht="51" spans="1:4">
       <c r="A95" s="39"/>
       <c r="B95" s="41" t="s">
-        <v>235</v>
+        <v>244</v>
       </c>
       <c r="C95" s="40"/>
       <c r="D95" s="27"/>
@@ -15009,7 +15134,7 @@
     <row r="96" s="13" customFormat="1" ht="38.25" spans="1:4">
       <c r="A96" s="39"/>
       <c r="B96" s="41" t="s">
-        <v>236</v>
+        <v>245</v>
       </c>
       <c r="C96" s="40"/>
       <c r="D96" s="27"/>
@@ -15017,7 +15142,7 @@
     <row r="97" s="13" customFormat="1" ht="38.25" spans="1:4">
       <c r="A97" s="39"/>
       <c r="B97" s="41" t="s">
-        <v>237</v>
+        <v>246</v>
       </c>
       <c r="C97" s="40"/>
       <c r="D97" s="27"/>
@@ -15025,7 +15150,7 @@
     <row r="98" s="13" customFormat="1" ht="38.25" spans="1:4">
       <c r="A98" s="39"/>
       <c r="B98" s="41" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="C98" s="40"/>
       <c r="D98" s="27"/>
@@ -15033,7 +15158,7 @@
     <row r="99" s="13" customFormat="1" ht="38.25" spans="1:4">
       <c r="A99" s="39"/>
       <c r="B99" s="41" t="s">
-        <v>239</v>
+        <v>248</v>
       </c>
       <c r="C99" s="40"/>
       <c r="D99" s="27"/>
@@ -15041,7 +15166,7 @@
     <row r="100" s="13" customFormat="1" ht="25.5" spans="1:4">
       <c r="A100" s="39"/>
       <c r="B100" s="20" t="s">
-        <v>240</v>
+        <v>249</v>
       </c>
       <c r="C100" s="40"/>
       <c r="D100" s="27"/>
@@ -15049,7 +15174,7 @@
     <row r="101" s="13" customFormat="1" ht="51" spans="1:4">
       <c r="A101" s="39"/>
       <c r="B101" s="20" t="s">
-        <v>241</v>
+        <v>250</v>
       </c>
       <c r="C101" s="40"/>
       <c r="D101" s="27"/>
@@ -15057,7 +15182,7 @@
     <row r="102" s="13" customFormat="1" ht="38.25" spans="1:4">
       <c r="A102" s="39"/>
       <c r="B102" s="41" t="s">
-        <v>242</v>
+        <v>251</v>
       </c>
       <c r="C102" s="40"/>
       <c r="D102" s="27"/>
@@ -15065,7 +15190,7 @@
     <row r="103" s="13" customFormat="1" ht="25.5" spans="1:4">
       <c r="A103" s="39"/>
       <c r="B103" s="20" t="s">
-        <v>243</v>
+        <v>252</v>
       </c>
       <c r="C103" s="40"/>
       <c r="D103" s="27"/>
@@ -15073,7 +15198,7 @@
     <row r="104" s="13" customFormat="1" ht="38.25" spans="1:4">
       <c r="A104" s="39"/>
       <c r="B104" s="20" t="s">
-        <v>244</v>
+        <v>253</v>
       </c>
       <c r="C104" s="40"/>
       <c r="D104" s="27"/>
@@ -15081,33 +15206,33 @@
     <row r="105" s="13" customFormat="1" ht="153" spans="1:4">
       <c r="A105" s="39"/>
       <c r="B105" s="42" t="s">
-        <v>245</v>
+        <v>254</v>
       </c>
       <c r="C105" s="37" t="s">
-        <v>246</v>
+        <v>255</v>
       </c>
       <c r="D105" s="18" t="s">
-        <v>247</v>
+        <v>256</v>
       </c>
     </row>
     <row r="106" s="13" customFormat="1" ht="51" spans="1:4">
       <c r="A106" s="39"/>
       <c r="B106" s="42"/>
       <c r="C106" s="37" t="s">
-        <v>248</v>
+        <v>257</v>
       </c>
       <c r="D106" s="18" t="s">
-        <v>249</v>
+        <v>258</v>
       </c>
     </row>
     <row r="107" s="13" customFormat="1" ht="306" spans="1:4">
       <c r="A107" s="39"/>
       <c r="B107" s="42"/>
       <c r="C107" s="37" t="s">
-        <v>250</v>
+        <v>259</v>
       </c>
       <c r="D107" s="27" t="s">
-        <v>251</v>
+        <v>260</v>
       </c>
     </row>
     <row r="108" s="13" customFormat="1" ht="229.5" spans="1:4">
@@ -15115,27 +15240,27 @@
       <c r="B108" s="42"/>
       <c r="C108" s="37"/>
       <c r="D108" s="27" t="s">
-        <v>252</v>
+        <v>261</v>
       </c>
     </row>
     <row r="109" s="13" customFormat="1" ht="242.25" spans="1:4">
       <c r="A109" s="39"/>
       <c r="B109" s="42"/>
       <c r="C109" s="37" t="s">
-        <v>253</v>
+        <v>262</v>
       </c>
       <c r="D109" s="27" t="s">
-        <v>254</v>
+        <v>263</v>
       </c>
     </row>
     <row r="110" s="13" customFormat="1" ht="216.75" spans="1:4">
       <c r="A110" s="39"/>
       <c r="B110" s="42"/>
       <c r="C110" s="37" t="s">
-        <v>255</v>
+        <v>264</v>
       </c>
       <c r="D110" s="27" t="s">
-        <v>256</v>
+        <v>265</v>
       </c>
     </row>
     <row r="111" s="13" customFormat="1" ht="369.75" spans="1:4">
@@ -15143,47 +15268,47 @@
       <c r="B111" s="42"/>
       <c r="C111" s="37"/>
       <c r="D111" s="27" t="s">
-        <v>257</v>
+        <v>266</v>
       </c>
     </row>
     <row r="112" s="13" customFormat="1" ht="382.5" spans="1:4">
       <c r="A112" s="39"/>
       <c r="B112" s="42"/>
       <c r="C112" s="37" t="s">
-        <v>258</v>
+        <v>267</v>
       </c>
       <c r="D112" s="27" t="s">
-        <v>259</v>
+        <v>268</v>
       </c>
     </row>
     <row r="113" s="13" customFormat="1" ht="255" spans="1:4">
       <c r="A113" s="39"/>
       <c r="B113" s="43"/>
       <c r="C113" s="37" t="s">
-        <v>260</v>
+        <v>269</v>
       </c>
       <c r="D113" s="18" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
     </row>
     <row r="114" s="13" customFormat="1" ht="165.75" spans="1:4">
       <c r="A114" s="39"/>
       <c r="B114" s="43"/>
       <c r="C114" s="37" t="s">
-        <v>262</v>
+        <v>271</v>
       </c>
       <c r="D114" s="18" t="s">
-        <v>263</v>
+        <v>272</v>
       </c>
     </row>
     <row r="115" s="13" customFormat="1" ht="89.25" spans="1:4">
       <c r="A115" s="39"/>
       <c r="B115" s="43"/>
       <c r="C115" s="37" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="D115" s="18" t="s">
-        <v>265</v>
+        <v>274</v>
       </c>
     </row>
     <row r="116" s="13" customFormat="1" ht="89.25" spans="1:4">
@@ -15191,26 +15316,26 @@
       <c r="B116" s="43"/>
       <c r="C116" s="37"/>
       <c r="D116" s="18" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
     </row>
     <row r="117" s="13" customFormat="1" ht="63.75" spans="1:4">
       <c r="A117" s="39"/>
       <c r="B117" s="43"/>
       <c r="C117" s="37" t="s">
-        <v>267</v>
+        <v>276</v>
       </c>
       <c r="D117" s="18" t="s">
-        <v>268</v>
+        <v>277</v>
       </c>
     </row>
     <row r="118" s="13" customFormat="1" ht="274.5" customHeight="1" spans="1:4">
       <c r="A118" s="39"/>
       <c r="B118" s="37" t="s">
-        <v>269</v>
+        <v>278</v>
       </c>
       <c r="C118" s="18" t="s">
-        <v>270</v>
+        <v>279</v>
       </c>
       <c r="D118" s="18"/>
     </row>
@@ -15218,17 +15343,17 @@
       <c r="A119" s="39"/>
       <c r="B119" s="37"/>
       <c r="C119" s="18" t="s">
-        <v>271</v>
+        <v>280</v>
       </c>
       <c r="D119" s="18"/>
     </row>
     <row r="120" s="13" customFormat="1" ht="391.5" customHeight="1" spans="1:4">
       <c r="A120" s="39"/>
       <c r="B120" s="37" t="s">
-        <v>272</v>
+        <v>281</v>
       </c>
       <c r="C120" s="18" t="s">
-        <v>273</v>
+        <v>282</v>
       </c>
       <c r="D120" s="18"/>
     </row>
@@ -15236,91 +15361,91 @@
       <c r="A121" s="39"/>
       <c r="B121" s="37"/>
       <c r="C121" s="18" t="s">
-        <v>274</v>
+        <v>283</v>
       </c>
       <c r="D121" s="18"/>
     </row>
     <row r="122" s="13" customFormat="1" ht="45" customHeight="1" spans="1:4">
       <c r="A122" s="44" t="s">
-        <v>275</v>
+        <v>284</v>
       </c>
       <c r="B122" s="37" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="C122" s="18" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="D122" s="18"/>
     </row>
     <row r="123" s="13" customFormat="1" ht="12.75" spans="1:4">
       <c r="A123" s="39"/>
       <c r="B123" s="37" t="s">
-        <v>278</v>
+        <v>287</v>
       </c>
       <c r="C123" s="37" t="s">
-        <v>279</v>
+        <v>288</v>
       </c>
       <c r="D123" s="18" t="s">
-        <v>280</v>
+        <v>289</v>
       </c>
     </row>
     <row r="124" s="13" customFormat="1" ht="12.75" spans="1:4">
       <c r="A124" s="39"/>
       <c r="B124" s="37"/>
       <c r="C124" s="37" t="s">
-        <v>281</v>
+        <v>290</v>
       </c>
       <c r="D124" s="18" t="s">
-        <v>282</v>
+        <v>291</v>
       </c>
     </row>
     <row r="125" s="13" customFormat="1" ht="25.5" spans="1:4">
       <c r="A125" s="39"/>
       <c r="B125" s="37"/>
       <c r="C125" s="37" t="s">
-        <v>283</v>
+        <v>292</v>
       </c>
       <c r="D125" s="18" t="s">
-        <v>284</v>
+        <v>293</v>
       </c>
     </row>
     <row r="126" s="13" customFormat="1" ht="25.5" spans="1:4">
       <c r="A126" s="39"/>
       <c r="B126" s="37"/>
       <c r="C126" s="37" t="s">
-        <v>285</v>
+        <v>294</v>
       </c>
       <c r="D126" s="18" t="s">
-        <v>286</v>
+        <v>295</v>
       </c>
     </row>
     <row r="127" s="13" customFormat="1" ht="51" spans="1:4">
       <c r="A127" s="39"/>
       <c r="B127" s="37" t="s">
-        <v>287</v>
+        <v>296</v>
       </c>
       <c r="C127" s="37" t="s">
-        <v>288</v>
+        <v>297</v>
       </c>
       <c r="D127" s="18" t="s">
-        <v>289</v>
+        <v>298</v>
       </c>
     </row>
     <row r="128" s="13" customFormat="1" ht="51" spans="1:4">
       <c r="A128" s="39"/>
       <c r="B128" s="37"/>
       <c r="C128" s="37" t="s">
-        <v>290</v>
+        <v>299</v>
       </c>
       <c r="D128" s="18" t="s">
-        <v>291</v>
+        <v>300</v>
       </c>
     </row>
     <row r="129" s="13" customFormat="1" ht="25.5" spans="1:4">
       <c r="A129" s="39"/>
       <c r="B129" s="37"/>
       <c r="C129" s="18" t="s">
-        <v>292</v>
+        <v>301</v>
       </c>
       <c r="D129" s="18"/>
     </row>
@@ -15328,7 +15453,7 @@
       <c r="A130" s="39"/>
       <c r="B130" s="37"/>
       <c r="C130" s="18" t="s">
-        <v>293</v>
+        <v>302</v>
       </c>
       <c r="D130" s="18"/>
     </row>
@@ -15336,7 +15461,7 @@
       <c r="A131" s="39"/>
       <c r="B131" s="37"/>
       <c r="C131" s="18" t="s">
-        <v>294</v>
+        <v>303</v>
       </c>
       <c r="D131" s="18"/>
     </row>
@@ -15344,17 +15469,17 @@
       <c r="A132" s="39"/>
       <c r="B132" s="37"/>
       <c r="C132" s="18" t="s">
-        <v>295</v>
+        <v>304</v>
       </c>
       <c r="D132" s="18"/>
     </row>
     <row r="133" s="13" customFormat="1" ht="25.5" spans="1:4">
       <c r="A133" s="39"/>
       <c r="B133" s="37" t="s">
-        <v>296</v>
+        <v>305</v>
       </c>
       <c r="C133" s="18" t="s">
-        <v>297</v>
+        <v>306</v>
       </c>
       <c r="D133" s="18"/>
     </row>
@@ -15362,7 +15487,7 @@
       <c r="A134" s="39"/>
       <c r="B134" s="37"/>
       <c r="C134" s="18" t="s">
-        <v>298</v>
+        <v>307</v>
       </c>
       <c r="D134" s="18"/>
     </row>
@@ -15370,14 +15495,14 @@
       <c r="A135" s="39"/>
       <c r="B135" s="37"/>
       <c r="C135" s="18" t="s">
-        <v>299</v>
+        <v>308</v>
       </c>
       <c r="D135" s="18"/>
     </row>
     <row r="136" s="13" customFormat="1" ht="12.75" spans="1:4">
       <c r="A136" s="39"/>
       <c r="B136" s="37" t="s">
-        <v>300</v>
+        <v>309</v>
       </c>
       <c r="C136" s="18"/>
       <c r="D136" s="18"/>
@@ -15470,7 +15595,7 @@
   <sheetData>
     <row r="1" ht="12.75" spans="1:1">
       <c r="A1" s="31" t="s">
-        <v>301</v>
+        <v>310</v>
       </c>
     </row>
     <row r="2" ht="12.75" spans="1:3">
@@ -15568,22 +15693,22 @@
     </row>
     <row r="26" ht="17.25" spans="1:2">
       <c r="A26" s="31" t="s">
-        <v>302</v>
+        <v>311</v>
       </c>
       <c r="B26" s="29" t="s">
-        <v>303</v>
+        <v>312</v>
       </c>
     </row>
     <row r="27" ht="17.25" spans="1:2">
       <c r="A27" s="31"/>
       <c r="B27" s="29" t="s">
-        <v>304</v>
+        <v>313</v>
       </c>
     </row>
     <row r="28" ht="17.25" spans="1:2">
       <c r="A28" s="31"/>
       <c r="B28" s="29" t="s">
-        <v>305</v>
+        <v>314</v>
       </c>
     </row>
     <row r="29" spans="1:1">
@@ -15591,74 +15716,74 @@
     </row>
     <row r="30" ht="12.75" spans="1:3">
       <c r="A30" s="31" t="s">
-        <v>306</v>
+        <v>315</v>
       </c>
       <c r="B30" s="29" t="s">
-        <v>307</v>
+        <v>316</v>
       </c>
       <c r="C30" s="30" t="s">
-        <v>308</v>
+        <v>317</v>
       </c>
     </row>
     <row r="31" ht="12.75" spans="1:3">
       <c r="A31" s="31"/>
       <c r="C31" s="30" t="s">
-        <v>309</v>
+        <v>318</v>
       </c>
     </row>
     <row r="32" ht="12.75" spans="1:3">
       <c r="A32" s="31"/>
       <c r="C32" s="30" t="s">
-        <v>310</v>
+        <v>319</v>
       </c>
     </row>
     <row r="33" ht="12.75" spans="1:3">
       <c r="A33" s="31"/>
       <c r="C33" s="30" t="s">
-        <v>311</v>
+        <v>320</v>
       </c>
     </row>
     <row r="35" ht="114.75" spans="1:3">
       <c r="A35" s="31" t="s">
-        <v>312</v>
+        <v>321</v>
       </c>
       <c r="B35" s="29" t="s">
-        <v>313</v>
-      </c>
-      <c r="C35" s="71" t="s">
-        <v>314</v>
+        <v>322</v>
+      </c>
+      <c r="C35" s="70" t="s">
+        <v>323</v>
       </c>
     </row>
     <row r="36" ht="89.25" spans="1:3">
       <c r="A36" s="31"/>
       <c r="B36" s="29" t="s">
-        <v>315</v>
-      </c>
-      <c r="C36" s="71" t="s">
-        <v>316</v>
+        <v>324</v>
+      </c>
+      <c r="C36" s="70" t="s">
+        <v>325</v>
       </c>
     </row>
     <row r="37" ht="76.5" spans="1:3">
       <c r="A37" s="31"/>
       <c r="B37" s="29" t="s">
-        <v>317</v>
+        <v>326</v>
       </c>
       <c r="C37" s="35" t="s">
-        <v>318</v>
+        <v>327</v>
       </c>
     </row>
     <row r="38" ht="51" spans="1:3">
       <c r="A38" s="31"/>
       <c r="B38" s="29" t="s">
-        <v>319</v>
+        <v>328</v>
       </c>
       <c r="C38" s="35" t="s">
-        <v>320</v>
+        <v>329</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="31" t="s">
-        <v>321</v>
+        <v>330</v>
       </c>
     </row>
   </sheetData>
@@ -15693,12 +15818,12 @@
   <sheetData>
     <row r="1" ht="89.25" spans="4:4">
       <c r="D1" s="1" t="s">
-        <v>322</v>
+        <v>331</v>
       </c>
     </row>
     <row r="2" ht="350" customHeight="1" spans="4:4">
       <c r="D2" s="27" t="s">
-        <v>323</v>
+        <v>332</v>
       </c>
     </row>
   </sheetData>
@@ -15723,7 +15848,7 @@
   <sheetData>
     <row r="1" ht="76.5" spans="3:3">
       <c r="C1" s="27" t="s">
-        <v>324</v>
+        <v>333</v>
       </c>
     </row>
   </sheetData>
@@ -15749,140 +15874,140 @@
   <sheetData>
     <row r="1" ht="127.5" spans="1:3">
       <c r="A1" s="22" t="s">
-        <v>325</v>
-      </c>
-      <c r="B1" s="70" t="s">
-        <v>326</v>
+        <v>334</v>
+      </c>
+      <c r="B1" s="69" t="s">
+        <v>335</v>
       </c>
       <c r="C1" s="23" t="s">
-        <v>327</v>
+        <v>336</v>
       </c>
     </row>
     <row r="2" ht="200.25" customHeight="1" spans="1:2">
       <c r="A2" s="21" t="s">
-        <v>328</v>
+        <v>337</v>
       </c>
       <c r="B2" s="21" t="s">
-        <v>329</v>
+        <v>338</v>
       </c>
     </row>
     <row r="3" ht="102" spans="1:2">
       <c r="A3" s="21" t="s">
-        <v>330</v>
+        <v>339</v>
       </c>
       <c r="B3" s="21" t="s">
-        <v>331</v>
+        <v>340</v>
       </c>
     </row>
     <row r="4" ht="25.5" spans="1:2">
       <c r="A4" s="21" t="s">
-        <v>332</v>
-      </c>
-      <c r="B4" s="70" t="s">
-        <v>333</v>
+        <v>341</v>
+      </c>
+      <c r="B4" s="69" t="s">
+        <v>342</v>
       </c>
     </row>
     <row r="5" ht="25.5" spans="1:2">
       <c r="A5" s="21" t="s">
-        <v>334</v>
+        <v>343</v>
       </c>
       <c r="B5" s="21" t="s">
-        <v>335</v>
+        <v>344</v>
       </c>
     </row>
     <row r="6" ht="38.25" spans="1:1">
       <c r="A6" s="21" t="s">
-        <v>336</v>
+        <v>345</v>
       </c>
     </row>
     <row r="7" ht="38.25" spans="1:2">
       <c r="A7" s="21" t="s">
-        <v>337</v>
+        <v>346</v>
       </c>
       <c r="B7" s="21" t="s">
-        <v>338</v>
+        <v>347</v>
       </c>
     </row>
     <row r="8" ht="114.75" spans="1:2">
       <c r="A8" s="21" t="s">
-        <v>339</v>
+        <v>348</v>
       </c>
       <c r="B8" s="21" t="s">
-        <v>340</v>
+        <v>349</v>
       </c>
     </row>
     <row r="12" ht="51" spans="1:2">
       <c r="A12" s="21" t="s">
-        <v>341</v>
+        <v>350</v>
       </c>
       <c r="B12" s="21" t="s">
-        <v>342</v>
+        <v>351</v>
       </c>
     </row>
     <row r="13" ht="51" spans="1:2">
       <c r="A13" s="21" t="s">
-        <v>343</v>
+        <v>352</v>
       </c>
       <c r="B13" s="21" t="s">
-        <v>344</v>
+        <v>353</v>
       </c>
     </row>
     <row r="14" ht="89.25" spans="1:2">
       <c r="A14" s="21" t="s">
-        <v>345</v>
+        <v>354</v>
       </c>
       <c r="B14" s="21" t="s">
-        <v>346</v>
+        <v>355</v>
       </c>
     </row>
     <row r="15" ht="102" spans="1:2">
       <c r="A15" s="21" t="s">
-        <v>347</v>
+        <v>356</v>
       </c>
       <c r="B15" s="21" t="s">
-        <v>348</v>
+        <v>357</v>
       </c>
     </row>
     <row r="16" spans="1:2">
       <c r="A16" s="21" t="s">
-        <v>349</v>
+        <v>358</v>
       </c>
       <c r="B16" s="21" t="s">
-        <v>350</v>
+        <v>359</v>
       </c>
     </row>
     <row r="17" ht="178.5" spans="1:2">
       <c r="A17" s="21" t="s">
-        <v>351</v>
+        <v>360</v>
       </c>
       <c r="B17" s="21" t="s">
-        <v>352</v>
+        <v>361</v>
       </c>
     </row>
     <row r="18" ht="25.5" spans="1:2">
       <c r="A18" s="21" t="s">
-        <v>353</v>
+        <v>362</v>
       </c>
       <c r="B18" s="21" t="s">
-        <v>354</v>
+        <v>363</v>
       </c>
     </row>
     <row r="19" ht="280.5" spans="1:2">
       <c r="A19" s="21" t="s">
-        <v>355</v>
+        <v>364</v>
       </c>
       <c r="B19" s="21" t="s">
-        <v>356</v>
+        <v>365</v>
       </c>
     </row>
     <row r="20" spans="1:1">
       <c r="A20" s="21" t="s">
-        <v>357</v>
+        <v>366</v>
       </c>
     </row>
     <row r="22" spans="1:1">
       <c r="A22" s="21" t="s">
-        <v>358</v>
+        <v>367</v>
       </c>
     </row>
     <row r="23" spans="2:2">
@@ -15890,145 +16015,145 @@
     </row>
     <row r="25" spans="1:1">
       <c r="A25" s="21" t="s">
-        <v>359</v>
+        <v>368</v>
       </c>
     </row>
     <row r="28" spans="1:1">
       <c r="A28" s="21" t="s">
-        <v>360</v>
+        <v>369</v>
       </c>
     </row>
     <row r="31" spans="1:2">
       <c r="A31" s="21" t="s">
-        <v>361</v>
+        <v>370</v>
       </c>
       <c r="B31" s="21" t="s">
-        <v>362</v>
+        <v>371</v>
       </c>
     </row>
     <row r="33" ht="38.25" spans="1:2">
       <c r="A33" s="21" t="s">
-        <v>363</v>
+        <v>372</v>
       </c>
       <c r="B33" s="21" t="s">
-        <v>364</v>
+        <v>373</v>
       </c>
     </row>
     <row r="34" ht="114.75" spans="1:2">
       <c r="A34" s="21" t="s">
-        <v>365</v>
+        <v>374</v>
       </c>
       <c r="B34" s="21" t="s">
-        <v>366</v>
+        <v>375</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" s="21" t="s">
-        <v>367</v>
+        <v>376</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" s="21" t="s">
-        <v>368</v>
+        <v>377</v>
       </c>
     </row>
     <row r="40" spans="1:1">
       <c r="A40" s="21" t="s">
-        <v>369</v>
+        <v>378</v>
       </c>
     </row>
     <row r="42" spans="1:1">
       <c r="A42" s="21" t="s">
-        <v>370</v>
+        <v>379</v>
       </c>
     </row>
     <row r="44" spans="1:1">
       <c r="A44" s="21" t="s">
-        <v>371</v>
+        <v>380</v>
       </c>
     </row>
     <row r="46" spans="1:1">
       <c r="A46" s="21" t="s">
-        <v>372</v>
+        <v>381</v>
       </c>
     </row>
     <row r="48" spans="1:1">
       <c r="A48" s="21" t="s">
-        <v>373</v>
+        <v>382</v>
       </c>
     </row>
     <row r="50" spans="1:1">
       <c r="A50" s="21" t="s">
-        <v>374</v>
+        <v>383</v>
       </c>
     </row>
     <row r="52" spans="1:1">
       <c r="A52" s="21" t="s">
-        <v>375</v>
+        <v>384</v>
       </c>
     </row>
     <row r="54" spans="1:2">
       <c r="A54" s="25" t="s">
-        <v>376</v>
+        <v>385</v>
       </c>
       <c r="B54" s="21" t="s">
-        <v>377</v>
+        <v>386</v>
       </c>
     </row>
     <row r="55" spans="1:2">
       <c r="A55" s="25"/>
       <c r="B55" s="21" t="s">
-        <v>378</v>
+        <v>387</v>
       </c>
     </row>
     <row r="56" spans="1:2">
       <c r="A56" s="25"/>
       <c r="B56" s="21" t="s">
-        <v>379</v>
+        <v>388</v>
       </c>
     </row>
     <row r="58" ht="25.5" spans="1:2">
       <c r="A58" s="17" t="s">
-        <v>380</v>
+        <v>389</v>
       </c>
       <c r="B58" s="21" t="s">
-        <v>381</v>
+        <v>390</v>
       </c>
     </row>
     <row r="59" spans="1:2">
       <c r="A59" s="17"/>
       <c r="B59" s="26" t="s">
-        <v>382</v>
+        <v>391</v>
       </c>
     </row>
     <row r="60" spans="1:2">
       <c r="A60" s="17"/>
       <c r="B60" s="26" t="s">
-        <v>383</v>
+        <v>392</v>
       </c>
     </row>
     <row r="61" spans="1:2">
       <c r="A61" s="17"/>
       <c r="B61" s="26" t="s">
-        <v>384</v>
+        <v>393</v>
       </c>
     </row>
     <row r="62" spans="1:2">
       <c r="A62" s="17"/>
       <c r="B62" s="26" t="s">
-        <v>385</v>
+        <v>394</v>
       </c>
     </row>
     <row r="63" spans="1:2">
       <c r="A63" s="17"/>
       <c r="B63" s="26" t="s">
-        <v>386</v>
+        <v>395</v>
       </c>
     </row>
     <row r="64" spans="1:2">
       <c r="A64" s="17"/>
       <c r="B64" s="26" t="s">
-        <v>387</v>
+        <v>396</v>
       </c>
     </row>
   </sheetData>
@@ -16061,99 +16186,99 @@
   <sheetData>
     <row r="1" ht="267.75" spans="1:2">
       <c r="A1" s="17" t="s">
-        <v>388</v>
+        <v>397</v>
       </c>
       <c r="B1" s="18" t="s">
-        <v>389</v>
+        <v>398</v>
       </c>
     </row>
     <row r="2" ht="76.5" spans="1:2">
       <c r="A2" s="17" t="s">
-        <v>390</v>
+        <v>399</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>391</v>
+        <v>400</v>
       </c>
     </row>
     <row r="3" ht="38.25" spans="1:2">
       <c r="A3" s="17" t="s">
-        <v>392</v>
+        <v>401</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>393</v>
+        <v>402</v>
       </c>
     </row>
     <row r="4" ht="127.5" spans="1:2">
       <c r="A4" s="17" t="s">
-        <v>394</v>
+        <v>403</v>
       </c>
       <c r="B4" s="18" t="s">
-        <v>395</v>
+        <v>404</v>
       </c>
     </row>
     <row r="5" ht="114.75" spans="2:2">
       <c r="B5" s="18" t="s">
-        <v>396</v>
+        <v>405</v>
       </c>
     </row>
     <row r="6" ht="51" spans="1:2">
       <c r="A6" s="17" t="s">
-        <v>397</v>
+        <v>406</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>398</v>
+        <v>407</v>
       </c>
     </row>
     <row r="7" ht="63.75" spans="1:2">
       <c r="A7" s="17" t="s">
-        <v>399</v>
+        <v>408</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>400</v>
+        <v>409</v>
       </c>
     </row>
     <row r="8" ht="38.25" spans="1:2">
       <c r="A8" s="17" t="s">
-        <v>401</v>
+        <v>410</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>402</v>
+        <v>411</v>
       </c>
     </row>
     <row r="9" ht="38.25" spans="1:2">
       <c r="A9" s="17" t="s">
-        <v>403</v>
+        <v>412</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>404</v>
+        <v>413</v>
       </c>
     </row>
     <row r="10" ht="38.25" spans="1:2">
       <c r="A10" s="17" t="s">
-        <v>405</v>
+        <v>414</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>406</v>
+        <v>415</v>
       </c>
     </row>
     <row r="11" ht="127.5" spans="1:2">
       <c r="A11" s="20" t="s">
-        <v>407</v>
+        <v>416</v>
       </c>
       <c r="B11" s="18" t="s">
-        <v>408</v>
+        <v>417</v>
       </c>
     </row>
     <row r="12" ht="51" spans="1:2">
       <c r="A12" s="20"/>
       <c r="B12" s="18" t="s">
-        <v>409</v>
+        <v>418</v>
       </c>
     </row>
     <row r="13" ht="102" spans="1:2">
       <c r="A13" s="20"/>
       <c r="B13" s="2" t="s">
-        <v>410</v>
+        <v>419</v>
       </c>
     </row>
   </sheetData>

</xml_diff>